<commit_message>
17011401 米白色衬衫  by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="19100" windowHeight="8690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>产品标题</t>
   </si>
@@ -232,23 +232,33 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>衬衫</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>爬爬服</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>手套</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="4">
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
     <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,142 +292,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,194 +317,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -625,251 +326,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -889,19 +354,19 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -910,7 +375,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -926,63 +391,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1004,7 +424,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1042,7 +462,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1080,7 +500,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1118,7 +538,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1156,7 +576,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1194,7 +614,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1232,7 +652,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1270,7 +690,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1308,7 +728,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1346,7 +766,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1384,7 +804,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1422,7 +842,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1464,7 +884,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1502,7 +922,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1540,7 +960,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1578,7 +998,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1620,7 +1040,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1662,7 +1082,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1704,7 +1124,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1746,7 +1166,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1788,7 +1208,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1830,7 +1250,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1872,7 +1292,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1914,7 +1334,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1956,7 +1376,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1998,7 +1418,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2040,7 +1460,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2082,7 +1502,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2120,7 +1540,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2162,7 +1582,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2204,7 +1624,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2246,7 +1666,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2288,7 +1708,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2326,7 +1746,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2364,7 +1784,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2406,7 +1826,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2448,7 +1868,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2490,7 +1910,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2532,7 +1952,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2574,7 +1994,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2616,7 +2036,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2654,7 +2074,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2675,6 +2095,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>74545</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1017485</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1060175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="图片 45" descr="QQ截图20170114224128.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="74545" y="44988232"/>
+          <a:ext cx="942940" cy="944218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2687,7 +2145,7 @@
       <sheetName val="Sheet3"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1">
         <row r="26">
           <cell r="K26">
             <v>100</v>
@@ -2709,8 +2167,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3000,36 +2458,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="8.12727272727273" customWidth="1"/>
-    <col min="6" max="6" width="9.87272727272727" customWidth="1"/>
-    <col min="7" max="7" width="8.25454545454545" customWidth="1"/>
-    <col min="10" max="10" width="11.2545454545455" customWidth="1"/>
-    <col min="11" max="11" width="11.1272727272727" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="8.125" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="8.25" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3085,13 +2541,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>16072601</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -3113,11 +2569,11 @@
       </c>
       <c r="J2" s="10">
         <f t="shared" ref="J2:J14" si="0">(E2+F2+($K$46*H2+$M$46)*$L$46)/(1-G2)/(1-$O$46)/(1-I2)/$N$46</f>
-        <v>16.8747806027782</v>
+        <v>16.874780602778198</v>
       </c>
       <c r="K2" s="11">
         <f t="shared" ref="K2:K14" si="1">(E2+F2+($K$46*H2+$M$46)*$L$46)/(1-G2)/(1-$P$46)/(1-I2)/$N$46</f>
-        <v>18.2644684171246</v>
+        <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2:L14" si="2">E2+F2+($K$46*H2+$M$46)*$L$46</f>
@@ -3129,7 +2585,7 @@
       </c>
       <c r="N2" s="12">
         <f t="shared" ref="N2:N14" si="4">L2/(1-G2)/(1-$P$46)/$N$46</f>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O2" s="12">
         <f>L2/(1-G2)/$N$46</f>
@@ -3137,7 +2593,7 @@
       </c>
       <c r="P2" s="13">
         <f>O2*$N$46-L2</f>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -3146,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>16072701</v>
@@ -3174,27 +2630,27 @@
       </c>
       <c r="J3" s="10">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619209999</v>
       </c>
       <c r="K3" s="11">
         <f t="shared" si="1"/>
-        <v>11.9338715878508</v>
+        <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" si="2"/>
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="12">
         <f t="shared" si="3"/>
-        <v>8.2693947144075</v>
+        <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="12">
         <f t="shared" si="4"/>
-        <v>8.95040369088812</v>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="12">
         <f>L3/(1-G3)/$N$46</f>
-        <v>7.6078431372549</v>
+        <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="13">
         <f>O3*$N$46-L3</f>
@@ -3207,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>16072901</v>
@@ -3235,11 +2691,11 @@
       </c>
       <c r="J4" s="10">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962898</v>
       </c>
       <c r="K4" s="11">
         <f t="shared" si="1"/>
-        <v>20.6953369583127</v>
+        <v>20.695336958312701</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="2"/>
@@ -3247,11 +2703,11 @@
       </c>
       <c r="M4" s="12">
         <f t="shared" si="3"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="12">
         <f t="shared" si="4"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818899</v>
       </c>
       <c r="O4" s="12">
         <f>L4/(1-G4)/$N$46</f>
@@ -3259,7 +2715,7 @@
       </c>
       <c r="P4" s="13">
         <f>O4*$N$46-L4</f>
-        <v>20.9333333333333</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -3268,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>16073001</v>
@@ -3296,11 +2752,11 @@
       </c>
       <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119699</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" si="1"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047199</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="2"/>
@@ -3312,7 +2768,7 @@
       </c>
       <c r="N5" s="12">
         <f t="shared" si="4"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790099</v>
       </c>
       <c r="O5" s="12">
         <f>L5/(1-G5)/$N$46</f>
@@ -3320,7 +2776,7 @@
       </c>
       <c r="P5" s="13">
         <f>O5*$N$46-L5</f>
-        <v>24.2666666666667</v>
+        <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -3329,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>16073002</v>
@@ -3361,7 +2817,7 @@
       </c>
       <c r="K6" s="11">
         <f t="shared" si="1"/>
-        <v>16.6140850803989</v>
+        <v>16.614085080398901</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="2"/>
@@ -3381,7 +2837,7 @@
       </c>
       <c r="P6" s="13">
         <f t="shared" ref="P6:P14" si="6">O6*$N$46-L6</f>
-        <v>16.325</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -3393,7 +2849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>16080301</v>
@@ -3421,11 +2877,11 @@
       </c>
       <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871301</v>
       </c>
       <c r="K7" s="11">
         <f t="shared" si="1"/>
-        <v>18.671551665649</v>
+        <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="2"/>
@@ -3433,7 +2889,7 @@
       </c>
       <c r="M7" s="12">
         <f t="shared" si="3"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="4"/>
@@ -3441,11 +2897,11 @@
       </c>
       <c r="O7" s="12">
         <f t="shared" si="5"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P7" s="13">
         <f t="shared" si="6"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -3454,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -3481,11 +2937,11 @@
       </c>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907897</v>
       </c>
       <c r="K8" s="11">
         <f t="shared" si="1"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159202</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="2"/>
@@ -3493,19 +2949,19 @@
       </c>
       <c r="M8" s="12">
         <f t="shared" si="3"/>
-        <v>17.792918797954</v>
+        <v>17.792918797954002</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="4"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079601</v>
       </c>
       <c r="O8" s="12">
         <f t="shared" si="5"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117599</v>
       </c>
       <c r="P8" s="13">
         <f t="shared" si="6"/>
-        <v>22.2625</v>
+        <v>22.262499999999999</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -3514,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -3541,11 +2997,11 @@
       </c>
       <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695599</v>
       </c>
       <c r="K9" s="11">
         <f t="shared" si="1"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058801</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="2"/>
@@ -3553,11 +3009,11 @@
       </c>
       <c r="M9" s="12">
         <f t="shared" si="3"/>
-        <v>16.8478260869565</v>
+        <v>16.847826086956498</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="4"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647101</v>
       </c>
       <c r="O9" s="12">
         <f t="shared" si="5"/>
@@ -3574,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -3601,11 +3057,11 @@
       </c>
       <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914598</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="1"/>
-        <v>40.467951886637</v>
+        <v>40.467951886637003</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="2"/>
@@ -3613,7 +3069,7 @@
       </c>
       <c r="M10" s="12">
         <f t="shared" si="3"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640201</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="4"/>
@@ -3621,11 +3077,11 @@
       </c>
       <c r="O10" s="12">
         <f t="shared" si="5"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549002</v>
       </c>
       <c r="P10" s="13">
         <f t="shared" si="6"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333302</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -3634,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -3661,15 +3117,15 @@
       </c>
       <c r="J11" s="10">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720503</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="1"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320998</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="2"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="12">
         <f t="shared" si="3"/>
@@ -3677,11 +3133,11 @@
       </c>
       <c r="N11" s="12">
         <f t="shared" si="4"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622799</v>
       </c>
       <c r="O11" s="12">
         <f t="shared" si="5"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529399</v>
       </c>
       <c r="P11" s="13">
         <f t="shared" si="6"/>
@@ -3694,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -3721,7 +3177,7 @@
       </c>
       <c r="J12" s="10">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419602</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="1"/>
@@ -3729,23 +3185,23 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="2"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="3"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506699</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="4"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666001</v>
       </c>
       <c r="O12" s="12">
         <f t="shared" si="5"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666098</v>
       </c>
       <c r="P12" s="13">
         <f t="shared" si="6"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729701</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3754,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -3801,11 +3257,11 @@
       </c>
       <c r="O13" s="12">
         <f t="shared" si="5"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607799</v>
       </c>
       <c r="P13" s="13">
         <f t="shared" si="6"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333302</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -3814,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -3841,27 +3297,27 @@
       </c>
       <c r="J14" s="10">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874698</v>
       </c>
       <c r="K14" s="11">
         <f t="shared" si="1"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193804</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="2"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="12">
         <f t="shared" si="3"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437299</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="4"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096902</v>
       </c>
       <c r="O14" s="12">
         <f t="shared" si="5"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882401</v>
       </c>
       <c r="P14" s="13">
         <f t="shared" si="6"/>
@@ -3874,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -3901,11 +3357,11 @@
       </c>
       <c r="J15" s="10">
         <f>(E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46)/(1-G15)/(1-Sheet1!$O$46)/(1-I15)/Sheet1!$N$46</f>
-        <v>23.0179028132992</v>
+        <v>23.017902813299202</v>
       </c>
       <c r="K15" s="11">
         <f>(E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46)/(1-G15)/(1-Sheet1!$P$46)/(1-I15)/Sheet1!$N$46</f>
-        <v>24.9134948096886</v>
+        <v>24.913494809688601</v>
       </c>
       <c r="L15" s="1">
         <f>E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46</f>
@@ -3913,11 +3369,11 @@
       </c>
       <c r="M15" s="12">
         <f>L15/(1-G15)/(1-Sheet1!$O$46)/Sheet1!$N$46</f>
-        <v>19.5652173913043</v>
+        <v>19.565217391304301</v>
       </c>
       <c r="N15" s="12">
         <f>L15/(1-G15)/(1-Sheet1!$P$46)/Sheet1!$N$46</f>
-        <v>21.1764705882353</v>
+        <v>21.176470588235301</v>
       </c>
       <c r="O15" s="12">
         <f>L15/(1-G15)/Sheet1!$N$46</f>
@@ -3934,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -3965,7 +3421,7 @@
       </c>
       <c r="K16" s="11">
         <f>(E16+F16+(Sheet1!$K$46*H16+Sheet1!$M$46)*Sheet1!$L$46)/(1-G16)/(1-Sheet1!$P$46)/(1-I16)/Sheet1!$N$46</f>
-        <v>12.6297577854671</v>
+        <v>12.629757785467101</v>
       </c>
       <c r="L16" s="1">
         <f>E16+F16+(Sheet1!$K$46*H16+Sheet1!$M$46)*Sheet1!$L$46</f>
@@ -3973,15 +3429,15 @@
       </c>
       <c r="M16" s="12">
         <f>L16/(1-G16)/(1-Sheet1!$O$46)/Sheet1!$N$46</f>
-        <v>8.75159846547314</v>
+        <v>8.7515984654731405</v>
       </c>
       <c r="N16" s="12">
         <f>L16/(1-G16)/(1-Sheet1!$P$46)/Sheet1!$N$46</f>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003491</v>
       </c>
       <c r="O16" s="12">
         <f>L16/(1-G16)/Sheet1!$N$46</f>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352899</v>
       </c>
       <c r="P16" s="13">
         <f>O16*Sheet1!$N$46-L16</f>
@@ -3994,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -4021,11 +3477,11 @@
       </c>
       <c r="J17" s="10">
         <f>(E17+F17+([1]Sheet1!$K$26*H17+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G17)/(1-[1]Sheet1!$O$26)/(1-I17)/[1]Sheet1!$N$26</f>
-        <v>16.1015730055978</v>
+        <v>16.101573005597775</v>
       </c>
       <c r="K17" s="11">
         <f>(E17+F17+([1]Sheet1!$K$26*H17+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G17)/(1-[1]Sheet1!$P$26)/(1-I17)/[1]Sheet1!$N$26</f>
-        <v>17.9958757121387</v>
+        <v>17.995875712138687</v>
       </c>
       <c r="L17" s="1">
         <f>E17+F17+([1]Sheet1!$K$26*H17+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4033,19 +3489,19 @@
       </c>
       <c r="M17" s="12">
         <f>L17/(1-G17)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.6863370547581</v>
+        <v>13.686337054758109</v>
       </c>
       <c r="N17" s="12">
         <f>L17/(1-G17)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>15.2964943553179</v>
+        <v>15.296494355317884</v>
       </c>
       <c r="O17" s="12">
         <f>L17/(1-G17)/[1]Sheet1!$N$26</f>
-        <v>13.0020202020202</v>
+        <v>13.002020202020203</v>
       </c>
       <c r="P17" s="13">
         <f>O17*[1]Sheet1!$N$26-L17</f>
-        <v>21.4533333333333</v>
+        <v>21.453333333333333</v>
       </c>
       <c r="Q17" s="14">
         <v>0.15</v>
@@ -4054,7 +3510,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -4081,11 +3537,11 @@
       </c>
       <c r="J18" s="10">
         <f>(E18+F18+([1]Sheet1!$K$26*H18+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G18)/(1-[1]Sheet1!$O$26)/(1-I18)/[1]Sheet1!$N$26</f>
-        <v>16.1015730055978</v>
+        <v>16.101573005597775</v>
       </c>
       <c r="K18" s="11">
         <f>(E18+F18+([1]Sheet1!$K$26*H18+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G18)/(1-[1]Sheet1!$P$26)/(1-I18)/[1]Sheet1!$N$26</f>
-        <v>17.9958757121387</v>
+        <v>17.995875712138687</v>
       </c>
       <c r="L18" s="1">
         <f>E18+F18+([1]Sheet1!$K$26*H18+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4093,19 +3549,19 @@
       </c>
       <c r="M18" s="12">
         <f>L18/(1-G18)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.6863370547581</v>
+        <v>13.686337054758109</v>
       </c>
       <c r="N18" s="12">
         <f>L18/(1-G18)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>15.2964943553179</v>
+        <v>15.296494355317884</v>
       </c>
       <c r="O18" s="12">
         <f>L18/(1-G18)/[1]Sheet1!$N$26</f>
-        <v>13.0020202020202</v>
+        <v>13.002020202020203</v>
       </c>
       <c r="P18" s="13">
         <f>O18*[1]Sheet1!$N$26-L18</f>
-        <v>21.4533333333333</v>
+        <v>21.453333333333333</v>
       </c>
       <c r="Q18" s="14">
         <v>0.15</v>
@@ -4114,11 +3570,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D19" s="7" t="s">
         <v>42</v>
       </c>
@@ -4139,11 +3597,11 @@
       </c>
       <c r="J19" s="10">
         <f>(E19+F19+([1]Sheet1!$K$26*H19+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G19)/(1-[1]Sheet1!$O$26)/(1-I19)/[1]Sheet1!$N$26</f>
-        <v>16.7400318979266</v>
+        <v>16.740031897926634</v>
       </c>
       <c r="K19" s="11">
         <f>(E19+F19+([1]Sheet1!$K$26*H19+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G19)/(1-[1]Sheet1!$P$26)/(1-I19)/[1]Sheet1!$N$26</f>
-        <v>18.7094474153298</v>
+        <v>18.70944741532977</v>
       </c>
       <c r="L19" s="1">
         <f>E19+F19+([1]Sheet1!$K$26*H19+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4151,19 +3609,19 @@
       </c>
       <c r="M19" s="12">
         <f>L19/(1-G19)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>8.37001594896332</v>
+        <v>8.3700159489633172</v>
       </c>
       <c r="N19" s="12">
         <f>L19/(1-G19)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>9.35472370766488</v>
+        <v>9.3547237076648848</v>
       </c>
       <c r="O19" s="12">
         <f>L19/(1-G19)/[1]Sheet1!$N$26</f>
-        <v>7.95151515151515</v>
+        <v>7.9515151515151512</v>
       </c>
       <c r="P19" s="13">
         <f>O19*[1]Sheet1!$N$26-L19</f>
-        <v>13.12</v>
+        <v>13.119999999999997</v>
       </c>
       <c r="Q19">
         <v>15</v>
@@ -4172,11 +3630,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D20" s="7" t="s">
         <v>43</v>
       </c>
@@ -4197,11 +3657,11 @@
       </c>
       <c r="J20" s="10">
         <f>(E20+F20+([1]Sheet1!$K$26*H20+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G20)/(1-[1]Sheet1!$O$26)/(1-I20)/[1]Sheet1!$N$26</f>
-        <v>18.1240981240981</v>
+        <v>18.124098124098129</v>
       </c>
       <c r="K20" s="11">
         <f>(E20+F20+([1]Sheet1!$K$26*H20+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G20)/(1-[1]Sheet1!$P$26)/(1-I20)/[1]Sheet1!$N$26</f>
-        <v>20.2563449622273</v>
+        <v>20.256344962227317</v>
       </c>
       <c r="L20" s="1">
         <f>E20+F20+([1]Sheet1!$K$26*H20+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4209,25 +3669,25 @@
       </c>
       <c r="M20" s="12">
         <f>L20/(1-G20)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>12.6868686868687</v>
+        <v>12.686868686868687</v>
       </c>
       <c r="N20" s="12">
         <f>L20/(1-G20)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.1794414735591</v>
+        <v>14.179441473559123</v>
       </c>
       <c r="O20" s="12">
         <f>L20/(1-G20)/[1]Sheet1!$N$26</f>
-        <v>12.0525252525253</v>
+        <v>12.052525252525253</v>
       </c>
       <c r="P20" s="13">
         <f>O20*[1]Sheet1!$N$26-L20</f>
-        <v>19.8866666666667</v>
+        <v>19.88666666666667</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -4254,11 +3714,11 @@
       </c>
       <c r="J21" s="10">
         <f>(E21+F21+([1]Sheet1!$K$26*H21+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G21)/(1-[1]Sheet1!$O$26)/(1-I21)/[1]Sheet1!$N$26</f>
-        <v>25.541539799913</v>
+        <v>25.541539799913004</v>
       </c>
       <c r="K21" s="11">
         <f>(E21+F21+([1]Sheet1!$K$26*H21+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G21)/(1-[1]Sheet1!$P$26)/(1-I21)/[1]Sheet1!$N$26</f>
-        <v>28.5464268351969</v>
+        <v>28.54642683519689</v>
       </c>
       <c r="L21" s="1">
         <f>E21+F21+([1]Sheet1!$K$26*H21+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4266,28 +3726,31 @@
       </c>
       <c r="M21" s="12">
         <f>L21/(1-G21)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.0478468899522</v>
+        <v>14.047846889952154</v>
       </c>
       <c r="N21" s="12">
         <f>L21/(1-G21)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>15.7005347593583</v>
+        <v>15.700534759358289</v>
       </c>
       <c r="O21" s="12">
         <f>L21/(1-G21)/[1]Sheet1!$N$26</f>
-        <v>13.3454545454545</v>
+        <v>13.345454545454546</v>
       </c>
       <c r="P21" s="13">
         <f>O21*[1]Sheet1!$N$26-L21</f>
-        <v>22.02</v>
+        <v>22.019999999999996</v>
       </c>
       <c r="R21">
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D22" s="7" t="s">
         <v>45</v>
       </c>
@@ -4308,11 +3771,11 @@
       </c>
       <c r="J22" s="10">
         <f>(E22+F22+([1]Sheet1!$K$26*H22+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G22)/(1-[1]Sheet1!$O$26)/(1-I22)/[1]Sheet1!$N$26</f>
-        <v>25.541539799913</v>
+        <v>25.541539799913004</v>
       </c>
       <c r="K22" s="11">
         <f>(E22+F22+([1]Sheet1!$K$26*H22+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G22)/(1-[1]Sheet1!$P$26)/(1-I22)/[1]Sheet1!$N$26</f>
-        <v>28.5464268351969</v>
+        <v>28.54642683519689</v>
       </c>
       <c r="L22" s="1">
         <f>E22+F22+([1]Sheet1!$K$26*H22+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4320,28 +3783,31 @@
       </c>
       <c r="M22" s="12">
         <f>L22/(1-G22)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.0478468899522</v>
+        <v>14.047846889952154</v>
       </c>
       <c r="N22" s="12">
         <f>L22/(1-G22)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>15.7005347593583</v>
+        <v>15.700534759358289</v>
       </c>
       <c r="O22" s="12">
         <f>L22/(1-G22)/[1]Sheet1!$N$26</f>
-        <v>13.3454545454545</v>
+        <v>13.345454545454546</v>
       </c>
       <c r="P22" s="13">
         <f>O22*[1]Sheet1!$N$26-L22</f>
-        <v>22.02</v>
+        <v>22.019999999999996</v>
       </c>
       <c r="R22">
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
       <c r="D23" s="7" t="s">
         <v>46</v>
       </c>
@@ -4362,11 +3828,11 @@
       </c>
       <c r="J23" s="10">
         <f>(E23+F23+([1]Sheet1!$K$26*H23+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G23)/(1-[1]Sheet1!$O$26)/(1-I23)/[1]Sheet1!$N$26</f>
-        <v>27.0881059397806</v>
+        <v>27.088105939780586</v>
       </c>
       <c r="K23" s="11">
         <f>(E23+F23+([1]Sheet1!$K$26*H23+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G23)/(1-[1]Sheet1!$P$26)/(1-I23)/[1]Sheet1!$N$26</f>
-        <v>30.2749419326959</v>
+        <v>30.274941932695945</v>
       </c>
       <c r="L23" s="1">
         <f>E23+F23+([1]Sheet1!$K$26*H23+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4374,25 +3840,25 @@
       </c>
       <c r="M23" s="12">
         <f>L23/(1-G23)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.8984582668793</v>
+        <v>14.898458266879324</v>
       </c>
       <c r="N23" s="12">
         <f>L23/(1-G23)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>16.6512180629828</v>
+        <v>16.651218062982771</v>
       </c>
       <c r="O23" s="12">
         <f>L23/(1-G23)/[1]Sheet1!$N$26</f>
-        <v>14.1535353535354</v>
+        <v>14.153535353535355</v>
       </c>
       <c r="P23" s="13">
         <f>O23*[1]Sheet1!$N$26-L23</f>
-        <v>23.3533333333333</v>
+        <v>23.353333333333339</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -4419,11 +3885,11 @@
       </c>
       <c r="J24" s="10">
         <f>(E24+F24+([1]Sheet1!$K$26*H24+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G24)/(1-[1]Sheet1!$O$26)/(1-I24)/[1]Sheet1!$N$26</f>
-        <v>25.9281813348799</v>
+        <v>25.928181334879902</v>
       </c>
       <c r="K24" s="11">
         <f>(E24+F24+([1]Sheet1!$K$26*H24+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G24)/(1-[1]Sheet1!$P$26)/(1-I24)/[1]Sheet1!$N$26</f>
-        <v>28.9785556095717</v>
+        <v>28.978555609571654</v>
       </c>
       <c r="L24" s="1">
         <f>E24+F24+([1]Sheet1!$K$26*H24+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4431,25 +3897,25 @@
       </c>
       <c r="M24" s="12">
         <f>L24/(1-G24)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.2604997341839</v>
+        <v>14.260499734183947</v>
       </c>
       <c r="N24" s="12">
         <f>L24/(1-G24)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>15.9382055852644</v>
+        <v>15.938205585264411</v>
       </c>
       <c r="O24" s="12">
         <f>L24/(1-G24)/[1]Sheet1!$N$26</f>
-        <v>13.5474747474747</v>
+        <v>13.54747474747475</v>
       </c>
       <c r="P24" s="13">
         <f>O24*[1]Sheet1!$N$26-L24</f>
-        <v>22.3533333333333</v>
+        <v>22.353333333333339</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -4476,27 +3942,27 @@
       </c>
       <c r="J25" s="10">
         <f>(E25+F25+([1]Sheet1!$K$26*H25+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G25)/(1-[1]Sheet1!$O$26)/(1-I25)/[1]Sheet1!$N$26</f>
-        <v>24.9016480595428</v>
+        <v>24.901648059542801</v>
       </c>
       <c r="K25" s="11">
         <f>(E25+F25+([1]Sheet1!$K$26*H25+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G25)/(1-[1]Sheet1!$P$26)/(1-I25)/[1]Sheet1!$N$26</f>
-        <v>27.8312537136067</v>
+        <v>27.831253713606657</v>
       </c>
       <c r="L25" s="1">
         <f>E25+F25+([1]Sheet1!$K$26*H25+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>70.26</v>
+        <v>70.259999999999991</v>
       </c>
       <c r="M25" s="12">
         <f>L25/(1-G25)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.9409888357257</v>
+        <v>14.940988835725678</v>
       </c>
       <c r="N25" s="12">
         <f>L25/(1-G25)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>16.698752228164</v>
+        <v>16.698752228163993</v>
       </c>
       <c r="O25" s="12">
         <f>L25/(1-G25)/[1]Sheet1!$N$26</f>
-        <v>14.1939393939394</v>
+        <v>14.193939393939393</v>
       </c>
       <c r="P25" s="13">
         <f>O25*[1]Sheet1!$N$26-L25</f>
@@ -4506,7 +3972,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -4537,7 +4003,7 @@
       </c>
       <c r="K26" s="11">
         <f>(E26+F26+([1]Sheet1!$K$26*H26+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G26)/(1-[1]Sheet1!$P$26)/(1-I26)/[1]Sheet1!$N$26</f>
-        <v>24.9792038027332</v>
+        <v>24.979203802733217</v>
       </c>
       <c r="L26" s="1">
         <f>E26+F26+([1]Sheet1!$K$26*H26+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4545,25 +4011,25 @@
       </c>
       <c r="M26" s="12">
         <f>L26/(1-G26)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.4098883572568</v>
+        <v>13.409888357256781</v>
       </c>
       <c r="N26" s="12">
         <f>L26/(1-G26)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.9875222816399</v>
+        <v>14.987522281639929</v>
       </c>
       <c r="O26" s="12">
         <f>L26/(1-G26)/[1]Sheet1!$N$26</f>
-        <v>12.7393939393939</v>
+        <v>12.73939393939394</v>
       </c>
       <c r="P26" s="13">
         <f>O26*[1]Sheet1!$N$26-L26</f>
-        <v>21.02</v>
+        <v>21.019999999999996</v>
       </c>
       <c r="R26">
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -4590,31 +4056,31 @@
       </c>
       <c r="J27" s="10">
         <f>(E27+F27+([1]Sheet1!$K$26*H27+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G27)/(1-[1]Sheet1!$O$26)/(1-I27)/[1]Sheet1!$N$26</f>
-        <v>19.0172400698717</v>
+        <v>19.017240069871651</v>
       </c>
       <c r="K27" s="11">
         <f>(E27+F27+([1]Sheet1!$K$26*H27+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G27)/(1-[1]Sheet1!$P$26)/(1-I27)/[1]Sheet1!$N$26</f>
-        <v>21.254562431033</v>
+        <v>21.254562431033019</v>
       </c>
       <c r="L27" s="1">
         <f>E27+F27+([1]Sheet1!$K$26*H27+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>62.6</v>
+        <v>62.599999999999994</v>
       </c>
       <c r="M27" s="12">
         <f>L27/(1-G27)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.3120680489102</v>
+        <v>13.312068048910154</v>
       </c>
       <c r="N27" s="12">
         <f>L27/(1-G27)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.8781937017231</v>
+        <v>14.878193701723113</v>
       </c>
       <c r="O27" s="12">
         <f>L27/(1-G27)/[1]Sheet1!$N$26</f>
-        <v>12.6464646464646</v>
+        <v>12.646464646464645</v>
       </c>
       <c r="P27" s="13">
         <f>O27*[1]Sheet1!$N$26-L27</f>
-        <v>20.8666666666667</v>
+        <v>20.86666666666666</v>
       </c>
       <c r="Q27">
         <v>40</v>
@@ -4623,7 +4089,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -4650,31 +4116,31 @@
       </c>
       <c r="J28" s="10">
         <f>(E28+F28+([1]Sheet1!$K$26*H28+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G28)/(1-[1]Sheet1!$O$26)/(1-I28)/[1]Sheet1!$N$26</f>
-        <v>28.0160456237011</v>
+        <v>28.016045623701128</v>
       </c>
       <c r="K28" s="11">
         <f>(E28+F28+([1]Sheet1!$K$26*H28+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G28)/(1-[1]Sheet1!$P$26)/(1-I28)/[1]Sheet1!$N$26</f>
-        <v>31.3120509911954</v>
+        <v>31.312050991195381</v>
       </c>
       <c r="L28" s="1">
         <f>E28+F28+([1]Sheet1!$K$26*H28+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>72.46</v>
+        <v>72.460000000000008</v>
       </c>
       <c r="M28" s="12">
         <f>L28/(1-G28)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>15.4088250930356</v>
+        <v>15.408825093035622</v>
       </c>
       <c r="N28" s="12">
         <f>L28/(1-G28)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>17.2216280451575</v>
+        <v>17.221628045157463</v>
       </c>
       <c r="O28" s="12">
         <f>L28/(1-G28)/[1]Sheet1!$N$26</f>
-        <v>14.6383838383838</v>
+        <v>14.638383838383842</v>
       </c>
       <c r="P28" s="13">
         <f>O28*[1]Sheet1!$N$26-L28</f>
-        <v>24.1533333333333</v>
+        <v>24.153333333333336</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -4683,7 +4149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -4710,31 +4176,31 @@
       </c>
       <c r="J29" s="10">
         <f>(E29+F29+([1]Sheet1!$K$26*H29+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G29)/(1-[1]Sheet1!$O$26)/(1-I29)/[1]Sheet1!$N$26</f>
-        <v>21.1121743753323</v>
+        <v>21.112174375332273</v>
       </c>
       <c r="K29" s="11">
         <f>(E29+F29+([1]Sheet1!$K$26*H29+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G29)/(1-[1]Sheet1!$P$26)/(1-I29)/[1]Sheet1!$N$26</f>
-        <v>23.5959595959596</v>
+        <v>23.595959595959602</v>
       </c>
       <c r="L29" s="1">
         <f>E29+F29+([1]Sheet1!$K$26*H29+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>74.46</v>
+        <v>74.460000000000008</v>
       </c>
       <c r="M29" s="12">
         <f>L29/(1-G29)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>15.8341307814992</v>
+        <v>15.834130781499207</v>
       </c>
       <c r="N29" s="12">
         <f>L29/(1-G29)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>17.6969696969697</v>
+        <v>17.696969696969703</v>
       </c>
       <c r="O29" s="12">
         <f>L29/(1-G29)/[1]Sheet1!$N$26</f>
-        <v>15.0424242424242</v>
+        <v>15.042424242424245</v>
       </c>
       <c r="P29" s="13">
         <f>O29*[1]Sheet1!$N$26-L29</f>
-        <v>24.82</v>
+        <v>24.820000000000007</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -4743,7 +4209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -4770,11 +4236,11 @@
       </c>
       <c r="J30" s="10">
         <f>(E30+F30+([1]Sheet1!$K$26*H30+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G30)/(1-[1]Sheet1!$O$26)/(1-I30)/[1]Sheet1!$N$26</f>
-        <v>26.04417379537</v>
+        <v>26.044173795369968</v>
       </c>
       <c r="K30" s="11">
         <f>(E30+F30+([1]Sheet1!$K$26*H30+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G30)/(1-[1]Sheet1!$P$26)/(1-I30)/[1]Sheet1!$N$26</f>
-        <v>29.1081942418841</v>
+        <v>29.108194241884085</v>
       </c>
       <c r="L30" s="1">
         <f>E30+F30+([1]Sheet1!$K$26*H30+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4782,19 +4248,19 @@
       </c>
       <c r="M30" s="12">
         <f>L30/(1-G30)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.3242955874535</v>
+        <v>14.324295587453484</v>
       </c>
       <c r="N30" s="12">
         <f>L30/(1-G30)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>16.0095068330362</v>
+        <v>16.009506833036248</v>
       </c>
       <c r="O30" s="12">
         <f>L30/(1-G30)/[1]Sheet1!$N$26</f>
-        <v>13.6080808080808</v>
+        <v>13.608080808080809</v>
       </c>
       <c r="P30" s="13">
         <f>O30*[1]Sheet1!$N$26-L30</f>
-        <v>22.4533333333333</v>
+        <v>22.453333333333333</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -4803,7 +4269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -4830,11 +4296,11 @@
       </c>
       <c r="J31" s="10">
         <f>(E31+F31+([1]Sheet1!$K$26*H31+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G31)/(1-[1]Sheet1!$O$26)/(1-I31)/[1]Sheet1!$N$26</f>
-        <v>12.5093035619351</v>
+        <v>12.509303561935141</v>
       </c>
       <c r="K31" s="11">
         <f>(E31+F31+([1]Sheet1!$K$26*H31+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G31)/(1-[1]Sheet1!$P$26)/(1-I31)/[1]Sheet1!$N$26</f>
-        <v>13.9809863339275</v>
+        <v>13.980986333927513</v>
       </c>
       <c r="L31" s="1">
         <f>E31+F31+([1]Sheet1!$K$26*H31+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4842,19 +4308,19 @@
       </c>
       <c r="M31" s="12">
         <f>L31/(1-G31)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>10.0074428495481</v>
+        <v>10.007442849548115</v>
       </c>
       <c r="N31" s="12">
         <f>L31/(1-G31)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>11.184789067142</v>
+        <v>11.18478906714201</v>
       </c>
       <c r="O31" s="12">
         <f>L31/(1-G31)/[1]Sheet1!$N$26</f>
-        <v>9.50707070707071</v>
+        <v>9.5070707070707083</v>
       </c>
       <c r="P31" s="13">
         <f>O31*[1]Sheet1!$N$26-L31</f>
-        <v>15.6866666666667</v>
+        <v>15.686666666666667</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -4863,7 +4329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -4890,31 +4356,31 @@
       </c>
       <c r="J32" s="10">
         <f>(E32+F32+([1]Sheet1!$K$26*H32+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G32)/(1-[1]Sheet1!$O$26)/(1-I32)/[1]Sheet1!$N$26</f>
-        <v>17.7068934963672</v>
+        <v>17.706893496367179</v>
       </c>
       <c r="K32" s="11">
         <f>(E32+F32+([1]Sheet1!$K$26*H32+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G32)/(1-[1]Sheet1!$P$26)/(1-I32)/[1]Sheet1!$N$26</f>
-        <v>19.7900574371163</v>
+        <v>19.790057437116261</v>
       </c>
       <c r="L32" s="1">
         <f>E32+F32+([1]Sheet1!$K$26*H32+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>49.96</v>
+        <v>49.959999999999994</v>
       </c>
       <c r="M32" s="12">
         <f>L32/(1-G32)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>10.6241360978203</v>
+        <v>10.624136097820308</v>
       </c>
       <c r="N32" s="12">
         <f>L32/(1-G32)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>11.8740344622698</v>
+        <v>11.874034462269755</v>
       </c>
       <c r="O32" s="12">
         <f>L32/(1-G32)/[1]Sheet1!$N$26</f>
-        <v>10.0929292929293</v>
+        <v>10.092929292929293</v>
       </c>
       <c r="P32" s="13">
         <f>O32*[1]Sheet1!$N$26-L32</f>
-        <v>16.6533333333333</v>
+        <v>16.653333333333336</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -4923,7 +4389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -4950,11 +4416,11 @@
       </c>
       <c r="J33" s="10">
         <f>(E33+F33+([1]Sheet1!$K$26*H33+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G33)/(1-[1]Sheet1!$O$26)/(1-I33)/[1]Sheet1!$N$26</f>
-        <v>25.5802039534097</v>
+        <v>25.58020395340969</v>
       </c>
       <c r="K33" s="11">
         <f>(E33+F33+([1]Sheet1!$K$26*H33+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G33)/(1-[1]Sheet1!$P$26)/(1-I33)/[1]Sheet1!$N$26</f>
-        <v>28.5896397126344</v>
+        <v>28.589639712634362</v>
       </c>
       <c r="L33" s="1">
         <f>E33+F33+([1]Sheet1!$K$26*H33+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -4962,7 +4428,7 @@
       </c>
       <c r="M33" s="12">
         <f>L33/(1-G33)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.0691121743753</v>
+        <v>14.069112174375331</v>
       </c>
       <c r="N33" s="12">
         <f>L33/(1-G33)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
@@ -4970,11 +4436,11 @@
       </c>
       <c r="O33" s="12">
         <f>L33/(1-G33)/[1]Sheet1!$N$26</f>
-        <v>13.3656565656566</v>
+        <v>13.365656565656565</v>
       </c>
       <c r="P33" s="13">
         <f>O33*[1]Sheet1!$N$26-L33</f>
-        <v>22.0533333333333</v>
+        <v>22.053333333333327</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -4983,7 +4449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -5010,11 +4476,11 @@
       </c>
       <c r="J34" s="10">
         <f>(E34+F34+([1]Sheet1!$K$26*H34+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G34)/(1-[1]Sheet1!$O$26)/(1-I34)/[1]Sheet1!$N$26</f>
-        <v>19.6094276094276</v>
+        <v>19.609427609427609</v>
       </c>
       <c r="K34" s="11">
         <f>(E34+F34+([1]Sheet1!$K$26*H34+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G34)/(1-[1]Sheet1!$P$26)/(1-I34)/[1]Sheet1!$N$26</f>
-        <v>21.9164190928897</v>
+        <v>21.916419092889683</v>
       </c>
       <c r="L34" s="1">
         <f>E34+F34+([1]Sheet1!$K$26*H34+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5022,19 +4488,19 @@
       </c>
       <c r="M34" s="12">
         <f>L34/(1-G34)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>14.7070707070707</v>
+        <v>14.707070707070708</v>
       </c>
       <c r="N34" s="12">
         <f>L34/(1-G34)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>16.4373143196673</v>
+        <v>16.437314319667262</v>
       </c>
       <c r="O34" s="12">
         <f>L34/(1-G34)/[1]Sheet1!$N$26</f>
-        <v>13.9717171717172</v>
+        <v>13.97171717171717</v>
       </c>
       <c r="P34" s="13">
         <f>O34*[1]Sheet1!$N$26-L34</f>
-        <v>23.0533333333333</v>
+        <v>23.053333333333327</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -5043,7 +4509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -5070,11 +4536,11 @@
       </c>
       <c r="J35" s="10">
         <f>(E35+F35+([1]Sheet1!$K$26*H35+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G35)/(1-[1]Sheet1!$O$26)/(1-I35)/[1]Sheet1!$N$26</f>
-        <v>15.725677830941</v>
+        <v>15.725677830940988</v>
       </c>
       <c r="K35" s="11">
         <f>(E35+F35+([1]Sheet1!$K$26*H35+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G35)/(1-[1]Sheet1!$P$26)/(1-I35)/[1]Sheet1!$N$26</f>
-        <v>17.5757575757576</v>
+        <v>17.575757575757574</v>
       </c>
       <c r="L35" s="1">
         <f>E35+F35+([1]Sheet1!$K$26*H35+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5082,15 +4548,15 @@
       </c>
       <c r="M35" s="12">
         <f>L35/(1-G35)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>12.5805422647528</v>
+        <v>12.580542264752792</v>
       </c>
       <c r="N35" s="12">
         <f>L35/(1-G35)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.0606060606061</v>
+        <v>14.060606060606061</v>
       </c>
       <c r="O35" s="12">
         <f>L35/(1-G35)/[1]Sheet1!$N$26</f>
-        <v>11.9515151515152</v>
+        <v>11.951515151515151</v>
       </c>
       <c r="P35" s="13">
         <f>O35*[1]Sheet1!$N$26-L35</f>
@@ -5100,7 +4566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -5125,11 +4591,11 @@
       </c>
       <c r="J36" s="10">
         <f>(E36+F36+([1]Sheet1!$K$26*H36+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G36)/(1-[1]Sheet1!$O$26)/(1-I36)/[1]Sheet1!$N$26</f>
-        <v>24.0336378135421</v>
+        <v>24.033637813542118</v>
       </c>
       <c r="K36" s="11">
         <f>(E36+F36+([1]Sheet1!$K$26*H36+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G36)/(1-[1]Sheet1!$P$26)/(1-I36)/[1]Sheet1!$N$26</f>
-        <v>26.8611246151353</v>
+        <v>26.861124615135306</v>
       </c>
       <c r="L36" s="1">
         <f>E36+F36+([1]Sheet1!$K$26*H36+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5137,15 +4603,15 @@
       </c>
       <c r="M36" s="12">
         <f>L36/(1-G36)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.2185007974482</v>
+        <v>13.218500797448167</v>
       </c>
       <c r="N36" s="12">
         <f>L36/(1-G36)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.7736185383244</v>
+        <v>14.773618538324421</v>
       </c>
       <c r="O36" s="12">
         <f>L36/(1-G36)/[1]Sheet1!$N$26</f>
-        <v>12.5575757575758</v>
+        <v>12.557575757575757</v>
       </c>
       <c r="P36" s="13">
         <f>O36*[1]Sheet1!$N$26-L36</f>
@@ -5155,7 +4621,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -5180,11 +4646,11 @@
       </c>
       <c r="J37" s="10">
         <f>(E37+F37+([1]Sheet1!$K$26*H37+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G37)/(1-[1]Sheet1!$O$26)/(1-I37)/[1]Sheet1!$N$26</f>
-        <v>7.1398192450824</v>
+        <v>7.1398192450824025</v>
       </c>
       <c r="K37" s="11">
         <f>(E37+F37+([1]Sheet1!$K$26*H37+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G37)/(1-[1]Sheet1!$P$26)/(1-I37)/[1]Sheet1!$N$26</f>
-        <v>7.97979797979798</v>
+        <v>7.9797979797979801</v>
       </c>
       <c r="L37" s="1">
         <f>E37+F37+([1]Sheet1!$K$26*H37+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5192,25 +4658,25 @@
       </c>
       <c r="M37" s="12">
         <f>L37/(1-G37)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>5.71185539606592</v>
+        <v>5.7118553960659231</v>
       </c>
       <c r="N37" s="12">
         <f>L37/(1-G37)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>6.38383838383838</v>
+        <v>6.3838383838383841</v>
       </c>
       <c r="O37" s="12">
         <f>L37/(1-G37)/[1]Sheet1!$N$26</f>
-        <v>5.42626262626263</v>
+        <v>5.4262626262626261</v>
       </c>
       <c r="P37" s="13">
         <f>O37*[1]Sheet1!$N$26-L37</f>
-        <v>8.95333333333333</v>
+        <v>8.9533333333333331</v>
       </c>
       <c r="Q37">
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -5235,11 +4701,11 @@
       </c>
       <c r="J38" s="10">
         <f>(E38+F38+([1]Sheet1!$K$26*H38+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G38)/(1-[1]Sheet1!$O$26)/(1-I38)/[1]Sheet1!$N$26</f>
-        <v>16.0595427963849</v>
+        <v>16.059542796384903</v>
       </c>
       <c r="K38" s="11">
         <f>(E38+F38+([1]Sheet1!$K$26*H38+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G38)/(1-[1]Sheet1!$P$26)/(1-I38)/[1]Sheet1!$N$26</f>
-        <v>17.9489007724302</v>
+        <v>17.948900772430182</v>
       </c>
       <c r="L38" s="1">
         <f>E38+F38+([1]Sheet1!$K$26*H38+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5247,19 +4713,19 @@
       </c>
       <c r="M38" s="12">
         <f>L38/(1-G38)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>8.02977139819245</v>
+        <v>8.0297713981924517</v>
       </c>
       <c r="N38" s="12">
         <f>L38/(1-G38)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>8.97445038621509</v>
+        <v>8.9744503862150911</v>
       </c>
       <c r="O38" s="12">
         <f>L38/(1-G38)/[1]Sheet1!$N$26</f>
-        <v>7.62828282828283</v>
+        <v>7.6282828282828286</v>
       </c>
       <c r="P38" s="13">
         <f>O38*[1]Sheet1!$N$26-L38</f>
-        <v>12.5866666666667</v>
+        <v>12.586666666666666</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -5268,7 +4734,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -5295,31 +4761,31 @@
       </c>
       <c r="J39" s="10">
         <f>(E39+F39+([1]Sheet1!$K$26*H39+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G39)/(1-[1]Sheet1!$O$26)/(1-I39)/[1]Sheet1!$N$26</f>
-        <v>17.7068934963672</v>
+        <v>17.706893496367179</v>
       </c>
       <c r="K39" s="11">
         <f>(E39+F39+([1]Sheet1!$K$26*H39+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G39)/(1-[1]Sheet1!$P$26)/(1-I39)/[1]Sheet1!$N$26</f>
-        <v>19.7900574371163</v>
+        <v>19.790057437116261</v>
       </c>
       <c r="L39" s="1">
         <f>E39+F39+([1]Sheet1!$K$26*H39+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>49.96</v>
+        <v>49.959999999999994</v>
       </c>
       <c r="M39" s="12">
         <f>L39/(1-G39)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>10.6241360978203</v>
+        <v>10.624136097820308</v>
       </c>
       <c r="N39" s="12">
         <f>L39/(1-G39)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>11.8740344622698</v>
+        <v>11.874034462269755</v>
       </c>
       <c r="O39" s="12">
         <f>L39/(1-G39)/[1]Sheet1!$N$26</f>
-        <v>10.0929292929293</v>
+        <v>10.092929292929293</v>
       </c>
       <c r="P39" s="13">
         <f>O39*[1]Sheet1!$N$26-L39</f>
-        <v>16.6533333333333</v>
+        <v>16.653333333333336</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -5328,7 +4794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -5355,31 +4821,31 @@
       </c>
       <c r="J40" s="10">
         <f>(E40+F40+([1]Sheet1!$K$26*H40+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G40)/(1-[1]Sheet1!$O$26)/(1-I40)/[1]Sheet1!$N$26</f>
-        <v>18.1566864820453</v>
+        <v>18.15668648204533</v>
       </c>
       <c r="K40" s="11">
         <f>(E40+F40+([1]Sheet1!$K$26*H40+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G40)/(1-[1]Sheet1!$P$26)/(1-I40)/[1]Sheet1!$N$26</f>
-        <v>20.2927672446389</v>
+        <v>20.292767244638899</v>
       </c>
       <c r="L40" s="1">
         <f>E40+F40+([1]Sheet1!$K$26*H40+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
-        <v>46.96</v>
+        <v>46.959999999999994</v>
       </c>
       <c r="M40" s="12">
         <f>L40/(1-G40)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>9.98617756512493</v>
+        <v>9.9861775651249332</v>
       </c>
       <c r="N40" s="12">
         <f>L40/(1-G40)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>11.1610219845514</v>
+        <v>11.161021984551397</v>
       </c>
       <c r="O40" s="12">
         <f>L40/(1-G40)/[1]Sheet1!$N$26</f>
-        <v>9.48686868686869</v>
+        <v>9.4868686868686858</v>
       </c>
       <c r="P40" s="13">
         <f>O40*[1]Sheet1!$N$26-L40</f>
-        <v>15.6533333333333</v>
+        <v>15.653333333333329</v>
       </c>
       <c r="Q40">
         <v>20</v>
@@ -5388,7 +4854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -5415,11 +4881,11 @@
       </c>
       <c r="J41" s="10">
         <f>(E41+F41+([1]Sheet1!$K$26*H41+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G41)/(1-[1]Sheet1!$O$26)/(1-I41)/[1]Sheet1!$N$26</f>
-        <v>11.25075314549</v>
+        <v>11.250753145489988</v>
       </c>
       <c r="K41" s="11">
         <f>(E41+F41+([1]Sheet1!$K$26*H41+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G41)/(1-[1]Sheet1!$P$26)/(1-I41)/[1]Sheet1!$N$26</f>
-        <v>12.5743711626065</v>
+        <v>12.574371162606457</v>
       </c>
       <c r="L41" s="1">
         <f>E41+F41+([1]Sheet1!$K$26*H41+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5427,19 +4893,19 @@
       </c>
       <c r="M41" s="12">
         <f>L41/(1-G41)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>8.43806485911749</v>
+        <v>8.4380648591174907</v>
       </c>
       <c r="N41" s="12">
         <f>L41/(1-G41)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>9.43077837195484</v>
+        <v>9.4307783719548421</v>
       </c>
       <c r="O41" s="12">
         <f>L41/(1-G41)/[1]Sheet1!$N$26</f>
-        <v>8.01616161616162</v>
+        <v>8.0161616161616163</v>
       </c>
       <c r="P41" s="13">
         <f>O41*[1]Sheet1!$N$26-L41</f>
-        <v>13.2266666666667</v>
+        <v>13.226666666666667</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -5448,7 +4914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -5475,11 +4941,11 @@
       </c>
       <c r="J42" s="10">
         <f>(E42+F42+([1]Sheet1!$K$26*H42+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G42)/(1-[1]Sheet1!$O$26)/(1-I42)/[1]Sheet1!$N$26</f>
-        <v>24.3816151950123</v>
+        <v>24.381615195012326</v>
       </c>
       <c r="K42" s="11">
         <f>(E42+F42+([1]Sheet1!$K$26*H42+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G42)/(1-[1]Sheet1!$P$26)/(1-I42)/[1]Sheet1!$N$26</f>
-        <v>27.2500405120726</v>
+        <v>27.250040512072598</v>
       </c>
       <c r="L42" s="1">
         <f>E42+F42+([1]Sheet1!$K$26*H42+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
@@ -5487,19 +4953,19 @@
       </c>
       <c r="M42" s="12">
         <f>L42/(1-G42)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
-        <v>13.4098883572568</v>
+        <v>13.409888357256781</v>
       </c>
       <c r="N42" s="12">
         <f>L42/(1-G42)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
-        <v>14.9875222816399</v>
+        <v>14.987522281639929</v>
       </c>
       <c r="O42" s="12">
         <f>L42/(1-G42)/[1]Sheet1!$N$26</f>
-        <v>12.7393939393939</v>
+        <v>12.73939393939394</v>
       </c>
       <c r="P42" s="13">
         <f>O42*[1]Sheet1!$N$26-L42</f>
-        <v>21.02</v>
+        <v>21.019999999999996</v>
       </c>
       <c r="Q42">
         <v>45</v>
@@ -5508,20 +4974,67 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="3:16">
-      <c r="C43" s="1"/>
-      <c r="D43" s="6"/>
-      <c r="G43" s="3"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="13"/>
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B43">
+        <v>17011401</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43">
+        <v>19</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H43">
+        <v>0.2</v>
+      </c>
+      <c r="I43" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J43" s="10">
+        <f>(E43+F43+([1]Sheet1!$K$26*H43+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G43)/(1-[1]Sheet1!$O$26)/(1-I43)/[1]Sheet1!$N$26</f>
+        <v>12.464292043239411</v>
+      </c>
+      <c r="K43" s="11">
+        <f>(E43+F43+([1]Sheet1!$K$26*H43+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G43)/(1-[1]Sheet1!$P$26)/(1-I43)/[1]Sheet1!$N$26</f>
+        <v>13.930679342444044</v>
+      </c>
+      <c r="L43" s="1">
+        <f>E43+F43+([1]Sheet1!$K$26*H43+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
+        <v>43.959999999999994</v>
+      </c>
+      <c r="M43" s="12">
+        <f>L43/(1-G43)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
+        <v>9.348219032429558</v>
+      </c>
+      <c r="N43" s="12">
+        <f>L43/(1-G43)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
+        <v>10.448009506833035</v>
+      </c>
+      <c r="O43" s="12">
+        <f>L43/(1-G43)/[1]Sheet1!$N$26</f>
+        <v>8.8808080808080803</v>
+      </c>
+      <c r="P43" s="13">
+        <f>O43*[1]Sheet1!$N$26-L43</f>
+        <v>14.653333333333336</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>25</v>
+      </c>
     </row>
-    <row r="45" spans="11:16">
+    <row r="45" spans="2:18">
       <c r="K45" s="15" t="s">
         <v>64</v>
       </c>
@@ -5541,7 +5054,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="11:16">
+    <row r="46" spans="2:18">
       <c r="K46" s="16">
         <v>100</v>
       </c>
@@ -5562,94 +5075,86 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27 C41 C42 C2:C16 C29:C30">
-      <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C28 C43 C17:C21 C24:C26 C31:C40">
-      <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
       <formula1>"0,1"</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
+      <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17011501 格子连衣裙 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>产品标题</t>
   </si>
@@ -246,6 +246,10 @@
   </si>
   <si>
     <t>手套</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2125,6 +2129,44 @@
         <a:xfrm>
           <a:off x="74545" y="44988232"/>
           <a:ext cx="942940" cy="944218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33131</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>16568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>997851</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>977350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="图片 47" descr="QQ截图20170115132517.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33131" y="47169459"/>
+          <a:ext cx="964720" cy="960782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2459,11 +2501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2568,31 +2610,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="10">
-        <f t="shared" ref="J2:J14" si="0">(E2+F2+($K$46*H2+$M$46)*$L$46)/(1-G2)/(1-$O$46)/(1-I2)/$N$46</f>
+        <f t="shared" ref="J2:J14" si="0">(E2+F2+($K$47*H2+$M$47)*$L$47)/(1-G2)/(1-$O$47)/(1-I2)/$N$47</f>
         <v>16.874780602778198</v>
       </c>
       <c r="K2" s="11">
-        <f t="shared" ref="K2:K14" si="1">(E2+F2+($K$46*H2+$M$46)*$L$46)/(1-G2)/(1-$P$46)/(1-I2)/$N$46</f>
+        <f t="shared" ref="K2:K14" si="1">(E2+F2+($K$47*H2+$M$47)*$L$47)/(1-G2)/(1-$P$47)/(1-I2)/$N$47</f>
         <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2:L14" si="2">E2+F2+($K$46*H2+$M$46)*$L$46</f>
+        <f t="shared" ref="L2:L14" si="2">E2+F2+($K$47*H2+$M$47)*$L$47</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="12">
-        <f t="shared" ref="M2:M14" si="3">L2/(1-G2)/(1-$O$46)/$N$46</f>
+        <f t="shared" ref="M2:M14" si="3">L2/(1-G2)/(1-$O$47)/$N$47</f>
         <v>14.3435635123615</v>
       </c>
       <c r="N2" s="12">
-        <f t="shared" ref="N2:N14" si="4">L2/(1-G2)/(1-$P$46)/$N$46</f>
+        <f t="shared" ref="N2:N14" si="4">L2/(1-G2)/(1-$P$47)/$N$47</f>
         <v>15.524798154555899</v>
       </c>
       <c r="O2" s="12">
-        <f>L2/(1-G2)/$N$46</f>
+        <f>L2/(1-G2)/$N$47</f>
         <v>13.1960784313726</v>
       </c>
       <c r="P2" s="13">
-        <f>O2*$N$46-L2</f>
+        <f>O2*$N$47-L2</f>
         <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
@@ -2649,11 +2691,11 @@
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="12">
-        <f>L3/(1-G3)/$N$46</f>
+        <f>L3/(1-G3)/$N$47</f>
         <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="13">
-        <f>O3*$N$46-L3</f>
+        <f>O3*$N$47-L3</f>
         <v>12.9333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -2710,11 +2752,11 @@
         <v>14.486735870818899</v>
       </c>
       <c r="O4" s="12">
-        <f>L4/(1-G4)/$N$46</f>
+        <f>L4/(1-G4)/$N$47</f>
         <v>12.3137254901961</v>
       </c>
       <c r="P4" s="13">
-        <f>O4*$N$46-L4</f>
+        <f>O4*$N$47-L4</f>
         <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="1">
@@ -2771,11 +2813,11 @@
         <v>16.793540945790099</v>
       </c>
       <c r="O5" s="12">
-        <f>L5/(1-G5)/$N$46</f>
+        <f>L5/(1-G5)/$N$47</f>
         <v>14.2745098039216</v>
       </c>
       <c r="P5" s="13">
-        <f>O5*$N$46-L5</f>
+        <f>O5*$N$47-L5</f>
         <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="1">
@@ -2832,11 +2874,11 @@
         <v>14.1219723183391</v>
       </c>
       <c r="O6" s="12">
-        <f t="shared" ref="O6:O14" si="5">L6/(1-G6)/$N$46</f>
+        <f t="shared" ref="O6:O14" si="5">L6/(1-G6)/$N$47</f>
         <v>12.0036764705882</v>
       </c>
       <c r="P6" s="13">
-        <f t="shared" ref="P6:P14" si="6">O6*$N$46-L6</f>
+        <f t="shared" ref="P6:P14" si="6">O6*$N$47-L6</f>
         <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="1">
@@ -3356,32 +3398,32 @@
         <v>0.15</v>
       </c>
       <c r="J15" s="10">
-        <f>(E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46)/(1-G15)/(1-Sheet1!$O$46)/(1-I15)/Sheet1!$N$46</f>
-        <v>23.017902813299202</v>
+        <f>(E15+F15+(Sheet1!$K$47*H15+Sheet1!$M$47)*Sheet1!$L$47)/(1-G15)/(1-Sheet1!$O$47)/(1-I15)/Sheet1!$N$47</f>
+        <v>23.017902813299234</v>
       </c>
       <c r="K15" s="11">
-        <f>(E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46)/(1-G15)/(1-Sheet1!$P$46)/(1-I15)/Sheet1!$N$46</f>
-        <v>24.913494809688601</v>
+        <f>(E15+F15+(Sheet1!$K$47*H15+Sheet1!$M$47)*Sheet1!$L$47)/(1-G15)/(1-Sheet1!$P$47)/(1-I15)/Sheet1!$N$47</f>
+        <v>24.913494809688583</v>
       </c>
       <c r="L15" s="1">
-        <f>E15+F15+(Sheet1!$K$46*H15+Sheet1!$M$46)*Sheet1!$L$46</f>
+        <f>E15+F15+(Sheet1!$K$47*H15+Sheet1!$M$47)*Sheet1!$L$47</f>
         <v>91.8</v>
       </c>
       <c r="M15" s="12">
-        <f>L15/(1-G15)/(1-Sheet1!$O$46)/Sheet1!$N$46</f>
-        <v>19.565217391304301</v>
+        <f>L15/(1-G15)/(1-Sheet1!$O$47)/Sheet1!$N$47</f>
+        <v>19.565217391304348</v>
       </c>
       <c r="N15" s="12">
-        <f>L15/(1-G15)/(1-Sheet1!$P$46)/Sheet1!$N$46</f>
-        <v>21.176470588235301</v>
+        <f>L15/(1-G15)/(1-Sheet1!$P$47)/Sheet1!$N$47</f>
+        <v>21.176470588235293</v>
       </c>
       <c r="O15" s="12">
-        <f>L15/(1-G15)/Sheet1!$N$46</f>
+        <f>L15/(1-G15)/Sheet1!$N$47</f>
         <v>18</v>
       </c>
       <c r="P15" s="13">
-        <f>O15*Sheet1!$N$46-L15</f>
-        <v>30.6</v>
+        <f>O15*Sheet1!$N$47-L15</f>
+        <v>30.599999999999994</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -3416,32 +3458,32 @@
         <v>0.25</v>
       </c>
       <c r="J16" s="10">
-        <f>(E16+F16+(Sheet1!$K$46*H16+Sheet1!$M$46)*Sheet1!$L$46)/(1-G16)/(1-Sheet1!$O$46)/(1-I16)/Sheet1!$N$46</f>
-        <v>11.6687979539642</v>
+        <f>(E16+F16+(Sheet1!$K$47*H16+Sheet1!$M$47)*Sheet1!$L$47)/(1-G16)/(1-Sheet1!$O$47)/(1-I16)/Sheet1!$N$47</f>
+        <v>11.668797953964194</v>
       </c>
       <c r="K16" s="11">
-        <f>(E16+F16+(Sheet1!$K$46*H16+Sheet1!$M$46)*Sheet1!$L$46)/(1-G16)/(1-Sheet1!$P$46)/(1-I16)/Sheet1!$N$46</f>
-        <v>12.629757785467101</v>
+        <f>(E16+F16+(Sheet1!$K$47*H16+Sheet1!$M$47)*Sheet1!$L$47)/(1-G16)/(1-Sheet1!$P$47)/(1-I16)/Sheet1!$N$47</f>
+        <v>12.629757785467127</v>
       </c>
       <c r="L16" s="1">
-        <f>E16+F16+(Sheet1!$K$46*H16+Sheet1!$M$46)*Sheet1!$L$46</f>
+        <f>E16+F16+(Sheet1!$K$47*H16+Sheet1!$M$47)*Sheet1!$L$47</f>
         <v>43.8</v>
       </c>
       <c r="M16" s="12">
-        <f>L16/(1-G16)/(1-Sheet1!$O$46)/Sheet1!$N$46</f>
-        <v>8.7515984654731405</v>
+        <f>L16/(1-G16)/(1-Sheet1!$O$47)/Sheet1!$N$47</f>
+        <v>8.751598465473144</v>
       </c>
       <c r="N16" s="12">
-        <f>L16/(1-G16)/(1-Sheet1!$P$46)/Sheet1!$N$46</f>
-        <v>9.4723183391003491</v>
+        <f>L16/(1-G16)/(1-Sheet1!$P$47)/Sheet1!$N$47</f>
+        <v>9.4723183391003456</v>
       </c>
       <c r="O16" s="12">
-        <f>L16/(1-G16)/Sheet1!$N$46</f>
-        <v>8.0514705882352899</v>
+        <f>L16/(1-G16)/Sheet1!$N$47</f>
+        <v>8.0514705882352935</v>
       </c>
       <c r="P16" s="13">
-        <f>O16*Sheet1!$N$46-L16</f>
-        <v>10.95</v>
+        <f>O16*Sheet1!$N$47-L16</f>
+        <v>10.949999999999996</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -5034,43 +5076,103 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="2:18">
-      <c r="K45" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L45" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="M45" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="N45" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="O45" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="P45" s="15" t="s">
-        <v>69</v>
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B44">
+        <v>17011501</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44">
+        <v>26</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H44">
+        <v>0.3</v>
+      </c>
+      <c r="I44" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J44" s="10">
+        <f>(E44+F44+([1]Sheet1!$K$26*H44+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G44)/(1-[1]Sheet1!$O$26)/(1-I44)/[1]Sheet1!$N$26</f>
+        <v>16.774056353003722</v>
+      </c>
+      <c r="K44" s="11">
+        <f>(E44+F44+([1]Sheet1!$K$26*H44+[1]Sheet1!$M$26)*[1]Sheet1!$L$26)/(1-G44)/(1-[1]Sheet1!$P$26)/(1-I44)/[1]Sheet1!$N$26</f>
+        <v>18.747474747474747</v>
+      </c>
+      <c r="L44" s="1">
+        <f>E44+F44+([1]Sheet1!$K$26*H44+[1]Sheet1!$M$26)*[1]Sheet1!$L$26</f>
+        <v>59.16</v>
+      </c>
+      <c r="M44" s="12">
+        <f>L44/(1-G44)/(1-[1]Sheet1!$O$26)/[1]Sheet1!$N$26</f>
+        <v>12.580542264752792</v>
+      </c>
+      <c r="N44" s="12">
+        <f>L44/(1-G44)/(1-[1]Sheet1!$P$26)/[1]Sheet1!$N$26</f>
+        <v>14.060606060606061</v>
+      </c>
+      <c r="O44" s="12">
+        <f>L44/(1-G44)/[1]Sheet1!$N$26</f>
+        <v>11.951515151515151</v>
+      </c>
+      <c r="P44" s="13">
+        <f>O44*[1]Sheet1!$N$26-L44</f>
+        <v>19.72</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="2:18">
-      <c r="K46" s="16">
+      <c r="K46" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L46" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M46" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N46" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O46" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P46" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18">
+      <c r="K47" s="16">
         <v>100</v>
       </c>
-      <c r="L46" s="14">
+      <c r="L47" s="14">
         <v>0.85</v>
       </c>
-      <c r="M46">
+      <c r="M47">
         <v>8</v>
       </c>
-      <c r="N46">
+      <c r="N47">
         <v>6.8</v>
       </c>
-      <c r="O46" s="14">
+      <c r="O47" s="14">
         <v>0.08</v>
       </c>
-      <c r="P46" s="14">
+      <c r="P47" s="14">
         <v>0.15</v>
       </c>
     </row>
@@ -5083,7 +5185,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C44">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5124,10 +5226,11 @@
     <hyperlink ref="D41" r:id="rId34"/>
     <hyperlink ref="D42" r:id="rId35"/>
     <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId37"/>
+  <drawing r:id="rId38"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17011602 外套 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="19100" windowHeight="8690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
   <si>
     <t>产品标题</t>
   </si>
@@ -253,23 +254,23 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/527560763616.html?spm=b26110380.sw311.0.0.p4j2tp</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,142 +304,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,194 +329,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -646,251 +338,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -907,34 +363,34 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -943,67 +399,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1025,7 +436,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1063,7 +474,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1101,7 +512,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1139,7 +550,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1177,7 +588,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1215,7 +626,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1253,7 +664,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1291,7 +702,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1329,7 +740,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1367,7 +778,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1405,7 +816,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1443,7 +854,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1485,7 +896,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1523,7 +934,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1561,7 +972,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1599,7 +1010,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1641,7 +1052,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1683,7 +1094,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1725,7 +1136,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1767,7 +1178,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1809,7 +1220,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1851,7 +1262,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1893,7 +1304,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1935,7 +1346,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1977,7 +1388,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2019,7 +1430,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2061,7 +1472,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2103,7 +1514,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2141,7 +1552,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2183,7 +1594,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2225,7 +1636,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2267,7 +1678,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2309,7 +1720,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2347,7 +1758,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2385,7 +1796,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2427,7 +1838,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2469,7 +1880,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2511,7 +1922,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2553,7 +1964,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2595,7 +2006,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2637,7 +2048,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2675,7 +2086,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2717,7 +2128,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId43" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2755,7 +2166,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId44" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2793,7 +2204,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId45" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2835,7 +2246,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId46" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2873,7 +2284,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId47" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2911,7 +2322,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId48"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2928,6 +2339,44 @@
         <a:ln w="9525">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1013267</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1076740</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="图片 49" descr="QQ截图20170116215948.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="52975565"/>
+          <a:ext cx="1013266" cy="1010479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3219,37 +2668,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="7.26363636363636" customWidth="1"/>
-    <col min="6" max="6" width="8.92727272727273" customWidth="1"/>
-    <col min="7" max="7" width="7.50909090909091" customWidth="1"/>
-    <col min="8" max="8" width="7.34545454545455" customWidth="1"/>
-    <col min="10" max="10" width="11.2545454545455" customWidth="1"/>
-    <col min="11" max="11" width="10.5090909090909" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3305,7 +2752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>16072601</v>
@@ -3332,12 +2779,12 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="10">
-        <f t="shared" ref="J2:J47" si="0">(E2+F2+($K$55*H2+$M$55)*$L$55)/(1-G2)/(1-$O$55)/(1-I2)/$N$55</f>
-        <v>16.8747806027782</v>
+        <f t="shared" ref="J2:J45" si="0">(E2+F2+($K$55*H2+$M$55)*$L$55)/(1-G2)/(1-$O$55)/(1-I2)/$N$55</f>
+        <v>16.874780602778198</v>
       </c>
       <c r="K2" s="11">
         <f t="shared" ref="K2" si="1">(E2+F2+($K$55*H2+$M$55)*$L$55)/(1-G2)/(1-$P$55)/(1-I2)/$N$55</f>
-        <v>18.2644684171246</v>
+        <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2" si="2">E2+F2+($K$55*H2+$M$55)*$L$55</f>
@@ -3349,7 +2796,7 @@
       </c>
       <c r="N2" s="12">
         <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$55)/$N$55</f>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O2" s="12">
         <f>L2/(1-G2)/$N$55</f>
@@ -3357,7 +2804,7 @@
       </c>
       <c r="P2" s="13">
         <f>O2*$N$55-L2</f>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -3366,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>16072701</v>
@@ -3394,27 +2841,27 @@
       </c>
       <c r="J3" s="10">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619209999</v>
       </c>
       <c r="K3" s="11">
         <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$55*H3+$M$55)*$L$55)/(1-G3)/(1-$P$55)/(1-I3)/$N$55</f>
-        <v>11.9338715878508</v>
+        <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L6" si="6">E3+F3+($K$55*H3+$M$55)*$L$55</f>
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="12">
         <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$55)/$N$55</f>
-        <v>8.2693947144075</v>
+        <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="12">
         <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$55)/$N$55</f>
-        <v>8.95040369088812</v>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="12">
         <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$55</f>
-        <v>7.6078431372549</v>
+        <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="13">
         <f t="shared" ref="P3:P6" si="10">O3*$N$55-L3</f>
@@ -3427,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>16072901</v>
@@ -3455,11 +2902,11 @@
       </c>
       <c r="J4" s="10">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962898</v>
       </c>
       <c r="K4" s="11">
         <f t="shared" si="5"/>
-        <v>20.6953369583127</v>
+        <v>20.695336958312701</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="6"/>
@@ -3467,11 +2914,11 @@
       </c>
       <c r="M4" s="12">
         <f t="shared" si="7"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="12">
         <f t="shared" si="8"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818899</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" si="9"/>
@@ -3479,7 +2926,7 @@
       </c>
       <c r="P4" s="13">
         <f t="shared" si="10"/>
-        <v>20.9333333333333</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -3488,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>16073001</v>
@@ -3516,11 +2963,11 @@
       </c>
       <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119699</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" si="5"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047199</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="6"/>
@@ -3532,7 +2979,7 @@
       </c>
       <c r="N5" s="12">
         <f t="shared" si="8"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790099</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="9"/>
@@ -3540,7 +2987,7 @@
       </c>
       <c r="P5" s="13">
         <f t="shared" si="10"/>
-        <v>24.2666666666667</v>
+        <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -3549,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>16073002</v>
@@ -3581,7 +3028,7 @@
       </c>
       <c r="K6" s="11">
         <f t="shared" si="5"/>
-        <v>16.6140850803989</v>
+        <v>16.614085080398901</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="6"/>
@@ -3601,7 +3048,7 @@
       </c>
       <c r="P6" s="13">
         <f t="shared" si="10"/>
-        <v>16.325</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -3613,7 +3060,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>16080301</v>
@@ -3641,31 +3088,31 @@
       </c>
       <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871301</v>
       </c>
       <c r="K7" s="11">
-        <f t="shared" ref="K7:K47" si="11">(E7+F7+($K$55*H7+$M$55)*$L$55)/(1-G7)/(1-$P$55)/(1-I7)/$N$55</f>
-        <v>18.671551665649</v>
+        <f t="shared" ref="K7:K45" si="11">(E7+F7+($K$55*H7+$M$55)*$L$55)/(1-G7)/(1-$P$55)/(1-I7)/$N$55</f>
+        <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L47" si="12">E7+F7+($K$55*H7+$M$55)*$L$55</f>
+        <f t="shared" ref="L7:L45" si="12">E7+F7+($K$55*H7+$M$55)*$L$55</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="12">
-        <f t="shared" ref="M7:M47" si="13">L7/(1-G7)/(1-$O$55)/$N$55</f>
-        <v>14.6632566069906</v>
+        <f t="shared" ref="M7:M45" si="13">L7/(1-G7)/(1-$O$55)/$N$55</f>
+        <v>14.663256606990601</v>
       </c>
       <c r="N7" s="12">
-        <f t="shared" ref="N7:N47" si="14">L7/(1-G7)/(1-$P$55)/$N$55</f>
+        <f t="shared" ref="N7:N45" si="14">L7/(1-G7)/(1-$P$55)/$N$55</f>
         <v>15.8708189158016</v>
       </c>
       <c r="O7" s="12">
-        <f t="shared" ref="O7:O47" si="15">L7/(1-G7)/$N$55</f>
-        <v>13.4901960784314</v>
+        <f t="shared" ref="O7:O45" si="15">L7/(1-G7)/$N$55</f>
+        <v>13.490196078431399</v>
       </c>
       <c r="P7" s="13">
-        <f t="shared" ref="P7:P47" si="16">O7*$N$55-L7</f>
-        <v>22.9333333333333</v>
+        <f t="shared" ref="P7:P45" si="16">O7*$N$55-L7</f>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -3674,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -3701,11 +3148,11 @@
       </c>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907897</v>
       </c>
       <c r="K8" s="11">
         <f t="shared" si="11"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159202</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="12"/>
@@ -3713,19 +3160,19 @@
       </c>
       <c r="M8" s="12">
         <f t="shared" si="13"/>
-        <v>17.792918797954</v>
+        <v>17.792918797954002</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="14"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079601</v>
       </c>
       <c r="O8" s="12">
         <f t="shared" si="15"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117599</v>
       </c>
       <c r="P8" s="13">
         <f t="shared" si="16"/>
-        <v>22.2625</v>
+        <v>22.262499999999999</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -3734,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -3761,11 +3208,11 @@
       </c>
       <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695599</v>
       </c>
       <c r="K9" s="11">
         <f t="shared" si="11"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058801</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="12"/>
@@ -3773,11 +3220,11 @@
       </c>
       <c r="M9" s="12">
         <f t="shared" si="13"/>
-        <v>16.8478260869565</v>
+        <v>16.847826086956498</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="14"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647101</v>
       </c>
       <c r="O9" s="12">
         <f t="shared" si="15"/>
@@ -3794,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -3821,11 +3268,11 @@
       </c>
       <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914598</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="11"/>
-        <v>40.467951886637</v>
+        <v>40.467951886637003</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="12"/>
@@ -3833,7 +3280,7 @@
       </c>
       <c r="M10" s="12">
         <f t="shared" si="13"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640201</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="14"/>
@@ -3841,11 +3288,11 @@
       </c>
       <c r="O10" s="12">
         <f t="shared" si="15"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549002</v>
       </c>
       <c r="P10" s="13">
         <f t="shared" si="16"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333302</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -3854,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -3881,15 +3328,15 @@
       </c>
       <c r="J11" s="10">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720503</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="11"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320998</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="12"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="12">
         <f t="shared" si="13"/>
@@ -3897,11 +3344,11 @@
       </c>
       <c r="N11" s="12">
         <f t="shared" si="14"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622799</v>
       </c>
       <c r="O11" s="12">
         <f t="shared" si="15"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529399</v>
       </c>
       <c r="P11" s="13">
         <f t="shared" si="16"/>
@@ -3914,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -3941,7 +3388,7 @@
       </c>
       <c r="J12" s="10">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419602</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="11"/>
@@ -3949,23 +3396,23 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="12"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="13"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506699</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="14"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666001</v>
       </c>
       <c r="O12" s="12">
         <f t="shared" si="15"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666098</v>
       </c>
       <c r="P12" s="13">
         <f t="shared" si="16"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729701</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -3974,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -4021,11 +3468,11 @@
       </c>
       <c r="O13" s="12">
         <f t="shared" si="15"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607799</v>
       </c>
       <c r="P13" s="13">
         <f t="shared" si="16"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333302</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -4034,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -4061,27 +3508,27 @@
       </c>
       <c r="J14" s="10">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874698</v>
       </c>
       <c r="K14" s="11">
         <f t="shared" si="11"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193804</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="12"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="12">
         <f t="shared" si="13"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437299</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="14"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096902</v>
       </c>
       <c r="O14" s="12">
         <f t="shared" si="15"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882401</v>
       </c>
       <c r="P14" s="13">
         <f t="shared" si="16"/>
@@ -4094,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -4121,11 +3568,11 @@
       </c>
       <c r="J15" s="10">
         <f t="shared" si="0"/>
-        <v>23.0179028132992</v>
+        <v>23.017902813299202</v>
       </c>
       <c r="K15" s="11">
         <f t="shared" si="11"/>
-        <v>24.9134948096886</v>
+        <v>24.913494809688601</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="12"/>
@@ -4133,11 +3580,11 @@
       </c>
       <c r="M15" s="12">
         <f t="shared" si="13"/>
-        <v>19.5652173913043</v>
+        <v>19.565217391304301</v>
       </c>
       <c r="N15" s="12">
         <f t="shared" si="14"/>
-        <v>21.1764705882353</v>
+        <v>21.176470588235301</v>
       </c>
       <c r="O15" s="12">
         <f t="shared" si="15"/>
@@ -4154,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -4185,7 +3632,7 @@
       </c>
       <c r="K16" s="11">
         <f t="shared" si="11"/>
-        <v>12.6297577854671</v>
+        <v>12.629757785467101</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="12"/>
@@ -4193,15 +3640,15 @@
       </c>
       <c r="M16" s="12">
         <f t="shared" si="13"/>
-        <v>8.75159846547314</v>
+        <v>8.7515984654731405</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="14"/>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003491</v>
       </c>
       <c r="O16" s="12">
         <f t="shared" si="15"/>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352899</v>
       </c>
       <c r="P16" s="13">
         <f t="shared" si="16"/>
@@ -4214,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -4241,11 +3688,11 @@
       </c>
       <c r="J17" s="10">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K17" s="11">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="12"/>
@@ -4253,7 +3700,7 @@
       </c>
       <c r="M17" s="12">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="14"/>
@@ -4261,11 +3708,11 @@
       </c>
       <c r="O17" s="12">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P17" s="13">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q17" s="14">
         <v>0.15</v>
@@ -4274,7 +3721,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -4301,11 +3748,11 @@
       </c>
       <c r="J18" s="10">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K18" s="11">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="12"/>
@@ -4313,7 +3760,7 @@
       </c>
       <c r="M18" s="12">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N18" s="12">
         <f t="shared" si="14"/>
@@ -4321,11 +3768,11 @@
       </c>
       <c r="O18" s="12">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P18" s="13">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q18" s="14">
         <v>0.15</v>
@@ -4334,7 +3781,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
@@ -4361,27 +3808,27 @@
       </c>
       <c r="J19" s="10">
         <f t="shared" si="0"/>
-        <v>17.0716112531969</v>
+        <v>17.071611253196899</v>
       </c>
       <c r="K19" s="11">
         <f t="shared" si="11"/>
-        <v>18.477508650519</v>
+        <v>18.477508650518999</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="12"/>
-        <v>40.05</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="12">
         <f t="shared" si="13"/>
-        <v>8.53580562659847</v>
+        <v>8.5358056265984708</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="14"/>
-        <v>9.23875432525952</v>
+        <v>9.2387543252595208</v>
       </c>
       <c r="O19" s="12">
         <f t="shared" si="15"/>
-        <v>7.85294117647059</v>
+        <v>7.8529411764705896</v>
       </c>
       <c r="P19" s="13">
         <f t="shared" si="16"/>
@@ -4394,7 +3841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
@@ -4421,11 +3868,11 @@
       </c>
       <c r="J20" s="10">
         <f t="shared" si="0"/>
-        <v>18.5117525270978</v>
+        <v>18.511752527097801</v>
       </c>
       <c r="K20" s="11">
         <f t="shared" si="11"/>
-        <v>20.0362497940353</v>
+        <v>20.036249794035299</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="12"/>
@@ -4433,11 +3880,11 @@
       </c>
       <c r="M20" s="12">
         <f t="shared" si="13"/>
-        <v>12.9582267689685</v>
+        <v>12.958226768968499</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="14"/>
-        <v>14.0253748558247</v>
+        <v>14.025374855824699</v>
       </c>
       <c r="O20" s="12">
         <f t="shared" si="15"/>
@@ -4445,13 +3892,13 @@
       </c>
       <c r="P20" s="13">
         <f t="shared" si="16"/>
-        <v>20.2666666666667</v>
+        <v>20.266666666666701</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -4482,7 +3929,7 @@
       </c>
       <c r="K21" s="11">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="12"/>
@@ -4494,11 +3941,11 @@
       </c>
       <c r="N21" s="12">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O21" s="12">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P21" s="13">
         <f t="shared" si="16"/>
@@ -4508,7 +3955,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
@@ -4539,7 +3986,7 @@
       </c>
       <c r="K22" s="11">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="12"/>
@@ -4551,11 +3998,11 @@
       </c>
       <c r="N22" s="12">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O22" s="12">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P22" s="13">
         <f t="shared" si="16"/>
@@ -4565,7 +4012,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
@@ -4592,11 +4039,11 @@
       </c>
       <c r="J23" s="10">
         <f t="shared" si="0"/>
-        <v>27.5323568162443</v>
+        <v>27.532356816244299</v>
       </c>
       <c r="K23" s="11">
         <f t="shared" si="11"/>
-        <v>29.799727377582</v>
+        <v>29.799727377581998</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="12"/>
@@ -4604,25 +4051,25 @@
       </c>
       <c r="M23" s="12">
         <f t="shared" si="13"/>
-        <v>15.1427962489344</v>
+        <v>15.142796248934401</v>
       </c>
       <c r="N23" s="12">
         <f t="shared" si="14"/>
-        <v>16.3898500576701</v>
+        <v>16.389850057670099</v>
       </c>
       <c r="O23" s="12">
         <f t="shared" si="15"/>
-        <v>13.9313725490196</v>
+        <v>13.931372549019599</v>
       </c>
       <c r="P23" s="13">
         <f t="shared" si="16"/>
-        <v>23.6833333333333</v>
+        <v>23.683333333333302</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -4649,11 +4096,11 @@
       </c>
       <c r="J24" s="10">
         <f t="shared" si="0"/>
-        <v>26.3698364721383</v>
+        <v>26.369836472138299</v>
       </c>
       <c r="K24" s="11">
         <f t="shared" si="11"/>
-        <v>28.5414700639614</v>
+        <v>28.541470063961398</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="12"/>
@@ -4665,7 +4112,7 @@
       </c>
       <c r="N24" s="12">
         <f t="shared" si="14"/>
-        <v>15.6978085351788</v>
+        <v>15.697808535178799</v>
       </c>
       <c r="O24" s="12">
         <f t="shared" si="15"/>
@@ -4673,13 +4120,13 @@
       </c>
       <c r="P24" s="13">
         <f t="shared" si="16"/>
-        <v>22.6833333333333</v>
+        <v>22.683333333333302</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -4706,7 +4153,7 @@
       </c>
       <c r="J25" s="10">
         <f t="shared" si="0"/>
-        <v>25.4156010230179</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="11">
         <f t="shared" si="11"/>
@@ -4718,11 +4165,11 @@
       </c>
       <c r="M25" s="12">
         <f t="shared" si="13"/>
-        <v>15.2493606138107</v>
+        <v>15.249360613810699</v>
       </c>
       <c r="N25" s="12">
         <f t="shared" si="14"/>
-        <v>16.5051903114187</v>
+        <v>16.505190311418701</v>
       </c>
       <c r="O25" s="12">
         <f t="shared" si="15"/>
@@ -4736,7 +4183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -4763,7 +4210,7 @@
       </c>
       <c r="J26" s="10">
         <f t="shared" si="0"/>
-        <v>22.7514919011083</v>
+        <v>22.751491901108299</v>
       </c>
       <c r="K26" s="11">
         <f t="shared" si="11"/>
@@ -4793,7 +4240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -4820,11 +4267,11 @@
       </c>
       <c r="J27" s="10">
         <f t="shared" si="0"/>
-        <v>19.3338204847156</v>
+        <v>19.333820484715599</v>
       </c>
       <c r="K27" s="11">
         <f t="shared" si="11"/>
-        <v>20.9260174658099</v>
+        <v>20.926017465809899</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="12"/>
@@ -4836,7 +4283,7 @@
       </c>
       <c r="N27" s="12">
         <f t="shared" si="14"/>
-        <v>14.6482122260669</v>
+        <v>14.648212226066899</v>
       </c>
       <c r="O27" s="12">
         <f t="shared" si="15"/>
@@ -4853,7 +4300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -4880,11 +4327,11 @@
       </c>
       <c r="J28" s="10">
         <f t="shared" si="0"/>
-        <v>28.6948771603503</v>
+        <v>28.694877160350298</v>
       </c>
       <c r="K28" s="11">
         <f t="shared" si="11"/>
-        <v>31.0579846912027</v>
+        <v>31.057984691202702</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="12"/>
@@ -4892,7 +4339,7 @@
       </c>
       <c r="M28" s="12">
         <f t="shared" si="13"/>
-        <v>15.7821824381927</v>
+        <v>15.782182438192701</v>
       </c>
       <c r="N28" s="12">
         <f t="shared" si="14"/>
@@ -4900,11 +4347,11 @@
       </c>
       <c r="O28" s="12">
         <f t="shared" si="15"/>
-        <v>14.5196078431373</v>
+        <v>14.519607843137299</v>
       </c>
       <c r="P28" s="13">
         <f t="shared" si="16"/>
-        <v>24.6833333333333</v>
+        <v>24.683333333333302</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -4913,7 +4360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -4952,7 +4399,7 @@
       </c>
       <c r="M29" s="12">
         <f t="shared" si="13"/>
-        <v>16.2084398976982</v>
+        <v>16.208439897698199</v>
       </c>
       <c r="N29" s="12">
         <f t="shared" si="14"/>
@@ -4960,7 +4407,7 @@
       </c>
       <c r="O29" s="12">
         <f t="shared" si="15"/>
-        <v>14.9117647058824</v>
+        <v>14.911764705882399</v>
       </c>
       <c r="P29" s="13">
         <f t="shared" si="16"/>
@@ -4973,7 +4420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -5000,11 +4447,11 @@
       </c>
       <c r="J30" s="10">
         <f t="shared" si="0"/>
-        <v>26.6604665581648</v>
+        <v>26.660466558164799</v>
       </c>
       <c r="K30" s="11">
         <f t="shared" si="11"/>
-        <v>28.8560343923666</v>
+        <v>28.856034392366599</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="12"/>
@@ -5012,7 +4459,7 @@
       </c>
       <c r="M30" s="12">
         <f t="shared" si="13"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N30" s="12">
         <f t="shared" si="14"/>
@@ -5020,11 +4467,11 @@
       </c>
       <c r="O30" s="12">
         <f t="shared" si="15"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P30" s="13">
         <f t="shared" si="16"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -5033,7 +4480,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -5060,11 +4507,11 @@
       </c>
       <c r="J31" s="10">
         <f t="shared" si="0"/>
-        <v>12.8010443307758</v>
+        <v>12.801044330775801</v>
       </c>
       <c r="K31" s="11">
         <f t="shared" si="11"/>
-        <v>13.8552479815456</v>
+        <v>13.855247981545601</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="12"/>
@@ -5080,11 +4527,11 @@
       </c>
       <c r="O31" s="12">
         <f t="shared" si="15"/>
-        <v>9.42156862745098</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="13">
         <f t="shared" si="16"/>
-        <v>16.0166666666667</v>
+        <v>16.016666666666701</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -5093,7 +4540,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -5124,7 +4571,7 @@
       </c>
       <c r="K32" s="11">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="12"/>
@@ -5132,7 +4579,7 @@
       </c>
       <c r="M32" s="12">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N32" s="12">
         <f t="shared" si="14"/>
@@ -5140,11 +4587,11 @@
       </c>
       <c r="O32" s="12">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="13">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -5153,7 +4600,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -5184,7 +4631,7 @@
       </c>
       <c r="K33" s="11">
         <f t="shared" si="11"/>
-        <v>28.2269057355563</v>
+        <v>28.226905735556301</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="12"/>
@@ -5196,7 +4643,7 @@
       </c>
       <c r="N33" s="12">
         <f t="shared" si="14"/>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O33" s="12">
         <f t="shared" si="15"/>
@@ -5204,7 +4651,7 @@
       </c>
       <c r="P33" s="13">
         <f t="shared" si="16"/>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -5213,7 +4660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -5240,11 +4687,11 @@
       </c>
       <c r="J34" s="10">
         <f t="shared" si="0"/>
-        <v>19.9772662688264</v>
+        <v>19.977266268826401</v>
       </c>
       <c r="K34" s="11">
         <f t="shared" si="11"/>
-        <v>21.6224529027297</v>
+        <v>21.622452902729702</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="12"/>
@@ -5264,7 +4711,7 @@
       </c>
       <c r="P34" s="13">
         <f t="shared" si="16"/>
-        <v>23.4333333333333</v>
+        <v>23.433333333333302</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -5273,7 +4720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -5300,11 +4747,11 @@
       </c>
       <c r="J35" s="10">
         <f t="shared" si="0"/>
-        <v>16.0645780051151</v>
+        <v>16.064578005115099</v>
       </c>
       <c r="K35" s="11">
         <f t="shared" si="11"/>
-        <v>17.3875432525952</v>
+        <v>17.387543252595201</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="12"/>
@@ -5312,25 +4759,25 @@
       </c>
       <c r="M35" s="12">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N35" s="12">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O35" s="12">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P35" s="13">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="R35">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -5359,7 +4806,7 @@
       </c>
       <c r="K36" s="11">
         <f t="shared" si="11"/>
-        <v>26.5492293173954</v>
+        <v>26.549229317395401</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="12"/>
@@ -5367,7 +4814,7 @@
       </c>
       <c r="M36" s="12">
         <f t="shared" si="13"/>
-        <v>13.4910485933504</v>
+        <v>13.491048593350399</v>
       </c>
       <c r="N36" s="12">
         <f t="shared" si="14"/>
@@ -5375,7 +4822,7 @@
       </c>
       <c r="O36" s="12">
         <f t="shared" si="15"/>
-        <v>12.4117647058824</v>
+        <v>12.411764705882399</v>
       </c>
       <c r="P36" s="13">
         <f t="shared" si="16"/>
@@ -5385,7 +4832,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -5410,11 +4857,11 @@
       </c>
       <c r="J37" s="10">
         <f t="shared" si="0"/>
-        <v>7.33962063086104</v>
+        <v>7.3396206308610399</v>
       </c>
       <c r="K37" s="11">
         <f t="shared" si="11"/>
-        <v>7.94405997693195</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="12"/>
@@ -5422,15 +4869,15 @@
       </c>
       <c r="M37" s="12">
         <f t="shared" si="13"/>
-        <v>5.87169650468883</v>
+        <v>5.8716965046888303</v>
       </c>
       <c r="N37" s="12">
         <f t="shared" si="14"/>
-        <v>6.35524798154556</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="12">
         <f t="shared" si="15"/>
-        <v>5.40196078431373</v>
+        <v>5.4019607843137303</v>
       </c>
       <c r="P37" s="13">
         <f t="shared" si="16"/>
@@ -5440,7 +4887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -5465,19 +4912,19 @@
       </c>
       <c r="J38" s="10">
         <f t="shared" si="0"/>
-        <v>16.3256606990622</v>
+        <v>16.325660699062201</v>
       </c>
       <c r="K38" s="11">
         <f t="shared" si="11"/>
-        <v>17.6701268742791</v>
+        <v>17.670126874279099</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="12"/>
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="12">
         <f t="shared" si="13"/>
-        <v>8.16283034953112</v>
+        <v>8.1628303495311201</v>
       </c>
       <c r="N38" s="12">
         <f t="shared" si="14"/>
@@ -5485,11 +4932,11 @@
       </c>
       <c r="O38" s="12">
         <f t="shared" si="15"/>
-        <v>7.50980392156863</v>
+        <v>7.5098039215686301</v>
       </c>
       <c r="P38" s="13">
         <f t="shared" si="16"/>
-        <v>12.7666666666667</v>
+        <v>12.766666666666699</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -5498,7 +4945,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -5529,7 +4976,7 @@
       </c>
       <c r="K39" s="11">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="12"/>
@@ -5537,7 +4984,7 @@
       </c>
       <c r="M39" s="12">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N39" s="12">
         <f t="shared" si="14"/>
@@ -5545,11 +4992,11 @@
       </c>
       <c r="O39" s="12">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="13">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -5558,7 +5005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -5618,7 +5065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -5649,7 +5096,7 @@
       </c>
       <c r="K41" s="11">
         <f t="shared" si="11"/>
-        <v>12.4259900038447</v>
+        <v>12.425990003844699</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="12"/>
@@ -5657,19 +5104,19 @@
       </c>
       <c r="M41" s="12">
         <f t="shared" si="13"/>
-        <v>8.61040068201194</v>
+        <v>8.6104006820119405</v>
       </c>
       <c r="N41" s="12">
         <f t="shared" si="14"/>
-        <v>9.31949250288351</v>
+        <v>9.3194925028835094</v>
       </c>
       <c r="O41" s="12">
         <f t="shared" si="15"/>
-        <v>7.92156862745098</v>
+        <v>7.9215686274509798</v>
       </c>
       <c r="P41" s="13">
         <f t="shared" si="16"/>
-        <v>13.4666666666667</v>
+        <v>13.466666666666701</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -5678,7 +5125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -5709,7 +5156,7 @@
       </c>
       <c r="K42" s="11">
         <f t="shared" si="11"/>
-        <v>26.8637936458006</v>
+        <v>26.863793645800602</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="12"/>
@@ -5738,7 +5185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="2:18">
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
       <c r="B43">
         <v>17011401</v>
       </c>
@@ -5769,7 +5216,7 @@
       </c>
       <c r="K43" s="11">
         <f t="shared" si="11"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827801</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="12"/>
@@ -5777,15 +5224,15 @@
       </c>
       <c r="M43" s="12">
         <f t="shared" si="13"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241194</v>
       </c>
       <c r="N43" s="12">
         <f t="shared" si="14"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870801</v>
       </c>
       <c r="O43" s="12">
         <f t="shared" si="15"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254902004</v>
       </c>
       <c r="P43" s="13">
         <f t="shared" si="16"/>
@@ -5798,7 +5245,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" ht="90.75" customHeight="1" spans="2:18">
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
       <c r="B44">
         <v>17011501</v>
       </c>
@@ -5825,11 +5272,11 @@
       </c>
       <c r="J44" s="10">
         <f t="shared" si="0"/>
-        <v>17.1355498721228</v>
+        <v>17.135549872122802</v>
       </c>
       <c r="K44" s="11">
         <f t="shared" si="11"/>
-        <v>18.5467128027682</v>
+        <v>18.546712802768202</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="12"/>
@@ -5837,19 +5284,19 @@
       </c>
       <c r="M44" s="12">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N44" s="12">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O44" s="12">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P44" s="13">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -5858,7 +5305,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="90.75" customHeight="1" spans="2:18">
+    <row r="45" spans="2:18" ht="90.75" customHeight="1">
       <c r="B45">
         <v>17011502</v>
       </c>
@@ -5885,11 +5332,11 @@
       </c>
       <c r="J45" s="10">
         <f t="shared" si="0"/>
-        <v>21.3322483143455</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="11">
         <f t="shared" si="11"/>
-        <v>23.0890217049387</v>
+        <v>23.089021704938698</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="12"/>
@@ -5897,7 +5344,7 @@
       </c>
       <c r="M45" s="12">
         <f t="shared" si="13"/>
-        <v>11.73273657289</v>
+        <v>11.732736572889999</v>
       </c>
       <c r="N45" s="12">
         <f t="shared" si="14"/>
@@ -5905,11 +5352,11 @@
       </c>
       <c r="O45" s="12">
         <f t="shared" si="15"/>
-        <v>10.7941176470588</v>
+        <v>10.794117647058799</v>
       </c>
       <c r="P45" s="13">
         <f t="shared" si="16"/>
-        <v>18.35</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -5918,7 +5365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" ht="90.75" customHeight="1" spans="2:18">
+    <row r="46" spans="2:18" ht="90.75" customHeight="1">
       <c r="B46">
         <v>17011601</v>
       </c>
@@ -5949,7 +5396,7 @@
       </c>
       <c r="K46" s="11">
         <f>(E46+F46+($K$55*H46+$M$55)*$L$55)/(1-G46)/(1-$P$55)/(1-I46)/$N$55</f>
-        <v>22.2501834958582</v>
+        <v>22.250183495858199</v>
       </c>
       <c r="L46" s="1">
         <f>E46+F46+($K$55*H46+$M$55)*$L$55</f>
@@ -5961,15 +5408,15 @@
       </c>
       <c r="N46" s="12">
         <f>L46/(1-G46)/(1-$P$55)/$N$55</f>
-        <v>12.237600922722</v>
+        <v>12.237600922722001</v>
       </c>
       <c r="O46" s="12">
         <f>L46/(1-G46)/$N$55</f>
-        <v>10.4019607843137</v>
+        <v>10.401960784313699</v>
       </c>
       <c r="P46" s="13">
         <f>O46*$N$55-L46</f>
-        <v>17.6833333333333</v>
+        <v>17.683333333333302</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -5978,7 +5425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="90.75" customHeight="1" spans="2:18">
+    <row r="47" spans="2:18" ht="90.75" customHeight="1">
       <c r="B47">
         <v>17011503</v>
       </c>
@@ -6009,7 +5456,7 @@
       </c>
       <c r="K47" s="11">
         <f>(E47+F47+($K$55*H47+$M$55)*$L$55)/(1-G47)/(1-$P$55)/(1-I47)/$N$55</f>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L47" s="1">
         <f>E47+F47+($K$55*H47+$M$55)*$L$55</f>
@@ -6021,15 +5468,15 @@
       </c>
       <c r="N47" s="12">
         <f>L47/(1-G47)/(1-$P$55)/$N$55</f>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O47" s="12">
         <f>L47/(1-G47)/$N$55</f>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P47" s="13">
         <f>O47*$N$55-L47</f>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -6038,7 +5485,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" ht="90.75" customHeight="1" spans="2:18">
+    <row r="48" spans="2:18" ht="90.75" customHeight="1">
       <c r="B48">
         <v>17011504</v>
       </c>
@@ -6069,7 +5516,7 @@
       </c>
       <c r="K48" s="11">
         <f>(E48+F48+($K$55*H48+$M$55)*$L$55)/(1-G48)/(1-$P$55)/(1-I48)/$N$55</f>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L48" s="1">
         <f>E48+F48+($K$55*H48+$M$55)*$L$55</f>
@@ -6081,15 +5528,15 @@
       </c>
       <c r="N48" s="12">
         <f>L48/(1-G48)/(1-$P$55)/$N$55</f>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O48" s="12">
         <f>L48/(1-G48)/$N$55</f>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P48" s="13">
         <f>O48*$N$55-L48</f>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -6098,20 +5545,67 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" ht="90.75" customHeight="1" spans="3:16">
-      <c r="C49" s="1"/>
-      <c r="D49" s="9"/>
-      <c r="G49" s="3"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="13"/>
+    <row r="49" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B49">
+        <v>17011602</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49">
+        <v>28</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H49">
+        <v>0.25</v>
+      </c>
+      <c r="I49" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J49" s="10">
+        <f>(E49+F49+($K$55*H49+$M$55)*$L$55)/(1-G49)/(1-$O$55)/(1-I49)/$N$55</f>
+        <v>16.496163682864449</v>
+      </c>
+      <c r="K49" s="11">
+        <f>(E49+F49+($K$55*H49+$M$55)*$L$55)/(1-G49)/(1-$P$55)/(1-I49)/$N$55</f>
+        <v>17.854671280276815</v>
+      </c>
+      <c r="L49" s="1">
+        <f>E49+F49+($K$55*H49+$M$55)*$L$55</f>
+        <v>58.05</v>
+      </c>
+      <c r="M49" s="12">
+        <f>L49/(1-G49)/(1-$O$55)/$N$55</f>
+        <v>12.372122762148337</v>
+      </c>
+      <c r="N49" s="12">
+        <f>L49/(1-G49)/(1-$P$55)/$N$55</f>
+        <v>13.391003460207612</v>
+      </c>
+      <c r="O49" s="12">
+        <f>L49/(1-G49)/$N$55</f>
+        <v>11.382352941176469</v>
+      </c>
+      <c r="P49" s="13">
+        <f>O49*$N$55-L49</f>
+        <v>19.349999999999994</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>25</v>
+      </c>
     </row>
-    <row r="50" ht="90.75" customHeight="1" spans="3:16">
+    <row r="50" spans="2:18" ht="90.75" customHeight="1">
       <c r="C50" s="1"/>
       <c r="D50" s="9"/>
       <c r="G50" s="3"/>
@@ -6124,7 +5618,7 @@
       <c r="O50" s="12"/>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" ht="90.75" customHeight="1" spans="3:16">
+    <row r="51" spans="2:18" ht="90.75" customHeight="1">
       <c r="C51" s="1"/>
       <c r="D51" s="9"/>
       <c r="G51" s="3"/>
@@ -6137,7 +5631,7 @@
       <c r="O51" s="12"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" ht="90.75" customHeight="1" spans="3:16">
+    <row r="52" spans="2:18" ht="90.75" customHeight="1">
       <c r="C52" s="1"/>
       <c r="D52" s="9"/>
       <c r="G52" s="3"/>
@@ -6150,7 +5644,7 @@
       <c r="O52" s="12"/>
       <c r="P52" s="13"/>
     </row>
-    <row r="54" spans="11:16">
+    <row r="54" spans="2:18">
       <c r="K54" s="15" t="s">
         <v>72</v>
       </c>
@@ -6170,7 +5664,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="11:16">
+    <row r="55" spans="2:18">
       <c r="K55" s="16">
         <v>100</v>
       </c>
@@ -6191,11 +5685,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C46 C49 C50 C51 C52 C2:C45 C47:C48">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C52">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -6203,83 +5698,77 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
-    <hyperlink ref="D43" r:id="rId34" display="https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp"/>
-    <hyperlink ref="D44" r:id="rId35" display="https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW"/>
-    <hyperlink ref="D45" r:id="rId36" display="https://detail.1688.com/offer/525494755952.html?spm=a2615.7691456.0.0.2qsBMx"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://detail.1688.com/offer/525529106954.html?spm=a2615.7691456.0.0.4Tm2o6"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D49" r:id="rId40"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId41"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17011902 海军连衣裙 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="19100" windowHeight="8690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19095" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>产品标题</t>
   </si>
@@ -259,23 +259,22 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/543771981018.html?spm=b26110380.8015204.tkhy006.41.WybDGh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,140 +310,17 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,194 +333,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -652,251 +342,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -913,34 +367,34 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -949,67 +403,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1031,7 +440,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1069,7 +478,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1107,7 +516,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1145,7 +554,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1183,7 +592,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1221,7 +630,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1259,7 +668,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1297,7 +706,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1335,7 +744,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1373,7 +782,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1411,7 +820,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1449,7 +858,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1491,7 +900,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1529,7 +938,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1567,7 +976,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1605,7 +1014,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1647,7 +1056,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1689,7 +1098,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1731,7 +1140,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1773,7 +1182,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1815,7 +1224,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1857,7 +1266,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1899,7 +1308,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1941,7 +1350,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1983,7 +1392,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2025,7 +1434,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2067,7 +1476,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2109,7 +1518,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2147,7 +1556,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2189,7 +1598,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2231,7 +1640,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2273,7 +1682,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2315,7 +1724,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2353,7 +1762,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2391,7 +1800,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2433,7 +1842,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2475,7 +1884,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2517,7 +1926,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2559,7 +1968,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2601,7 +2010,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2643,7 +2052,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2681,7 +2090,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2723,7 +2132,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId43" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2761,7 +2170,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId44" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2799,7 +2208,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId45" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2841,7 +2250,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId46" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2879,7 +2288,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId47" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2917,7 +2326,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId48"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2959,7 +2368,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId49" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2979,15 +2388,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
+      <xdr:colOff>64328</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>41413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>938530</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>996508</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1097032</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2997,15 +2406,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId50"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6350" y="54197250"/>
-          <a:ext cx="932180" cy="1095375"/>
+          <a:off x="64328" y="54102000"/>
+          <a:ext cx="932180" cy="1055619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3014,6 +2423,44 @@
         <a:ln w="9525">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1031288</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>1027042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="图片 51" descr="QQ截图20170117234407.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16565" y="55236717"/>
+          <a:ext cx="1014723" cy="1002195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3305,37 +2752,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="O51" sqref="O51"/>
+      <selection pane="bottomLeft" activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="7.25454545454545" customWidth="1"/>
-    <col min="6" max="6" width="8.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="7.37272727272727" customWidth="1"/>
-    <col min="10" max="10" width="11.2545454545455" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3391,7 +2836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>16072601</v>
@@ -3419,11 +2864,11 @@
       </c>
       <c r="J2" s="10">
         <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$55*H2+$M$55)*$L$55)/(1-G2)/(1-$O$55)/(1-I2)/$N$55</f>
-        <v>16.8747806027782</v>
+        <v>16.874780602778198</v>
       </c>
       <c r="K2" s="11">
         <f t="shared" ref="K2" si="1">(E2+F2+($K$55*H2+$M$55)*$L$55)/(1-G2)/(1-$P$55)/(1-I2)/$N$55</f>
-        <v>18.2644684171246</v>
+        <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2" si="2">E2+F2+($K$55*H2+$M$55)*$L$55</f>
@@ -3435,7 +2880,7 @@
       </c>
       <c r="N2" s="12">
         <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$55)/$N$55</f>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O2" s="12">
         <f>L2/(1-G2)/$N$55</f>
@@ -3443,7 +2888,7 @@
       </c>
       <c r="P2" s="13">
         <f>O2*$N$55-L2</f>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -3452,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>16072701</v>
@@ -3480,27 +2925,27 @@
       </c>
       <c r="J3" s="10">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619209999</v>
       </c>
       <c r="K3" s="11">
         <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$55*H3+$M$55)*$L$55)/(1-G3)/(1-$P$55)/(1-I3)/$N$55</f>
-        <v>11.9338715878508</v>
+        <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L6" si="6">E3+F3+($K$55*H3+$M$55)*$L$55</f>
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="12">
         <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$55)/$N$55</f>
-        <v>8.2693947144075</v>
+        <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="12">
         <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$55)/$N$55</f>
-        <v>8.95040369088812</v>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="12">
         <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$55</f>
-        <v>7.6078431372549</v>
+        <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="13">
         <f t="shared" ref="P3:P6" si="10">O3*$N$55-L3</f>
@@ -3513,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>16072901</v>
@@ -3541,11 +2986,11 @@
       </c>
       <c r="J4" s="10">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962898</v>
       </c>
       <c r="K4" s="11">
         <f t="shared" si="5"/>
-        <v>20.6953369583127</v>
+        <v>20.695336958312701</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="6"/>
@@ -3553,11 +2998,11 @@
       </c>
       <c r="M4" s="12">
         <f t="shared" si="7"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="12">
         <f t="shared" si="8"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818899</v>
       </c>
       <c r="O4" s="12">
         <f t="shared" si="9"/>
@@ -3565,7 +3010,7 @@
       </c>
       <c r="P4" s="13">
         <f t="shared" si="10"/>
-        <v>20.9333333333333</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -3574,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>16073001</v>
@@ -3602,11 +3047,11 @@
       </c>
       <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119699</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" si="5"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047199</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="6"/>
@@ -3618,7 +3063,7 @@
       </c>
       <c r="N5" s="12">
         <f t="shared" si="8"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790099</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="9"/>
@@ -3626,7 +3071,7 @@
       </c>
       <c r="P5" s="13">
         <f t="shared" si="10"/>
-        <v>24.2666666666667</v>
+        <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -3635,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>16073002</v>
@@ -3667,7 +3112,7 @@
       </c>
       <c r="K6" s="11">
         <f t="shared" si="5"/>
-        <v>16.6140850803989</v>
+        <v>16.614085080398901</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="6"/>
@@ -3687,7 +3132,7 @@
       </c>
       <c r="P6" s="13">
         <f t="shared" si="10"/>
-        <v>16.325</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -3699,7 +3144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>16080301</v>
@@ -3727,11 +3172,11 @@
       </c>
       <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871301</v>
       </c>
       <c r="K7" s="11">
         <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$55*H7+$M$55)*$L$55)/(1-G7)/(1-$P$55)/(1-I7)/$N$55</f>
-        <v>18.671551665649</v>
+        <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L49" si="12">E7+F7+($K$55*H7+$M$55)*$L$55</f>
@@ -3739,7 +3184,7 @@
       </c>
       <c r="M7" s="12">
         <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$55)/$N$55</f>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$55)/$N$55</f>
@@ -3747,11 +3192,11 @@
       </c>
       <c r="O7" s="12">
         <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$55</f>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P7" s="13">
         <f t="shared" ref="P7:P49" si="16">O7*$N$55-L7</f>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -3760,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -3787,11 +3232,11 @@
       </c>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907897</v>
       </c>
       <c r="K8" s="11">
         <f t="shared" si="11"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159202</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="12"/>
@@ -3799,19 +3244,19 @@
       </c>
       <c r="M8" s="12">
         <f t="shared" si="13"/>
-        <v>17.792918797954</v>
+        <v>17.792918797954002</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="14"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079601</v>
       </c>
       <c r="O8" s="12">
         <f t="shared" si="15"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117599</v>
       </c>
       <c r="P8" s="13">
         <f t="shared" si="16"/>
-        <v>22.2625</v>
+        <v>22.262499999999999</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -3820,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -3847,11 +3292,11 @@
       </c>
       <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695599</v>
       </c>
       <c r="K9" s="11">
         <f t="shared" si="11"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058801</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="12"/>
@@ -3859,11 +3304,11 @@
       </c>
       <c r="M9" s="12">
         <f t="shared" si="13"/>
-        <v>16.8478260869565</v>
+        <v>16.847826086956498</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="14"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647101</v>
       </c>
       <c r="O9" s="12">
         <f t="shared" si="15"/>
@@ -3880,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -3907,11 +3352,11 @@
       </c>
       <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914598</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="11"/>
-        <v>40.467951886637</v>
+        <v>40.467951886637003</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="12"/>
@@ -3919,7 +3364,7 @@
       </c>
       <c r="M10" s="12">
         <f t="shared" si="13"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640201</v>
       </c>
       <c r="N10" s="12">
         <f t="shared" si="14"/>
@@ -3927,11 +3372,11 @@
       </c>
       <c r="O10" s="12">
         <f t="shared" si="15"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549002</v>
       </c>
       <c r="P10" s="13">
         <f t="shared" si="16"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333302</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -3940,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -3967,15 +3412,15 @@
       </c>
       <c r="J11" s="10">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720503</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="11"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320998</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="12"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="12">
         <f t="shared" si="13"/>
@@ -3983,11 +3428,11 @@
       </c>
       <c r="N11" s="12">
         <f t="shared" si="14"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622799</v>
       </c>
       <c r="O11" s="12">
         <f t="shared" si="15"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529399</v>
       </c>
       <c r="P11" s="13">
         <f t="shared" si="16"/>
@@ -4000,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -4027,7 +3472,7 @@
       </c>
       <c r="J12" s="10">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419602</v>
       </c>
       <c r="K12" s="11">
         <f t="shared" si="11"/>
@@ -4035,23 +3480,23 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="12"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="13"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506699</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="14"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666001</v>
       </c>
       <c r="O12" s="12">
         <f t="shared" si="15"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666098</v>
       </c>
       <c r="P12" s="13">
         <f t="shared" si="16"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729701</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -4060,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -4107,11 +3552,11 @@
       </c>
       <c r="O13" s="12">
         <f t="shared" si="15"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607799</v>
       </c>
       <c r="P13" s="13">
         <f t="shared" si="16"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333302</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -4120,7 +3565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -4147,27 +3592,27 @@
       </c>
       <c r="J14" s="10">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874698</v>
       </c>
       <c r="K14" s="11">
         <f t="shared" si="11"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193804</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="12"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="12">
         <f t="shared" si="13"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437299</v>
       </c>
       <c r="N14" s="12">
         <f t="shared" si="14"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096902</v>
       </c>
       <c r="O14" s="12">
         <f t="shared" si="15"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882401</v>
       </c>
       <c r="P14" s="13">
         <f t="shared" si="16"/>
@@ -4180,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -4207,11 +3652,11 @@
       </c>
       <c r="J15" s="10">
         <f t="shared" si="0"/>
-        <v>23.0179028132992</v>
+        <v>23.017902813299202</v>
       </c>
       <c r="K15" s="11">
         <f t="shared" si="11"/>
-        <v>24.9134948096886</v>
+        <v>24.913494809688601</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="12"/>
@@ -4219,11 +3664,11 @@
       </c>
       <c r="M15" s="12">
         <f t="shared" si="13"/>
-        <v>19.5652173913043</v>
+        <v>19.565217391304301</v>
       </c>
       <c r="N15" s="12">
         <f t="shared" si="14"/>
-        <v>21.1764705882353</v>
+        <v>21.176470588235301</v>
       </c>
       <c r="O15" s="12">
         <f t="shared" si="15"/>
@@ -4240,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -4271,7 +3716,7 @@
       </c>
       <c r="K16" s="11">
         <f t="shared" si="11"/>
-        <v>12.6297577854671</v>
+        <v>12.629757785467101</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="12"/>
@@ -4279,15 +3724,15 @@
       </c>
       <c r="M16" s="12">
         <f t="shared" si="13"/>
-        <v>8.75159846547314</v>
+        <v>8.7515984654731405</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="14"/>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003491</v>
       </c>
       <c r="O16" s="12">
         <f t="shared" si="15"/>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352899</v>
       </c>
       <c r="P16" s="13">
         <f t="shared" si="16"/>
@@ -4300,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -4327,11 +3772,11 @@
       </c>
       <c r="J17" s="10">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K17" s="11">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="12"/>
@@ -4339,7 +3784,7 @@
       </c>
       <c r="M17" s="12">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N17" s="12">
         <f t="shared" si="14"/>
@@ -4347,11 +3792,11 @@
       </c>
       <c r="O17" s="12">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P17" s="13">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q17" s="14">
         <v>0.15</v>
@@ -4360,7 +3805,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -4387,11 +3832,11 @@
       </c>
       <c r="J18" s="10">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K18" s="11">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="12"/>
@@ -4399,7 +3844,7 @@
       </c>
       <c r="M18" s="12">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N18" s="12">
         <f t="shared" si="14"/>
@@ -4407,11 +3852,11 @@
       </c>
       <c r="O18" s="12">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P18" s="13">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q18" s="14">
         <v>0.15</v>
@@ -4420,7 +3865,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
@@ -4447,27 +3892,27 @@
       </c>
       <c r="J19" s="10">
         <f t="shared" si="0"/>
-        <v>17.0716112531969</v>
+        <v>17.071611253196899</v>
       </c>
       <c r="K19" s="11">
         <f t="shared" si="11"/>
-        <v>18.477508650519</v>
+        <v>18.477508650518999</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="12"/>
-        <v>40.05</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="12">
         <f t="shared" si="13"/>
-        <v>8.53580562659847</v>
+        <v>8.5358056265984708</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="14"/>
-        <v>9.23875432525952</v>
+        <v>9.2387543252595208</v>
       </c>
       <c r="O19" s="12">
         <f t="shared" si="15"/>
-        <v>7.85294117647059</v>
+        <v>7.8529411764705896</v>
       </c>
       <c r="P19" s="13">
         <f t="shared" si="16"/>
@@ -4480,7 +3925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
@@ -4507,11 +3952,11 @@
       </c>
       <c r="J20" s="10">
         <f t="shared" si="0"/>
-        <v>18.5117525270978</v>
+        <v>18.511752527097801</v>
       </c>
       <c r="K20" s="11">
         <f t="shared" si="11"/>
-        <v>20.0362497940353</v>
+        <v>20.036249794035299</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="12"/>
@@ -4519,11 +3964,11 @@
       </c>
       <c r="M20" s="12">
         <f t="shared" si="13"/>
-        <v>12.9582267689685</v>
+        <v>12.958226768968499</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="14"/>
-        <v>14.0253748558247</v>
+        <v>14.025374855824699</v>
       </c>
       <c r="O20" s="12">
         <f t="shared" si="15"/>
@@ -4531,13 +3976,13 @@
       </c>
       <c r="P20" s="13">
         <f t="shared" si="16"/>
-        <v>20.2666666666667</v>
+        <v>20.266666666666701</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -4568,7 +4013,7 @@
       </c>
       <c r="K21" s="11">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="12"/>
@@ -4580,11 +4025,11 @@
       </c>
       <c r="N21" s="12">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O21" s="12">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P21" s="13">
         <f t="shared" si="16"/>
@@ -4594,7 +4039,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
@@ -4625,7 +4070,7 @@
       </c>
       <c r="K22" s="11">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="12"/>
@@ -4637,11 +4082,11 @@
       </c>
       <c r="N22" s="12">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O22" s="12">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P22" s="13">
         <f t="shared" si="16"/>
@@ -4651,7 +4096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
@@ -4678,11 +4123,11 @@
       </c>
       <c r="J23" s="10">
         <f t="shared" si="0"/>
-        <v>27.5323568162443</v>
+        <v>27.532356816244299</v>
       </c>
       <c r="K23" s="11">
         <f t="shared" si="11"/>
-        <v>29.799727377582</v>
+        <v>29.799727377581998</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="12"/>
@@ -4690,25 +4135,25 @@
       </c>
       <c r="M23" s="12">
         <f t="shared" si="13"/>
-        <v>15.1427962489344</v>
+        <v>15.142796248934401</v>
       </c>
       <c r="N23" s="12">
         <f t="shared" si="14"/>
-        <v>16.3898500576701</v>
+        <v>16.389850057670099</v>
       </c>
       <c r="O23" s="12">
         <f t="shared" si="15"/>
-        <v>13.9313725490196</v>
+        <v>13.931372549019599</v>
       </c>
       <c r="P23" s="13">
         <f t="shared" si="16"/>
-        <v>23.6833333333333</v>
+        <v>23.683333333333302</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -4735,11 +4180,11 @@
       </c>
       <c r="J24" s="10">
         <f t="shared" si="0"/>
-        <v>26.3698364721383</v>
+        <v>26.369836472138299</v>
       </c>
       <c r="K24" s="11">
         <f t="shared" si="11"/>
-        <v>28.5414700639614</v>
+        <v>28.541470063961398</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="12"/>
@@ -4751,7 +4196,7 @@
       </c>
       <c r="N24" s="12">
         <f t="shared" si="14"/>
-        <v>15.6978085351788</v>
+        <v>15.697808535178799</v>
       </c>
       <c r="O24" s="12">
         <f t="shared" si="15"/>
@@ -4759,13 +4204,13 @@
       </c>
       <c r="P24" s="13">
         <f t="shared" si="16"/>
-        <v>22.6833333333333</v>
+        <v>22.683333333333302</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -4792,7 +4237,7 @@
       </c>
       <c r="J25" s="10">
         <f t="shared" si="0"/>
-        <v>25.4156010230179</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="11">
         <f t="shared" si="11"/>
@@ -4804,11 +4249,11 @@
       </c>
       <c r="M25" s="12">
         <f t="shared" si="13"/>
-        <v>15.2493606138107</v>
+        <v>15.249360613810699</v>
       </c>
       <c r="N25" s="12">
         <f t="shared" si="14"/>
-        <v>16.5051903114187</v>
+        <v>16.505190311418701</v>
       </c>
       <c r="O25" s="12">
         <f t="shared" si="15"/>
@@ -4822,7 +4267,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -4849,7 +4294,7 @@
       </c>
       <c r="J26" s="10">
         <f t="shared" si="0"/>
-        <v>22.7514919011083</v>
+        <v>22.751491901108299</v>
       </c>
       <c r="K26" s="11">
         <f t="shared" si="11"/>
@@ -4879,7 +4324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -4906,11 +4351,11 @@
       </c>
       <c r="J27" s="10">
         <f t="shared" si="0"/>
-        <v>19.3338204847156</v>
+        <v>19.333820484715599</v>
       </c>
       <c r="K27" s="11">
         <f t="shared" si="11"/>
-        <v>20.9260174658099</v>
+        <v>20.926017465809899</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="12"/>
@@ -4922,7 +4367,7 @@
       </c>
       <c r="N27" s="12">
         <f t="shared" si="14"/>
-        <v>14.6482122260669</v>
+        <v>14.648212226066899</v>
       </c>
       <c r="O27" s="12">
         <f t="shared" si="15"/>
@@ -4939,7 +4384,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -4966,11 +4411,11 @@
       </c>
       <c r="J28" s="10">
         <f t="shared" si="0"/>
-        <v>28.6948771603503</v>
+        <v>28.694877160350298</v>
       </c>
       <c r="K28" s="11">
         <f t="shared" si="11"/>
-        <v>31.0579846912027</v>
+        <v>31.057984691202702</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="12"/>
@@ -4978,7 +4423,7 @@
       </c>
       <c r="M28" s="12">
         <f t="shared" si="13"/>
-        <v>15.7821824381927</v>
+        <v>15.782182438192701</v>
       </c>
       <c r="N28" s="12">
         <f t="shared" si="14"/>
@@ -4986,11 +4431,11 @@
       </c>
       <c r="O28" s="12">
         <f t="shared" si="15"/>
-        <v>14.5196078431373</v>
+        <v>14.519607843137299</v>
       </c>
       <c r="P28" s="13">
         <f t="shared" si="16"/>
-        <v>24.6833333333333</v>
+        <v>24.683333333333302</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -4999,7 +4444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -5038,7 +4483,7 @@
       </c>
       <c r="M29" s="12">
         <f t="shared" si="13"/>
-        <v>16.2084398976982</v>
+        <v>16.208439897698199</v>
       </c>
       <c r="N29" s="12">
         <f t="shared" si="14"/>
@@ -5046,7 +4491,7 @@
       </c>
       <c r="O29" s="12">
         <f t="shared" si="15"/>
-        <v>14.9117647058824</v>
+        <v>14.911764705882399</v>
       </c>
       <c r="P29" s="13">
         <f t="shared" si="16"/>
@@ -5059,7 +4504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -5086,11 +4531,11 @@
       </c>
       <c r="J30" s="10">
         <f t="shared" si="0"/>
-        <v>26.6604665581648</v>
+        <v>26.660466558164799</v>
       </c>
       <c r="K30" s="11">
         <f t="shared" si="11"/>
-        <v>28.8560343923666</v>
+        <v>28.856034392366599</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="12"/>
@@ -5098,7 +4543,7 @@
       </c>
       <c r="M30" s="12">
         <f t="shared" si="13"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N30" s="12">
         <f t="shared" si="14"/>
@@ -5106,11 +4551,11 @@
       </c>
       <c r="O30" s="12">
         <f t="shared" si="15"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P30" s="13">
         <f t="shared" si="16"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -5119,7 +4564,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -5146,11 +4591,11 @@
       </c>
       <c r="J31" s="10">
         <f t="shared" si="0"/>
-        <v>12.8010443307758</v>
+        <v>12.801044330775801</v>
       </c>
       <c r="K31" s="11">
         <f t="shared" si="11"/>
-        <v>13.8552479815456</v>
+        <v>13.855247981545601</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="12"/>
@@ -5166,11 +4611,11 @@
       </c>
       <c r="O31" s="12">
         <f t="shared" si="15"/>
-        <v>9.42156862745098</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="13">
         <f t="shared" si="16"/>
-        <v>16.0166666666667</v>
+        <v>16.016666666666701</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -5179,7 +4624,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -5210,7 +4655,7 @@
       </c>
       <c r="K32" s="11">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="12"/>
@@ -5218,7 +4663,7 @@
       </c>
       <c r="M32" s="12">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N32" s="12">
         <f t="shared" si="14"/>
@@ -5226,11 +4671,11 @@
       </c>
       <c r="O32" s="12">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="13">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -5239,7 +4684,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -5270,7 +4715,7 @@
       </c>
       <c r="K33" s="11">
         <f t="shared" si="11"/>
-        <v>28.2269057355563</v>
+        <v>28.226905735556301</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="12"/>
@@ -5282,7 +4727,7 @@
       </c>
       <c r="N33" s="12">
         <f t="shared" si="14"/>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O33" s="12">
         <f t="shared" si="15"/>
@@ -5290,7 +4735,7 @@
       </c>
       <c r="P33" s="13">
         <f t="shared" si="16"/>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -5299,7 +4744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -5326,11 +4771,11 @@
       </c>
       <c r="J34" s="10">
         <f t="shared" si="0"/>
-        <v>19.9772662688264</v>
+        <v>19.977266268826401</v>
       </c>
       <c r="K34" s="11">
         <f t="shared" si="11"/>
-        <v>21.6224529027297</v>
+        <v>21.622452902729702</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="12"/>
@@ -5350,7 +4795,7 @@
       </c>
       <c r="P34" s="13">
         <f t="shared" si="16"/>
-        <v>23.4333333333333</v>
+        <v>23.433333333333302</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -5359,7 +4804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -5386,11 +4831,11 @@
       </c>
       <c r="J35" s="10">
         <f t="shared" si="0"/>
-        <v>16.0645780051151</v>
+        <v>16.064578005115099</v>
       </c>
       <c r="K35" s="11">
         <f t="shared" si="11"/>
-        <v>17.3875432525952</v>
+        <v>17.387543252595201</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="12"/>
@@ -5398,25 +4843,25 @@
       </c>
       <c r="M35" s="12">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N35" s="12">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O35" s="12">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P35" s="13">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="R35">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -5445,7 +4890,7 @@
       </c>
       <c r="K36" s="11">
         <f t="shared" si="11"/>
-        <v>26.5492293173954</v>
+        <v>26.549229317395401</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="12"/>
@@ -5453,7 +4898,7 @@
       </c>
       <c r="M36" s="12">
         <f t="shared" si="13"/>
-        <v>13.4910485933504</v>
+        <v>13.491048593350399</v>
       </c>
       <c r="N36" s="12">
         <f t="shared" si="14"/>
@@ -5461,7 +4906,7 @@
       </c>
       <c r="O36" s="12">
         <f t="shared" si="15"/>
-        <v>12.4117647058824</v>
+        <v>12.411764705882399</v>
       </c>
       <c r="P36" s="13">
         <f t="shared" si="16"/>
@@ -5471,7 +4916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -5496,11 +4941,11 @@
       </c>
       <c r="J37" s="10">
         <f t="shared" si="0"/>
-        <v>7.33962063086104</v>
+        <v>7.3396206308610399</v>
       </c>
       <c r="K37" s="11">
         <f t="shared" si="11"/>
-        <v>7.94405997693195</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="12"/>
@@ -5508,15 +4953,15 @@
       </c>
       <c r="M37" s="12">
         <f t="shared" si="13"/>
-        <v>5.87169650468883</v>
+        <v>5.8716965046888303</v>
       </c>
       <c r="N37" s="12">
         <f t="shared" si="14"/>
-        <v>6.35524798154556</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="12">
         <f t="shared" si="15"/>
-        <v>5.40196078431373</v>
+        <v>5.4019607843137303</v>
       </c>
       <c r="P37" s="13">
         <f t="shared" si="16"/>
@@ -5526,7 +4971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -5551,19 +4996,19 @@
       </c>
       <c r="J38" s="10">
         <f t="shared" si="0"/>
-        <v>16.3256606990622</v>
+        <v>16.325660699062201</v>
       </c>
       <c r="K38" s="11">
         <f t="shared" si="11"/>
-        <v>17.6701268742791</v>
+        <v>17.670126874279099</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="12"/>
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="12">
         <f t="shared" si="13"/>
-        <v>8.16283034953112</v>
+        <v>8.1628303495311201</v>
       </c>
       <c r="N38" s="12">
         <f t="shared" si="14"/>
@@ -5571,11 +5016,11 @@
       </c>
       <c r="O38" s="12">
         <f t="shared" si="15"/>
-        <v>7.50980392156863</v>
+        <v>7.5098039215686301</v>
       </c>
       <c r="P38" s="13">
         <f t="shared" si="16"/>
-        <v>12.7666666666667</v>
+        <v>12.766666666666699</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -5584,7 +5029,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -5615,7 +5060,7 @@
       </c>
       <c r="K39" s="11">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="12"/>
@@ -5623,7 +5068,7 @@
       </c>
       <c r="M39" s="12">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N39" s="12">
         <f t="shared" si="14"/>
@@ -5631,11 +5076,11 @@
       </c>
       <c r="O39" s="12">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="13">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -5644,7 +5089,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -5704,7 +5149,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -5735,7 +5180,7 @@
       </c>
       <c r="K41" s="11">
         <f t="shared" si="11"/>
-        <v>12.4259900038447</v>
+        <v>12.425990003844699</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="12"/>
@@ -5743,19 +5188,19 @@
       </c>
       <c r="M41" s="12">
         <f t="shared" si="13"/>
-        <v>8.61040068201194</v>
+        <v>8.6104006820119405</v>
       </c>
       <c r="N41" s="12">
         <f t="shared" si="14"/>
-        <v>9.31949250288351</v>
+        <v>9.3194925028835094</v>
       </c>
       <c r="O41" s="12">
         <f t="shared" si="15"/>
-        <v>7.92156862745098</v>
+        <v>7.9215686274509798</v>
       </c>
       <c r="P41" s="13">
         <f t="shared" si="16"/>
-        <v>13.4666666666667</v>
+        <v>13.466666666666701</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -5764,7 +5209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -5795,7 +5240,7 @@
       </c>
       <c r="K42" s="11">
         <f t="shared" si="11"/>
-        <v>26.8637936458006</v>
+        <v>26.863793645800602</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="12"/>
@@ -5824,7 +5269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="2:18">
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
       <c r="B43">
         <v>17011401</v>
       </c>
@@ -5855,7 +5300,7 @@
       </c>
       <c r="K43" s="11">
         <f t="shared" si="11"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827801</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="12"/>
@@ -5863,15 +5308,15 @@
       </c>
       <c r="M43" s="12">
         <f t="shared" si="13"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241194</v>
       </c>
       <c r="N43" s="12">
         <f t="shared" si="14"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870801</v>
       </c>
       <c r="O43" s="12">
         <f t="shared" si="15"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254902004</v>
       </c>
       <c r="P43" s="13">
         <f t="shared" si="16"/>
@@ -5884,7 +5329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" ht="90.75" customHeight="1" spans="2:18">
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
       <c r="B44">
         <v>17011501</v>
       </c>
@@ -5911,11 +5356,11 @@
       </c>
       <c r="J44" s="10">
         <f t="shared" si="0"/>
-        <v>17.1355498721228</v>
+        <v>17.135549872122802</v>
       </c>
       <c r="K44" s="11">
         <f t="shared" si="11"/>
-        <v>18.5467128027682</v>
+        <v>18.546712802768202</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="12"/>
@@ -5923,19 +5368,19 @@
       </c>
       <c r="M44" s="12">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N44" s="12">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O44" s="12">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P44" s="13">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -5944,7 +5389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="90.75" customHeight="1" spans="2:18">
+    <row r="45" spans="2:18" ht="90.75" customHeight="1">
       <c r="B45">
         <v>17011502</v>
       </c>
@@ -5971,11 +5416,11 @@
       </c>
       <c r="J45" s="10">
         <f t="shared" si="0"/>
-        <v>21.3322483143455</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="11">
         <f t="shared" si="11"/>
-        <v>23.0890217049387</v>
+        <v>23.089021704938698</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="12"/>
@@ -5983,7 +5428,7 @@
       </c>
       <c r="M45" s="12">
         <f t="shared" si="13"/>
-        <v>11.73273657289</v>
+        <v>11.732736572889999</v>
       </c>
       <c r="N45" s="12">
         <f t="shared" si="14"/>
@@ -5991,11 +5436,11 @@
       </c>
       <c r="O45" s="12">
         <f t="shared" si="15"/>
-        <v>10.7941176470588</v>
+        <v>10.794117647058799</v>
       </c>
       <c r="P45" s="13">
         <f t="shared" si="16"/>
-        <v>18.35</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -6004,7 +5449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" ht="90.75" customHeight="1" spans="2:18">
+    <row r="46" spans="2:18" ht="90.75" customHeight="1">
       <c r="B46">
         <v>17011601</v>
       </c>
@@ -6035,7 +5480,7 @@
       </c>
       <c r="K46" s="11">
         <f t="shared" si="11"/>
-        <v>22.2501834958582</v>
+        <v>22.250183495858199</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="12"/>
@@ -6047,15 +5492,15 @@
       </c>
       <c r="N46" s="12">
         <f t="shared" si="14"/>
-        <v>12.237600922722</v>
+        <v>12.237600922722001</v>
       </c>
       <c r="O46" s="12">
         <f t="shared" si="15"/>
-        <v>10.4019607843137</v>
+        <v>10.401960784313699</v>
       </c>
       <c r="P46" s="13">
         <f t="shared" si="16"/>
-        <v>17.6833333333333</v>
+        <v>17.683333333333302</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -6064,7 +5509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="90.75" customHeight="1" spans="2:18">
+    <row r="47" spans="2:18" ht="90.75" customHeight="1">
       <c r="B47">
         <v>17011503</v>
       </c>
@@ -6095,7 +5540,7 @@
       </c>
       <c r="K47" s="11">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="12"/>
@@ -6107,15 +5552,15 @@
       </c>
       <c r="N47" s="12">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O47" s="12">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P47" s="13">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -6124,7 +5569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" ht="90.75" customHeight="1" spans="2:18">
+    <row r="48" spans="2:18" ht="90.75" customHeight="1">
       <c r="B48">
         <v>17011504</v>
       </c>
@@ -6155,7 +5600,7 @@
       </c>
       <c r="K48" s="11">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="12"/>
@@ -6167,15 +5612,15 @@
       </c>
       <c r="N48" s="12">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O48" s="12">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P48" s="13">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -6184,7 +5629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" ht="90.75" customHeight="1" spans="2:18">
+    <row r="49" spans="2:18" ht="90.75" customHeight="1">
       <c r="B49">
         <v>17011602</v>
       </c>
@@ -6211,11 +5656,11 @@
       </c>
       <c r="J49" s="10">
         <f t="shared" si="0"/>
-        <v>16.4961636828644</v>
+        <v>16.496163682864399</v>
       </c>
       <c r="K49" s="11">
         <f t="shared" si="11"/>
-        <v>17.8546712802768</v>
+        <v>17.854671280276801</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="12"/>
@@ -6223,7 +5668,7 @@
       </c>
       <c r="M49" s="12">
         <f t="shared" si="13"/>
-        <v>12.3721227621483</v>
+        <v>12.372122762148299</v>
       </c>
       <c r="N49" s="12">
         <f t="shared" si="14"/>
@@ -6231,11 +5676,11 @@
       </c>
       <c r="O49" s="12">
         <f t="shared" si="15"/>
-        <v>11.3823529411765</v>
+        <v>11.382352941176499</v>
       </c>
       <c r="P49" s="13">
         <f t="shared" si="16"/>
-        <v>19.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -6244,7 +5689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" ht="90.75" customHeight="1" spans="2:18">
+    <row r="50" spans="2:18" ht="90.75" customHeight="1">
       <c r="B50">
         <v>17011901</v>
       </c>
@@ -6271,11 +5716,11 @@
       </c>
       <c r="J50" s="10">
         <f>(E50+F50+($K$55*H50+$M$55)*$L$55)/(1-G50)/(1-$O$55)/(1-I50)/$N$55</f>
-        <v>17.0696737192901</v>
+        <v>17.069673719290101</v>
       </c>
       <c r="K50" s="11">
         <f>(E50+F50+($K$55*H50+$M$55)*$L$55)/(1-G50)/(1-$P$55)/(1-I50)/$N$55</f>
-        <v>18.4754115549963</v>
+        <v>18.475411554996299</v>
       </c>
       <c r="L50" s="1">
         <f>E50+F50+($K$55*H50+$M$55)*$L$55</f>
@@ -6283,7 +5728,7 @@
       </c>
       <c r="M50" s="12">
         <f>L50/(1-G50)/(1-$O$55)/$N$55</f>
-        <v>9.38832054560955</v>
+        <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="12">
         <f>L50/(1-G50)/(1-$P$55)/$N$55</f>
@@ -6291,7 +5736,7 @@
       </c>
       <c r="O50" s="12">
         <f>L50/(1-G50)/$N$55</f>
-        <v>8.63725490196078</v>
+        <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="13">
         <f>O50*$N$55-L50</f>
@@ -6304,20 +5749,67 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" ht="90.75" customHeight="1" spans="3:16">
-      <c r="C51" s="1"/>
-      <c r="D51" s="9"/>
-      <c r="G51" s="3"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="13"/>
+    <row r="51" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B51">
+        <v>17011902</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51">
+        <v>28</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H51">
+        <v>0.2</v>
+      </c>
+      <c r="I51" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J51" s="10">
+        <f>(E51+F51+($K$55*H51+$M$55)*$L$55)/(1-G51)/(1-$O$55)/(1-I51)/$N$55</f>
+        <v>14.332907075873825</v>
+      </c>
+      <c r="K51" s="11">
+        <f>(E51+F51+($K$55*H51+$M$55)*$L$55)/(1-G51)/(1-$P$55)/(1-I51)/$N$55</f>
+        <v>15.51326412918108</v>
+      </c>
+      <c r="L51" s="1">
+        <f>E51+F51+($K$55*H51+$M$55)*$L$55</f>
+        <v>53.8</v>
+      </c>
+      <c r="M51" s="12">
+        <f>L51/(1-G51)/(1-$O$55)/$N$55</f>
+        <v>10.749680306905368</v>
+      </c>
+      <c r="N51" s="12">
+        <f>L51/(1-G51)/(1-$P$55)/$N$55</f>
+        <v>11.634948096885811</v>
+      </c>
+      <c r="O51" s="12">
+        <f>L51/(1-G51)/$N$55</f>
+        <v>9.8897058823529385</v>
+      </c>
+      <c r="P51" s="13">
+        <f>O51*$N$55-L51</f>
+        <v>13.449999999999989</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>25</v>
+      </c>
     </row>
-    <row r="52" ht="90.75" customHeight="1" spans="3:16">
+    <row r="52" spans="2:18" ht="90.75" customHeight="1">
       <c r="C52" s="1"/>
       <c r="D52" s="9"/>
       <c r="G52" s="3"/>
@@ -6330,7 +5822,7 @@
       <c r="O52" s="12"/>
       <c r="P52" s="13"/>
     </row>
-    <row r="54" spans="11:16">
+    <row r="54" spans="2:18">
       <c r="K54" s="15" t="s">
         <v>74</v>
       </c>
@@ -6350,7 +5842,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="11:16">
+    <row r="55" spans="2:18">
       <c r="K55" s="16">
         <v>100</v>
       </c>
@@ -6371,6 +5863,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
@@ -6383,85 +5876,78 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
-    <hyperlink ref="D43" r:id="rId34" display="https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp"/>
-    <hyperlink ref="D44" r:id="rId35" display="https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW"/>
-    <hyperlink ref="D45" r:id="rId36" display="https://detail.1688.com/offer/525494755952.html?spm=a2615.7691456.0.0.2qsBMx"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://detail.1688.com/offer/525529106954.html?spm=a2615.7691456.0.0.4Tm2o6"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://detail.1688.com/offer/527560763616.html?spm=b26110380.sw311.0.0.p4j2tp"/>
-    <hyperlink ref="D50" r:id="rId39" display="https://detail.1688.com/offer/542627436877.html?spm=b26110380.sw1037004.0.0.aYzCim&amp;sk=consign"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D49" r:id="rId40"/>
+    <hyperlink ref="D50" r:id="rId41"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17020601 牛仔 外套 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
   <si>
     <t>产品标题</t>
   </si>
@@ -270,6 +270,14 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>外套</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/45277079052.html?spm=a261y.7663282.0.0.8G3JEy&amp;sk=consign</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2600,6 +2608,44 @@
         <a:xfrm>
           <a:off x="24850" y="57539285"/>
           <a:ext cx="1013228" cy="1010478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1075197</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>1118152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="图片 53" descr="QQ截图20170206230345.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="58707129"/>
+          <a:ext cx="1075197" cy="1076740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2899,8 +2945,8 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6073,17 +6119,64 @@
       </c>
     </row>
     <row r="54" spans="2:18" ht="90.75" customHeight="1">
-      <c r="C54" s="1"/>
-      <c r="D54" s="9"/>
-      <c r="G54" s="3"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="13"/>
+      <c r="B54">
+        <v>17020601</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54">
+        <v>37</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H54">
+        <v>0.3</v>
+      </c>
+      <c r="I54" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="J54" s="10">
+        <f>(E54+F54+($K$58*H54+$M$58)*$L$58)/(1-G54)/(1-$O$58)/(1-I54)/$N$58</f>
+        <v>20.35189075630252</v>
+      </c>
+      <c r="K54" s="11">
+        <f>(E54+F54+($K$58*H54+$M$58)*$L$58)/(1-G54)/(1-$P$58)/(1-I54)/$N$58</f>
+        <v>22.027928818586258</v>
+      </c>
+      <c r="L54" s="1">
+        <f>E54+F54+($K$58*H54+$M$58)*$L$58</f>
+        <v>71.3</v>
+      </c>
+      <c r="M54" s="12">
+        <f>L54/(1-G54)/(1-$O$58)/$N$58</f>
+        <v>14.246323529411763</v>
+      </c>
+      <c r="N54" s="12">
+        <f>L54/(1-G54)/(1-$P$58)/$N$58</f>
+        <v>15.41955017301038</v>
+      </c>
+      <c r="O54" s="12">
+        <f>L54/(1-G54)/$N$58</f>
+        <v>13.106617647058822</v>
+      </c>
+      <c r="P54" s="13">
+        <f>O54*$N$58-L54</f>
+        <v>17.824999999999989</v>
+      </c>
+      <c r="Q54">
+        <v>30</v>
+      </c>
+      <c r="R54">
+        <v>25</v>
+      </c>
     </row>
     <row r="55" spans="2:18" ht="90.75" customHeight="1">
       <c r="C55" s="1"/>
@@ -6196,10 +6289,11 @@
     <hyperlink ref="D52" r:id="rId42"/>
     <hyperlink ref="D51" r:id="rId43"/>
     <hyperlink ref="D53" r:id="rId44"/>
+    <hyperlink ref="D54" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
 
@@ -6227,6 +6321,6 @@
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17020701 绣花礼服 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>产品标题</t>
   </si>
@@ -2646,6 +2646,44 @@
         <a:xfrm>
           <a:off x="0" y="58707129"/>
           <a:ext cx="1075197" cy="1076740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1018761</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>1118151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="图片 55" descr="QQ截图20170207224810.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="59817000"/>
+          <a:ext cx="1018761" cy="1118151"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2945,8 +2983,8 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5904,31 +5942,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="10">
-        <f>(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$O$58)/(1-I50)/$N$58</f>
+        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$O$58)/(1-I50)/$N$58</f>
         <v>17.069673719290101</v>
       </c>
       <c r="K50" s="11">
-        <f>(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$P$58)/(1-I50)/$N$58</f>
+        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$P$58)/(1-I50)/$N$58</f>
         <v>18.475411554996299</v>
       </c>
       <c r="L50" s="1">
-        <f>E50+F50+($K$58*H50+$M$58)*$L$58</f>
+        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$58*H50+$M$58)*$L$58</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="12">
-        <f>L50/(1-G50)/(1-$O$58)/$N$58</f>
+        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$58)/$N$58</f>
         <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="12">
-        <f>L50/(1-G50)/(1-$P$58)/$N$58</f>
+        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$58)/$N$58</f>
         <v>10.161476355248</v>
       </c>
       <c r="O50" s="12">
-        <f>L50/(1-G50)/$N$58</f>
+        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$58</f>
         <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="13">
-        <f>O50*$N$58-L50</f>
+        <f t="shared" ref="P50:P55" si="23">O50*$N$58-L50</f>
         <v>14.6833333333333</v>
       </c>
       <c r="Q50">
@@ -5964,31 +6002,31 @@
         <v>0.25</v>
       </c>
       <c r="J51" s="10">
-        <f>(E51+F51+($K$58*H51+$M$58)*$L$58)/(1-G51)/(1-$O$58)/(1-I51)/$N$58</f>
+        <f t="shared" si="17"/>
         <v>14.332907075873825</v>
       </c>
       <c r="K51" s="11">
-        <f>(E51+F51+($K$58*H51+$M$58)*$L$58)/(1-G51)/(1-$P$58)/(1-I51)/$N$58</f>
+        <f t="shared" si="18"/>
         <v>15.51326412918108</v>
       </c>
       <c r="L51" s="1">
-        <f>E51+F51+($K$58*H51+$M$58)*$L$58</f>
+        <f t="shared" si="19"/>
         <v>53.8</v>
       </c>
       <c r="M51" s="12">
-        <f>L51/(1-G51)/(1-$O$58)/$N$58</f>
+        <f t="shared" si="20"/>
         <v>10.749680306905368</v>
       </c>
       <c r="N51" s="12">
-        <f>L51/(1-G51)/(1-$P$58)/$N$58</f>
+        <f t="shared" si="21"/>
         <v>11.634948096885811</v>
       </c>
       <c r="O51" s="12">
-        <f>L51/(1-G51)/$N$58</f>
+        <f t="shared" si="22"/>
         <v>9.8897058823529385</v>
       </c>
       <c r="P51" s="13">
-        <f>O51*$N$58-L51</f>
+        <f t="shared" si="23"/>
         <v>13.449999999999989</v>
       </c>
       <c r="Q51">
@@ -6024,31 +6062,31 @@
         <v>0.25</v>
       </c>
       <c r="J52" s="10">
-        <f>(E52+F52+($K$58*H52+$M$58)*$L$58)/(1-G52)/(1-$O$58)/(1-I52)/$N$58</f>
+        <f t="shared" si="17"/>
         <v>23.457480818414318</v>
       </c>
       <c r="K52" s="11">
-        <f>(E52+F52+($K$58*H52+$M$58)*$L$58)/(1-G52)/(1-$P$58)/(1-I52)/$N$58</f>
+        <f t="shared" si="18"/>
         <v>25.389273356401382</v>
       </c>
       <c r="L52" s="1">
-        <f>E52+F52+($K$58*H52+$M$58)*$L$58</f>
+        <f t="shared" si="19"/>
         <v>88.05</v>
       </c>
       <c r="M52" s="12">
-        <f>L52/(1-G52)/(1-$O$58)/$N$58</f>
+        <f t="shared" si="20"/>
         <v>17.593110613810737</v>
       </c>
       <c r="N52" s="12">
-        <f>L52/(1-G52)/(1-$P$58)/$N$58</f>
+        <f t="shared" si="21"/>
         <v>19.041955017301035</v>
       </c>
       <c r="O52" s="12">
-        <f>L52/(1-G52)/$N$58</f>
+        <f t="shared" si="22"/>
         <v>16.18566176470588</v>
       </c>
       <c r="P52" s="13">
-        <f>O52*$N$58-L52</f>
+        <f t="shared" si="23"/>
         <v>22.012499999999989</v>
       </c>
       <c r="Q52">
@@ -6084,31 +6122,31 @@
         <v>0.3</v>
       </c>
       <c r="J53" s="10">
-        <f>(E53+F53+($K$58*H53+$M$58)*$L$58)/(1-G53)/(1-$O$58)/(1-I53)/$N$58</f>
+        <f t="shared" si="17"/>
         <v>24.27744553198854</v>
       </c>
       <c r="K53" s="11">
-        <f>(E53+F53+($K$58*H53+$M$58)*$L$58)/(1-G53)/(1-$P$58)/(1-I53)/$N$58</f>
+        <f t="shared" si="18"/>
         <v>26.276764575799358</v>
       </c>
       <c r="L53" s="1">
-        <f>E53+F53+($K$58*H53+$M$58)*$L$58</f>
+        <f t="shared" si="19"/>
         <v>80.8</v>
       </c>
       <c r="M53" s="12">
-        <f>L53/(1-G53)/(1-$O$58)/$N$58</f>
+        <f t="shared" si="20"/>
         <v>16.994211872391976</v>
       </c>
       <c r="N53" s="12">
-        <f>L53/(1-G53)/(1-$P$58)/$N$58</f>
+        <f t="shared" si="21"/>
         <v>18.393735203059553</v>
       </c>
       <c r="O53" s="12">
-        <f>L53/(1-G53)/$N$58</f>
+        <f t="shared" si="22"/>
         <v>15.634674922600619</v>
       </c>
       <c r="P53" s="13">
-        <f>O53*$N$58-L53</f>
+        <f t="shared" si="23"/>
         <v>25.515789473684208</v>
       </c>
       <c r="Q53">
@@ -6144,31 +6182,31 @@
         <v>0.3</v>
       </c>
       <c r="J54" s="10">
-        <f>(E54+F54+($K$58*H54+$M$58)*$L$58)/(1-G54)/(1-$O$58)/(1-I54)/$N$58</f>
+        <f t="shared" si="17"/>
         <v>20.35189075630252</v>
       </c>
       <c r="K54" s="11">
-        <f>(E54+F54+($K$58*H54+$M$58)*$L$58)/(1-G54)/(1-$P$58)/(1-I54)/$N$58</f>
+        <f t="shared" si="18"/>
         <v>22.027928818586258</v>
       </c>
       <c r="L54" s="1">
-        <f>E54+F54+($K$58*H54+$M$58)*$L$58</f>
+        <f t="shared" si="19"/>
         <v>71.3</v>
       </c>
       <c r="M54" s="12">
-        <f>L54/(1-G54)/(1-$O$58)/$N$58</f>
+        <f t="shared" si="20"/>
         <v>14.246323529411763</v>
       </c>
       <c r="N54" s="12">
-        <f>L54/(1-G54)/(1-$P$58)/$N$58</f>
+        <f t="shared" si="21"/>
         <v>15.41955017301038</v>
       </c>
       <c r="O54" s="12">
-        <f>L54/(1-G54)/$N$58</f>
+        <f t="shared" si="22"/>
         <v>13.106617647058822</v>
       </c>
       <c r="P54" s="13">
-        <f>O54*$N$58-L54</f>
+        <f t="shared" si="23"/>
         <v>17.824999999999989</v>
       </c>
       <c r="Q54">
@@ -6179,17 +6217,64 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="90.75" customHeight="1">
-      <c r="C55" s="1"/>
-      <c r="D55" s="9"/>
-      <c r="G55" s="3"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="13"/>
+      <c r="B55">
+        <v>17020701</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55">
+        <v>60</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H55">
+        <v>0.2</v>
+      </c>
+      <c r="I55" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="J55" s="10">
+        <f t="shared" si="17"/>
+        <v>24.490774570697841</v>
+      </c>
+      <c r="K55" s="11">
+        <f t="shared" si="18"/>
+        <v>26.507661888284723</v>
+      </c>
+      <c r="L55" s="1">
+        <f t="shared" si="19"/>
+        <v>85.8</v>
+      </c>
+      <c r="M55" s="12">
+        <f t="shared" si="20"/>
+        <v>17.14354219948849</v>
+      </c>
+      <c r="N55" s="12">
+        <f t="shared" si="21"/>
+        <v>18.555363321799305</v>
+      </c>
+      <c r="O55" s="12">
+        <f t="shared" si="22"/>
+        <v>15.772058823529409</v>
+      </c>
+      <c r="P55" s="13">
+        <f t="shared" si="23"/>
+        <v>21.449999999999989</v>
+      </c>
+      <c r="Q55">
+        <v>30</v>
+      </c>
+      <c r="R55">
+        <v>25</v>
+      </c>
     </row>
     <row r="57" spans="2:18">
       <c r="K57" s="15" t="s">
@@ -6290,10 +6375,11 @@
     <hyperlink ref="D51" r:id="rId43"/>
     <hyperlink ref="D53" r:id="rId44"/>
     <hyperlink ref="D54" r:id="rId45"/>
+    <hyperlink ref="D55" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId46"/>
+  <drawing r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -6307,7 +6393,7 @@
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17020801 by rabbit clothing set by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="101">
   <si>
     <t>产品标题</t>
   </si>
@@ -279,6 +279,55 @@
   <si>
     <t>https://detail.1688.com/offer/45277079052.html?spm=a261y.7663282.0.0.8G3JEy&amp;sk=consign</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/38711199781.html?spm=b26110380.8015204.tkhy006.2.g0hkme</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t> 9-12</t>
+  </si>
+  <si>
+    <t> 24.5</t>
+  </si>
+  <si>
+    <t> 30</t>
+  </si>
+  <si>
+    <t> 34</t>
+  </si>
+  <si>
+    <t> 20</t>
+  </si>
+  <si>
+    <t> 12-18</t>
+  </si>
+  <si>
+    <t> 26</t>
+  </si>
+  <si>
+    <t> 31</t>
+  </si>
+  <si>
+    <t> 37</t>
+  </si>
+  <si>
+    <t> 21</t>
+  </si>
+  <si>
+    <t> 18-24</t>
+  </si>
+  <si>
+    <t> 27</t>
+  </si>
+  <si>
+    <t> 32</t>
+  </si>
+  <si>
+    <t> 38</t>
+  </si>
+  <si>
+    <t> 22</t>
   </si>
 </sst>
 </file>
@@ -291,7 +340,7 @@
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +385,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,13 +405,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -371,7 +447,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -423,6 +499,9 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -2675,7 +2754,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2684,6 +2763,44 @@
         <a:xfrm>
           <a:off x="0" y="59817000"/>
           <a:ext cx="1018761" cy="1118151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>74544</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1067811</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1109869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="图片 57" descr="1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="email"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="61042827"/>
+          <a:ext cx="1067811" cy="1035325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2980,11 +3097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3090,31 +3207,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="10">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$58*H2+$M$58)*$L$58)/(1-G2)/(1-$O$58)/(1-I2)/$N$58</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$60*H2+$M$60)*$L$60)/(1-G2)/(1-$O$60)/(1-I2)/$N$60</f>
         <v>16.874780602778198</v>
       </c>
       <c r="K2" s="11">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$58*H2+$M$58)*$L$58)/(1-G2)/(1-$P$58)/(1-I2)/$N$58</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$60*H2+$M$60)*$L$60)/(1-G2)/(1-$P$60)/(1-I2)/$N$60</f>
         <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$58*H2+$M$58)*$L$58</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$60*H2+$M$60)*$L$60</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="12">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$58)/$N$58</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$60)/$N$60</f>
         <v>14.3435635123615</v>
       </c>
       <c r="N2" s="12">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$58)/$N$58</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$60)/$N$60</f>
         <v>15.524798154555899</v>
       </c>
       <c r="O2" s="12">
-        <f>L2/(1-G2)/$N$58</f>
+        <f>L2/(1-G2)/$N$60</f>
         <v>13.1960784313726</v>
       </c>
       <c r="P2" s="13">
-        <f>O2*$N$58-L2</f>
+        <f>O2*$N$60-L2</f>
         <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
@@ -3155,27 +3272,27 @@
         <v>11.025859619209999</v>
       </c>
       <c r="K3" s="11">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$58*H3+$M$58)*$L$58)/(1-G3)/(1-$P$58)/(1-I3)/$N$58</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$60*H3+$M$60)*$L$60)/(1-G3)/(1-$P$60)/(1-I3)/$N$60</f>
         <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$58*H3+$M$58)*$L$58</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$60*H3+$M$60)*$L$60</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="12">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$58)/$N$58</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$60)/$N$60</f>
         <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="12">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$58)/$N$58</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$60)/$N$60</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="12">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$58</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$60</f>
         <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="13">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$58-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$60-L3</f>
         <v>12.9333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -3402,27 +3519,27 @@
         <v>17.250890125871301</v>
       </c>
       <c r="K7" s="11">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$58*H7+$M$58)*$L$58)/(1-G7)/(1-$P$58)/(1-I7)/$N$58</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$60*H7+$M$60)*$L$60)/(1-G7)/(1-$P$60)/(1-I7)/$N$60</f>
         <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$58*H7+$M$58)*$L$58</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$60*H7+$M$60)*$L$60</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="12">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$58)/$N$58</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$60)/$N$60</f>
         <v>14.663256606990601</v>
       </c>
       <c r="N7" s="12">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$58)/$N$58</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$60)/$N$60</f>
         <v>15.8708189158016</v>
       </c>
       <c r="O7" s="12">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$58</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$60</f>
         <v>13.490196078431399</v>
       </c>
       <c r="P7" s="13">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$58-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$60-L7</f>
         <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
@@ -5942,31 +6059,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="10">
-        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$O$58)/(1-I50)/$N$58</f>
+        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$60*H50+$M$60)*$L$60)/(1-G50)/(1-$O$60)/(1-I50)/$N$60</f>
         <v>17.069673719290101</v>
       </c>
       <c r="K50" s="11">
-        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$58*H50+$M$58)*$L$58)/(1-G50)/(1-$P$58)/(1-I50)/$N$58</f>
+        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$60*H50+$M$60)*$L$60)/(1-G50)/(1-$P$60)/(1-I50)/$N$60</f>
         <v>18.475411554996299</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$58*H50+$M$58)*$L$58</f>
+        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$60*H50+$M$60)*$L$60</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="12">
-        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$58)/$N$58</f>
+        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$60)/$N$60</f>
         <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="12">
-        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$58)/$N$58</f>
+        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$60)/$N$60</f>
         <v>10.161476355248</v>
       </c>
       <c r="O50" s="12">
-        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$58</f>
+        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$60</f>
         <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="13">
-        <f t="shared" ref="P50:P55" si="23">O50*$N$58-L50</f>
+        <f t="shared" ref="P50:P55" si="23">O50*$N$60-L50</f>
         <v>14.6833333333333</v>
       </c>
       <c r="Q50">
@@ -6276,43 +6393,116 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="2:18">
-      <c r="K57" s="15" t="s">
+    <row r="56" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B56">
+        <v>17020801</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56">
+        <v>24.5</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H56">
+        <v>0.18</v>
+      </c>
+      <c r="I56" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" ref="J56" si="24">(E56+F56+($K$60*H56+$M$60)*$L$60)/(1-G56)/(1-$O$60)/(1-I56)/$N$60</f>
+        <v>13.872396784800875</v>
+      </c>
+      <c r="K56" s="11">
+        <f t="shared" ref="K56" si="25">(E56+F56+($K$60*H56+$M$60)*$L$60)/(1-G56)/(1-$P$60)/(1-I56)/$N$60</f>
+        <v>15.014829461196243</v>
+      </c>
+      <c r="L56" s="1">
+        <f t="shared" ref="L56" si="26">E56+F56+($K$60*H56+$M$60)*$L$60</f>
+        <v>48.599999999999994</v>
+      </c>
+      <c r="M56" s="12">
+        <f t="shared" ref="M56" si="27">L56/(1-G56)/(1-$O$60)/$N$60</f>
+        <v>9.7106777493606113</v>
+      </c>
+      <c r="N56" s="12">
+        <f t="shared" ref="N56" si="28">L56/(1-G56)/(1-$P$60)/$N$60</f>
+        <v>10.510380622837371</v>
+      </c>
+      <c r="O56" s="12">
+        <f t="shared" ref="O56" si="29">L56/(1-G56)/$N$60</f>
+        <v>8.9338235294117645</v>
+      </c>
+      <c r="P56" s="13">
+        <f t="shared" ref="P56" si="30">O56*$N$60-L56</f>
+        <v>12.150000000000006</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" ht="90.75" customHeight="1">
+      <c r="C57" s="1"/>
+      <c r="D57" s="9"/>
+      <c r="G57" s="3"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="13"/>
+    </row>
+    <row r="59" spans="2:18">
+      <c r="K59" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="L57" s="15" t="s">
+      <c r="L59" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="M57" s="15" t="s">
+      <c r="M59" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="N57" s="15" t="s">
+      <c r="N59" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="O57" s="15" t="s">
+      <c r="O59" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="P57" s="15" t="s">
+      <c r="P59" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="2:18">
-      <c r="K58" s="16">
+    <row r="60" spans="2:18">
+      <c r="K60" s="16">
         <v>100</v>
       </c>
-      <c r="L58" s="14">
+      <c r="L60" s="14">
         <v>0.85</v>
       </c>
-      <c r="M58">
+      <c r="M60">
         <v>8</v>
       </c>
-      <c r="N58">
+      <c r="N60">
         <v>6.8</v>
       </c>
-      <c r="O58" s="14">
+      <c r="O60" s="14">
         <v>0.08</v>
       </c>
-      <c r="P58" s="14">
+      <c r="P60" s="14">
         <v>0.15</v>
       </c>
     </row>
@@ -6322,7 +6512,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C55">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C57">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -6376,21 +6566,76 @@
     <hyperlink ref="D53" r:id="rId44"/>
     <hyperlink ref="D54" r:id="rId45"/>
     <hyperlink ref="D55" r:id="rId46"/>
+    <hyperlink ref="D56" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId47"/>
+  <drawing r:id="rId48"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
17021101-03  魔法精灵提交 by  hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="18540" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t>产品标题</t>
   </si>
@@ -286,23 +286,30 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/544516029305.html?spm=0.0.0.0.D3IAEt</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/541801369107.html?spm=0.0.0.0.D3IAEt</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/542163784708.html?spm=0.0.0.0.D3IAEt</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
     <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,140 +345,26 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,194 +377,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -679,255 +386,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -943,22 +414,22 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -967,7 +438,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -982,64 +453,22 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1061,7 +490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1103,7 +532,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1145,7 +574,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1187,7 +616,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1229,7 +658,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1271,7 +700,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1313,7 +742,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1355,7 +784,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1397,7 +826,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1439,7 +868,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1481,7 +910,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1523,7 +952,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1565,7 +994,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1607,7 +1036,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1649,7 +1078,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1691,7 +1120,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1733,7 +1162,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1775,7 +1204,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1817,7 +1246,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1859,7 +1288,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1901,7 +1330,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1943,7 +1372,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1985,7 +1414,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2027,7 +1456,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2069,7 +1498,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2111,7 +1540,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2153,7 +1582,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2195,7 +1624,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2237,7 +1666,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2279,7 +1708,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2321,7 +1750,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2363,7 +1792,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2405,7 +1834,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2447,7 +1876,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2489,7 +1918,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2531,7 +1960,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2573,7 +2002,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2615,7 +2044,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2657,7 +2086,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2699,7 +2128,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2741,7 +2170,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2783,7 +2212,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2825,7 +2254,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId43" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2867,7 +2296,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId44" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2909,7 +2338,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId45" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2951,7 +2380,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId46" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2993,7 +2422,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId47"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3035,7 +2464,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId48" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3077,7 +2506,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId49"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3119,7 +2548,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId50" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3161,7 +2590,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId51" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3203,7 +2632,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId52" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3241,7 +2670,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId53" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3279,7 +2708,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId54" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3317,7 +2746,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId55" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3355,7 +2784,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId56" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3397,7 +2826,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId57" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3435,7 +2864,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId58"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3473,7 +2902,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId59"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3490,6 +2919,120 @@
         <a:ln w="9525">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>24847</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>57979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1051890</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>1093770</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="图片 68" descr="QQ截图20170211150609.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24847" y="64523179"/>
+          <a:ext cx="1027043" cy="1035791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>49696</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1061079</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>1051891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="图片 69" descr="QQ截图20170211153103.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="49696" y="65642573"/>
+          <a:ext cx="1011383" cy="1027043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2004</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>1060174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="图片 70" descr="QQ截图20170211154419.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="66836512"/>
+          <a:ext cx="1078329" cy="993912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3781,37 +3324,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:S63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="S59" sqref="S59"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="7.25454545454545" customWidth="1"/>
-    <col min="6" max="6" width="8.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="7.37272727272727" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="11.1272727272727" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3867,7 +3408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>16072601</v>
@@ -3894,32 +3435,32 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$63*H2+$M$63)*$L$63)/(1-G2)/(1-$O$63)/(1-I2)/$N$63</f>
-        <v>16.8747806027782</v>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$68*H2+$M$68)*$L$68)/(1-G2)/(1-$O$68)/(1-I2)/$N$68</f>
+        <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$63*H2+$M$63)*$L$63)/(1-G2)/(1-$P$63)/(1-I2)/$N$63</f>
-        <v>18.2644684171246</v>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$68*H2+$M$68)*$L$68)/(1-G2)/(1-$P$68)/(1-I2)/$N$68</f>
+        <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$63*H2+$M$63)*$L$63</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$68*H2+$M$68)*$L$68</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$63)/$N$63</f>
-        <v>14.3435635123615</v>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$68)/$N$68</f>
+        <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$63)/$N$63</f>
-        <v>15.5247981545559</v>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$68)/$N$68</f>
+        <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$63</f>
-        <v>13.1960784313726</v>
+        <f>L2/(1-G2)/$N$68</f>
+        <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$63-L2</f>
-        <v>22.4333333333333</v>
+        <f>O2*$N$68-L2</f>
+        <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -3928,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>16072701</v>
@@ -3956,31 +3497,31 @@
       </c>
       <c r="J3" s="11">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$63*H3+$M$63)*$L$63)/(1-G3)/(1-$P$63)/(1-I3)/$N$63</f>
-        <v>11.9338715878508</v>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$68*H3+$M$68)*$L$68)/(1-G3)/(1-$P$68)/(1-I3)/$N$68</f>
+        <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$63*H3+$M$63)*$L$63</f>
-        <v>38.8</v>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$68*H3+$M$68)*$L$68</f>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$63)/$N$63</f>
-        <v>8.2693947144075</v>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$68)/$N$68</f>
+        <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$63)/$N$63</f>
-        <v>8.95040369088812</v>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$68)/$N$68</f>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$63</f>
-        <v>7.6078431372549</v>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$68</f>
+        <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$63-L3</f>
-        <v>12.9333333333333</v>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$68-L3</f>
+        <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
@@ -3989,7 +3530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>16072901</v>
@@ -4017,11 +3558,11 @@
       </c>
       <c r="J4" s="11">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962856</v>
       </c>
       <c r="K4" s="12">
         <f t="shared" si="5"/>
-        <v>20.6953369583127</v>
+        <v>20.69533695831274</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="6"/>
@@ -4029,19 +3570,19 @@
       </c>
       <c r="M4" s="13">
         <f t="shared" si="7"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" si="8"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818917</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="9"/>
-        <v>12.3137254901961</v>
+        <v>12.313725490196079</v>
       </c>
       <c r="P4" s="14">
         <f t="shared" si="10"/>
-        <v>20.9333333333333</v>
+        <v>20.933333333333337</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -4050,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>16073001</v>
@@ -4078,11 +3619,11 @@
       </c>
       <c r="J5" s="11">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119653</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" si="5"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047156</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="6"/>
@@ -4090,19 +3631,19 @@
       </c>
       <c r="M5" s="13">
         <f t="shared" si="7"/>
-        <v>15.5157715260017</v>
+        <v>15.515771526001704</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" si="8"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790081</v>
       </c>
       <c r="O5" s="13">
         <f t="shared" si="9"/>
-        <v>14.2745098039216</v>
+        <v>14.274509803921568</v>
       </c>
       <c r="P5" s="14">
         <f t="shared" si="10"/>
-        <v>24.2666666666667</v>
+        <v>24.266666666666666</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -4111,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>16073002</v>
@@ -4139,11 +3680,11 @@
       </c>
       <c r="J6" s="11">
         <f t="shared" si="0"/>
-        <v>15.3499699112381</v>
+        <v>15.34996991123815</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" si="5"/>
-        <v>16.6140850803989</v>
+        <v>16.61408508039894</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="6"/>
@@ -4151,19 +3692,19 @@
       </c>
       <c r="M6" s="13">
         <f t="shared" si="7"/>
-        <v>13.0474744245524</v>
+        <v>13.047474424552426</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" si="8"/>
-        <v>14.1219723183391</v>
+        <v>14.121972318339099</v>
       </c>
       <c r="O6" s="13">
         <f t="shared" si="9"/>
-        <v>12.0036764705882</v>
+        <v>12.003676470588234</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="10"/>
-        <v>16.325</v>
+        <v>16.324999999999989</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -4175,7 +3716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>16080301</v>
@@ -4203,31 +3744,31 @@
       </c>
       <c r="J7" s="11">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$63*H7+$M$63)*$L$63)/(1-G7)/(1-$P$63)/(1-I7)/$N$63</f>
-        <v>18.671551665649</v>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$68*H7+$M$68)*$L$68)/(1-G7)/(1-$P$68)/(1-I7)/$N$68</f>
+        <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$63*H7+$M$63)*$L$63</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$68*H7+$M$68)*$L$68</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$63)/$N$63</f>
-        <v>14.6632566069906</v>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$68)/$N$68</f>
+        <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$63)/$N$63</f>
-        <v>15.8708189158016</v>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$68)/$N$68</f>
+        <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$63</f>
-        <v>13.4901960784314</v>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$68</f>
+        <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$63-L7</f>
-        <v>22.9333333333333</v>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$68-L7</f>
+        <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -4236,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -4263,11 +3804,11 @@
       </c>
       <c r="J8" s="11">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907925</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="11"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159166</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="12"/>
@@ -4275,19 +3816,19 @@
       </c>
       <c r="M8" s="13">
         <f t="shared" si="13"/>
-        <v>17.792918797954</v>
+        <v>17.792918797953963</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="14"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079583</v>
       </c>
       <c r="O8" s="13">
         <f t="shared" si="15"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117645</v>
       </c>
       <c r="P8" s="14">
         <f t="shared" si="16"/>
-        <v>22.2625</v>
+        <v>22.262499999999989</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -4296,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -4323,11 +3864,11 @@
       </c>
       <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695649</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="11"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058822</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="12"/>
@@ -4335,11 +3876,11 @@
       </c>
       <c r="M9" s="13">
         <f t="shared" si="13"/>
-        <v>16.8478260869565</v>
+        <v>16.84782608695652</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="14"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647058</v>
       </c>
       <c r="O9" s="13">
         <f t="shared" si="15"/>
@@ -4347,7 +3888,7 @@
       </c>
       <c r="P9" s="14">
         <f t="shared" si="16"/>
-        <v>26.35</v>
+        <v>26.349999999999994</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -4356,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -4383,11 +3924,11 @@
       </c>
       <c r="J10" s="11">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914626</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="11"/>
-        <v>40.467951886637</v>
+        <v>40.46795188663701</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="12"/>
@@ -4395,19 +3936,19 @@
       </c>
       <c r="M10" s="13">
         <f t="shared" si="13"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640237</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="14"/>
-        <v>28.3275663206459</v>
+        <v>28.327566320645907</v>
       </c>
       <c r="O10" s="13">
         <f t="shared" si="15"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549019</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="16"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333323</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -4416,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -4443,31 +3984,31 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720474</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="11"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320991</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="12"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="13">
         <f t="shared" si="13"/>
-        <v>27.8772378516624</v>
+        <v>27.877237851662404</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="14"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622841</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="15"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529413</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="16"/>
-        <v>43.6</v>
+        <v>43.599999999999994</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -4476,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -4503,7 +4044,7 @@
       </c>
       <c r="J12" s="11">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419616</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="11"/>
@@ -4511,23 +4052,23 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="12"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="13"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506674</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="14"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666044</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="15"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666137</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="16"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729729</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -4536,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -4563,11 +4104,11 @@
       </c>
       <c r="J13" s="11">
         <f t="shared" si="0"/>
-        <v>15.1822877488591</v>
+        <v>15.182287748859135</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" si="11"/>
-        <v>16.4325937987652</v>
+        <v>16.432593798765183</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="12"/>
@@ -4575,19 +4116,19 @@
       </c>
       <c r="M13" s="13">
         <f t="shared" si="13"/>
-        <v>12.9049445865303</v>
+        <v>12.904944586530265</v>
       </c>
       <c r="N13" s="13">
         <f t="shared" si="14"/>
-        <v>13.9677047289504</v>
+        <v>13.967704728950405</v>
       </c>
       <c r="O13" s="13">
         <f t="shared" si="15"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607844</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="16"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333337</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -4596,7 +4137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -4623,31 +4164,31 @@
       </c>
       <c r="J14" s="11">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874677</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="11"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193776</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="12"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="13">
         <f t="shared" si="13"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437338</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="14"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096888</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="15"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882355</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="16"/>
-        <v>46.6</v>
+        <v>46.599999999999994</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -4656,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -4683,11 +4224,11 @@
       </c>
       <c r="J15" s="11">
         <f t="shared" si="0"/>
-        <v>23.0179028132992</v>
+        <v>23.017902813299234</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="11"/>
-        <v>24.9134948096886</v>
+        <v>24.913494809688583</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="12"/>
@@ -4695,11 +4236,11 @@
       </c>
       <c r="M15" s="13">
         <f t="shared" si="13"/>
-        <v>19.5652173913043</v>
+        <v>19.565217391304348</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="14"/>
-        <v>21.1764705882353</v>
+        <v>21.176470588235293</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="15"/>
@@ -4707,7 +4248,7 @@
       </c>
       <c r="P15" s="14">
         <f t="shared" si="16"/>
-        <v>30.6</v>
+        <v>30.599999999999994</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -4716,7 +4257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -4743,11 +4284,11 @@
       </c>
       <c r="J16" s="11">
         <f t="shared" si="0"/>
-        <v>11.6687979539642</v>
+        <v>11.668797953964194</v>
       </c>
       <c r="K16" s="12">
         <f t="shared" si="11"/>
-        <v>12.6297577854671</v>
+        <v>12.629757785467127</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="12"/>
@@ -4755,19 +4296,19 @@
       </c>
       <c r="M16" s="13">
         <f t="shared" si="13"/>
-        <v>8.75159846547314</v>
+        <v>8.751598465473144</v>
       </c>
       <c r="N16" s="13">
         <f t="shared" si="14"/>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003456</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="15"/>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352935</v>
       </c>
       <c r="P16" s="14">
         <f t="shared" si="16"/>
-        <v>10.95</v>
+        <v>10.949999999999996</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -4776,7 +4317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -4803,11 +4344,11 @@
       </c>
       <c r="J17" s="11">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685071</v>
       </c>
       <c r="K17" s="12">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600313</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="12"/>
@@ -4815,19 +4356,19 @@
       </c>
       <c r="M17" s="13">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.02387041773231</v>
       </c>
       <c r="N17" s="13">
         <f t="shared" si="14"/>
-        <v>15.1787773933103</v>
+        <v>15.178777393310266</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313726</v>
       </c>
       <c r="P17" s="14">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333337</v>
       </c>
       <c r="Q17" s="15">
         <v>0.15</v>
@@ -4836,7 +4377,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -4863,11 +4404,11 @@
       </c>
       <c r="J18" s="11">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685071</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600313</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="12"/>
@@ -4875,19 +4416,19 @@
       </c>
       <c r="M18" s="13">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.02387041773231</v>
       </c>
       <c r="N18" s="13">
         <f t="shared" si="14"/>
-        <v>15.1787773933103</v>
+        <v>15.178777393310266</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313726</v>
       </c>
       <c r="P18" s="14">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333337</v>
       </c>
       <c r="Q18" s="15">
         <v>0.15</v>
@@ -4896,7 +4437,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
@@ -4923,31 +4464,31 @@
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>17.0716112531969</v>
+        <v>17.071611253196931</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="11"/>
-        <v>18.477508650519</v>
+        <v>18.477508650519031</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="12"/>
-        <v>40.05</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="13">
         <f t="shared" si="13"/>
-        <v>8.53580562659847</v>
+        <v>8.5358056265984654</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" si="14"/>
-        <v>9.23875432525952</v>
+        <v>9.2387543252595155</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="15"/>
-        <v>7.85294117647059</v>
+        <v>7.8529411764705879</v>
       </c>
       <c r="P19" s="14">
         <f t="shared" si="16"/>
-        <v>13.35</v>
+        <v>13.350000000000001</v>
       </c>
       <c r="Q19">
         <v>15</v>
@@ -4956,7 +4497,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
@@ -4983,11 +4524,11 @@
       </c>
       <c r="J20" s="11">
         <f t="shared" si="0"/>
-        <v>18.5117525270978</v>
+        <v>18.511752527097798</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="11"/>
-        <v>20.0362497940353</v>
+        <v>20.03624979403526</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="12"/>
@@ -4995,25 +4536,25 @@
       </c>
       <c r="M20" s="13">
         <f t="shared" si="13"/>
-        <v>12.9582267689685</v>
+        <v>12.958226768968457</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="14"/>
-        <v>14.0253748558247</v>
+        <v>14.025374855824683</v>
       </c>
       <c r="O20" s="13">
         <f t="shared" si="15"/>
-        <v>11.921568627451</v>
+        <v>11.921568627450981</v>
       </c>
       <c r="P20" s="14">
         <f t="shared" si="16"/>
-        <v>20.2666666666667</v>
+        <v>20.266666666666666</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -5040,11 +4581,11 @@
       </c>
       <c r="J21" s="11">
         <f t="shared" si="0"/>
-        <v>25.9823296907696</v>
+        <v>25.982329690769582</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421202</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="12"/>
@@ -5052,25 +4593,25 @@
       </c>
       <c r="M21" s="13">
         <f t="shared" si="13"/>
-        <v>14.2902813299233</v>
+        <v>14.290281329923273</v>
       </c>
       <c r="N21" s="13">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.46712802768166</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529411</v>
       </c>
       <c r="P21" s="14">
         <f t="shared" si="16"/>
-        <v>22.35</v>
+        <v>22.349999999999994</v>
       </c>
       <c r="R21">
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
@@ -5097,11 +4638,11 @@
       </c>
       <c r="J22" s="11">
         <f t="shared" si="0"/>
-        <v>25.9823296907696</v>
+        <v>25.982329690769582</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421202</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="12"/>
@@ -5109,25 +4650,25 @@
       </c>
       <c r="M22" s="13">
         <f t="shared" si="13"/>
-        <v>14.2902813299233</v>
+        <v>14.290281329923273</v>
       </c>
       <c r="N22" s="13">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.46712802768166</v>
       </c>
       <c r="O22" s="13">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529411</v>
       </c>
       <c r="P22" s="14">
         <f t="shared" si="16"/>
-        <v>22.35</v>
+        <v>22.349999999999994</v>
       </c>
       <c r="R22">
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
@@ -5154,11 +4695,11 @@
       </c>
       <c r="J23" s="11">
         <f t="shared" si="0"/>
-        <v>27.5323568162443</v>
+        <v>27.532356816244285</v>
       </c>
       <c r="K23" s="12">
         <f t="shared" si="11"/>
-        <v>29.799727377582</v>
+        <v>29.799727377582048</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="12"/>
@@ -5166,25 +4707,25 @@
       </c>
       <c r="M23" s="13">
         <f t="shared" si="13"/>
-        <v>15.1427962489344</v>
+        <v>15.142796248934356</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="14"/>
-        <v>16.3898500576701</v>
+        <v>16.389850057670127</v>
       </c>
       <c r="O23" s="13">
         <f t="shared" si="15"/>
-        <v>13.9313725490196</v>
+        <v>13.931372549019608</v>
       </c>
       <c r="P23" s="14">
         <f t="shared" si="16"/>
-        <v>23.6833333333333</v>
+        <v>23.683333333333337</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -5211,11 +4752,11 @@
       </c>
       <c r="J24" s="11">
         <f t="shared" si="0"/>
-        <v>26.3698364721383</v>
+        <v>26.36983647213826</v>
       </c>
       <c r="K24" s="12">
         <f t="shared" si="11"/>
-        <v>28.5414700639614</v>
+        <v>28.541470063961413</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="12"/>
@@ -5223,25 +4764,25 @@
       </c>
       <c r="M24" s="13">
         <f t="shared" si="13"/>
-        <v>14.503410059676</v>
+        <v>14.503410059676044</v>
       </c>
       <c r="N24" s="13">
         <f t="shared" si="14"/>
-        <v>15.6978085351788</v>
+        <v>15.697808535178778</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" si="15"/>
-        <v>13.343137254902</v>
+        <v>13.343137254901961</v>
       </c>
       <c r="P24" s="14">
         <f t="shared" si="16"/>
-        <v>22.6833333333333</v>
+        <v>22.683333333333337</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -5268,11 +4809,11 @@
       </c>
       <c r="J25" s="11">
         <f t="shared" si="0"/>
-        <v>25.4156010230179</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="12">
         <f t="shared" si="11"/>
-        <v>27.5086505190311</v>
+        <v>27.508650519031143</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="12"/>
@@ -5280,25 +4821,25 @@
       </c>
       <c r="M25" s="13">
         <f t="shared" si="13"/>
-        <v>15.2493606138107</v>
+        <v>15.24936061381074</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="14"/>
-        <v>16.5051903114187</v>
+        <v>16.505190311418687</v>
       </c>
       <c r="O25" s="13">
         <f t="shared" si="15"/>
-        <v>14.0294117647059</v>
+        <v>14.029411764705882</v>
       </c>
       <c r="P25" s="14">
         <f t="shared" si="16"/>
-        <v>23.85</v>
+        <v>23.849999999999994</v>
       </c>
       <c r="R25">
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -5325,11 +4866,11 @@
       </c>
       <c r="J26" s="11">
         <f t="shared" si="0"/>
-        <v>22.7514919011083</v>
+        <v>22.751491901108267</v>
       </c>
       <c r="K26" s="12">
         <f t="shared" si="11"/>
-        <v>24.6251441753172</v>
+        <v>24.625144175317189</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="12"/>
@@ -5337,25 +4878,25 @@
       </c>
       <c r="M26" s="13">
         <f t="shared" si="13"/>
-        <v>13.650895140665</v>
+        <v>13.650895140664959</v>
       </c>
       <c r="N26" s="13">
         <f t="shared" si="14"/>
-        <v>14.7750865051903</v>
+        <v>14.775086505190311</v>
       </c>
       <c r="O26" s="13">
         <f t="shared" si="15"/>
-        <v>12.5588235294118</v>
+        <v>12.558823529411764</v>
       </c>
       <c r="P26" s="14">
         <f t="shared" si="16"/>
-        <v>21.35</v>
+        <v>21.349999999999994</v>
       </c>
       <c r="R26">
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -5382,11 +4923,11 @@
       </c>
       <c r="J27" s="11">
         <f t="shared" si="0"/>
-        <v>19.3338204847156</v>
+        <v>19.333820484715627</v>
       </c>
       <c r="K27" s="12">
         <f t="shared" si="11"/>
-        <v>20.9260174658099</v>
+        <v>20.926017465809856</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="12"/>
@@ -5394,19 +4935,19 @@
       </c>
       <c r="M27" s="13">
         <f t="shared" si="13"/>
-        <v>13.5336743393009</v>
+        <v>13.533674339300937</v>
       </c>
       <c r="N27" s="13">
         <f t="shared" si="14"/>
-        <v>14.6482122260669</v>
+        <v>14.648212226066898</v>
       </c>
       <c r="O27" s="13">
         <f t="shared" si="15"/>
-        <v>12.4509803921569</v>
+        <v>12.450980392156863</v>
       </c>
       <c r="P27" s="14">
         <f t="shared" si="16"/>
-        <v>21.1666666666667</v>
+        <v>21.166666666666671</v>
       </c>
       <c r="Q27">
         <v>40</v>
@@ -5415,7 +4956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -5442,11 +4983,11 @@
       </c>
       <c r="J28" s="11">
         <f t="shared" si="0"/>
-        <v>28.6948771603503</v>
+        <v>28.694877160350305</v>
       </c>
       <c r="K28" s="12">
         <f t="shared" si="11"/>
-        <v>31.0579846912027</v>
+        <v>31.057984691202684</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="12"/>
@@ -5454,19 +4995,19 @@
       </c>
       <c r="M28" s="13">
         <f t="shared" si="13"/>
-        <v>15.7821824381927</v>
+        <v>15.782182438192669</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="14"/>
-        <v>17.0818915801615</v>
+        <v>17.081891580161475</v>
       </c>
       <c r="O28" s="13">
         <f t="shared" si="15"/>
-        <v>14.5196078431373</v>
+        <v>14.519607843137255</v>
       </c>
       <c r="P28" s="14">
         <f t="shared" si="16"/>
-        <v>24.6833333333333</v>
+        <v>24.683333333333337</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -5475,7 +5016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -5502,11 +5043,11 @@
       </c>
       <c r="J29" s="11">
         <f t="shared" si="0"/>
-        <v>21.6112531969309</v>
+        <v>21.611253196930942</v>
       </c>
       <c r="K29" s="12">
         <f t="shared" si="11"/>
-        <v>23.3910034602076</v>
+        <v>23.39100346020761</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="12"/>
@@ -5514,19 +5055,19 @@
       </c>
       <c r="M29" s="13">
         <f t="shared" si="13"/>
-        <v>16.2084398976982</v>
+        <v>16.208439897698209</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="14"/>
-        <v>17.5432525951557</v>
+        <v>17.543252595155707</v>
       </c>
       <c r="O29" s="13">
         <f t="shared" si="15"/>
-        <v>14.9117647058824</v>
+        <v>14.911764705882351</v>
       </c>
       <c r="P29" s="14">
         <f t="shared" si="16"/>
-        <v>25.35</v>
+        <v>25.349999999999994</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -5535,7 +5076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -5562,11 +5103,11 @@
       </c>
       <c r="J30" s="11">
         <f t="shared" si="0"/>
-        <v>26.6604665581648</v>
+        <v>26.660466558164767</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="11"/>
-        <v>28.8560343923666</v>
+        <v>28.856034392366574</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="12"/>
@@ -5574,19 +5115,19 @@
       </c>
       <c r="M30" s="13">
         <f t="shared" si="13"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990624</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="14"/>
-        <v>15.8708189158016</v>
+        <v>15.870818915801616</v>
       </c>
       <c r="O30" s="13">
         <f t="shared" si="15"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431373</v>
       </c>
       <c r="P30" s="14">
         <f t="shared" si="16"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333337</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -5595,7 +5136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -5622,11 +5163,11 @@
       </c>
       <c r="J31" s="11">
         <f t="shared" si="0"/>
-        <v>12.8010443307758</v>
+        <v>12.801044330775786</v>
       </c>
       <c r="K31" s="12">
         <f t="shared" si="11"/>
-        <v>13.8552479815456</v>
+        <v>13.85524798154556</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="12"/>
@@ -5634,19 +5175,19 @@
       </c>
       <c r="M31" s="13">
         <f t="shared" si="13"/>
-        <v>10.2408354646206</v>
+        <v>10.240835464620631</v>
       </c>
       <c r="N31" s="13">
         <f t="shared" si="14"/>
-        <v>11.0841983852364</v>
+        <v>11.084198385236448</v>
       </c>
       <c r="O31" s="13">
         <f t="shared" si="15"/>
-        <v>9.42156862745098</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="14">
         <f t="shared" si="16"/>
-        <v>16.0166666666667</v>
+        <v>16.016666666666666</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -5655,7 +5196,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -5682,11 +5223,11 @@
       </c>
       <c r="J32" s="11">
         <f t="shared" si="0"/>
-        <v>18.0448991190679</v>
+        <v>18.044899119067917</v>
       </c>
       <c r="K32" s="12">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755864</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="12"/>
@@ -5694,19 +5235,19 @@
       </c>
       <c r="M32" s="13">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440749</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="14"/>
-        <v>11.7185697808535</v>
+        <v>11.718569780853519</v>
       </c>
       <c r="O32" s="13">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="14">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333337</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -5715,7 +5256,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -5742,11 +5283,11 @@
       </c>
       <c r="J33" s="11">
         <f t="shared" si="0"/>
-        <v>26.0792063861118</v>
+        <v>26.079206386111757</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" si="11"/>
-        <v>28.2269057355563</v>
+        <v>28.226905735556254</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="12"/>
@@ -5754,19 +5295,19 @@
       </c>
       <c r="M33" s="13">
         <f t="shared" si="13"/>
-        <v>14.3435635123615</v>
+        <v>14.343563512361467</v>
       </c>
       <c r="N33" s="13">
         <f t="shared" si="14"/>
-        <v>15.5247981545559</v>
+        <v>15.524798154555942</v>
       </c>
       <c r="O33" s="13">
         <f t="shared" si="15"/>
-        <v>13.1960784313726</v>
+        <v>13.19607843137255</v>
       </c>
       <c r="P33" s="14">
         <f t="shared" si="16"/>
-        <v>22.4333333333333</v>
+        <v>22.433333333333337</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -5775,7 +5316,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -5802,11 +5343,11 @@
       </c>
       <c r="J34" s="11">
         <f t="shared" si="0"/>
-        <v>19.9772662688264</v>
+        <v>19.977266268826373</v>
       </c>
       <c r="K34" s="12">
         <f t="shared" si="11"/>
-        <v>21.6224529027297</v>
+        <v>21.622452902729723</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="12"/>
@@ -5814,19 +5355,19 @@
       </c>
       <c r="M34" s="13">
         <f t="shared" si="13"/>
-        <v>14.9829497016198</v>
+        <v>14.982949701619777</v>
       </c>
       <c r="N34" s="13">
         <f t="shared" si="14"/>
-        <v>16.2168396770473</v>
+        <v>16.21683967704729</v>
       </c>
       <c r="O34" s="13">
         <f t="shared" si="15"/>
-        <v>13.7843137254902</v>
+        <v>13.784313725490197</v>
       </c>
       <c r="P34" s="14">
         <f t="shared" si="16"/>
-        <v>23.4333333333333</v>
+        <v>23.433333333333337</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -5835,7 +5376,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -5862,11 +5403,11 @@
       </c>
       <c r="J35" s="11">
         <f t="shared" si="0"/>
-        <v>16.0645780051151</v>
+        <v>16.064578005115088</v>
       </c>
       <c r="K35" s="12">
         <f t="shared" si="11"/>
-        <v>17.3875432525952</v>
+        <v>17.387543252595155</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="12"/>
@@ -5874,25 +5415,25 @@
       </c>
       <c r="M35" s="13">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092071</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076124</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764705</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.099999999999994</v>
       </c>
       <c r="R35">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -5917,11 +5458,11 @@
       </c>
       <c r="J36" s="11">
         <f t="shared" si="0"/>
-        <v>24.5291792606371</v>
+        <v>24.529179260637054</v>
       </c>
       <c r="K36" s="12">
         <f t="shared" si="11"/>
-        <v>26.5492293173954</v>
+        <v>26.549229317395405</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="12"/>
@@ -5929,25 +5470,25 @@
       </c>
       <c r="M36" s="13">
         <f t="shared" si="13"/>
-        <v>13.4910485933504</v>
+        <v>13.491048593350381</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="14"/>
-        <v>14.6020761245675</v>
+        <v>14.602076124567473</v>
       </c>
       <c r="O36" s="13">
         <f t="shared" si="15"/>
-        <v>12.4117647058824</v>
+        <v>12.411764705882351</v>
       </c>
       <c r="P36" s="14">
         <f t="shared" si="16"/>
-        <v>21.1</v>
+        <v>21.099999999999994</v>
       </c>
       <c r="Q36">
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -5972,11 +5513,11 @@
       </c>
       <c r="J37" s="11">
         <f t="shared" si="0"/>
-        <v>7.33962063086104</v>
+        <v>7.339620630861039</v>
       </c>
       <c r="K37" s="12">
         <f t="shared" si="11"/>
-        <v>7.94405997693195</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="12"/>
@@ -5984,25 +5525,25 @@
       </c>
       <c r="M37" s="13">
         <f t="shared" si="13"/>
-        <v>5.87169650468883</v>
+        <v>5.8716965046888321</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="14"/>
-        <v>6.35524798154556</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="13">
         <f t="shared" si="15"/>
-        <v>5.40196078431373</v>
+        <v>5.4019607843137258</v>
       </c>
       <c r="P37" s="14">
         <f t="shared" si="16"/>
-        <v>9.18333333333333</v>
+        <v>9.1833333333333336</v>
       </c>
       <c r="Q37">
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -6027,31 +5568,31 @@
       </c>
       <c r="J38" s="11">
         <f t="shared" si="0"/>
-        <v>16.3256606990622</v>
+        <v>16.325660699062233</v>
       </c>
       <c r="K38" s="12">
         <f t="shared" si="11"/>
-        <v>17.6701268742791</v>
+        <v>17.670126874279124</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="12"/>
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="13">
         <f t="shared" si="13"/>
-        <v>8.16283034953112</v>
+        <v>8.1628303495311165</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="14"/>
-        <v>8.83506343713956</v>
+        <v>8.8350634371395618</v>
       </c>
       <c r="O38" s="13">
         <f t="shared" si="15"/>
-        <v>7.50980392156863</v>
+        <v>7.5098039215686274</v>
       </c>
       <c r="P38" s="14">
         <f t="shared" si="16"/>
-        <v>12.7666666666667</v>
+        <v>12.766666666666666</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -6060,7 +5601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -6087,11 +5628,11 @@
       </c>
       <c r="J39" s="11">
         <f t="shared" si="0"/>
-        <v>18.0448991190679</v>
+        <v>18.044899119067917</v>
       </c>
       <c r="K39" s="12">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755864</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="12"/>
@@ -6099,19 +5640,19 @@
       </c>
       <c r="M39" s="13">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440749</v>
       </c>
       <c r="N39" s="13">
         <f t="shared" si="14"/>
-        <v>11.7185697808535</v>
+        <v>11.718569780853519</v>
       </c>
       <c r="O39" s="13">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="14">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333337</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -6120,7 +5661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -6147,11 +5688,11 @@
       </c>
       <c r="J40" s="11">
         <f t="shared" si="0"/>
-        <v>18.5228241494226</v>
+        <v>18.522824149422608</v>
       </c>
       <c r="K40" s="12">
         <f t="shared" si="11"/>
-        <v>20.0482331970221</v>
+        <v>20.048233197022117</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="12"/>
@@ -6159,19 +5700,19 @@
       </c>
       <c r="M40" s="13">
         <f t="shared" si="13"/>
-        <v>10.1875532821824</v>
+        <v>10.187553282182437</v>
       </c>
       <c r="N40" s="13">
         <f t="shared" si="14"/>
-        <v>11.0265282583622</v>
+        <v>11.026528258362168</v>
       </c>
       <c r="O40" s="13">
         <f t="shared" si="15"/>
-        <v>9.37254901960784</v>
+        <v>9.3725490196078418</v>
       </c>
       <c r="P40" s="14">
         <f t="shared" si="16"/>
-        <v>15.9333333333333</v>
+        <v>15.933333333333323</v>
       </c>
       <c r="Q40">
         <v>20</v>
@@ -6180,7 +5721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -6207,11 +5748,11 @@
       </c>
       <c r="J41" s="11">
         <f t="shared" si="0"/>
-        <v>11.4805342426826</v>
+        <v>11.480534242682578</v>
       </c>
       <c r="K41" s="12">
         <f t="shared" si="11"/>
-        <v>12.4259900038447</v>
+        <v>12.425990003844674</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="12"/>
@@ -6219,19 +5760,19 @@
       </c>
       <c r="M41" s="13">
         <f t="shared" si="13"/>
-        <v>8.61040068201194</v>
+        <v>8.6104006820119352</v>
       </c>
       <c r="N41" s="13">
         <f t="shared" si="14"/>
-        <v>9.31949250288351</v>
+        <v>9.3194925028835076</v>
       </c>
       <c r="O41" s="13">
         <f t="shared" si="15"/>
-        <v>7.92156862745098</v>
+        <v>7.9215686274509807</v>
       </c>
       <c r="P41" s="14">
         <f t="shared" si="16"/>
-        <v>13.4666666666667</v>
+        <v>13.466666666666669</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -6240,7 +5781,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -6267,11 +5808,11 @@
       </c>
       <c r="J42" s="11">
         <f t="shared" si="0"/>
-        <v>24.8198093466636</v>
+        <v>24.819809346663558</v>
       </c>
       <c r="K42" s="12">
         <f t="shared" si="11"/>
-        <v>26.8637936458006</v>
+        <v>26.863793645800566</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="12"/>
@@ -6279,19 +5820,19 @@
       </c>
       <c r="M42" s="13">
         <f t="shared" si="13"/>
-        <v>13.650895140665</v>
+        <v>13.650895140664959</v>
       </c>
       <c r="N42" s="13">
         <f t="shared" si="14"/>
-        <v>14.7750865051903</v>
+        <v>14.775086505190311</v>
       </c>
       <c r="O42" s="13">
         <f t="shared" si="15"/>
-        <v>12.5588235294118</v>
+        <v>12.558823529411764</v>
       </c>
       <c r="P42" s="14">
         <f t="shared" si="16"/>
-        <v>21.35</v>
+        <v>21.349999999999994</v>
       </c>
       <c r="Q42">
         <v>45</v>
@@ -6300,7 +5841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="2:18">
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
       <c r="B43">
         <v>17011401</v>
       </c>
@@ -6327,11 +5868,11 @@
       </c>
       <c r="J43" s="11">
         <f t="shared" si="0"/>
-        <v>12.7308894572322</v>
+        <v>12.730889457232166</v>
       </c>
       <c r="K43" s="12">
         <f t="shared" si="11"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827758</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="12"/>
@@ -6339,19 +5880,19 @@
       </c>
       <c r="M43" s="13">
         <f t="shared" si="13"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241247</v>
       </c>
       <c r="N43" s="13">
         <f t="shared" si="14"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870819</v>
       </c>
       <c r="O43" s="13">
         <f t="shared" si="15"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254901951</v>
       </c>
       <c r="P43" s="14">
         <f t="shared" si="16"/>
-        <v>14.9333333333333</v>
+        <v>14.93333333333333</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -6360,7 +5901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" ht="90.75" customHeight="1" spans="2:18">
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
       <c r="B44">
         <v>17011501</v>
       </c>
@@ -6387,11 +5928,11 @@
       </c>
       <c r="J44" s="11">
         <f t="shared" si="0"/>
-        <v>17.1355498721228</v>
+        <v>17.135549872122759</v>
       </c>
       <c r="K44" s="12">
         <f t="shared" si="11"/>
-        <v>18.5467128027682</v>
+        <v>18.546712802768166</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="12"/>
@@ -6399,19 +5940,19 @@
       </c>
       <c r="M44" s="13">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092071</v>
       </c>
       <c r="N44" s="13">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076124</v>
       </c>
       <c r="O44" s="13">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764705</v>
       </c>
       <c r="P44" s="14">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.099999999999994</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -6420,7 +5961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="90.75" customHeight="1" spans="2:18">
+    <row r="45" spans="2:18" ht="90.75" customHeight="1">
       <c r="B45">
         <v>17011502</v>
       </c>
@@ -6447,11 +5988,11 @@
       </c>
       <c r="J45" s="11">
         <f t="shared" si="0"/>
-        <v>21.3322483143455</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="12">
         <f t="shared" si="11"/>
-        <v>23.0890217049387</v>
+        <v>23.089021704938656</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="12"/>
@@ -6459,19 +6000,19 @@
       </c>
       <c r="M45" s="13">
         <f t="shared" si="13"/>
-        <v>11.73273657289</v>
+        <v>11.732736572890024</v>
       </c>
       <c r="N45" s="13">
         <f t="shared" si="14"/>
-        <v>12.6989619377163</v>
+        <v>12.698961937716263</v>
       </c>
       <c r="O45" s="13">
         <f t="shared" si="15"/>
-        <v>10.7941176470588</v>
+        <v>10.794117647058822</v>
       </c>
       <c r="P45" s="14">
         <f t="shared" si="16"/>
-        <v>18.35</v>
+        <v>18.349999999999994</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -6480,7 +6021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" ht="90.75" customHeight="1" spans="2:18">
+    <row r="46" spans="2:18" ht="90.75" customHeight="1">
       <c r="B46">
         <v>17011601</v>
       </c>
@@ -6507,11 +6048,11 @@
       </c>
       <c r="J46" s="11">
         <f t="shared" si="0"/>
-        <v>20.5572347516081</v>
+        <v>20.557234751608149</v>
       </c>
       <c r="K46" s="12">
         <f t="shared" si="11"/>
-        <v>22.2501834958582</v>
+        <v>22.250183495858234</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="12"/>
@@ -6519,19 +6060,19 @@
       </c>
       <c r="M46" s="13">
         <f t="shared" si="13"/>
-        <v>11.3064791133845</v>
+        <v>11.306479113384484</v>
       </c>
       <c r="N46" s="13">
         <f t="shared" si="14"/>
-        <v>12.237600922722</v>
+        <v>12.237600922722031</v>
       </c>
       <c r="O46" s="13">
         <f t="shared" si="15"/>
-        <v>10.4019607843137</v>
+        <v>10.401960784313726</v>
       </c>
       <c r="P46" s="14">
         <f t="shared" si="16"/>
-        <v>17.6833333333333</v>
+        <v>17.683333333333337</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -6540,7 +6081,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="90.75" customHeight="1" spans="2:18">
+    <row r="47" spans="2:18" ht="90.75" customHeight="1">
       <c r="B47">
         <v>17011503</v>
       </c>
@@ -6567,11 +6108,11 @@
       </c>
       <c r="J47" s="11">
         <f t="shared" si="0"/>
-        <v>15.7315643648764</v>
+        <v>15.731564364876382</v>
       </c>
       <c r="K47" s="12">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630908</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="12"/>
@@ -6579,19 +6120,19 @@
       </c>
       <c r="M47" s="13">
         <f t="shared" si="13"/>
-        <v>11.7986732736573</v>
+        <v>11.798673273657286</v>
       </c>
       <c r="N47" s="13">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723182</v>
       </c>
       <c r="O47" s="13">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764705</v>
       </c>
       <c r="P47" s="14">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999989</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -6600,7 +6141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" ht="90.75" customHeight="1" spans="2:18">
+    <row r="48" spans="2:18" ht="90.75" customHeight="1">
       <c r="B48">
         <v>17011504</v>
       </c>
@@ -6627,11 +6168,11 @@
       </c>
       <c r="J48" s="11">
         <f t="shared" si="0"/>
-        <v>15.7315643648764</v>
+        <v>15.731564364876382</v>
       </c>
       <c r="K48" s="12">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630908</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="12"/>
@@ -6639,19 +6180,19 @@
       </c>
       <c r="M48" s="13">
         <f t="shared" si="13"/>
-        <v>11.7986732736573</v>
+        <v>11.798673273657286</v>
       </c>
       <c r="N48" s="13">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723182</v>
       </c>
       <c r="O48" s="13">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764705</v>
       </c>
       <c r="P48" s="14">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999989</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -6660,7 +6201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" ht="90.75" customHeight="1" spans="2:18">
+    <row r="49" spans="2:18" ht="90.75" customHeight="1">
       <c r="B49">
         <v>17011602</v>
       </c>
@@ -6687,11 +6228,11 @@
       </c>
       <c r="J49" s="11">
         <f t="shared" si="0"/>
-        <v>16.4961636828644</v>
+        <v>16.496163682864449</v>
       </c>
       <c r="K49" s="12">
         <f t="shared" si="11"/>
-        <v>17.8546712802768</v>
+        <v>17.854671280276815</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="12"/>
@@ -6699,19 +6240,19 @@
       </c>
       <c r="M49" s="13">
         <f t="shared" si="13"/>
-        <v>12.3721227621483</v>
+        <v>12.372122762148337</v>
       </c>
       <c r="N49" s="13">
         <f t="shared" si="14"/>
-        <v>13.3910034602076</v>
+        <v>13.391003460207612</v>
       </c>
       <c r="O49" s="13">
         <f t="shared" si="15"/>
-        <v>11.3823529411765</v>
+        <v>11.382352941176469</v>
       </c>
       <c r="P49" s="14">
         <f t="shared" si="16"/>
-        <v>19.35</v>
+        <v>19.349999999999994</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -6720,7 +6261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" ht="90.75" customHeight="1" spans="2:18">
+    <row r="50" spans="2:18" ht="90.75" customHeight="1">
       <c r="B50">
         <v>17011901</v>
       </c>
@@ -6746,32 +6287,32 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$63*H50+$M$63)*$L$63)/(1-G50)/(1-$O$63)/(1-I50)/$N$63</f>
-        <v>17.0696737192901</v>
+        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$68*H50+$M$68)*$L$68)/(1-G50)/(1-$O$68)/(1-I50)/$N$68</f>
+        <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$63*H50+$M$63)*$L$63)/(1-G50)/(1-$P$63)/(1-I50)/$N$63</f>
-        <v>18.4754115549963</v>
+        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$68*H50+$M$68)*$L$68)/(1-G50)/(1-$P$68)/(1-I50)/$N$68</f>
+        <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$63*H50+$M$63)*$L$63</f>
+        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$68*H50+$M$68)*$L$68</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$63)/$N$63</f>
-        <v>9.38832054560955</v>
+        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$68)/$N$68</f>
+        <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$63)/$N$63</f>
-        <v>10.161476355248</v>
+        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$68)/$N$68</f>
+        <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$63</f>
-        <v>8.63725490196078</v>
+        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$68</f>
+        <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P55" si="23">O50*$N$63-L50</f>
-        <v>14.6833333333333</v>
+        <f t="shared" ref="P50:P55" si="23">O50*$N$68-L50</f>
+        <v>14.68333333333333</v>
       </c>
       <c r="Q50">
         <v>25</v>
@@ -6780,7 +6321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" ht="90.75" customHeight="1" spans="2:18">
+    <row r="51" spans="2:18" ht="90.75" customHeight="1">
       <c r="B51">
         <v>17011902</v>
       </c>
@@ -6807,11 +6348,11 @@
       </c>
       <c r="J51" s="11">
         <f t="shared" si="17"/>
-        <v>14.3329070758738</v>
+        <v>14.332907075873825</v>
       </c>
       <c r="K51" s="12">
         <f t="shared" si="18"/>
-        <v>15.5132641291811</v>
+        <v>15.51326412918108</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="19"/>
@@ -6819,19 +6360,19 @@
       </c>
       <c r="M51" s="13">
         <f t="shared" si="20"/>
-        <v>10.7496803069054</v>
+        <v>10.749680306905368</v>
       </c>
       <c r="N51" s="13">
         <f t="shared" si="21"/>
-        <v>11.6349480968858</v>
+        <v>11.634948096885811</v>
       </c>
       <c r="O51" s="13">
         <f t="shared" si="22"/>
-        <v>9.88970588235294</v>
+        <v>9.8897058823529385</v>
       </c>
       <c r="P51" s="14">
         <f t="shared" si="23"/>
-        <v>13.45</v>
+        <v>13.449999999999989</v>
       </c>
       <c r="Q51">
         <v>0</v>
@@ -6840,7 +6381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" ht="90.75" customHeight="1" spans="2:18">
+    <row r="52" spans="2:18" ht="90.75" customHeight="1">
       <c r="B52">
         <v>17020501</v>
       </c>
@@ -6867,11 +6408,11 @@
       </c>
       <c r="J52" s="11">
         <f t="shared" si="17"/>
-        <v>23.4574808184143</v>
+        <v>23.457480818414318</v>
       </c>
       <c r="K52" s="12">
         <f t="shared" si="18"/>
-        <v>25.3892733564014</v>
+        <v>25.389273356401382</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" si="19"/>
@@ -6879,19 +6420,19 @@
       </c>
       <c r="M52" s="13">
         <f t="shared" si="20"/>
-        <v>17.5931106138107</v>
+        <v>17.593110613810737</v>
       </c>
       <c r="N52" s="13">
         <f t="shared" si="21"/>
-        <v>19.041955017301</v>
+        <v>19.041955017301035</v>
       </c>
       <c r="O52" s="13">
         <f t="shared" si="22"/>
-        <v>16.1856617647059</v>
+        <v>16.18566176470588</v>
       </c>
       <c r="P52" s="14">
         <f t="shared" si="23"/>
-        <v>22.0125</v>
+        <v>22.012499999999989</v>
       </c>
       <c r="Q52">
         <v>30</v>
@@ -6900,7 +6441,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" ht="90.75" customHeight="1" spans="2:18">
+    <row r="53" spans="2:18" ht="90.75" customHeight="1">
       <c r="B53">
         <v>17020502</v>
       </c>
@@ -6927,11 +6468,11 @@
       </c>
       <c r="J53" s="11">
         <f t="shared" si="17"/>
-        <v>24.2774455319885</v>
+        <v>24.27744553198854</v>
       </c>
       <c r="K53" s="12">
         <f t="shared" si="18"/>
-        <v>26.2767645757994</v>
+        <v>26.276764575799358</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" si="19"/>
@@ -6939,19 +6480,19 @@
       </c>
       <c r="M53" s="13">
         <f t="shared" si="20"/>
-        <v>16.994211872392</v>
+        <v>16.994211872391976</v>
       </c>
       <c r="N53" s="13">
         <f t="shared" si="21"/>
-        <v>18.3937352030596</v>
+        <v>18.393735203059553</v>
       </c>
       <c r="O53" s="13">
         <f t="shared" si="22"/>
-        <v>15.6346749226006</v>
+        <v>15.634674922600619</v>
       </c>
       <c r="P53" s="14">
         <f t="shared" si="23"/>
-        <v>25.5157894736842</v>
+        <v>25.515789473684208</v>
       </c>
       <c r="Q53">
         <v>30</v>
@@ -6960,7 +6501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" ht="90.75" customHeight="1" spans="2:18">
+    <row r="54" spans="2:18" ht="90.75" customHeight="1">
       <c r="B54">
         <v>17020601</v>
       </c>
@@ -6987,11 +6528,11 @@
       </c>
       <c r="J54" s="11">
         <f t="shared" si="17"/>
-        <v>20.3518907563025</v>
+        <v>20.35189075630252</v>
       </c>
       <c r="K54" s="12">
         <f t="shared" si="18"/>
-        <v>22.0279288185863</v>
+        <v>22.027928818586258</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" si="19"/>
@@ -6999,19 +6540,19 @@
       </c>
       <c r="M54" s="13">
         <f t="shared" si="20"/>
-        <v>14.2463235294118</v>
+        <v>14.246323529411763</v>
       </c>
       <c r="N54" s="13">
         <f t="shared" si="21"/>
-        <v>15.4195501730104</v>
+        <v>15.41955017301038</v>
       </c>
       <c r="O54" s="13">
         <f t="shared" si="22"/>
-        <v>13.1066176470588</v>
+        <v>13.106617647058822</v>
       </c>
       <c r="P54" s="14">
         <f t="shared" si="23"/>
-        <v>17.825</v>
+        <v>17.824999999999989</v>
       </c>
       <c r="Q54">
         <v>30</v>
@@ -7020,7 +6561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" ht="90.75" customHeight="1" spans="2:18">
+    <row r="55" spans="2:18" ht="90.75" customHeight="1">
       <c r="B55">
         <v>17020701</v>
       </c>
@@ -7047,11 +6588,11 @@
       </c>
       <c r="J55" s="11">
         <f t="shared" si="17"/>
-        <v>24.4907745706978</v>
+        <v>24.490774570697841</v>
       </c>
       <c r="K55" s="12">
         <f t="shared" si="18"/>
-        <v>26.5076618882847</v>
+        <v>26.507661888284723</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="19"/>
@@ -7059,19 +6600,19 @@
       </c>
       <c r="M55" s="13">
         <f t="shared" si="20"/>
-        <v>17.1435421994885</v>
+        <v>17.14354219948849</v>
       </c>
       <c r="N55" s="13">
         <f t="shared" si="21"/>
-        <v>18.5553633217993</v>
+        <v>18.555363321799305</v>
       </c>
       <c r="O55" s="13">
         <f t="shared" si="22"/>
-        <v>15.7720588235294</v>
+        <v>15.772058823529409</v>
       </c>
       <c r="P55" s="14">
         <f t="shared" si="23"/>
-        <v>21.45</v>
+        <v>21.449999999999989</v>
       </c>
       <c r="Q55">
         <v>30</v>
@@ -7080,7 +6621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" ht="90.75" customHeight="1" spans="2:18">
+    <row r="56" spans="2:18" ht="90.75" customHeight="1">
       <c r="B56">
         <v>17020801</v>
       </c>
@@ -7106,32 +6647,32 @@
         <v>0.25</v>
       </c>
       <c r="J56" s="11">
-        <f t="shared" ref="J56:J60" si="24">(E56+F56+($K$63*H56+$M$63)*$L$63)/(1-G56)/(1-$O$63)/(1-I56)/$N$63</f>
-        <v>12.9475703324808</v>
+        <f>(E56+F56+($K$68*H56+$M$68)*$L$68)/(1-G56)/(1-$O$68)/(1-I56)/$N$68</f>
+        <v>12.947570332480817</v>
       </c>
       <c r="K56" s="12">
-        <f t="shared" ref="K56:K60" si="25">(E56+F56+($K$63*H56+$M$63)*$L$63)/(1-G56)/(1-$P$63)/(1-I56)/$N$63</f>
-        <v>14.0138408304498</v>
+        <f>(E56+F56+($K$68*H56+$M$68)*$L$68)/(1-G56)/(1-$P$68)/(1-I56)/$N$68</f>
+        <v>14.013840830449828</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" ref="L56:L60" si="26">E56+F56+($K$63*H56+$M$63)*$L$63</f>
-        <v>48.6</v>
+        <f>E56+F56+($K$68*H56+$M$68)*$L$68</f>
+        <v>48.599999999999994</v>
       </c>
       <c r="M56" s="13">
-        <f t="shared" ref="M56:M60" si="27">L56/(1-G56)/(1-$O$63)/$N$63</f>
-        <v>9.71067774936061</v>
+        <f>L56/(1-G56)/(1-$O$68)/$N$68</f>
+        <v>9.7106777493606113</v>
       </c>
       <c r="N56" s="13">
-        <f t="shared" ref="N56:N60" si="28">L56/(1-G56)/(1-$P$63)/$N$63</f>
-        <v>10.5103806228374</v>
+        <f>L56/(1-G56)/(1-$P$68)/$N$68</f>
+        <v>10.510380622837371</v>
       </c>
       <c r="O56" s="13">
-        <f t="shared" ref="O56:O60" si="29">L56/(1-G56)/$N$63</f>
-        <v>8.93382352941176</v>
+        <f>L56/(1-G56)/$N$68</f>
+        <v>8.9338235294117645</v>
       </c>
       <c r="P56" s="14">
-        <f t="shared" ref="P56:P60" si="30">O56*$N$63-L56</f>
-        <v>12.15</v>
+        <f>O56*$N$68-L56</f>
+        <v>12.150000000000006</v>
       </c>
       <c r="Q56">
         <v>30</v>
@@ -7140,7 +6681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" ht="90.75" customHeight="1" spans="2:18">
+    <row r="57" spans="2:18" ht="90.75" customHeight="1">
       <c r="B57">
         <v>17020901</v>
       </c>
@@ -7166,32 +6707,32 @@
         <v>0.45</v>
       </c>
       <c r="J57" s="11">
-        <f t="shared" si="24"/>
-        <v>19.6538595675424</v>
+        <f>(E57+F57+($K$68*H57+$M$68)*$L$68)/(1-G57)/(1-$O$68)/(1-I57)/$N$68</f>
+        <v>19.653859567542423</v>
       </c>
       <c r="K57" s="12">
-        <f t="shared" si="25"/>
-        <v>21.2724127083989</v>
+        <f>(E57+F57+($K$68*H57+$M$68)*$L$68)/(1-G57)/(1-$P$68)/(1-I57)/$N$68</f>
+        <v>21.272412708398864</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="26"/>
-        <v>54.1</v>
+        <f>E57+F57+($K$68*H57+$M$68)*$L$68</f>
+        <v>54.099999999999994</v>
       </c>
       <c r="M57" s="13">
-        <f t="shared" si="27"/>
-        <v>10.8096227621483</v>
+        <f>L57/(1-G57)/(1-$O$68)/$N$68</f>
+        <v>10.809622762148335</v>
       </c>
       <c r="N57" s="13">
-        <f t="shared" si="28"/>
-        <v>11.6998269896194</v>
+        <f>L57/(1-G57)/(1-$P$68)/$N$68</f>
+        <v>11.699826989619377</v>
       </c>
       <c r="O57" s="13">
-        <f t="shared" si="29"/>
-        <v>9.94485294117647</v>
+        <f>L57/(1-G57)/$N$68</f>
+        <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="14">
-        <f t="shared" si="30"/>
-        <v>13.525</v>
+        <f>O57*$N$68-L57</f>
+        <v>13.524999999999991</v>
       </c>
       <c r="Q57">
         <v>45</v>
@@ -7200,7 +6741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" ht="90.75" customHeight="1" spans="2:18">
+    <row r="58" spans="2:18" ht="90.75" customHeight="1">
       <c r="B58">
         <v>17020901</v>
       </c>
@@ -7226,32 +6767,32 @@
         <v>0.4</v>
       </c>
       <c r="J58" s="11">
-        <f t="shared" si="24"/>
-        <v>24.9094202898551</v>
+        <f>(E58+F58+($K$68*H58+$M$68)*$L$68)/(1-G58)/(1-$O$68)/(1-I58)/$N$68</f>
+        <v>24.909420289855071</v>
       </c>
       <c r="K58" s="12">
-        <f t="shared" si="25"/>
-        <v>26.9607843137255</v>
+        <f>(E58+F58+($K$68*H58+$M$68)*$L$68)/(1-G58)/(1-$P$68)/(1-I58)/$N$68</f>
+        <v>26.960784313725487</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" si="26"/>
+        <f>E58+F58+($K$68*H58+$M$68)*$L$68</f>
         <v>74.8</v>
       </c>
       <c r="M58" s="13">
-        <f t="shared" si="27"/>
-        <v>14.945652173913</v>
+        <f>L58/(1-G58)/(1-$O$68)/$N$68</f>
+        <v>14.945652173913041</v>
       </c>
       <c r="N58" s="13">
-        <f t="shared" si="28"/>
-        <v>16.1764705882353</v>
+        <f>L58/(1-G58)/(1-$P$68)/$N$68</f>
+        <v>16.176470588235293</v>
       </c>
       <c r="O58" s="13">
-        <f t="shared" si="29"/>
-        <v>13.75</v>
+        <f>L58/(1-G58)/$N$68</f>
+        <v>13.749999999999998</v>
       </c>
       <c r="P58" s="14">
-        <f t="shared" si="30"/>
-        <v>18.7</v>
+        <f>O58*$N$68-L58</f>
+        <v>18.699999999999989</v>
       </c>
       <c r="Q58">
         <v>0</v>
@@ -7260,9 +6801,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" ht="90.75" customHeight="1" spans="2:18">
+    <row r="59" spans="2:18" ht="90.75" customHeight="1">
       <c r="B59">
-        <v>17020904</v>
+        <v>17021104</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -7286,32 +6827,32 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" si="24"/>
-        <v>15.6421264157837</v>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$68*H59+$M$68)*$L$68)/(1-G59)/(1-$O$68)/(1-I59)/$N$68</f>
+        <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" si="25"/>
-        <v>16.9303015323777</v>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$68*H59+$M$68)*$L$68)/(1-G59)/(1-$P$68)/(1-I59)/$N$68</f>
+        <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$68*H59+$M$68)*$L$68</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" si="27"/>
-        <v>10.9494884910486</v>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$68)/$N$68</f>
+        <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" si="28"/>
-        <v>11.8512110726644</v>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$68)/$N$68</f>
+        <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" si="29"/>
-        <v>10.0735294117647</v>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$68</f>
+        <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" si="30"/>
-        <v>13.7</v>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$68-L59</f>
+        <v>13.699999999999989</v>
       </c>
       <c r="Q59">
         <v>30</v>
@@ -7320,9 +6861,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" ht="90.75" customHeight="1" spans="2:18">
+    <row r="60" spans="2:18" ht="90.75" customHeight="1">
       <c r="B60">
-        <v>17020905</v>
+        <v>17021105</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>21</v>
@@ -7347,11 +6888,11 @@
       </c>
       <c r="J60" s="11">
         <f t="shared" si="24"/>
-        <v>15.6421264157837</v>
+        <v>15.642126415783704</v>
       </c>
       <c r="K60" s="12">
         <f t="shared" si="25"/>
-        <v>16.9303015323777</v>
+        <v>16.930301532377655</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" si="26"/>
@@ -7359,19 +6900,19 @@
       </c>
       <c r="M60" s="13">
         <f t="shared" si="27"/>
-        <v>10.9494884910486</v>
+        <v>10.949488491048593</v>
       </c>
       <c r="N60" s="13">
         <f t="shared" si="28"/>
-        <v>11.8512110726644</v>
+        <v>11.851211072664359</v>
       </c>
       <c r="O60" s="13">
         <f t="shared" si="29"/>
-        <v>10.0735294117647</v>
+        <v>10.073529411764705</v>
       </c>
       <c r="P60" s="14">
         <f t="shared" si="30"/>
-        <v>13.7</v>
+        <v>13.699999999999989</v>
       </c>
       <c r="Q60">
         <v>30</v>
@@ -7380,52 +6921,259 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="11:16">
-      <c r="K62" s="16" t="s">
+    <row r="61" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B61">
+        <v>17021101</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61">
+        <v>26</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H61">
+        <v>0.09</v>
+      </c>
+      <c r="I61" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J61" s="11">
+        <f>(E61+F61+($K$68*H61+$M$68)*$L$68)/(1-G61)/(1-$O$68)/(1-I61)/$N$68</f>
+        <v>11.309143222506394</v>
+      </c>
+      <c r="K61" s="12">
+        <f>(E61+F61+($K$68*H61+$M$68)*$L$68)/(1-G61)/(1-$P$68)/(1-I61)/$N$68</f>
+        <v>12.240484429065743</v>
+      </c>
+      <c r="L61" s="1">
+        <f>E61+F61+($K$68*H61+$M$68)*$L$68</f>
+        <v>42.45</v>
+      </c>
+      <c r="M61" s="13">
+        <f>L61/(1-G61)/(1-$O$68)/$N$68</f>
+        <v>8.4818574168797962</v>
+      </c>
+      <c r="N61" s="13">
+        <f>L61/(1-G61)/(1-$P$68)/$N$68</f>
+        <v>9.1803633217993088</v>
+      </c>
+      <c r="O61" s="13">
+        <f>L61/(1-G61)/$N$68</f>
+        <v>7.8033088235294121</v>
+      </c>
+      <c r="P61" s="14">
+        <f>O61*$N$68-L61</f>
+        <v>10.612499999999997</v>
+      </c>
+      <c r="Q61">
+        <v>25</v>
+      </c>
+      <c r="R61">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B62">
+        <v>17021102</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62">
+        <v>24</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H62">
+        <v>0.1</v>
+      </c>
+      <c r="I62" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J62" s="11">
+        <f>(E62+F62+($K$68*H62+$M$68)*$L$68)/(1-G62)/(1-$O$68)/(1-I62)/$N$68</f>
+        <v>11.736288718385904</v>
+      </c>
+      <c r="K62" s="12">
+        <f>(E62+F62+($K$68*H62+$M$68)*$L$68)/(1-G62)/(1-$P$68)/(1-I62)/$N$68</f>
+        <v>12.702806612841213</v>
+      </c>
+      <c r="L62" s="1">
+        <f>E62+F62+($K$68*H62+$M$68)*$L$68</f>
+        <v>41.3</v>
+      </c>
+      <c r="M62" s="13">
+        <f>L62/(1-G62)/(1-$O$68)/$N$68</f>
+        <v>8.8022165387894287</v>
+      </c>
+      <c r="N62" s="13">
+        <f>L62/(1-G62)/(1-$P$68)/$N$68</f>
+        <v>9.5271049596309112</v>
+      </c>
+      <c r="O62" s="13">
+        <f>L62/(1-G62)/$N$68</f>
+        <v>8.0980392156862742</v>
+      </c>
+      <c r="P62" s="14">
+        <f>O62*$N$68-L62</f>
+        <v>13.766666666666666</v>
+      </c>
+      <c r="Q62">
+        <v>25</v>
+      </c>
+      <c r="R62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" ht="90.75" customHeight="1">
+      <c r="B63">
+        <v>17021103</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63">
+        <v>24</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H63">
+        <v>0.1</v>
+      </c>
+      <c r="I63" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J63" s="11">
+        <f>(E63+F63+($K$68*H63+$M$68)*$L$68)/(1-G63)/(1-$O$68)/(1-I63)/$N$68</f>
+        <v>14.670360897982381</v>
+      </c>
+      <c r="K63" s="12">
+        <f>(E63+F63+($K$68*H63+$M$68)*$L$68)/(1-G63)/(1-$P$68)/(1-I63)/$N$68</f>
+        <v>15.878508266051519</v>
+      </c>
+      <c r="L63" s="1">
+        <f>E63+F63+($K$68*H63+$M$68)*$L$68</f>
+        <v>41.3</v>
+      </c>
+      <c r="M63" s="13">
+        <f>L63/(1-G63)/(1-$O$68)/$N$68</f>
+        <v>8.8022165387894287</v>
+      </c>
+      <c r="N63" s="13">
+        <f>L63/(1-G63)/(1-$P$68)/$N$68</f>
+        <v>9.5271049596309112</v>
+      </c>
+      <c r="O63" s="13">
+        <f>L63/(1-G63)/$N$68</f>
+        <v>8.0980392156862742</v>
+      </c>
+      <c r="P63" s="14">
+        <f>O63*$N$68-L63</f>
+        <v>13.766666666666666</v>
+      </c>
+      <c r="Q63">
+        <v>25</v>
+      </c>
+      <c r="R63">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" ht="90.75" customHeight="1">
+      <c r="C64" s="1"/>
+      <c r="D64" s="9"/>
+      <c r="G64" s="3"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="13"/>
+      <c r="N64" s="13"/>
+      <c r="O64" s="13"/>
+      <c r="P64" s="14"/>
+    </row>
+    <row r="65" spans="3:16" ht="90.75" customHeight="1">
+      <c r="C65" s="1"/>
+      <c r="D65" s="9"/>
+      <c r="G65" s="3"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="13"/>
+      <c r="P65" s="14"/>
+    </row>
+    <row r="67" spans="3:16">
+      <c r="K67" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L62" s="16" t="s">
+      <c r="L67" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="M62" s="16" t="s">
+      <c r="M67" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="N62" s="16" t="s">
+      <c r="N67" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O62" s="16" t="s">
+      <c r="O67" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="P62" s="16" t="s">
+      <c r="P67" s="16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="11:16">
-      <c r="K63" s="17">
+    <row r="68" spans="3:16">
+      <c r="K68" s="17">
         <v>100</v>
       </c>
-      <c r="L63" s="15">
+      <c r="L68" s="15">
         <v>0.85</v>
       </c>
-      <c r="M63">
+      <c r="M68">
         <v>8</v>
       </c>
-      <c r="N63">
+      <c r="N68">
         <v>6.8</v>
       </c>
-      <c r="O63" s="15">
+      <c r="O68" s="15">
         <v>0.08</v>
       </c>
-      <c r="P63" s="15">
+      <c r="P68" s="15">
         <v>0.15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C59 C60 C2:C58">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -7433,95 +7181,91 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
-    <hyperlink ref="D43" r:id="rId34" display="https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp"/>
-    <hyperlink ref="D44" r:id="rId35" display="https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW"/>
-    <hyperlink ref="D45" r:id="rId36" display="https://detail.1688.com/offer/525494755952.html?spm=a2615.7691456.0.0.2qsBMx"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://detail.1688.com/offer/525529106954.html?spm=a2615.7691456.0.0.4Tm2o6"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://detail.1688.com/offer/527560763616.html?spm=b26110380.sw311.0.0.p4j2tp"/>
-    <hyperlink ref="D50" r:id="rId39" display="https://detail.1688.com/offer/542627436877.html?spm=b26110380.sw1037004.0.0.aYzCim&amp;sk=consign"/>
-    <hyperlink ref="D52" r:id="rId40" display="https://detail.1688.com/offer/543024612109.html?spm=0.0.0.0.QG7IU6"/>
-    <hyperlink ref="D51" r:id="rId41" display="https://detail.1688.com/offer/543614766781.html?spm=b26110380.8015204.tkhy006.2.m9SOm8"/>
-    <hyperlink ref="D53" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D54" r:id="rId43" display="https://detail.1688.com/offer/45277079052.html?spm=a261y.7663282.0.0.8G3JEy&amp;sk=consign"/>
-    <hyperlink ref="D55" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D56" r:id="rId44" display="https://detail.1688.com/offer/38711199781.html?spm=b26110380.8015204.tkhy006.2.g0hkme"/>
-    <hyperlink ref="D57" r:id="rId45" display="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
-    <hyperlink ref="D58" r:id="rId46" display="https://detail.1688.com/offer/536596301611.html?spm=a2615.7691456.0.0.HFQWm0"/>
-    <hyperlink ref="D59" r:id="rId47" display="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
-    <hyperlink ref="D60" r:id="rId48" display="https://detail.1688.com/offer/543879481659.html?spm=a2615.7691456.0.0.UWc1Wy"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D49" r:id="rId40"/>
+    <hyperlink ref="D50" r:id="rId41"/>
+    <hyperlink ref="D52" r:id="rId42"/>
+    <hyperlink ref="D51" r:id="rId43"/>
+    <hyperlink ref="D53" r:id="rId44"/>
+    <hyperlink ref="D54" r:id="rId45"/>
+    <hyperlink ref="D55" r:id="rId46"/>
+    <hyperlink ref="D56" r:id="rId47"/>
+    <hyperlink ref="D57" r:id="rId48" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
+    <hyperlink ref="D58" r:id="rId49"/>
+    <hyperlink ref="D60" r:id="rId50"/>
+    <hyperlink ref="D63" r:id="rId51"/>
+    <hyperlink ref="D59" r:id="rId52" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId53"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17021106 牛仔 衬衫 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>产品标题</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/536596301611.html?spm=a2615.7691456.0.0.HFQWm0</t>
   </si>
   <si>
     <t>https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy</t>
@@ -296,6 +293,14 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/542163784708.html?spm=0.0.0.0.D3IAEt</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/536596301611.html?spm=a2615.7691456.0.0.HFQWm0</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/520727227145.html?spm=b26110380.7927930.tkhy006.2.4cRHSy</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -3029,6 +3034,44 @@
         <a:xfrm>
           <a:off x="0" y="66836512"/>
           <a:ext cx="1078329" cy="993912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>49697</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1067242</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>1109871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="图片 64" descr="QQ截图20170211233428.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="70228240"/>
+          <a:ext cx="1067242" cy="1060174"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3328,8 +3371,8 @@
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6748,8 +6791,8 @@
       <c r="C58" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>80</v>
+      <c r="D58" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E58">
         <v>49</v>
@@ -6809,7 +6852,7 @@
         <v>21</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E59">
         <v>29</v>
@@ -6869,7 +6912,7 @@
         <v>21</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E60">
         <v>29</v>
@@ -6929,7 +6972,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61">
         <v>26</v>
@@ -6989,7 +7032,7 @@
         <v>21</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E62">
         <v>24</v>
@@ -7049,7 +7092,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63">
         <v>24</v>
@@ -7102,17 +7145,64 @@
       </c>
     </row>
     <row r="64" spans="2:18" ht="90.75" customHeight="1">
-      <c r="C64" s="1"/>
-      <c r="D64" s="9"/>
-      <c r="G64" s="3"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
-      <c r="P64" s="14"/>
+      <c r="B64">
+        <v>17021106</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64">
+        <v>32</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H64">
+        <v>0.2</v>
+      </c>
+      <c r="I64" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J64" s="11">
+        <f>(E64+F64+($K$68*H64+$M$68)*$L$68)/(1-G64)/(1-$O$68)/(1-I64)/$N$68</f>
+        <v>19.248188405797102</v>
+      </c>
+      <c r="K64" s="12">
+        <f>(E64+F64+($K$68*H64+$M$68)*$L$68)/(1-G64)/(1-$P$68)/(1-I64)/$N$68</f>
+        <v>20.833333333333332</v>
+      </c>
+      <c r="L64" s="1">
+        <f>E64+F64+($K$68*H64+$M$68)*$L$68</f>
+        <v>57.8</v>
+      </c>
+      <c r="M64" s="13">
+        <f>L64/(1-G64)/(1-$O$68)/$N$68</f>
+        <v>11.548913043478258</v>
+      </c>
+      <c r="N64" s="13">
+        <f>L64/(1-G64)/(1-$P$68)/$N$68</f>
+        <v>12.499999999999998</v>
+      </c>
+      <c r="O64" s="13">
+        <f>L64/(1-G64)/$N$68</f>
+        <v>10.624999999999998</v>
+      </c>
+      <c r="P64" s="14">
+        <f>O64*$N$68-L64</f>
+        <v>14.449999999999989</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>25</v>
+      </c>
     </row>
     <row r="65" spans="3:16" ht="90.75" customHeight="1">
       <c r="C65" s="1"/>
@@ -7129,22 +7219,22 @@
     </row>
     <row r="67" spans="3:16">
       <c r="K67" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L67" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L67" s="16" t="s">
+      <c r="M67" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="M67" s="16" t="s">
+      <c r="N67" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="N67" s="16" t="s">
+      <c r="O67" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O67" s="16" t="s">
+      <c r="P67" s="16" t="s">
         <v>87</v>
-      </c>
-      <c r="P67" s="16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="68" spans="3:16">
@@ -7233,10 +7323,11 @@
     <hyperlink ref="D60" r:id="rId50"/>
     <hyperlink ref="D63" r:id="rId51"/>
     <hyperlink ref="D59" r:id="rId52" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
+    <hyperlink ref="D64" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId53"/>
+  <drawing r:id="rId54"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17021201 by hjx 滑雪裤上传
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
   <si>
     <t>产品标题</t>
   </si>
@@ -302,6 +302,17 @@
   <si>
     <t>https://detail.1688.com/offer/520727227145.html?spm=b26110380.7927930.tkhy006.2.4cRHSy</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/45288474070.html?spm=0.0.0.0.ROTFEe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/542800642320.html?spm=b26110380.7927930.xshy005.529.St2Fw9</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/45422676746.html?spm=b26110380.8015204.xshy005.17.K9Fn6R</t>
   </si>
 </sst>
 </file>
@@ -403,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -461,6 +472,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -3072,6 +3086,44 @@
         <a:xfrm>
           <a:off x="0" y="70228240"/>
           <a:ext cx="1067242" cy="1060174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1060173</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>1068456</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="图片 65" descr="QQ截图20170212223004.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33130" y="71371239"/>
+          <a:ext cx="1027043" cy="1027043"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3368,11 +3420,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
+      <selection pane="bottomLeft" activeCell="L66" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3478,31 +3530,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$68*H2+$M$68)*$L$68)/(1-G2)/(1-$O$68)/(1-I2)/$N$68</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$69*H2+$M$69)*$L$69)/(1-G2)/(1-$O$69)/(1-I2)/$N$69</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$68*H2+$M$68)*$L$68)/(1-G2)/(1-$P$68)/(1-I2)/$N$68</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$69*H2+$M$69)*$L$69)/(1-G2)/(1-$P$69)/(1-I2)/$N$69</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$68*H2+$M$68)*$L$68</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$69*H2+$M$69)*$L$69</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$68)/$N$68</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$69)/$N$69</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$68)/$N$68</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$69)/$N$69</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$68</f>
+        <f>L2/(1-G2)/$N$69</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$68-L2</f>
+        <f>O2*$N$69-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -3543,27 +3595,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$68*H3+$M$68)*$L$68)/(1-G3)/(1-$P$68)/(1-I3)/$N$68</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$69*H3+$M$69)*$L$69)/(1-G3)/(1-$P$69)/(1-I3)/$N$69</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$68*H3+$M$68)*$L$68</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$69*H3+$M$69)*$L$69</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$68)/$N$68</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$69)/$N$69</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$68)/$N$68</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$69)/$N$69</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$68</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$69</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$68-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$69-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -3790,27 +3842,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$68*H7+$M$68)*$L$68)/(1-G7)/(1-$P$68)/(1-I7)/$N$68</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$69*H7+$M$69)*$L$69)/(1-G7)/(1-$P$69)/(1-I7)/$N$69</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$68*H7+$M$68)*$L$68</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$69*H7+$M$69)*$L$69</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$68)/$N$68</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$69)/$N$69</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$68)/$N$68</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$69)/$N$69</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$68</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$69</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$68-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$69-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -6330,31 +6382,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$68*H50+$M$68)*$L$68)/(1-G50)/(1-$O$68)/(1-I50)/$N$68</f>
+        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$69*H50+$M$69)*$L$69)/(1-G50)/(1-$O$69)/(1-I50)/$N$69</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$68*H50+$M$68)*$L$68)/(1-G50)/(1-$P$68)/(1-I50)/$N$68</f>
+        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$69*H50+$M$69)*$L$69)/(1-G50)/(1-$P$69)/(1-I50)/$N$69</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$68*H50+$M$68)*$L$68</f>
+        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$69*H50+$M$69)*$L$69</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$68)/$N$68</f>
+        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$69)/$N$69</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$68)/$N$68</f>
+        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$69)/$N$69</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$68</f>
+        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$69</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P55" si="23">O50*$N$68-L50</f>
+        <f t="shared" ref="P50:P55" si="23">O50*$N$69-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -6690,31 +6742,31 @@
         <v>0.25</v>
       </c>
       <c r="J56" s="11">
-        <f>(E56+F56+($K$68*H56+$M$68)*$L$68)/(1-G56)/(1-$O$68)/(1-I56)/$N$68</f>
+        <f>(E56+F56+($K$69*H56+$M$69)*$L$69)/(1-G56)/(1-$O$69)/(1-I56)/$N$69</f>
         <v>12.947570332480817</v>
       </c>
       <c r="K56" s="12">
-        <f>(E56+F56+($K$68*H56+$M$68)*$L$68)/(1-G56)/(1-$P$68)/(1-I56)/$N$68</f>
+        <f>(E56+F56+($K$69*H56+$M$69)*$L$69)/(1-G56)/(1-$P$69)/(1-I56)/$N$69</f>
         <v>14.013840830449828</v>
       </c>
       <c r="L56" s="1">
-        <f>E56+F56+($K$68*H56+$M$68)*$L$68</f>
+        <f>E56+F56+($K$69*H56+$M$69)*$L$69</f>
         <v>48.599999999999994</v>
       </c>
       <c r="M56" s="13">
-        <f>L56/(1-G56)/(1-$O$68)/$N$68</f>
+        <f>L56/(1-G56)/(1-$O$69)/$N$69</f>
         <v>9.7106777493606113</v>
       </c>
       <c r="N56" s="13">
-        <f>L56/(1-G56)/(1-$P$68)/$N$68</f>
+        <f>L56/(1-G56)/(1-$P$69)/$N$69</f>
         <v>10.510380622837371</v>
       </c>
       <c r="O56" s="13">
-        <f>L56/(1-G56)/$N$68</f>
+        <f>L56/(1-G56)/$N$69</f>
         <v>8.9338235294117645</v>
       </c>
       <c r="P56" s="14">
-        <f>O56*$N$68-L56</f>
+        <f>O56*$N$69-L56</f>
         <v>12.150000000000006</v>
       </c>
       <c r="Q56">
@@ -6750,31 +6802,31 @@
         <v>0.45</v>
       </c>
       <c r="J57" s="11">
-        <f>(E57+F57+($K$68*H57+$M$68)*$L$68)/(1-G57)/(1-$O$68)/(1-I57)/$N$68</f>
+        <f>(E57+F57+($K$69*H57+$M$69)*$L$69)/(1-G57)/(1-$O$69)/(1-I57)/$N$69</f>
         <v>19.653859567542423</v>
       </c>
       <c r="K57" s="12">
-        <f>(E57+F57+($K$68*H57+$M$68)*$L$68)/(1-G57)/(1-$P$68)/(1-I57)/$N$68</f>
+        <f>(E57+F57+($K$69*H57+$M$69)*$L$69)/(1-G57)/(1-$P$69)/(1-I57)/$N$69</f>
         <v>21.272412708398864</v>
       </c>
       <c r="L57" s="1">
-        <f>E57+F57+($K$68*H57+$M$68)*$L$68</f>
+        <f>E57+F57+($K$69*H57+$M$69)*$L$69</f>
         <v>54.099999999999994</v>
       </c>
       <c r="M57" s="13">
-        <f>L57/(1-G57)/(1-$O$68)/$N$68</f>
+        <f>L57/(1-G57)/(1-$O$69)/$N$69</f>
         <v>10.809622762148335</v>
       </c>
       <c r="N57" s="13">
-        <f>L57/(1-G57)/(1-$P$68)/$N$68</f>
+        <f>L57/(1-G57)/(1-$P$69)/$N$69</f>
         <v>11.699826989619377</v>
       </c>
       <c r="O57" s="13">
-        <f>L57/(1-G57)/$N$68</f>
+        <f>L57/(1-G57)/$N$69</f>
         <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="14">
-        <f>O57*$N$68-L57</f>
+        <f>O57*$N$69-L57</f>
         <v>13.524999999999991</v>
       </c>
       <c r="Q57">
@@ -6810,31 +6862,31 @@
         <v>0.4</v>
       </c>
       <c r="J58" s="11">
-        <f>(E58+F58+($K$68*H58+$M$68)*$L$68)/(1-G58)/(1-$O$68)/(1-I58)/$N$68</f>
+        <f>(E58+F58+($K$69*H58+$M$69)*$L$69)/(1-G58)/(1-$O$69)/(1-I58)/$N$69</f>
         <v>24.909420289855071</v>
       </c>
       <c r="K58" s="12">
-        <f>(E58+F58+($K$68*H58+$M$68)*$L$68)/(1-G58)/(1-$P$68)/(1-I58)/$N$68</f>
+        <f>(E58+F58+($K$69*H58+$M$69)*$L$69)/(1-G58)/(1-$P$69)/(1-I58)/$N$69</f>
         <v>26.960784313725487</v>
       </c>
       <c r="L58" s="1">
-        <f>E58+F58+($K$68*H58+$M$68)*$L$68</f>
+        <f>E58+F58+($K$69*H58+$M$69)*$L$69</f>
         <v>74.8</v>
       </c>
       <c r="M58" s="13">
-        <f>L58/(1-G58)/(1-$O$68)/$N$68</f>
+        <f>L58/(1-G58)/(1-$O$69)/$N$69</f>
         <v>14.945652173913041</v>
       </c>
       <c r="N58" s="13">
-        <f>L58/(1-G58)/(1-$P$68)/$N$68</f>
+        <f>L58/(1-G58)/(1-$P$69)/$N$69</f>
         <v>16.176470588235293</v>
       </c>
       <c r="O58" s="13">
-        <f>L58/(1-G58)/$N$68</f>
+        <f>L58/(1-G58)/$N$69</f>
         <v>13.749999999999998</v>
       </c>
       <c r="P58" s="14">
-        <f>O58*$N$68-L58</f>
+        <f>O58*$N$69-L58</f>
         <v>18.699999999999989</v>
       </c>
       <c r="Q58">
@@ -6870,31 +6922,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$68*H59+$M$68)*$L$68)/(1-G59)/(1-$O$68)/(1-I59)/$N$68</f>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$69*H59+$M$69)*$L$69)/(1-G59)/(1-$O$69)/(1-I59)/$N$69</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$68*H59+$M$68)*$L$68)/(1-G59)/(1-$P$68)/(1-I59)/$N$68</f>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$69*H59+$M$69)*$L$69)/(1-G59)/(1-$P$69)/(1-I59)/$N$69</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$68*H59+$M$68)*$L$68</f>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$69*H59+$M$69)*$L$69</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$68)/$N$68</f>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$69)/$N$69</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$68)/$N$68</f>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$69)/$N$69</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$68</f>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$69</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" ref="P59:P60" si="30">O59*$N$68-L59</f>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$69-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -6990,31 +7042,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f>(E61+F61+($K$68*H61+$M$68)*$L$68)/(1-G61)/(1-$O$68)/(1-I61)/$N$68</f>
+        <f>(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$O$69)/(1-I61)/$N$69</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f>(E61+F61+($K$68*H61+$M$68)*$L$68)/(1-G61)/(1-$P$68)/(1-I61)/$N$68</f>
+        <f>(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$P$69)/(1-I61)/$N$69</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f>E61+F61+($K$68*H61+$M$68)*$L$68</f>
+        <f>E61+F61+($K$69*H61+$M$69)*$L$69</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f>L61/(1-G61)/(1-$O$68)/$N$68</f>
+        <f>L61/(1-G61)/(1-$O$69)/$N$69</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f>L61/(1-G61)/(1-$P$68)/$N$68</f>
+        <f>L61/(1-G61)/(1-$P$69)/$N$69</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f>L61/(1-G61)/$N$68</f>
+        <f>L61/(1-G61)/$N$69</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f>O61*$N$68-L61</f>
+        <f>O61*$N$69-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -7050,31 +7102,31 @@
         <v>0.25</v>
       </c>
       <c r="J62" s="11">
-        <f>(E62+F62+($K$68*H62+$M$68)*$L$68)/(1-G62)/(1-$O$68)/(1-I62)/$N$68</f>
+        <f>(E62+F62+($K$69*H62+$M$69)*$L$69)/(1-G62)/(1-$O$69)/(1-I62)/$N$69</f>
         <v>11.736288718385904</v>
       </c>
       <c r="K62" s="12">
-        <f>(E62+F62+($K$68*H62+$M$68)*$L$68)/(1-G62)/(1-$P$68)/(1-I62)/$N$68</f>
+        <f>(E62+F62+($K$69*H62+$M$69)*$L$69)/(1-G62)/(1-$P$69)/(1-I62)/$N$69</f>
         <v>12.702806612841213</v>
       </c>
       <c r="L62" s="1">
-        <f>E62+F62+($K$68*H62+$M$68)*$L$68</f>
+        <f>E62+F62+($K$69*H62+$M$69)*$L$69</f>
         <v>41.3</v>
       </c>
       <c r="M62" s="13">
-        <f>L62/(1-G62)/(1-$O$68)/$N$68</f>
+        <f>L62/(1-G62)/(1-$O$69)/$N$69</f>
         <v>8.8022165387894287</v>
       </c>
       <c r="N62" s="13">
-        <f>L62/(1-G62)/(1-$P$68)/$N$68</f>
+        <f>L62/(1-G62)/(1-$P$69)/$N$69</f>
         <v>9.5271049596309112</v>
       </c>
       <c r="O62" s="13">
-        <f>L62/(1-G62)/$N$68</f>
+        <f>L62/(1-G62)/$N$69</f>
         <v>8.0980392156862742</v>
       </c>
       <c r="P62" s="14">
-        <f>O62*$N$68-L62</f>
+        <f>O62*$N$69-L62</f>
         <v>13.766666666666666</v>
       </c>
       <c r="Q62">
@@ -7110,31 +7162,31 @@
         <v>0.4</v>
       </c>
       <c r="J63" s="11">
-        <f>(E63+F63+($K$68*H63+$M$68)*$L$68)/(1-G63)/(1-$O$68)/(1-I63)/$N$68</f>
+        <f>(E63+F63+($K$69*H63+$M$69)*$L$69)/(1-G63)/(1-$O$69)/(1-I63)/$N$69</f>
         <v>14.670360897982381</v>
       </c>
       <c r="K63" s="12">
-        <f>(E63+F63+($K$68*H63+$M$68)*$L$68)/(1-G63)/(1-$P$68)/(1-I63)/$N$68</f>
+        <f>(E63+F63+($K$69*H63+$M$69)*$L$69)/(1-G63)/(1-$P$69)/(1-I63)/$N$69</f>
         <v>15.878508266051519</v>
       </c>
       <c r="L63" s="1">
-        <f>E63+F63+($K$68*H63+$M$68)*$L$68</f>
+        <f>E63+F63+($K$69*H63+$M$69)*$L$69</f>
         <v>41.3</v>
       </c>
       <c r="M63" s="13">
-        <f>L63/(1-G63)/(1-$O$68)/$N$68</f>
+        <f>L63/(1-G63)/(1-$O$69)/$N$69</f>
         <v>8.8022165387894287</v>
       </c>
       <c r="N63" s="13">
-        <f>L63/(1-G63)/(1-$P$68)/$N$68</f>
+        <f>L63/(1-G63)/(1-$P$69)/$N$69</f>
         <v>9.5271049596309112</v>
       </c>
       <c r="O63" s="13">
-        <f>L63/(1-G63)/$N$68</f>
+        <f>L63/(1-G63)/$N$69</f>
         <v>8.0980392156862742</v>
       </c>
       <c r="P63" s="14">
-        <f>O63*$N$68-L63</f>
+        <f>O63*$N$69-L63</f>
         <v>13.766666666666666</v>
       </c>
       <c r="Q63">
@@ -7167,93 +7219,160 @@
         <v>0.2</v>
       </c>
       <c r="I64" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J64" s="11">
+        <f>(E64+F64+($K$69*H64+$M$69)*$L$69)/(1-G64)/(1-$O$69)/(1-I64)/$N$69</f>
+        <v>15.398550724637678</v>
+      </c>
+      <c r="K64" s="12">
+        <f>(E64+F64+($K$69*H64+$M$69)*$L$69)/(1-G64)/(1-$P$69)/(1-I64)/$N$69</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="L64" s="1">
+        <f>E64+F64+($K$69*H64+$M$69)*$L$69</f>
+        <v>57.8</v>
+      </c>
+      <c r="M64" s="13">
+        <f>L64/(1-G64)/(1-$O$69)/$N$69</f>
+        <v>11.548913043478258</v>
+      </c>
+      <c r="N64" s="13">
+        <f>L64/(1-G64)/(1-$P$69)/$N$69</f>
+        <v>12.499999999999998</v>
+      </c>
+      <c r="O64" s="13">
+        <f>L64/(1-G64)/$N$69</f>
+        <v>10.624999999999998</v>
+      </c>
+      <c r="P64" s="14">
+        <f>O64*$N$69-L64</f>
+        <v>14.449999999999989</v>
+      </c>
+      <c r="Q64">
+        <v>25</v>
+      </c>
+      <c r="R64">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B65">
+        <v>17021201</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65">
+        <v>22</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="H65">
+        <v>0.2</v>
+      </c>
+      <c r="I65" s="15">
         <v>0.4</v>
       </c>
-      <c r="J64" s="11">
-        <f>(E64+F64+($K$68*H64+$M$68)*$L$68)/(1-G64)/(1-$O$68)/(1-I64)/$N$68</f>
-        <v>19.248188405797102</v>
-      </c>
-      <c r="K64" s="12">
-        <f>(E64+F64+($K$68*H64+$M$68)*$L$68)/(1-G64)/(1-$P$68)/(1-I64)/$N$68</f>
-        <v>20.833333333333332</v>
-      </c>
-      <c r="L64" s="1">
-        <f>E64+F64+($K$68*H64+$M$68)*$L$68</f>
-        <v>57.8</v>
-      </c>
-      <c r="M64" s="13">
-        <f>L64/(1-G64)/(1-$O$68)/$N$68</f>
-        <v>11.548913043478258</v>
-      </c>
-      <c r="N64" s="13">
-        <f>L64/(1-G64)/(1-$P$68)/$N$68</f>
-        <v>12.499999999999998</v>
-      </c>
-      <c r="O64" s="13">
-        <f>L64/(1-G64)/$N$68</f>
-        <v>10.624999999999998</v>
-      </c>
-      <c r="P64" s="14">
-        <f>O64*$N$68-L64</f>
-        <v>14.449999999999989</v>
-      </c>
-      <c r="Q64">
-        <v>0</v>
-      </c>
-      <c r="R64">
-        <v>25</v>
+      <c r="J65" s="11">
+        <f>(E65+F65+($K$69*H65+$M$69)*$L$69)/(1-G65)/(1-$O$69)/(1-I65)/$N$69</f>
+        <v>17.208704868551415</v>
+      </c>
+      <c r="K65" s="12">
+        <f>(E65+F65+($K$69*H65+$M$69)*$L$69)/(1-G65)/(1-$P$69)/(1-I65)/$N$69</f>
+        <v>18.625892328314475</v>
+      </c>
+      <c r="L65" s="1">
+        <f>E65+F65+($K$69*H65+$M$69)*$L$69</f>
+        <v>47.8</v>
+      </c>
+      <c r="M65" s="13">
+        <f>L65/(1-G65)/(1-$O$69)/$N$69</f>
+        <v>10.325222921130848</v>
+      </c>
+      <c r="N65" s="13">
+        <f>L65/(1-G65)/(1-$P$69)/$N$69</f>
+        <v>11.175535396988685</v>
+      </c>
+      <c r="O65" s="13">
+        <f>L65/(1-G65)/$N$69</f>
+        <v>9.4992050874403819</v>
+      </c>
+      <c r="P65" s="14">
+        <f>O65*$N$69-L65</f>
+        <v>16.794594594594599</v>
+      </c>
+      <c r="Q65">
+        <v>40</v>
+      </c>
+      <c r="R65">
+        <v>30</v>
+      </c>
+      <c r="S65" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="T65" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="65" spans="3:16" ht="90.75" customHeight="1">
-      <c r="C65" s="1"/>
-      <c r="D65" s="9"/>
-      <c r="G65" s="3"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
-      <c r="P65" s="14"/>
+    <row r="66" spans="2:20" ht="90.75" customHeight="1">
+      <c r="C66" s="1"/>
+      <c r="D66" s="9"/>
+      <c r="G66" s="3"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="13"/>
+      <c r="N66" s="13"/>
+      <c r="O66" s="13"/>
+      <c r="P66" s="14"/>
+      <c r="S66" s="19"/>
     </row>
-    <row r="67" spans="3:16">
-      <c r="K67" s="16" t="s">
+    <row r="68" spans="2:20">
+      <c r="K68" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L67" s="16" t="s">
+      <c r="L68" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="M67" s="16" t="s">
+      <c r="M68" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N67" s="16" t="s">
+      <c r="N68" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="O67" s="16" t="s">
+      <c r="O68" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="P67" s="16" t="s">
+      <c r="P68" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="3:16">
-      <c r="K68" s="17">
+    <row r="69" spans="2:20">
+      <c r="K69" s="17">
         <v>100</v>
       </c>
-      <c r="L68" s="15">
+      <c r="L69" s="15">
         <v>0.85</v>
       </c>
-      <c r="M68">
+      <c r="M69">
         <v>8</v>
       </c>
-      <c r="N68">
+      <c r="N69">
         <v>6.8</v>
       </c>
-      <c r="O68" s="15">
+      <c r="O69" s="15">
         <v>0.08</v>
       </c>
-      <c r="P68" s="15">
+      <c r="P69" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -7263,7 +7382,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C65">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C66">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -7324,10 +7443,12 @@
     <hyperlink ref="D63" r:id="rId51"/>
     <hyperlink ref="D59" r:id="rId52" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
     <hyperlink ref="D64" r:id="rId53"/>
+    <hyperlink ref="D65" r:id="rId54"/>
+    <hyperlink ref="S65" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId54"/>
+  <drawing r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17021301 topolino红色外套 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
   <si>
     <t>产品标题</t>
   </si>
@@ -313,6 +313,10 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/45422676746.html?spm=b26110380.8015204.xshy005.17.K9Fn6R</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3124,6 +3128,44 @@
         <a:xfrm>
           <a:off x="33130" y="71371239"/>
           <a:ext cx="1027043" cy="1027043"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1060175</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>1090124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="图片 66" descr="QQ截图20170213224326.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="72489393"/>
+          <a:ext cx="1060174" cy="1081840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3423,8 +3465,8 @@
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L66" sqref="L66"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7042,31 +7084,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f>(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$O$69)/(1-I61)/$N$69</f>
+        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$O$69)/(1-I61)/$N$69</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f>(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$P$69)/(1-I61)/$N$69</f>
+        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$P$69)/(1-I61)/$N$69</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f>E61+F61+($K$69*H61+$M$69)*$L$69</f>
+        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$69*H61+$M$69)*$L$69</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f>L61/(1-G61)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$69)/$N$69</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f>L61/(1-G61)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$69)/$N$69</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f>L61/(1-G61)/$N$69</f>
+        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$69</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f>O61*$N$69-L61</f>
+        <f t="shared" ref="P61:P66" si="37">O61*$N$69-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -7102,31 +7144,31 @@
         <v>0.25</v>
       </c>
       <c r="J62" s="11">
-        <f>(E62+F62+($K$69*H62+$M$69)*$L$69)/(1-G62)/(1-$O$69)/(1-I62)/$N$69</f>
+        <f t="shared" si="31"/>
         <v>11.736288718385904</v>
       </c>
       <c r="K62" s="12">
-        <f>(E62+F62+($K$69*H62+$M$69)*$L$69)/(1-G62)/(1-$P$69)/(1-I62)/$N$69</f>
+        <f t="shared" si="32"/>
         <v>12.702806612841213</v>
       </c>
       <c r="L62" s="1">
-        <f>E62+F62+($K$69*H62+$M$69)*$L$69</f>
+        <f t="shared" si="33"/>
         <v>41.3</v>
       </c>
       <c r="M62" s="13">
-        <f>L62/(1-G62)/(1-$O$69)/$N$69</f>
+        <f t="shared" si="34"/>
         <v>8.8022165387894287</v>
       </c>
       <c r="N62" s="13">
-        <f>L62/(1-G62)/(1-$P$69)/$N$69</f>
+        <f t="shared" si="35"/>
         <v>9.5271049596309112</v>
       </c>
       <c r="O62" s="13">
-        <f>L62/(1-G62)/$N$69</f>
+        <f t="shared" si="36"/>
         <v>8.0980392156862742</v>
       </c>
       <c r="P62" s="14">
-        <f>O62*$N$69-L62</f>
+        <f t="shared" si="37"/>
         <v>13.766666666666666</v>
       </c>
       <c r="Q62">
@@ -7162,31 +7204,31 @@
         <v>0.4</v>
       </c>
       <c r="J63" s="11">
-        <f>(E63+F63+($K$69*H63+$M$69)*$L$69)/(1-G63)/(1-$O$69)/(1-I63)/$N$69</f>
+        <f t="shared" si="31"/>
         <v>14.670360897982381</v>
       </c>
       <c r="K63" s="12">
-        <f>(E63+F63+($K$69*H63+$M$69)*$L$69)/(1-G63)/(1-$P$69)/(1-I63)/$N$69</f>
+        <f t="shared" si="32"/>
         <v>15.878508266051519</v>
       </c>
       <c r="L63" s="1">
-        <f>E63+F63+($K$69*H63+$M$69)*$L$69</f>
+        <f t="shared" si="33"/>
         <v>41.3</v>
       </c>
       <c r="M63" s="13">
-        <f>L63/(1-G63)/(1-$O$69)/$N$69</f>
+        <f t="shared" si="34"/>
         <v>8.8022165387894287</v>
       </c>
       <c r="N63" s="13">
-        <f>L63/(1-G63)/(1-$P$69)/$N$69</f>
+        <f t="shared" si="35"/>
         <v>9.5271049596309112</v>
       </c>
       <c r="O63" s="13">
-        <f>L63/(1-G63)/$N$69</f>
+        <f t="shared" si="36"/>
         <v>8.0980392156862742</v>
       </c>
       <c r="P63" s="14">
-        <f>O63*$N$69-L63</f>
+        <f t="shared" si="37"/>
         <v>13.766666666666666</v>
       </c>
       <c r="Q63">
@@ -7222,31 +7264,31 @@
         <v>0.25</v>
       </c>
       <c r="J64" s="11">
-        <f>(E64+F64+($K$69*H64+$M$69)*$L$69)/(1-G64)/(1-$O$69)/(1-I64)/$N$69</f>
+        <f t="shared" si="31"/>
         <v>15.398550724637678</v>
       </c>
       <c r="K64" s="12">
-        <f>(E64+F64+($K$69*H64+$M$69)*$L$69)/(1-G64)/(1-$P$69)/(1-I64)/$N$69</f>
+        <f t="shared" si="32"/>
         <v>16.666666666666664</v>
       </c>
       <c r="L64" s="1">
-        <f>E64+F64+($K$69*H64+$M$69)*$L$69</f>
+        <f t="shared" si="33"/>
         <v>57.8</v>
       </c>
       <c r="M64" s="13">
-        <f>L64/(1-G64)/(1-$O$69)/$N$69</f>
+        <f t="shared" si="34"/>
         <v>11.548913043478258</v>
       </c>
       <c r="N64" s="13">
-        <f>L64/(1-G64)/(1-$P$69)/$N$69</f>
+        <f t="shared" si="35"/>
         <v>12.499999999999998</v>
       </c>
       <c r="O64" s="13">
-        <f>L64/(1-G64)/$N$69</f>
+        <f t="shared" si="36"/>
         <v>10.624999999999998</v>
       </c>
       <c r="P64" s="14">
-        <f>O64*$N$69-L64</f>
+        <f t="shared" si="37"/>
         <v>14.449999999999989</v>
       </c>
       <c r="Q64">
@@ -7282,31 +7324,31 @@
         <v>0.4</v>
       </c>
       <c r="J65" s="11">
-        <f>(E65+F65+($K$69*H65+$M$69)*$L$69)/(1-G65)/(1-$O$69)/(1-I65)/$N$69</f>
+        <f t="shared" si="31"/>
         <v>17.208704868551415</v>
       </c>
       <c r="K65" s="12">
-        <f>(E65+F65+($K$69*H65+$M$69)*$L$69)/(1-G65)/(1-$P$69)/(1-I65)/$N$69</f>
+        <f t="shared" si="32"/>
         <v>18.625892328314475</v>
       </c>
       <c r="L65" s="1">
-        <f>E65+F65+($K$69*H65+$M$69)*$L$69</f>
+        <f t="shared" si="33"/>
         <v>47.8</v>
       </c>
       <c r="M65" s="13">
-        <f>L65/(1-G65)/(1-$O$69)/$N$69</f>
+        <f t="shared" si="34"/>
         <v>10.325222921130848</v>
       </c>
       <c r="N65" s="13">
-        <f>L65/(1-G65)/(1-$P$69)/$N$69</f>
+        <f t="shared" si="35"/>
         <v>11.175535396988685</v>
       </c>
       <c r="O65" s="13">
-        <f>L65/(1-G65)/$N$69</f>
+        <f t="shared" si="36"/>
         <v>9.4992050874403819</v>
       </c>
       <c r="P65" s="14">
-        <f>O65*$N$69-L65</f>
+        <f t="shared" si="37"/>
         <v>16.794594594594599</v>
       </c>
       <c r="Q65">
@@ -7323,17 +7365,64 @@
       </c>
     </row>
     <row r="66" spans="2:20" ht="90.75" customHeight="1">
-      <c r="C66" s="1"/>
-      <c r="D66" s="9"/>
-      <c r="G66" s="3"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="14"/>
+      <c r="B66">
+        <v>17021301</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E66">
+        <v>35</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H66">
+        <v>0.32</v>
+      </c>
+      <c r="I66" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="J66" s="11">
+        <f t="shared" si="31"/>
+        <v>20.266258677383998</v>
+      </c>
+      <c r="K66" s="12">
+        <f t="shared" si="32"/>
+        <v>21.935244686109741</v>
+      </c>
+      <c r="L66" s="1">
+        <f t="shared" si="33"/>
+        <v>71</v>
+      </c>
+      <c r="M66" s="13">
+        <f t="shared" si="34"/>
+        <v>14.186381074168798</v>
+      </c>
+      <c r="N66" s="13">
+        <f t="shared" si="35"/>
+        <v>15.354671280276818</v>
+      </c>
+      <c r="O66" s="13">
+        <f t="shared" si="36"/>
+        <v>13.051470588235295</v>
+      </c>
+      <c r="P66" s="14">
+        <f t="shared" si="37"/>
+        <v>17.75</v>
+      </c>
+      <c r="Q66">
+        <v>30</v>
+      </c>
+      <c r="R66">
+        <v>25</v>
+      </c>
       <c r="S66" s="19"/>
     </row>
     <row r="68" spans="2:20">
@@ -7445,10 +7534,11 @@
     <hyperlink ref="D64" r:id="rId53"/>
     <hyperlink ref="D65" r:id="rId54"/>
     <hyperlink ref="S65" r:id="rId55"/>
+    <hyperlink ref="D66" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId56"/>
+  <drawing r:id="rId57"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17021401 字母哈裙 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
   <si>
     <t>产品标题</t>
   </si>
@@ -317,6 +317,9 @@
   <si>
     <t>https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/542588347406.html?spm=0.0.0.0.uOstC8&amp;sk=consign</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +386,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -418,7 +428,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -479,6 +489,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -3166,6 +3179,44 @@
         <a:xfrm>
           <a:off x="1" y="72489393"/>
           <a:ext cx="1060174" cy="1081840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>49697</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>66262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>969066</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1051892</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="图片 67" descr="QQ截图20170214225337.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="49697" y="73698653"/>
+          <a:ext cx="919369" cy="985630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3462,11 +3513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3572,31 +3623,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$69*H2+$M$69)*$L$69)/(1-G2)/(1-$O$69)/(1-I2)/$N$69</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$72*H2+$M$72)*$L$72)/(1-G2)/(1-$O$72)/(1-I2)/$N$72</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$69*H2+$M$69)*$L$69)/(1-G2)/(1-$P$69)/(1-I2)/$N$69</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$72*H2+$M$72)*$L$72)/(1-G2)/(1-$P$72)/(1-I2)/$N$72</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$69*H2+$M$69)*$L$69</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$72*H2+$M$72)*$L$72</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$72)/$N$72</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$72)/$N$72</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$69</f>
+        <f>L2/(1-G2)/$N$72</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$69-L2</f>
+        <f>O2*$N$72-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -3637,27 +3688,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$69*H3+$M$69)*$L$69)/(1-G3)/(1-$P$69)/(1-I3)/$N$69</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$72*H3+$M$72)*$L$72)/(1-G3)/(1-$P$72)/(1-I3)/$N$72</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$69*H3+$M$69)*$L$69</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$72*H3+$M$72)*$L$72</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$72)/$N$72</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$72)/$N$72</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$69</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$72</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$69-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$72-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -3884,27 +3935,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$69*H7+$M$69)*$L$69)/(1-G7)/(1-$P$69)/(1-I7)/$N$69</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$72*H7+$M$72)*$L$72)/(1-G7)/(1-$P$72)/(1-I7)/$N$72</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$69*H7+$M$69)*$L$69</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$72*H7+$M$72)*$L$72</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$72)/$N$72</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$72)/$N$72</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$69</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$72</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$69-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$72-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -6424,31 +6475,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$69*H50+$M$69)*$L$69)/(1-G50)/(1-$O$69)/(1-I50)/$N$69</f>
+        <f t="shared" ref="J50:J55" si="17">(E50+F50+($K$72*H50+$M$72)*$L$72)/(1-G50)/(1-$O$72)/(1-I50)/$N$72</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$69*H50+$M$69)*$L$69)/(1-G50)/(1-$P$69)/(1-I50)/$N$69</f>
+        <f t="shared" ref="K50:K55" si="18">(E50+F50+($K$72*H50+$M$72)*$L$72)/(1-G50)/(1-$P$72)/(1-I50)/$N$72</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$69*H50+$M$69)*$L$69</f>
+        <f t="shared" ref="L50:L55" si="19">E50+F50+($K$72*H50+$M$72)*$L$72</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M50:M55" si="20">L50/(1-G50)/(1-$O$72)/$N$72</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N50:N55" si="21">L50/(1-G50)/(1-$P$72)/$N$72</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$69</f>
+        <f t="shared" ref="O50:O55" si="22">L50/(1-G50)/$N$72</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P55" si="23">O50*$N$69-L50</f>
+        <f t="shared" ref="P50:P55" si="23">O50*$N$72-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -6784,31 +6835,31 @@
         <v>0.25</v>
       </c>
       <c r="J56" s="11">
-        <f>(E56+F56+($K$69*H56+$M$69)*$L$69)/(1-G56)/(1-$O$69)/(1-I56)/$N$69</f>
+        <f>(E56+F56+($K$72*H56+$M$72)*$L$72)/(1-G56)/(1-$O$72)/(1-I56)/$N$72</f>
         <v>12.947570332480817</v>
       </c>
       <c r="K56" s="12">
-        <f>(E56+F56+($K$69*H56+$M$69)*$L$69)/(1-G56)/(1-$P$69)/(1-I56)/$N$69</f>
+        <f>(E56+F56+($K$72*H56+$M$72)*$L$72)/(1-G56)/(1-$P$72)/(1-I56)/$N$72</f>
         <v>14.013840830449828</v>
       </c>
       <c r="L56" s="1">
-        <f>E56+F56+($K$69*H56+$M$69)*$L$69</f>
+        <f>E56+F56+($K$72*H56+$M$72)*$L$72</f>
         <v>48.599999999999994</v>
       </c>
       <c r="M56" s="13">
-        <f>L56/(1-G56)/(1-$O$69)/$N$69</f>
+        <f>L56/(1-G56)/(1-$O$72)/$N$72</f>
         <v>9.7106777493606113</v>
       </c>
       <c r="N56" s="13">
-        <f>L56/(1-G56)/(1-$P$69)/$N$69</f>
+        <f>L56/(1-G56)/(1-$P$72)/$N$72</f>
         <v>10.510380622837371</v>
       </c>
       <c r="O56" s="13">
-        <f>L56/(1-G56)/$N$69</f>
+        <f>L56/(1-G56)/$N$72</f>
         <v>8.9338235294117645</v>
       </c>
       <c r="P56" s="14">
-        <f>O56*$N$69-L56</f>
+        <f>O56*$N$72-L56</f>
         <v>12.150000000000006</v>
       </c>
       <c r="Q56">
@@ -6844,31 +6895,31 @@
         <v>0.45</v>
       </c>
       <c r="J57" s="11">
-        <f>(E57+F57+($K$69*H57+$M$69)*$L$69)/(1-G57)/(1-$O$69)/(1-I57)/$N$69</f>
+        <f>(E57+F57+($K$72*H57+$M$72)*$L$72)/(1-G57)/(1-$O$72)/(1-I57)/$N$72</f>
         <v>19.653859567542423</v>
       </c>
       <c r="K57" s="12">
-        <f>(E57+F57+($K$69*H57+$M$69)*$L$69)/(1-G57)/(1-$P$69)/(1-I57)/$N$69</f>
+        <f>(E57+F57+($K$72*H57+$M$72)*$L$72)/(1-G57)/(1-$P$72)/(1-I57)/$N$72</f>
         <v>21.272412708398864</v>
       </c>
       <c r="L57" s="1">
-        <f>E57+F57+($K$69*H57+$M$69)*$L$69</f>
+        <f>E57+F57+($K$72*H57+$M$72)*$L$72</f>
         <v>54.099999999999994</v>
       </c>
       <c r="M57" s="13">
-        <f>L57/(1-G57)/(1-$O$69)/$N$69</f>
+        <f>L57/(1-G57)/(1-$O$72)/$N$72</f>
         <v>10.809622762148335</v>
       </c>
       <c r="N57" s="13">
-        <f>L57/(1-G57)/(1-$P$69)/$N$69</f>
+        <f>L57/(1-G57)/(1-$P$72)/$N$72</f>
         <v>11.699826989619377</v>
       </c>
       <c r="O57" s="13">
-        <f>L57/(1-G57)/$N$69</f>
+        <f>L57/(1-G57)/$N$72</f>
         <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="14">
-        <f>O57*$N$69-L57</f>
+        <f>O57*$N$72-L57</f>
         <v>13.524999999999991</v>
       </c>
       <c r="Q57">
@@ -6904,31 +6955,31 @@
         <v>0.4</v>
       </c>
       <c r="J58" s="11">
-        <f>(E58+F58+($K$69*H58+$M$69)*$L$69)/(1-G58)/(1-$O$69)/(1-I58)/$N$69</f>
+        <f>(E58+F58+($K$72*H58+$M$72)*$L$72)/(1-G58)/(1-$O$72)/(1-I58)/$N$72</f>
         <v>24.909420289855071</v>
       </c>
       <c r="K58" s="12">
-        <f>(E58+F58+($K$69*H58+$M$69)*$L$69)/(1-G58)/(1-$P$69)/(1-I58)/$N$69</f>
+        <f>(E58+F58+($K$72*H58+$M$72)*$L$72)/(1-G58)/(1-$P$72)/(1-I58)/$N$72</f>
         <v>26.960784313725487</v>
       </c>
       <c r="L58" s="1">
-        <f>E58+F58+($K$69*H58+$M$69)*$L$69</f>
+        <f>E58+F58+($K$72*H58+$M$72)*$L$72</f>
         <v>74.8</v>
       </c>
       <c r="M58" s="13">
-        <f>L58/(1-G58)/(1-$O$69)/$N$69</f>
+        <f>L58/(1-G58)/(1-$O$72)/$N$72</f>
         <v>14.945652173913041</v>
       </c>
       <c r="N58" s="13">
-        <f>L58/(1-G58)/(1-$P$69)/$N$69</f>
+        <f>L58/(1-G58)/(1-$P$72)/$N$72</f>
         <v>16.176470588235293</v>
       </c>
       <c r="O58" s="13">
-        <f>L58/(1-G58)/$N$69</f>
+        <f>L58/(1-G58)/$N$72</f>
         <v>13.749999999999998</v>
       </c>
       <c r="P58" s="14">
-        <f>O58*$N$69-L58</f>
+        <f>O58*$N$72-L58</f>
         <v>18.699999999999989</v>
       </c>
       <c r="Q58">
@@ -6964,31 +7015,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$69*H59+$M$69)*$L$69)/(1-G59)/(1-$O$69)/(1-I59)/$N$69</f>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$72*H59+$M$72)*$L$72)/(1-G59)/(1-$O$72)/(1-I59)/$N$72</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$69*H59+$M$69)*$L$69)/(1-G59)/(1-$P$69)/(1-I59)/$N$69</f>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$72*H59+$M$72)*$L$72)/(1-G59)/(1-$P$72)/(1-I59)/$N$72</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$69*H59+$M$69)*$L$69</f>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$72*H59+$M$72)*$L$72</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$72)/$N$72</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$72)/$N$72</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$69</f>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$72</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" ref="P59:P60" si="30">O59*$N$69-L59</f>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$72-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -7084,31 +7135,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$O$69)/(1-I61)/$N$69</f>
+        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$72*H61+$M$72)*$L$72)/(1-G61)/(1-$O$72)/(1-I61)/$N$72</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$69*H61+$M$69)*$L$69)/(1-G61)/(1-$P$69)/(1-I61)/$N$69</f>
+        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$72*H61+$M$72)*$L$72)/(1-G61)/(1-$P$72)/(1-I61)/$N$72</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$69*H61+$M$69)*$L$69</f>
+        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$72*H61+$M$72)*$L$72</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$69)/$N$69</f>
+        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$72)/$N$72</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$69)/$N$69</f>
+        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$72)/$N$72</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$69</f>
+        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$72</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="37">O61*$N$69-L61</f>
+        <f t="shared" ref="P61:P66" si="37">O61*$N$72-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -7425,43 +7476,132 @@
       </c>
       <c r="S66" s="19"/>
     </row>
-    <row r="68" spans="2:20">
-      <c r="K68" s="16" t="s">
+    <row r="67" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B67">
+        <v>17021301</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67">
+        <v>14</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H67">
+        <v>0.09</v>
+      </c>
+      <c r="I67" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J67" s="11">
+        <f t="shared" ref="J67" si="38">(E67+F67+($K$72*H67+$M$72)*$L$72)/(1-G67)/(1-$O$72)/(1-I67)/$N$72</f>
+        <v>8.3688547882921274</v>
+      </c>
+      <c r="K67" s="12">
+        <f t="shared" ref="K67" si="39">(E67+F67+($K$72*H67+$M$72)*$L$72)/(1-G67)/(1-$P$72)/(1-I67)/$N$72</f>
+        <v>9.0580545943867747</v>
+      </c>
+      <c r="L67" s="1">
+        <f t="shared" ref="L67" si="40">E67+F67+($K$72*H67+$M$72)*$L$72</f>
+        <v>29.45</v>
+      </c>
+      <c r="M67" s="13">
+        <f t="shared" ref="M67" si="41">L67/(1-G67)/(1-$O$72)/$N$72</f>
+        <v>6.276641091219096</v>
+      </c>
+      <c r="N67" s="13">
+        <f t="shared" ref="N67" si="42">L67/(1-G67)/(1-$P$72)/$N$72</f>
+        <v>6.7935409457900811</v>
+      </c>
+      <c r="O67" s="13">
+        <f t="shared" ref="O67" si="43">L67/(1-G67)/$N$72</f>
+        <v>5.7745098039215685</v>
+      </c>
+      <c r="P67" s="14">
+        <f t="shared" ref="P67" si="44">O67*$N$72-L67</f>
+        <v>9.8166666666666664</v>
+      </c>
+      <c r="Q67">
+        <v>30</v>
+      </c>
+      <c r="R67">
+        <v>25</v>
+      </c>
+      <c r="S67" s="19"/>
+    </row>
+    <row r="68" spans="2:20" ht="90.75" customHeight="1">
+      <c r="C68" s="1"/>
+      <c r="D68" s="9"/>
+      <c r="G68" s="3"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="14"/>
+      <c r="S68" s="19"/>
+    </row>
+    <row r="69" spans="2:20" ht="90.75" customHeight="1">
+      <c r="C69" s="1"/>
+      <c r="D69" s="9"/>
+      <c r="G69" s="3"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="14"/>
+      <c r="S69" s="19"/>
+    </row>
+    <row r="71" spans="2:20">
+      <c r="K71" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="16" t="s">
+      <c r="L71" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="M68" s="16" t="s">
+      <c r="M71" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N68" s="16" t="s">
+      <c r="N71" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="O68" s="16" t="s">
+      <c r="O71" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="P68" s="16" t="s">
+      <c r="P71" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="2:20">
-      <c r="K69" s="17">
+    <row r="72" spans="2:20">
+      <c r="K72" s="17">
         <v>100</v>
       </c>
-      <c r="L69" s="15">
+      <c r="L72" s="15">
         <v>0.85</v>
       </c>
-      <c r="M69">
+      <c r="M72">
         <v>8</v>
       </c>
-      <c r="N69">
+      <c r="N72">
         <v>6.8</v>
       </c>
-      <c r="O69" s="15">
+      <c r="O72" s="15">
         <v>0.08</v>
       </c>
-      <c r="P69" s="15">
+      <c r="P72" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -7471,7 +7611,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C66">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C69">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -7544,17 +7684,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C21"/>
+      <selection activeCell="H21" sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17021403 by hjx 蝙蝠哈裙
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="18540" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>产品标题</t>
   </si>
@@ -316,23 +316,23 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/544238732440.html?spm=0.0.0.0.XUpSK3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,7 +345,7 @@
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -383,140 +383,17 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,194 +406,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -724,251 +415,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -988,40 +443,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1030,70 +485,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1115,7 +525,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1157,7 +567,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1199,7 +609,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1241,7 +651,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1283,7 +693,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1325,7 +735,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1367,7 +777,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1409,7 +819,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1451,7 +861,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1493,7 +903,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1535,7 +945,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1577,7 +987,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1619,7 +1029,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1661,7 +1071,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1703,7 +1113,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1745,7 +1155,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1787,7 +1197,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1829,7 +1239,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1871,7 +1281,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1913,7 +1323,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1955,7 +1365,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1997,7 +1407,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2039,7 +1449,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2081,7 +1491,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2123,7 +1533,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2165,7 +1575,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2207,7 +1617,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2249,7 +1659,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2291,7 +1701,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2333,7 +1743,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2375,7 +1785,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2417,7 +1827,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2459,7 +1869,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2501,7 +1911,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2543,7 +1953,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2585,7 +1995,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2627,7 +2037,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2669,7 +2079,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2711,7 +2121,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2753,7 +2163,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2795,7 +2205,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2837,7 +2247,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2879,7 +2289,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId43" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2921,7 +2331,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId44" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2963,7 +2373,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId45" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3005,7 +2415,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId46" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3047,7 +2457,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId47"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3089,7 +2499,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId48" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3131,7 +2541,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId49"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3173,7 +2583,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId50" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3215,7 +2625,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId51" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3257,7 +2667,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId52" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3295,7 +2705,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId53" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3333,7 +2743,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId54" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3371,7 +2781,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId55" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3409,7 +2819,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId56" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3451,7 +2861,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId57" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3489,7 +2899,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId58"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3527,7 +2937,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId59" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3569,7 +2979,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId60" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3607,7 +3017,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId61" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3645,7 +3055,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId62" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3683,7 +3093,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId63" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3721,7 +3131,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId64" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3759,7 +3169,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId65" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3797,7 +3207,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId66" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3835,7 +3245,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId67"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3852,6 +3262,44 @@
         <a:ln w="9525">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>49699</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>57982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>969069</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>977352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="图片 71" descr="QQ截图20170214231711.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="49699" y="74895907"/>
+          <a:ext cx="919370" cy="919370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4143,37 +3591,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomLeft" activeCell="S70" sqref="S70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="7.25454545454545" customWidth="1"/>
-    <col min="6" max="6" width="8.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="7.37272727272727" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="11.1272727272727" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4229,7 +3675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>16072601</v>
@@ -4257,11 +3703,11 @@
       </c>
       <c r="J2" s="13">
         <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$72*H2+$M$72)*$L$72)/(1-G2)/(1-$O$72)/(1-I2)/$N$72</f>
-        <v>16.8747806027782</v>
+        <v>16.874780602778198</v>
       </c>
       <c r="K2" s="14">
         <f t="shared" ref="K2" si="1">(E2+F2+($K$72*H2+$M$72)*$L$72)/(1-G2)/(1-$P$72)/(1-I2)/$N$72</f>
-        <v>18.2644684171246</v>
+        <v>18.264468417124601</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ref="L2" si="2">E2+F2+($K$72*H2+$M$72)*$L$72</f>
@@ -4273,7 +3719,7 @@
       </c>
       <c r="N2" s="15">
         <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$72)/$N$72</f>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O2" s="15">
         <f>L2/(1-G2)/$N$72</f>
@@ -4281,7 +3727,7 @@
       </c>
       <c r="P2" s="16">
         <f>O2*$N$72-L2</f>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="2">
         <v>1</v>
@@ -4290,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2">
         <v>16072701</v>
@@ -4318,27 +3764,27 @@
       </c>
       <c r="J3" s="13">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619209999</v>
       </c>
       <c r="K3" s="14">
         <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$72*H3+$M$72)*$L$72)/(1-G3)/(1-$P$72)/(1-I3)/$N$72</f>
-        <v>11.9338715878508</v>
+        <v>11.933871587850801</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L6" si="6">E3+F3+($K$72*H3+$M$72)*$L$72</f>
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="15">
         <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$72)/$N$72</f>
-        <v>8.2693947144075</v>
+        <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="15">
         <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$72)/$N$72</f>
-        <v>8.95040369088812</v>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="15">
         <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$72</f>
-        <v>7.6078431372549</v>
+        <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="16">
         <f t="shared" ref="P3:P6" si="10">O3*$N$72-L3</f>
@@ -4351,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2">
         <v>16072901</v>
@@ -4379,11 +3825,11 @@
       </c>
       <c r="J4" s="13">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962898</v>
       </c>
       <c r="K4" s="14">
         <f t="shared" si="5"/>
-        <v>20.6953369583127</v>
+        <v>20.695336958312701</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" si="6"/>
@@ -4391,11 +3837,11 @@
       </c>
       <c r="M4" s="15">
         <f t="shared" si="7"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="15">
         <f t="shared" si="8"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818899</v>
       </c>
       <c r="O4" s="15">
         <f t="shared" si="9"/>
@@ -4403,7 +3849,7 @@
       </c>
       <c r="P4" s="16">
         <f t="shared" si="10"/>
-        <v>20.9333333333333</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="2">
         <v>1</v>
@@ -4412,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2">
         <v>16073001</v>
@@ -4440,11 +3886,11 @@
       </c>
       <c r="J5" s="13">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119699</v>
       </c>
       <c r="K5" s="14">
         <f t="shared" si="5"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047199</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="6"/>
@@ -4456,7 +3902,7 @@
       </c>
       <c r="N5" s="15">
         <f t="shared" si="8"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790099</v>
       </c>
       <c r="O5" s="15">
         <f t="shared" si="9"/>
@@ -4464,7 +3910,7 @@
       </c>
       <c r="P5" s="16">
         <f t="shared" si="10"/>
-        <v>24.2666666666667</v>
+        <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="2">
         <v>1</v>
@@ -4473,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="2">
         <v>16073002</v>
@@ -4505,7 +3951,7 @@
       </c>
       <c r="K6" s="14">
         <f t="shared" si="5"/>
-        <v>16.6140850803989</v>
+        <v>16.614085080398901</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="6"/>
@@ -4525,7 +3971,7 @@
       </c>
       <c r="P6" s="16">
         <f t="shared" si="10"/>
-        <v>16.325</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="2">
         <v>0</v>
@@ -4537,7 +3983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
         <v>16080301</v>
@@ -4565,11 +4011,11 @@
       </c>
       <c r="J7" s="13">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871301</v>
       </c>
       <c r="K7" s="14">
         <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$72*H7+$M$72)*$L$72)/(1-G7)/(1-$P$72)/(1-I7)/$N$72</f>
-        <v>18.671551665649</v>
+        <v>18.671551665649002</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ref="L7:L49" si="12">E7+F7+($K$72*H7+$M$72)*$L$72</f>
@@ -4577,7 +4023,7 @@
       </c>
       <c r="M7" s="15">
         <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$72)/$N$72</f>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N7" s="15">
         <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$72)/$N$72</f>
@@ -4585,11 +4031,11 @@
       </c>
       <c r="O7" s="15">
         <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$72</f>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P7" s="16">
         <f t="shared" ref="P7:P49" si="16">O7*$N$72-L7</f>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="2">
         <v>1</v>
@@ -4598,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -4625,11 +4071,11 @@
       </c>
       <c r="J8" s="13">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907897</v>
       </c>
       <c r="K8" s="14">
         <f t="shared" si="11"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159202</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" si="12"/>
@@ -4637,19 +4083,19 @@
       </c>
       <c r="M8" s="15">
         <f t="shared" si="13"/>
-        <v>17.792918797954</v>
+        <v>17.792918797954002</v>
       </c>
       <c r="N8" s="15">
         <f t="shared" si="14"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079601</v>
       </c>
       <c r="O8" s="15">
         <f t="shared" si="15"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117599</v>
       </c>
       <c r="P8" s="16">
         <f t="shared" si="16"/>
-        <v>22.2625</v>
+        <v>22.262499999999999</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -4658,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -4685,11 +4131,11 @@
       </c>
       <c r="J9" s="13">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695599</v>
       </c>
       <c r="K9" s="14">
         <f t="shared" si="11"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058801</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" si="12"/>
@@ -4697,11 +4143,11 @@
       </c>
       <c r="M9" s="15">
         <f t="shared" si="13"/>
-        <v>16.8478260869565</v>
+        <v>16.847826086956498</v>
       </c>
       <c r="N9" s="15">
         <f t="shared" si="14"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647101</v>
       </c>
       <c r="O9" s="15">
         <f t="shared" si="15"/>
@@ -4718,7 +4164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -4745,11 +4191,11 @@
       </c>
       <c r="J10" s="13">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914598</v>
       </c>
       <c r="K10" s="14">
         <f t="shared" si="11"/>
-        <v>40.467951886637</v>
+        <v>40.467951886637003</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="12"/>
@@ -4757,7 +4203,7 @@
       </c>
       <c r="M10" s="15">
         <f t="shared" si="13"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640201</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="14"/>
@@ -4765,11 +4211,11 @@
       </c>
       <c r="O10" s="15">
         <f t="shared" si="15"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549002</v>
       </c>
       <c r="P10" s="16">
         <f t="shared" si="16"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333302</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -4778,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -4805,15 +4251,15 @@
       </c>
       <c r="J11" s="13">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720503</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="11"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320998</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" si="12"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="13"/>
@@ -4821,11 +4267,11 @@
       </c>
       <c r="N11" s="15">
         <f t="shared" si="14"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622799</v>
       </c>
       <c r="O11" s="15">
         <f t="shared" si="15"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529399</v>
       </c>
       <c r="P11" s="16">
         <f t="shared" si="16"/>
@@ -4838,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -4865,7 +4311,7 @@
       </c>
       <c r="J12" s="13">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419602</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" si="11"/>
@@ -4873,23 +4319,23 @@
       </c>
       <c r="L12" s="2">
         <f t="shared" si="12"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="13"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506699</v>
       </c>
       <c r="N12" s="15">
         <f t="shared" si="14"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666001</v>
       </c>
       <c r="O12" s="15">
         <f t="shared" si="15"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666098</v>
       </c>
       <c r="P12" s="16">
         <f t="shared" si="16"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729701</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -4898,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -4945,11 +4391,11 @@
       </c>
       <c r="O13" s="15">
         <f t="shared" si="15"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607799</v>
       </c>
       <c r="P13" s="16">
         <f t="shared" si="16"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333302</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -4958,7 +4404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -4985,27 +4431,27 @@
       </c>
       <c r="J14" s="13">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874698</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="11"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193804</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="12"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="13"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437299</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="14"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096902</v>
       </c>
       <c r="O14" s="15">
         <f t="shared" si="15"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882401</v>
       </c>
       <c r="P14" s="16">
         <f t="shared" si="16"/>
@@ -5018,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -5045,11 +4491,11 @@
       </c>
       <c r="J15" s="13">
         <f t="shared" si="0"/>
-        <v>23.0179028132992</v>
+        <v>23.017902813299202</v>
       </c>
       <c r="K15" s="14">
         <f t="shared" si="11"/>
-        <v>24.9134948096886</v>
+        <v>24.913494809688601</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" si="12"/>
@@ -5057,11 +4503,11 @@
       </c>
       <c r="M15" s="15">
         <f t="shared" si="13"/>
-        <v>19.5652173913043</v>
+        <v>19.565217391304301</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="14"/>
-        <v>21.1764705882353</v>
+        <v>21.176470588235301</v>
       </c>
       <c r="O15" s="15">
         <f t="shared" si="15"/>
@@ -5078,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -5109,7 +4555,7 @@
       </c>
       <c r="K16" s="14">
         <f t="shared" si="11"/>
-        <v>12.6297577854671</v>
+        <v>12.629757785467101</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="12"/>
@@ -5117,15 +4563,15 @@
       </c>
       <c r="M16" s="15">
         <f t="shared" si="13"/>
-        <v>8.75159846547314</v>
+        <v>8.7515984654731405</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="14"/>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003491</v>
       </c>
       <c r="O16" s="15">
         <f t="shared" si="15"/>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352899</v>
       </c>
       <c r="P16" s="16">
         <f t="shared" si="16"/>
@@ -5138,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -5165,11 +4611,11 @@
       </c>
       <c r="J17" s="13">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K17" s="14">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="12"/>
@@ -5177,7 +4623,7 @@
       </c>
       <c r="M17" s="15">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="14"/>
@@ -5185,11 +4631,11 @@
       </c>
       <c r="O17" s="15">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P17" s="16">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q17" s="17">
         <v>0.15</v>
@@ -5198,7 +4644,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -5225,11 +4671,11 @@
       </c>
       <c r="J18" s="13">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K18" s="14">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="12"/>
@@ -5237,7 +4683,7 @@
       </c>
       <c r="M18" s="15">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="14"/>
@@ -5245,11 +4691,11 @@
       </c>
       <c r="O18" s="15">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P18" s="16">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q18" s="17">
         <v>0.15</v>
@@ -5258,7 +4704,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
@@ -5285,27 +4731,27 @@
       </c>
       <c r="J19" s="13">
         <f t="shared" si="0"/>
-        <v>17.0716112531969</v>
+        <v>17.071611253196899</v>
       </c>
       <c r="K19" s="14">
         <f t="shared" si="11"/>
-        <v>18.477508650519</v>
+        <v>18.477508650518999</v>
       </c>
       <c r="L19" s="2">
         <f t="shared" si="12"/>
-        <v>40.05</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="13"/>
-        <v>8.53580562659847</v>
+        <v>8.5358056265984708</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="14"/>
-        <v>9.23875432525952</v>
+        <v>9.2387543252595208</v>
       </c>
       <c r="O19" s="15">
         <f t="shared" si="15"/>
-        <v>7.85294117647059</v>
+        <v>7.8529411764705896</v>
       </c>
       <c r="P19" s="16">
         <f t="shared" si="16"/>
@@ -5318,7 +4764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
@@ -5345,11 +4791,11 @@
       </c>
       <c r="J20" s="13">
         <f t="shared" si="0"/>
-        <v>18.5117525270978</v>
+        <v>18.511752527097801</v>
       </c>
       <c r="K20" s="14">
         <f t="shared" si="11"/>
-        <v>20.0362497940353</v>
+        <v>20.036249794035299</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="12"/>
@@ -5357,11 +4803,11 @@
       </c>
       <c r="M20" s="15">
         <f t="shared" si="13"/>
-        <v>12.9582267689685</v>
+        <v>12.958226768968499</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="14"/>
-        <v>14.0253748558247</v>
+        <v>14.025374855824699</v>
       </c>
       <c r="O20" s="15">
         <f t="shared" si="15"/>
@@ -5369,13 +4815,13 @@
       </c>
       <c r="P20" s="16">
         <f t="shared" si="16"/>
-        <v>20.2666666666667</v>
+        <v>20.266666666666701</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -5406,7 +4852,7 @@
       </c>
       <c r="K21" s="14">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="12"/>
@@ -5418,11 +4864,11 @@
       </c>
       <c r="N21" s="15">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O21" s="15">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P21" s="16">
         <f t="shared" si="16"/>
@@ -5432,7 +4878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
@@ -5463,7 +4909,7 @@
       </c>
       <c r="K22" s="14">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="12"/>
@@ -5475,11 +4921,11 @@
       </c>
       <c r="N22" s="15">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O22" s="15">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P22" s="16">
         <f t="shared" si="16"/>
@@ -5489,7 +4935,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
@@ -5516,11 +4962,11 @@
       </c>
       <c r="J23" s="13">
         <f t="shared" si="0"/>
-        <v>27.5323568162443</v>
+        <v>27.532356816244299</v>
       </c>
       <c r="K23" s="14">
         <f t="shared" si="11"/>
-        <v>29.799727377582</v>
+        <v>29.799727377581998</v>
       </c>
       <c r="L23" s="2">
         <f t="shared" si="12"/>
@@ -5528,25 +4974,25 @@
       </c>
       <c r="M23" s="15">
         <f t="shared" si="13"/>
-        <v>15.1427962489344</v>
+        <v>15.142796248934401</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="14"/>
-        <v>16.3898500576701</v>
+        <v>16.389850057670099</v>
       </c>
       <c r="O23" s="15">
         <f t="shared" si="15"/>
-        <v>13.9313725490196</v>
+        <v>13.931372549019599</v>
       </c>
       <c r="P23" s="16">
         <f t="shared" si="16"/>
-        <v>23.6833333333333</v>
+        <v>23.683333333333302</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -5573,11 +5019,11 @@
       </c>
       <c r="J24" s="13">
         <f t="shared" si="0"/>
-        <v>26.3698364721383</v>
+        <v>26.369836472138299</v>
       </c>
       <c r="K24" s="14">
         <f t="shared" si="11"/>
-        <v>28.5414700639614</v>
+        <v>28.541470063961398</v>
       </c>
       <c r="L24" s="2">
         <f t="shared" si="12"/>
@@ -5589,7 +5035,7 @@
       </c>
       <c r="N24" s="15">
         <f t="shared" si="14"/>
-        <v>15.6978085351788</v>
+        <v>15.697808535178799</v>
       </c>
       <c r="O24" s="15">
         <f t="shared" si="15"/>
@@ -5597,13 +5043,13 @@
       </c>
       <c r="P24" s="16">
         <f t="shared" si="16"/>
-        <v>22.6833333333333</v>
+        <v>22.683333333333302</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -5630,7 +5076,7 @@
       </c>
       <c r="J25" s="13">
         <f t="shared" si="0"/>
-        <v>25.4156010230179</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="14">
         <f t="shared" si="11"/>
@@ -5642,11 +5088,11 @@
       </c>
       <c r="M25" s="15">
         <f t="shared" si="13"/>
-        <v>15.2493606138107</v>
+        <v>15.249360613810699</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="14"/>
-        <v>16.5051903114187</v>
+        <v>16.505190311418701</v>
       </c>
       <c r="O25" s="15">
         <f t="shared" si="15"/>
@@ -5660,7 +5106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -5687,7 +5133,7 @@
       </c>
       <c r="J26" s="13">
         <f t="shared" si="0"/>
-        <v>22.7514919011083</v>
+        <v>22.751491901108299</v>
       </c>
       <c r="K26" s="14">
         <f t="shared" si="11"/>
@@ -5717,7 +5163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -5744,11 +5190,11 @@
       </c>
       <c r="J27" s="13">
         <f t="shared" si="0"/>
-        <v>19.3338204847156</v>
+        <v>19.333820484715599</v>
       </c>
       <c r="K27" s="14">
         <f t="shared" si="11"/>
-        <v>20.9260174658099</v>
+        <v>20.926017465809899</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" si="12"/>
@@ -5760,7 +5206,7 @@
       </c>
       <c r="N27" s="15">
         <f t="shared" si="14"/>
-        <v>14.6482122260669</v>
+        <v>14.648212226066899</v>
       </c>
       <c r="O27" s="15">
         <f t="shared" si="15"/>
@@ -5777,7 +5223,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -5804,11 +5250,11 @@
       </c>
       <c r="J28" s="13">
         <f t="shared" si="0"/>
-        <v>28.6948771603503</v>
+        <v>28.694877160350298</v>
       </c>
       <c r="K28" s="14">
         <f t="shared" si="11"/>
-        <v>31.0579846912027</v>
+        <v>31.057984691202702</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" si="12"/>
@@ -5816,7 +5262,7 @@
       </c>
       <c r="M28" s="15">
         <f t="shared" si="13"/>
-        <v>15.7821824381927</v>
+        <v>15.782182438192701</v>
       </c>
       <c r="N28" s="15">
         <f t="shared" si="14"/>
@@ -5824,11 +5270,11 @@
       </c>
       <c r="O28" s="15">
         <f t="shared" si="15"/>
-        <v>14.5196078431373</v>
+        <v>14.519607843137299</v>
       </c>
       <c r="P28" s="16">
         <f t="shared" si="16"/>
-        <v>24.6833333333333</v>
+        <v>24.683333333333302</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -5837,7 +5283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -5876,7 +5322,7 @@
       </c>
       <c r="M29" s="15">
         <f t="shared" si="13"/>
-        <v>16.2084398976982</v>
+        <v>16.208439897698199</v>
       </c>
       <c r="N29" s="15">
         <f t="shared" si="14"/>
@@ -5884,7 +5330,7 @@
       </c>
       <c r="O29" s="15">
         <f t="shared" si="15"/>
-        <v>14.9117647058824</v>
+        <v>14.911764705882399</v>
       </c>
       <c r="P29" s="16">
         <f t="shared" si="16"/>
@@ -5897,7 +5343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -5924,11 +5370,11 @@
       </c>
       <c r="J30" s="13">
         <f t="shared" si="0"/>
-        <v>26.6604665581648</v>
+        <v>26.660466558164799</v>
       </c>
       <c r="K30" s="14">
         <f t="shared" si="11"/>
-        <v>28.8560343923666</v>
+        <v>28.856034392366599</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" si="12"/>
@@ -5936,7 +5382,7 @@
       </c>
       <c r="M30" s="15">
         <f t="shared" si="13"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N30" s="15">
         <f t="shared" si="14"/>
@@ -5944,11 +5390,11 @@
       </c>
       <c r="O30" s="15">
         <f t="shared" si="15"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P30" s="16">
         <f t="shared" si="16"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -5957,7 +5403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -5984,11 +5430,11 @@
       </c>
       <c r="J31" s="13">
         <f t="shared" si="0"/>
-        <v>12.8010443307758</v>
+        <v>12.801044330775801</v>
       </c>
       <c r="K31" s="14">
         <f t="shared" si="11"/>
-        <v>13.8552479815456</v>
+        <v>13.855247981545601</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" si="12"/>
@@ -6004,11 +5450,11 @@
       </c>
       <c r="O31" s="15">
         <f t="shared" si="15"/>
-        <v>9.42156862745098</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="16">
         <f t="shared" si="16"/>
-        <v>16.0166666666667</v>
+        <v>16.016666666666701</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -6017,7 +5463,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -6048,7 +5494,7 @@
       </c>
       <c r="K32" s="14">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" si="12"/>
@@ -6056,7 +5502,7 @@
       </c>
       <c r="M32" s="15">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N32" s="15">
         <f t="shared" si="14"/>
@@ -6064,11 +5510,11 @@
       </c>
       <c r="O32" s="15">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="16">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -6077,7 +5523,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -6108,7 +5554,7 @@
       </c>
       <c r="K33" s="14">
         <f t="shared" si="11"/>
-        <v>28.2269057355563</v>
+        <v>28.226905735556301</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" si="12"/>
@@ -6120,7 +5566,7 @@
       </c>
       <c r="N33" s="15">
         <f t="shared" si="14"/>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O33" s="15">
         <f t="shared" si="15"/>
@@ -6128,7 +5574,7 @@
       </c>
       <c r="P33" s="16">
         <f t="shared" si="16"/>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -6137,7 +5583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -6164,11 +5610,11 @@
       </c>
       <c r="J34" s="13">
         <f t="shared" si="0"/>
-        <v>19.9772662688264</v>
+        <v>19.977266268826401</v>
       </c>
       <c r="K34" s="14">
         <f t="shared" si="11"/>
-        <v>21.6224529027297</v>
+        <v>21.622452902729702</v>
       </c>
       <c r="L34" s="2">
         <f t="shared" si="12"/>
@@ -6188,7 +5634,7 @@
       </c>
       <c r="P34" s="16">
         <f t="shared" si="16"/>
-        <v>23.4333333333333</v>
+        <v>23.433333333333302</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -6197,7 +5643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -6224,11 +5670,11 @@
       </c>
       <c r="J35" s="13">
         <f t="shared" si="0"/>
-        <v>16.0645780051151</v>
+        <v>16.064578005115099</v>
       </c>
       <c r="K35" s="14">
         <f t="shared" si="11"/>
-        <v>17.3875432525952</v>
+        <v>17.387543252595201</v>
       </c>
       <c r="L35" s="2">
         <f t="shared" si="12"/>
@@ -6236,25 +5682,25 @@
       </c>
       <c r="M35" s="15">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N35" s="15">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O35" s="15">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P35" s="16">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="R35">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -6283,7 +5729,7 @@
       </c>
       <c r="K36" s="14">
         <f t="shared" si="11"/>
-        <v>26.5492293173954</v>
+        <v>26.549229317395401</v>
       </c>
       <c r="L36" s="2">
         <f t="shared" si="12"/>
@@ -6291,7 +5737,7 @@
       </c>
       <c r="M36" s="15">
         <f t="shared" si="13"/>
-        <v>13.4910485933504</v>
+        <v>13.491048593350399</v>
       </c>
       <c r="N36" s="15">
         <f t="shared" si="14"/>
@@ -6299,7 +5745,7 @@
       </c>
       <c r="O36" s="15">
         <f t="shared" si="15"/>
-        <v>12.4117647058824</v>
+        <v>12.411764705882399</v>
       </c>
       <c r="P36" s="16">
         <f t="shared" si="16"/>
@@ -6309,7 +5755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -6334,11 +5780,11 @@
       </c>
       <c r="J37" s="13">
         <f t="shared" si="0"/>
-        <v>7.33962063086104</v>
+        <v>7.3396206308610399</v>
       </c>
       <c r="K37" s="14">
         <f t="shared" si="11"/>
-        <v>7.94405997693195</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" si="12"/>
@@ -6346,15 +5792,15 @@
       </c>
       <c r="M37" s="15">
         <f t="shared" si="13"/>
-        <v>5.87169650468883</v>
+        <v>5.8716965046888303</v>
       </c>
       <c r="N37" s="15">
         <f t="shared" si="14"/>
-        <v>6.35524798154556</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="15">
         <f t="shared" si="15"/>
-        <v>5.40196078431373</v>
+        <v>5.4019607843137303</v>
       </c>
       <c r="P37" s="16">
         <f t="shared" si="16"/>
@@ -6364,7 +5810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -6389,19 +5835,19 @@
       </c>
       <c r="J38" s="13">
         <f t="shared" si="0"/>
-        <v>16.3256606990622</v>
+        <v>16.325660699062201</v>
       </c>
       <c r="K38" s="14">
         <f t="shared" si="11"/>
-        <v>17.6701268742791</v>
+        <v>17.670126874279099</v>
       </c>
       <c r="L38" s="2">
         <f t="shared" si="12"/>
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="15">
         <f t="shared" si="13"/>
-        <v>8.16283034953112</v>
+        <v>8.1628303495311201</v>
       </c>
       <c r="N38" s="15">
         <f t="shared" si="14"/>
@@ -6409,11 +5855,11 @@
       </c>
       <c r="O38" s="15">
         <f t="shared" si="15"/>
-        <v>7.50980392156863</v>
+        <v>7.5098039215686301</v>
       </c>
       <c r="P38" s="16">
         <f t="shared" si="16"/>
-        <v>12.7666666666667</v>
+        <v>12.766666666666699</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -6422,7 +5868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -6453,7 +5899,7 @@
       </c>
       <c r="K39" s="14">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L39" s="2">
         <f t="shared" si="12"/>
@@ -6461,7 +5907,7 @@
       </c>
       <c r="M39" s="15">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N39" s="15">
         <f t="shared" si="14"/>
@@ -6469,11 +5915,11 @@
       </c>
       <c r="O39" s="15">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="16">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -6482,7 +5928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -6542,7 +5988,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -6573,7 +6019,7 @@
       </c>
       <c r="K41" s="14">
         <f t="shared" si="11"/>
-        <v>12.4259900038447</v>
+        <v>12.425990003844699</v>
       </c>
       <c r="L41" s="2">
         <f t="shared" si="12"/>
@@ -6581,19 +6027,19 @@
       </c>
       <c r="M41" s="15">
         <f t="shared" si="13"/>
-        <v>8.61040068201194</v>
+        <v>8.6104006820119405</v>
       </c>
       <c r="N41" s="15">
         <f t="shared" si="14"/>
-        <v>9.31949250288351</v>
+        <v>9.3194925028835094</v>
       </c>
       <c r="O41" s="15">
         <f t="shared" si="15"/>
-        <v>7.92156862745098</v>
+        <v>7.9215686274509798</v>
       </c>
       <c r="P41" s="16">
         <f t="shared" si="16"/>
-        <v>13.4666666666667</v>
+        <v>13.466666666666701</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -6602,7 +6048,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -6633,7 +6079,7 @@
       </c>
       <c r="K42" s="14">
         <f t="shared" si="11"/>
-        <v>26.8637936458006</v>
+        <v>26.863793645800602</v>
       </c>
       <c r="L42" s="2">
         <f t="shared" si="12"/>
@@ -6662,7 +6108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="2:18">
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
       <c r="B43">
         <v>17011401</v>
       </c>
@@ -6693,7 +6139,7 @@
       </c>
       <c r="K43" s="14">
         <f t="shared" si="11"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827801</v>
       </c>
       <c r="L43" s="2">
         <f t="shared" si="12"/>
@@ -6701,15 +6147,15 @@
       </c>
       <c r="M43" s="15">
         <f t="shared" si="13"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241194</v>
       </c>
       <c r="N43" s="15">
         <f t="shared" si="14"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870801</v>
       </c>
       <c r="O43" s="15">
         <f t="shared" si="15"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254902004</v>
       </c>
       <c r="P43" s="16">
         <f t="shared" si="16"/>
@@ -6722,7 +6168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" ht="90.75" customHeight="1" spans="2:18">
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
       <c r="B44">
         <v>17011501</v>
       </c>
@@ -6749,11 +6195,11 @@
       </c>
       <c r="J44" s="13">
         <f t="shared" si="0"/>
-        <v>17.1355498721228</v>
+        <v>17.135549872122802</v>
       </c>
       <c r="K44" s="14">
         <f t="shared" si="11"/>
-        <v>18.5467128027682</v>
+        <v>18.546712802768202</v>
       </c>
       <c r="L44" s="2">
         <f t="shared" si="12"/>
@@ -6761,19 +6207,19 @@
       </c>
       <c r="M44" s="15">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N44" s="15">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O44" s="15">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P44" s="16">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -6782,7 +6228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="90.75" customHeight="1" spans="2:18">
+    <row r="45" spans="2:18" ht="90.75" customHeight="1">
       <c r="B45">
         <v>17011502</v>
       </c>
@@ -6809,11 +6255,11 @@
       </c>
       <c r="J45" s="13">
         <f t="shared" si="0"/>
-        <v>21.3322483143455</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="14">
         <f t="shared" si="11"/>
-        <v>23.0890217049387</v>
+        <v>23.089021704938698</v>
       </c>
       <c r="L45" s="2">
         <f t="shared" si="12"/>
@@ -6821,7 +6267,7 @@
       </c>
       <c r="M45" s="15">
         <f t="shared" si="13"/>
-        <v>11.73273657289</v>
+        <v>11.732736572889999</v>
       </c>
       <c r="N45" s="15">
         <f t="shared" si="14"/>
@@ -6829,11 +6275,11 @@
       </c>
       <c r="O45" s="15">
         <f t="shared" si="15"/>
-        <v>10.7941176470588</v>
+        <v>10.794117647058799</v>
       </c>
       <c r="P45" s="16">
         <f t="shared" si="16"/>
-        <v>18.35</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -6842,7 +6288,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" ht="90.75" customHeight="1" spans="2:18">
+    <row r="46" spans="2:18" ht="90.75" customHeight="1">
       <c r="B46">
         <v>17011601</v>
       </c>
@@ -6873,7 +6319,7 @@
       </c>
       <c r="K46" s="14">
         <f t="shared" si="11"/>
-        <v>22.2501834958582</v>
+        <v>22.250183495858199</v>
       </c>
       <c r="L46" s="2">
         <f t="shared" si="12"/>
@@ -6885,15 +6331,15 @@
       </c>
       <c r="N46" s="15">
         <f t="shared" si="14"/>
-        <v>12.237600922722</v>
+        <v>12.237600922722001</v>
       </c>
       <c r="O46" s="15">
         <f t="shared" si="15"/>
-        <v>10.4019607843137</v>
+        <v>10.401960784313699</v>
       </c>
       <c r="P46" s="16">
         <f t="shared" si="16"/>
-        <v>17.6833333333333</v>
+        <v>17.683333333333302</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -6902,7 +6348,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="90.75" customHeight="1" spans="2:18">
+    <row r="47" spans="2:18" ht="90.75" customHeight="1">
       <c r="B47">
         <v>17011503</v>
       </c>
@@ -6933,7 +6379,7 @@
       </c>
       <c r="K47" s="14">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L47" s="2">
         <f t="shared" si="12"/>
@@ -6945,15 +6391,15 @@
       </c>
       <c r="N47" s="15">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O47" s="15">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P47" s="16">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -6962,7 +6408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" ht="90.75" customHeight="1" spans="2:18">
+    <row r="48" spans="2:18" ht="90.75" customHeight="1">
       <c r="B48">
         <v>17011504</v>
       </c>
@@ -6993,7 +6439,7 @@
       </c>
       <c r="K48" s="14">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L48" s="2">
         <f t="shared" si="12"/>
@@ -7005,15 +6451,15 @@
       </c>
       <c r="N48" s="15">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O48" s="15">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P48" s="16">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -7022,7 +6468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" ht="90.75" customHeight="1" spans="2:18">
+    <row r="49" spans="2:18" ht="90.75" customHeight="1">
       <c r="B49">
         <v>17011602</v>
       </c>
@@ -7049,11 +6495,11 @@
       </c>
       <c r="J49" s="13">
         <f t="shared" si="0"/>
-        <v>16.4961636828644</v>
+        <v>16.496163682864399</v>
       </c>
       <c r="K49" s="14">
         <f t="shared" si="11"/>
-        <v>17.8546712802768</v>
+        <v>17.854671280276801</v>
       </c>
       <c r="L49" s="2">
         <f t="shared" si="12"/>
@@ -7061,7 +6507,7 @@
       </c>
       <c r="M49" s="15">
         <f t="shared" si="13"/>
-        <v>12.3721227621483</v>
+        <v>12.372122762148299</v>
       </c>
       <c r="N49" s="15">
         <f t="shared" si="14"/>
@@ -7069,11 +6515,11 @@
       </c>
       <c r="O49" s="15">
         <f t="shared" si="15"/>
-        <v>11.3823529411765</v>
+        <v>11.382352941176499</v>
       </c>
       <c r="P49" s="16">
         <f t="shared" si="16"/>
-        <v>19.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -7082,7 +6528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" ht="90.75" customHeight="1" spans="2:18">
+    <row r="50" spans="2:18" ht="90.75" customHeight="1">
       <c r="B50">
         <v>17011901</v>
       </c>
@@ -7109,11 +6555,11 @@
       </c>
       <c r="J50" s="13">
         <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$72*H50+$M$72)*$L$72)/(1-G50)/(1-$O$72)/(1-I50)/$N$72</f>
-        <v>17.0696737192901</v>
+        <v>17.069673719290101</v>
       </c>
       <c r="K50" s="14">
         <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$72*H50+$M$72)*$L$72)/(1-G50)/(1-$P$72)/(1-I50)/$N$72</f>
-        <v>18.4754115549963</v>
+        <v>18.475411554996299</v>
       </c>
       <c r="L50" s="2">
         <f t="shared" ref="L50:L58" si="19">E50+F50+($K$72*H50+$M$72)*$L$72</f>
@@ -7121,7 +6567,7 @@
       </c>
       <c r="M50" s="15">
         <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$72)/$N$72</f>
-        <v>9.38832054560955</v>
+        <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="15">
         <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$72)/$N$72</f>
@@ -7129,7 +6575,7 @@
       </c>
       <c r="O50" s="15">
         <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$72</f>
-        <v>8.63725490196078</v>
+        <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="16">
         <f t="shared" ref="P50:P58" si="23">O50*$N$72-L50</f>
@@ -7142,7 +6588,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" ht="90.75" customHeight="1" spans="2:18">
+    <row r="51" spans="2:18" ht="90.75" customHeight="1">
       <c r="B51">
         <v>17011902</v>
       </c>
@@ -7173,7 +6619,7 @@
       </c>
       <c r="K51" s="14">
         <f t="shared" si="18"/>
-        <v>15.5132641291811</v>
+        <v>15.513264129181101</v>
       </c>
       <c r="L51" s="2">
         <f t="shared" si="19"/>
@@ -7189,7 +6635,7 @@
       </c>
       <c r="O51" s="15">
         <f t="shared" si="22"/>
-        <v>9.88970588235294</v>
+        <v>9.8897058823529402</v>
       </c>
       <c r="P51" s="16">
         <f t="shared" si="23"/>
@@ -7202,7 +6648,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" ht="90.75" customHeight="1" spans="2:18">
+    <row r="52" spans="2:18" ht="90.75" customHeight="1">
       <c r="B52">
         <v>17020501</v>
       </c>
@@ -7241,19 +6687,19 @@
       </c>
       <c r="M52" s="15">
         <f t="shared" si="20"/>
-        <v>17.5931106138107</v>
+        <v>17.593110613810701</v>
       </c>
       <c r="N52" s="15">
         <f t="shared" si="21"/>
-        <v>19.041955017301</v>
+        <v>19.041955017300999</v>
       </c>
       <c r="O52" s="15">
         <f t="shared" si="22"/>
-        <v>16.1856617647059</v>
+        <v>16.185661764705898</v>
       </c>
       <c r="P52" s="16">
         <f t="shared" si="23"/>
-        <v>22.0125</v>
+        <v>22.012499999999999</v>
       </c>
       <c r="Q52">
         <v>30</v>
@@ -7262,7 +6708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" ht="90.75" customHeight="1" spans="2:18">
+    <row r="53" spans="2:18" ht="90.75" customHeight="1">
       <c r="B53">
         <v>17020502</v>
       </c>
@@ -7289,11 +6735,11 @@
       </c>
       <c r="J53" s="13">
         <f t="shared" si="17"/>
-        <v>24.2774455319885</v>
+        <v>24.277445531988501</v>
       </c>
       <c r="K53" s="14">
         <f t="shared" si="18"/>
-        <v>26.2767645757994</v>
+        <v>26.276764575799401</v>
       </c>
       <c r="L53" s="2">
         <f t="shared" si="19"/>
@@ -7305,15 +6751,15 @@
       </c>
       <c r="N53" s="15">
         <f t="shared" si="21"/>
-        <v>18.3937352030596</v>
+        <v>18.393735203059599</v>
       </c>
       <c r="O53" s="15">
         <f t="shared" si="22"/>
-        <v>15.6346749226006</v>
+        <v>15.634674922600601</v>
       </c>
       <c r="P53" s="16">
         <f t="shared" si="23"/>
-        <v>25.5157894736842</v>
+        <v>25.515789473684201</v>
       </c>
       <c r="Q53">
         <v>30</v>
@@ -7322,7 +6768,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" ht="90.75" customHeight="1" spans="2:18">
+    <row r="54" spans="2:18" ht="90.75" customHeight="1">
       <c r="B54">
         <v>17020601</v>
       </c>
@@ -7349,7 +6795,7 @@
       </c>
       <c r="J54" s="13">
         <f t="shared" si="17"/>
-        <v>20.3518907563025</v>
+        <v>20.351890756302499</v>
       </c>
       <c r="K54" s="14">
         <f t="shared" si="18"/>
@@ -7369,11 +6815,11 @@
       </c>
       <c r="O54" s="15">
         <f t="shared" si="22"/>
-        <v>13.1066176470588</v>
+        <v>13.106617647058799</v>
       </c>
       <c r="P54" s="16">
         <f t="shared" si="23"/>
-        <v>17.825</v>
+        <v>17.824999999999999</v>
       </c>
       <c r="Q54">
         <v>30</v>
@@ -7382,7 +6828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" ht="90.75" customHeight="1" spans="2:18">
+    <row r="55" spans="2:18" ht="90.75" customHeight="1">
       <c r="B55">
         <v>17020701</v>
       </c>
@@ -7409,11 +6855,11 @@
       </c>
       <c r="J55" s="13">
         <f t="shared" si="17"/>
-        <v>24.4907745706978</v>
+        <v>24.490774570697798</v>
       </c>
       <c r="K55" s="14">
         <f t="shared" si="18"/>
-        <v>26.5076618882847</v>
+        <v>26.507661888284701</v>
       </c>
       <c r="L55" s="2">
         <f t="shared" si="19"/>
@@ -7425,11 +6871,11 @@
       </c>
       <c r="N55" s="15">
         <f t="shared" si="21"/>
-        <v>18.5553633217993</v>
+        <v>18.555363321799302</v>
       </c>
       <c r="O55" s="15">
         <f t="shared" si="22"/>
-        <v>15.7720588235294</v>
+        <v>15.772058823529401</v>
       </c>
       <c r="P55" s="16">
         <f t="shared" si="23"/>
@@ -7442,7 +6888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" ht="90.75" customHeight="1" spans="2:18">
+    <row r="56" spans="2:18" ht="90.75" customHeight="1">
       <c r="B56">
         <v>17020801</v>
       </c>
@@ -7469,7 +6915,7 @@
       </c>
       <c r="J56" s="13">
         <f t="shared" si="17"/>
-        <v>12.9475703324808</v>
+        <v>12.947570332480799</v>
       </c>
       <c r="K56" s="14">
         <f t="shared" si="18"/>
@@ -7481,15 +6927,15 @@
       </c>
       <c r="M56" s="15">
         <f t="shared" si="20"/>
-        <v>9.71067774936061</v>
+        <v>9.7106777493606096</v>
       </c>
       <c r="N56" s="15">
         <f t="shared" si="21"/>
-        <v>10.5103806228374</v>
+        <v>10.510380622837401</v>
       </c>
       <c r="O56" s="15">
         <f t="shared" si="22"/>
-        <v>8.93382352941176</v>
+        <v>8.9338235294117592</v>
       </c>
       <c r="P56" s="16">
         <f t="shared" si="23"/>
@@ -7502,7 +6948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" ht="90.75" customHeight="1" spans="2:18">
+    <row r="57" spans="2:18" ht="90.75" customHeight="1">
       <c r="B57">
         <v>17020901</v>
       </c>
@@ -7529,7 +6975,7 @@
       </c>
       <c r="J57" s="13">
         <f t="shared" si="17"/>
-        <v>19.6538595675424</v>
+        <v>19.653859567542401</v>
       </c>
       <c r="K57" s="14">
         <f t="shared" si="18"/>
@@ -7541,7 +6987,7 @@
       </c>
       <c r="M57" s="15">
         <f t="shared" si="20"/>
-        <v>10.8096227621483</v>
+        <v>10.809622762148299</v>
       </c>
       <c r="N57" s="15">
         <f t="shared" si="21"/>
@@ -7549,7 +6995,7 @@
       </c>
       <c r="O57" s="15">
         <f t="shared" si="22"/>
-        <v>9.94485294117647</v>
+        <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="16">
         <f t="shared" si="23"/>
@@ -7562,7 +7008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" ht="90.75" customHeight="1" spans="2:18">
+    <row r="58" spans="2:18" ht="90.75" customHeight="1">
       <c r="B58">
         <v>17020901</v>
       </c>
@@ -7589,11 +7035,11 @@
       </c>
       <c r="J58" s="13">
         <f t="shared" si="17"/>
-        <v>24.9094202898551</v>
+        <v>24.909420289855099</v>
       </c>
       <c r="K58" s="14">
         <f t="shared" si="18"/>
-        <v>26.9607843137255</v>
+        <v>26.960784313725501</v>
       </c>
       <c r="L58" s="2">
         <f t="shared" si="19"/>
@@ -7605,7 +7051,7 @@
       </c>
       <c r="N58" s="15">
         <f t="shared" si="21"/>
-        <v>16.1764705882353</v>
+        <v>16.176470588235301</v>
       </c>
       <c r="O58" s="15">
         <f t="shared" si="22"/>
@@ -7622,7 +7068,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" ht="90.75" customHeight="1" spans="2:18">
+    <row r="59" spans="2:18" ht="90.75" customHeight="1">
       <c r="B59">
         <v>17021104</v>
       </c>
@@ -7653,7 +7099,7 @@
       </c>
       <c r="K59" s="14">
         <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$72*H59+$M$72)*$L$72)/(1-G59)/(1-$P$72)/(1-I59)/$N$72</f>
-        <v>16.9303015323777</v>
+        <v>16.930301532377701</v>
       </c>
       <c r="L59" s="2">
         <f t="shared" ref="L59:L60" si="26">E59+F59+($K$72*H59+$M$72)*$L$72</f>
@@ -7669,7 +7115,7 @@
       </c>
       <c r="O59" s="15">
         <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$72</f>
-        <v>10.0735294117647</v>
+        <v>10.073529411764699</v>
       </c>
       <c r="P59" s="16">
         <f t="shared" ref="P59:P60" si="30">O59*$N$72-L59</f>
@@ -7682,7 +7128,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" ht="90.75" customHeight="1" spans="2:18">
+    <row r="60" spans="2:18" ht="90.75" customHeight="1">
       <c r="B60">
         <v>17021105</v>
       </c>
@@ -7713,7 +7159,7 @@
       </c>
       <c r="K60" s="14">
         <f t="shared" si="25"/>
-        <v>16.9303015323777</v>
+        <v>16.930301532377701</v>
       </c>
       <c r="L60" s="2">
         <f t="shared" si="26"/>
@@ -7729,7 +7175,7 @@
       </c>
       <c r="O60" s="15">
         <f t="shared" si="29"/>
-        <v>10.0735294117647</v>
+        <v>10.073529411764699</v>
       </c>
       <c r="P60" s="16">
         <f t="shared" si="30"/>
@@ -7742,7 +7188,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" ht="90.75" customHeight="1" spans="2:18">
+    <row r="61" spans="2:18" ht="90.75" customHeight="1">
       <c r="B61">
         <v>17021101</v>
       </c>
@@ -7773,7 +7219,7 @@
       </c>
       <c r="K61" s="14">
         <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$72*H61+$M$72)*$L$72)/(1-G61)/(1-$P$72)/(1-I61)/$N$72</f>
-        <v>12.2404844290657</v>
+        <v>12.240484429065701</v>
       </c>
       <c r="L61" s="2">
         <f t="shared" ref="L61:L66" si="33">E61+F61+($K$72*H61+$M$72)*$L$72</f>
@@ -7781,19 +7227,19 @@
       </c>
       <c r="M61" s="15">
         <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$72)/$N$72</f>
-        <v>8.4818574168798</v>
+        <v>8.4818574168797998</v>
       </c>
       <c r="N61" s="15">
         <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$72)/$N$72</f>
-        <v>9.18036332179931</v>
+        <v>9.1803633217993106</v>
       </c>
       <c r="O61" s="15">
         <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$72</f>
-        <v>7.80330882352941</v>
+        <v>7.8033088235294104</v>
       </c>
       <c r="P61" s="16">
         <f t="shared" ref="P61:P66" si="37">O61*$N$72-L61</f>
-        <v>10.6125</v>
+        <v>10.612500000000001</v>
       </c>
       <c r="Q61">
         <v>25</v>
@@ -7802,7 +7248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" ht="90.75" customHeight="1" spans="2:18">
+    <row r="62" spans="2:18" ht="90.75" customHeight="1">
       <c r="B62">
         <v>17021102</v>
       </c>
@@ -7833,7 +7279,7 @@
       </c>
       <c r="K62" s="14">
         <f t="shared" si="32"/>
-        <v>12.7028066128412</v>
+        <v>12.702806612841201</v>
       </c>
       <c r="L62" s="2">
         <f t="shared" si="33"/>
@@ -7841,19 +7287,19 @@
       </c>
       <c r="M62" s="15">
         <f t="shared" si="34"/>
-        <v>8.80221653878943</v>
+        <v>8.8022165387894304</v>
       </c>
       <c r="N62" s="15">
         <f t="shared" si="35"/>
-        <v>9.52710495963091</v>
+        <v>9.5271049596309094</v>
       </c>
       <c r="O62" s="15">
         <f t="shared" si="36"/>
-        <v>8.09803921568627</v>
+        <v>8.0980392156862706</v>
       </c>
       <c r="P62" s="16">
         <f t="shared" si="37"/>
-        <v>13.7666666666667</v>
+        <v>13.766666666666699</v>
       </c>
       <c r="Q62">
         <v>25</v>
@@ -7862,7 +7308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" ht="90.75" customHeight="1" spans="2:18">
+    <row r="63" spans="2:18" ht="90.75" customHeight="1">
       <c r="B63">
         <v>17021103</v>
       </c>
@@ -7893,7 +7339,7 @@
       </c>
       <c r="K63" s="14">
         <f t="shared" si="32"/>
-        <v>15.8785082660515</v>
+        <v>15.878508266051499</v>
       </c>
       <c r="L63" s="2">
         <f t="shared" si="33"/>
@@ -7901,19 +7347,19 @@
       </c>
       <c r="M63" s="15">
         <f t="shared" si="34"/>
-        <v>8.80221653878943</v>
+        <v>8.8022165387894304</v>
       </c>
       <c r="N63" s="15">
         <f t="shared" si="35"/>
-        <v>9.52710495963091</v>
+        <v>9.5271049596309094</v>
       </c>
       <c r="O63" s="15">
         <f t="shared" si="36"/>
-        <v>8.09803921568627</v>
+        <v>8.0980392156862706</v>
       </c>
       <c r="P63" s="16">
         <f t="shared" si="37"/>
-        <v>13.7666666666667</v>
+        <v>13.766666666666699</v>
       </c>
       <c r="Q63">
         <v>25</v>
@@ -7922,7 +7368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" ht="90.75" customHeight="1" spans="2:18">
+    <row r="64" spans="2:18" ht="90.75" customHeight="1">
       <c r="B64">
         <v>17021106</v>
       </c>
@@ -7949,7 +7395,7 @@
       </c>
       <c r="J64" s="13">
         <f t="shared" si="31"/>
-        <v>15.3985507246377</v>
+        <v>15.398550724637699</v>
       </c>
       <c r="K64" s="14">
         <f t="shared" si="32"/>
@@ -7961,7 +7407,7 @@
       </c>
       <c r="M64" s="15">
         <f t="shared" si="34"/>
-        <v>11.5489130434783</v>
+        <v>11.548913043478301</v>
       </c>
       <c r="N64" s="15">
         <f t="shared" si="35"/>
@@ -7982,7 +7428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" ht="90.75" customHeight="1" spans="2:20">
+    <row r="65" spans="2:20" ht="90.75" customHeight="1">
       <c r="B65">
         <v>17021201</v>
       </c>
@@ -8009,11 +7455,11 @@
       </c>
       <c r="J65" s="13">
         <f t="shared" si="31"/>
-        <v>17.2087048685514</v>
+        <v>17.208704868551401</v>
       </c>
       <c r="K65" s="14">
         <f t="shared" si="32"/>
-        <v>18.6258923283145</v>
+        <v>18.625892328314499</v>
       </c>
       <c r="L65" s="2">
         <f t="shared" si="33"/>
@@ -8029,11 +7475,11 @@
       </c>
       <c r="O65" s="15">
         <f t="shared" si="36"/>
-        <v>9.49920508744038</v>
+        <v>9.4992050874403802</v>
       </c>
       <c r="P65" s="16">
         <f t="shared" si="37"/>
-        <v>16.7945945945946</v>
+        <v>16.794594594594599</v>
       </c>
       <c r="Q65">
         <v>40</v>
@@ -8048,7 +7494,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" ht="90.75" customHeight="1" spans="2:19">
+    <row r="66" spans="2:20" ht="90.75" customHeight="1">
       <c r="B66">
         <v>17021301</v>
       </c>
@@ -8075,11 +7521,11 @@
       </c>
       <c r="J66" s="13">
         <f t="shared" si="31"/>
-        <v>20.266258677384</v>
+        <v>20.266258677383998</v>
       </c>
       <c r="K66" s="14">
         <f t="shared" si="32"/>
-        <v>21.9352446861097</v>
+        <v>21.935244686109701</v>
       </c>
       <c r="L66" s="2">
         <f t="shared" si="33"/>
@@ -8091,11 +7537,11 @@
       </c>
       <c r="N66" s="15">
         <f t="shared" si="35"/>
-        <v>15.3546712802768</v>
+        <v>15.354671280276801</v>
       </c>
       <c r="O66" s="15">
         <f t="shared" si="36"/>
-        <v>13.0514705882353</v>
+        <v>13.051470588235301</v>
       </c>
       <c r="P66" s="16">
         <f t="shared" si="37"/>
@@ -8109,7 +7555,7 @@
       </c>
       <c r="S66" s="20"/>
     </row>
-    <row r="67" ht="90.75" customHeight="1" spans="2:19">
+    <row r="67" spans="2:20" ht="90.75" customHeight="1">
       <c r="B67">
         <v>17021401</v>
       </c>
@@ -8136,11 +7582,11 @@
       </c>
       <c r="J67" s="13">
         <f t="shared" ref="J67" si="38">(E67+F67+($K$72*H67+$M$72)*$L$72)/(1-G67)/(1-$O$72)/(1-I67)/$N$72</f>
-        <v>8.36885478829213</v>
+        <v>8.3688547882921291</v>
       </c>
       <c r="K67" s="14">
         <f t="shared" ref="K67" si="39">(E67+F67+($K$72*H67+$M$72)*$L$72)/(1-G67)/(1-$P$72)/(1-I67)/$N$72</f>
-        <v>9.05805459438677</v>
+        <v>9.0580545943867694</v>
       </c>
       <c r="L67" s="2">
         <f t="shared" ref="L67" si="40">E67+F67+($K$72*H67+$M$72)*$L$72</f>
@@ -8148,29 +7594,29 @@
       </c>
       <c r="M67" s="15">
         <f t="shared" ref="M67" si="41">L67/(1-G67)/(1-$O$72)/$N$72</f>
-        <v>6.2766410912191</v>
+        <v>6.2766410912191004</v>
       </c>
       <c r="N67" s="15">
         <f t="shared" ref="N67" si="42">L67/(1-G67)/(1-$P$72)/$N$72</f>
-        <v>6.79354094579008</v>
+        <v>6.7935409457900802</v>
       </c>
       <c r="O67" s="15">
         <f t="shared" ref="O67" si="43">L67/(1-G67)/$N$72</f>
-        <v>5.77450980392157</v>
+        <v>5.7745098039215703</v>
       </c>
       <c r="P67" s="16">
         <f t="shared" ref="P67" si="44">O67*$N$72-L67</f>
         <v>9.81666666666667</v>
       </c>
       <c r="Q67">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R67">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="S67" s="20"/>
     </row>
-    <row r="68" ht="90.75" customHeight="1" spans="2:19">
+    <row r="68" spans="2:20" ht="90.75" customHeight="1">
       <c r="B68">
         <v>17021402</v>
       </c>
@@ -8197,11 +7643,11 @@
       </c>
       <c r="J68" s="13">
         <f>(E68+F68+($K$72*H68+$M$72)*$L$72)/(1-G68)/(1-$O$72)/(1-I68)/$N$72</f>
-        <v>13.7952414167248</v>
+        <v>13.795241416724799</v>
       </c>
       <c r="K68" s="14">
         <f>(E68+F68+($K$72*H68+$M$72)*$L$72)/(1-G68)/(1-$P$72)/(1-I68)/$N$72</f>
-        <v>14.9313201216315</v>
+        <v>14.931320121631501</v>
       </c>
       <c r="L68" s="2">
         <f>E68+F68+($K$72*H68+$M$72)*$L$72</f>
@@ -8209,19 +7655,19 @@
       </c>
       <c r="M68" s="15">
         <f>L68/(1-G68)/(1-$O$72)/$N$72</f>
-        <v>7.58738277919864</v>
+        <v>7.5873827791986397</v>
       </c>
       <c r="N68" s="15">
         <f>L68/(1-G68)/(1-$P$72)/$N$72</f>
-        <v>8.21222606689735</v>
+        <v>8.2122260668973492</v>
       </c>
       <c r="O68" s="15">
         <f>L68/(1-G68)/$N$72</f>
-        <v>6.98039215686275</v>
+        <v>6.9803921568627496</v>
       </c>
       <c r="P68" s="16">
         <f>O68*$N$72-L68</f>
-        <v>11.8666666666667</v>
+        <v>11.866666666666699</v>
       </c>
       <c r="Q68">
         <v>45</v>
@@ -8231,21 +7677,68 @@
       </c>
       <c r="S68" s="20"/>
     </row>
-    <row r="69" ht="90.75" customHeight="1" spans="3:19">
-      <c r="C69" s="2"/>
-      <c r="D69" s="10"/>
-      <c r="G69" s="4"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="16"/>
+    <row r="69" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B69">
+        <v>17021403</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E69">
+        <v>20</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="H69">
+        <v>0.1</v>
+      </c>
+      <c r="I69" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="J69" s="13">
+        <f t="shared" ref="J69" si="45">(E69+F69+($K$72*H69+$M$72)*$L$72)/(1-G69)/(1-$O$72)/(1-I69)/$N$72</f>
+        <v>12.539073600454673</v>
+      </c>
+      <c r="K69" s="14">
+        <f t="shared" ref="K69" si="46">(E69+F69+($K$72*H69+$M$72)*$L$72)/(1-G69)/(1-$P$72)/(1-I69)/$N$72</f>
+        <v>13.571703191080355</v>
+      </c>
+      <c r="L69" s="2">
+        <f t="shared" ref="L69" si="47">E69+F69+($K$72*H69+$M$72)*$L$72</f>
+        <v>35.299999999999997</v>
+      </c>
+      <c r="M69" s="15">
+        <f t="shared" ref="M69" si="48">L69/(1-G69)/(1-$O$72)/$N$72</f>
+        <v>7.5234441602728035</v>
+      </c>
+      <c r="N69" s="15">
+        <f t="shared" ref="N69" si="49">L69/(1-G69)/(1-$P$72)/$N$72</f>
+        <v>8.1430219146482123</v>
+      </c>
+      <c r="O69" s="15">
+        <f t="shared" ref="O69" si="50">L69/(1-G69)/$N$72</f>
+        <v>6.9215686274509798</v>
+      </c>
+      <c r="P69" s="16">
+        <f t="shared" ref="P69" si="51">O69*$N$72-L69</f>
+        <v>11.766666666666666</v>
+      </c>
+      <c r="Q69">
+        <v>25</v>
+      </c>
+      <c r="R69">
+        <v>40</v>
+      </c>
       <c r="S69" s="20"/>
     </row>
-    <row r="71" spans="11:16">
+    <row r="71" spans="2:20">
       <c r="K71" s="18" t="s">
         <v>93</v>
       </c>
@@ -8265,7 +7758,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="11:16">
+    <row r="72" spans="2:20">
       <c r="K72" s="19">
         <v>100</v>
       </c>
@@ -8286,6 +7779,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C69">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
@@ -8298,81 +7792,80 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
-    <hyperlink ref="D43" r:id="rId34" display="https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp"/>
-    <hyperlink ref="D44" r:id="rId35" display="https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW"/>
-    <hyperlink ref="D45" r:id="rId36" display="https://detail.1688.com/offer/525494755952.html?spm=a2615.7691456.0.0.2qsBMx"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://detail.1688.com/offer/525529106954.html?spm=a2615.7691456.0.0.4Tm2o6"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://detail.1688.com/offer/527560763616.html?spm=b26110380.sw311.0.0.p4j2tp"/>
-    <hyperlink ref="D50" r:id="rId39" display="https://detail.1688.com/offer/542627436877.html?spm=b26110380.sw1037004.0.0.aYzCim&amp;sk=consign"/>
-    <hyperlink ref="D52" r:id="rId40" display="https://detail.1688.com/offer/543024612109.html?spm=0.0.0.0.QG7IU6"/>
-    <hyperlink ref="D51" r:id="rId41" display="https://detail.1688.com/offer/543614766781.html?spm=b26110380.8015204.tkhy006.2.m9SOm8"/>
-    <hyperlink ref="D53" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D54" r:id="rId43" display="https://detail.1688.com/offer/45277079052.html?spm=a261y.7663282.0.0.8G3JEy&amp;sk=consign"/>
-    <hyperlink ref="D55" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D56" r:id="rId44" display="https://detail.1688.com/offer/38711199781.html?spm=b26110380.8015204.tkhy006.2.g0hkme"/>
-    <hyperlink ref="D57" r:id="rId45" display="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
-    <hyperlink ref="D58" r:id="rId46" display="https://detail.1688.com/offer/536596301611.html?spm=a2615.7691456.0.0.HFQWm0"/>
-    <hyperlink ref="D60" r:id="rId47" display="https://detail.1688.com/offer/543879481659.html?spm=a2615.7691456.0.0.UWc1Wy"/>
-    <hyperlink ref="D63" r:id="rId48" display="https://detail.1688.com/offer/542163784708.html?spm=0.0.0.0.D3IAEt"/>
-    <hyperlink ref="D59" r:id="rId49" display="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
-    <hyperlink ref="D64" r:id="rId50" display="https://detail.1688.com/offer/520727227145.html?spm=b26110380.7927930.tkhy006.2.4cRHSy"/>
-    <hyperlink ref="D65" r:id="rId51" display="https://detail.1688.com/offer/45288474070.html?spm=0.0.0.0.ROTFEe"/>
-    <hyperlink ref="S65" r:id="rId52" display="https://detail.1688.com/offer/542800642320.html?spm=b26110380.7927930.xshy005.529.St2Fw9"/>
-    <hyperlink ref="D66" r:id="rId53" display="https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan"/>
-    <hyperlink ref="D68" r:id="rId54" display="https://detail.1688.com/offer/529253294546.html?spm=a2615.7691456.0.0.Q2HHFu"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D49" r:id="rId40"/>
+    <hyperlink ref="D50" r:id="rId41"/>
+    <hyperlink ref="D52" r:id="rId42"/>
+    <hyperlink ref="D51" r:id="rId43"/>
+    <hyperlink ref="D53" r:id="rId44"/>
+    <hyperlink ref="D54" r:id="rId45"/>
+    <hyperlink ref="D55" r:id="rId46"/>
+    <hyperlink ref="D56" r:id="rId47"/>
+    <hyperlink ref="D57" r:id="rId48" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
+    <hyperlink ref="D58" r:id="rId49"/>
+    <hyperlink ref="D60" r:id="rId50"/>
+    <hyperlink ref="D63" r:id="rId51"/>
+    <hyperlink ref="D59" r:id="rId52" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
+    <hyperlink ref="D64" r:id="rId53"/>
+    <hyperlink ref="D65" r:id="rId54"/>
+    <hyperlink ref="S65" r:id="rId55"/>
+    <hyperlink ref="D66" r:id="rId56"/>
+    <hyperlink ref="D68" r:id="rId57"/>
+    <hyperlink ref="D69" r:id="rId58"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId59"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1"/>
@@ -8395,25 +7888,22 @@
       <c r="C4" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
171603 by hjx topolino 大童外套
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>产品标题</t>
   </si>
@@ -288,139 +288,55 @@
     <t>https://detail.1688.com/offer/542800642320.html?spm=b26110380.7927930.xshy005.529.St2Fw9</t>
   </si>
   <si>
+    <t>https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/542588347406.html?spm=0.0.0.0.uOstC8&amp;sk=consign</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/529253294546.html?spm=a2615.7691456.0.0.Q2HHFu</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/544238732440.html?spm=0.0.0.0.XUpSK3</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/536547771377.html?spm=a2615.7691456.0.0.0h3eHa</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/530505809495.html?spm=a2615.7691456.0.0.mwCaVr</t>
+  </si>
+  <si>
+    <t>国际运费 1kg/￥</t>
+  </si>
+  <si>
+    <t>国际运费折扣</t>
+  </si>
+  <si>
+    <t>挂号费</t>
+  </si>
+  <si>
+    <t>汇率</t>
+  </si>
+  <si>
+    <t>速卖通费率</t>
+  </si>
+  <si>
+    <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/542553809977.html?spm=a2615.7691456.0.0.yQWyYp</t>
+  </si>
+  <si>
     <t>https://detail.1688.com/offer/45422676746.html?spm=b26110380.8015204.xshy005.17.K9Fn6R</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/542588347406.html?spm=0.0.0.0.uOstC8&amp;sk=consign</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/529253294546.html?spm=a2615.7691456.0.0.Q2HHFu</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/544238732440.html?spm=0.0.0.0.XUpSK3</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/536547771377.html?spm=a2615.7691456.0.0.0h3eHa</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/530505809495.html?spm=a2615.7691456.0.0.mwCaVr</t>
-  </si>
-  <si>
-    <t>国际运费 1kg/￥</t>
-  </si>
-  <si>
-    <t>国际运费折扣</t>
-  </si>
-  <si>
-    <t>挂号费</t>
-  </si>
-  <si>
-    <t>汇率</t>
-  </si>
-  <si>
-    <t>速卖通费率</t>
-  </si>
-  <si>
-    <t>wish费率</t>
-  </si>
-  <si>
-    <t>https://detail.1688.com/offer/542553809977.html?spm=a2615.7691456.0.0.yQWyYp</t>
-  </si>
-  <si>
-    <t>Product Size</t>
-  </si>
-  <si>
-    <t>Skirt Waist*2</t>
-  </si>
-  <si>
-    <t>80 ( 12M )</t>
-  </si>
-  <si>
-    <t>35 cm</t>
-  </si>
-  <si>
-    <t>26*2 cm</t>
-  </si>
-  <si>
-    <t>20 cm</t>
-  </si>
-  <si>
-    <t>19*2 cm</t>
-  </si>
-  <si>
-    <t>90 ( 24M )</t>
-  </si>
-  <si>
-    <t>37 cm</t>
-  </si>
-  <si>
-    <t>27*2 cm</t>
-  </si>
-  <si>
-    <t>23 cm</t>
-  </si>
-  <si>
-    <t>20*2 cm</t>
-  </si>
-  <si>
-    <t>100 ( 3T )</t>
-  </si>
-  <si>
-    <t>39 cm</t>
-  </si>
-  <si>
-    <t>28*2 cm</t>
-  </si>
-  <si>
-    <t>25 cm</t>
-  </si>
-  <si>
-    <t>21*2 cm</t>
-  </si>
-  <si>
-    <t>110 ( 4T )</t>
-  </si>
-  <si>
-    <t>41 cm</t>
-  </si>
-  <si>
-    <t>29*2 cm</t>
-  </si>
-  <si>
-    <t>27 cm</t>
-  </si>
-  <si>
-    <t>22*2 cm</t>
-  </si>
-  <si>
-    <t>120 ( 5T )</t>
-  </si>
-  <si>
-    <t>43 cm</t>
-  </si>
-  <si>
-    <t>30*2 cm</t>
-  </si>
-  <si>
-    <t>31 cm</t>
-  </si>
-  <si>
-    <t>24*2 cm</t>
-  </si>
-  <si>
-    <t>Skirt Length </t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top Bust*2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Top Length </t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/540415830695.html?spm=a2615.7691456.0.0.fxjODa</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/45288474070.html?spm=0.0.0.0.ROTFEe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -429,24 +345,17 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="180" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -500,7 +409,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -508,34 +417,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -548,53 +442,50 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3523,6 +3414,82 @@
         <a:xfrm>
           <a:off x="0" y="79438500"/>
           <a:ext cx="1022240" cy="1002196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>99392</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>57979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>977348</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>1086767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="图片 73" descr="QQ截图20170216225449.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="99392" y="80598066"/>
+          <a:ext cx="877956" cy="1028788"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>132523</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>977349</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>1119446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="图片 74" descr="QQ截图20170216234511.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="132523" y="81732783"/>
+          <a:ext cx="844826" cy="1078033"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3819,11 +3786,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T76"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R73" sqref="R73"/>
+      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3929,31 +3896,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$76*H2+$M$76)*$L$76)/(1-G2)/(1-$O$76)/(1-I2)/$N$76</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$78*H2+$M$78)*$L$78)/(1-G2)/(1-$O$78)/(1-I2)/$N$78</f>
         <v>16.874780602778198</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$76*H2+$M$76)*$L$76)/(1-G2)/(1-$P$76)/(1-I2)/$N$76</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$78*H2+$M$78)*$L$78)/(1-G2)/(1-$P$78)/(1-I2)/$N$78</f>
         <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$76*H2+$M$76)*$L$76</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$78*H2+$M$78)*$L$78</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$78)/$N$78</f>
         <v>14.3435635123615</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$78)/$N$78</f>
         <v>15.524798154555899</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$76</f>
+        <f>L2/(1-G2)/$N$78</f>
         <v>13.1960784313726</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$76-L2</f>
+        <f>O2*$N$78-L2</f>
         <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
@@ -3994,27 +3961,27 @@
         <v>11.025859619209999</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$76*H3+$M$76)*$L$76)/(1-G3)/(1-$P$76)/(1-I3)/$N$76</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$78*H3+$M$78)*$L$78)/(1-G3)/(1-$P$78)/(1-I3)/$N$78</f>
         <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$76*H3+$M$76)*$L$76</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$78*H3+$M$78)*$L$78</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$78)/$N$78</f>
         <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$78)/$N$78</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$76</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$78</f>
         <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$76-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$78-L3</f>
         <v>12.9333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -4241,27 +4208,27 @@
         <v>17.250890125871301</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$76*H7+$M$76)*$L$76)/(1-G7)/(1-$P$76)/(1-I7)/$N$76</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$78*H7+$M$78)*$L$78)/(1-G7)/(1-$P$78)/(1-I7)/$N$78</f>
         <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$76*H7+$M$76)*$L$76</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$78*H7+$M$78)*$L$78</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$78)/$N$78</f>
         <v>14.663256606990601</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$78)/$N$78</f>
         <v>15.8708189158016</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$76</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$78</f>
         <v>13.490196078431399</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$76-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$78-L7</f>
         <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
@@ -6781,31 +6748,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$76*H50+$M$76)*$L$76)/(1-G50)/(1-$O$76)/(1-I50)/$N$76</f>
+        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$78*H50+$M$78)*$L$78)/(1-G50)/(1-$O$78)/(1-I50)/$N$78</f>
         <v>17.069673719290101</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$76*H50+$M$76)*$L$76)/(1-G50)/(1-$P$76)/(1-I50)/$N$76</f>
+        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$78*H50+$M$78)*$L$78)/(1-G50)/(1-$P$78)/(1-I50)/$N$78</f>
         <v>18.475411554996299</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$76*H50+$M$76)*$L$76</f>
+        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$78*H50+$M$78)*$L$78</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$78)/$N$78</f>
         <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$78)/$N$78</f>
         <v>10.161476355248</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$76</f>
+        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$78</f>
         <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="23">O50*$N$76-L50</f>
+        <f t="shared" ref="P50:P58" si="23">O50*$N$78-L50</f>
         <v>14.6833333333333</v>
       </c>
       <c r="Q50">
@@ -7321,31 +7288,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$76*H59+$M$76)*$L$76)/(1-G59)/(1-$O$76)/(1-I59)/$N$76</f>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$78*H59+$M$78)*$L$78)/(1-G59)/(1-$O$78)/(1-I59)/$N$78</f>
         <v>15.6421264157837</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$76*H59+$M$76)*$L$76)/(1-G59)/(1-$P$76)/(1-I59)/$N$76</f>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$78*H59+$M$78)*$L$78)/(1-G59)/(1-$P$78)/(1-I59)/$N$78</f>
         <v>16.930301532377701</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$76*H59+$M$76)*$L$76</f>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$78*H59+$M$78)*$L$78</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$78)/$N$78</f>
         <v>10.9494884910486</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$78)/$N$78</f>
         <v>11.8512110726644</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$76</f>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$78</f>
         <v>10.073529411764699</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" ref="P59:P60" si="30">O59*$N$76-L59</f>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$78-L59</f>
         <v>13.7</v>
       </c>
       <c r="Q59">
@@ -7441,31 +7408,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$76*H61+$M$76)*$L$76)/(1-G61)/(1-$O$76)/(1-I61)/$N$76</f>
+        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$78*H61+$M$78)*$L$78)/(1-G61)/(1-$O$78)/(1-I61)/$N$78</f>
         <v>11.3091432225064</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$76*H61+$M$76)*$L$76)/(1-G61)/(1-$P$76)/(1-I61)/$N$76</f>
+        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$78*H61+$M$78)*$L$78)/(1-G61)/(1-$P$78)/(1-I61)/$N$78</f>
         <v>12.240484429065701</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$76*H61+$M$76)*$L$76</f>
+        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$78*H61+$M$78)*$L$78</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$78)/$N$78</f>
         <v>8.4818574168797998</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$78)/$N$78</f>
         <v>9.1803633217993106</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$76</f>
+        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$78</f>
         <v>7.8033088235294104</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="37">O61*$N$76-L61</f>
+        <f t="shared" ref="P61:P66" si="37">O61*$N$78-L61</f>
         <v>10.612500000000001</v>
       </c>
       <c r="Q61">
@@ -7717,8 +7684,8 @@
       <c r="S65" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="T65" t="s">
-        <v>89</v>
+      <c r="T65" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="66" spans="2:20" ht="90.75" customHeight="1">
@@ -7729,7 +7696,7 @@
         <v>28</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E66">
         <v>35</v>
@@ -7790,7 +7757,7 @@
         <v>21</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E67">
         <v>14</v>
@@ -7808,31 +7775,31 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$76*H67+$M$76)*$L$76)/(1-G67)/(1-$O$76)/(1-I67)/$N$76</f>
+        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$78*H67+$M$78)*$L$78)/(1-G67)/(1-$O$78)/(1-I67)/$N$78</f>
         <v>10.4610684853652</v>
       </c>
       <c r="K67" s="12">
-        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$76*H67+$M$76)*$L$76)/(1-G67)/(1-$P$76)/(1-I67)/$N$76</f>
+        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$78*H67+$M$78)*$L$78)/(1-G67)/(1-$P$78)/(1-I67)/$N$78</f>
         <v>11.3225682429835</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$76*H67+$M$76)*$L$76</f>
+        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$78*H67+$M$78)*$L$78</f>
         <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$78)/$N$78</f>
         <v>6.2766410912191004</v>
       </c>
       <c r="N67" s="13">
-        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$78)/$N$78</f>
         <v>6.7935409457900802</v>
       </c>
       <c r="O67" s="13">
-        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$76</f>
+        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$78</f>
         <v>5.7745098039215703</v>
       </c>
       <c r="P67" s="14">
-        <f t="shared" ref="P67:P68" si="44">O67*$N$76-L67</f>
+        <f t="shared" ref="P67:P68" si="44">O67*$N$78-L67</f>
         <v>9.81666666666667</v>
       </c>
       <c r="Q67">
@@ -7851,7 +7818,7 @@
         <v>21</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E68">
         <v>20</v>
@@ -7912,7 +7879,7 @@
         <v>21</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E69">
         <v>20</v>
@@ -7930,31 +7897,31 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69" si="45">(E69+F69+($K$76*H69+$M$76)*$L$76)/(1-G69)/(1-$O$76)/(1-I69)/$N$76</f>
+        <f t="shared" ref="J69" si="45">(E69+F69+($K$78*H69+$M$78)*$L$78)/(1-G69)/(1-$O$78)/(1-I69)/$N$78</f>
         <v>12.539073600454699</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69" si="46">(E69+F69+($K$76*H69+$M$76)*$L$76)/(1-G69)/(1-$P$76)/(1-I69)/$N$76</f>
+        <f t="shared" ref="K69" si="46">(E69+F69+($K$78*H69+$M$78)*$L$78)/(1-G69)/(1-$P$78)/(1-I69)/$N$78</f>
         <v>13.571703191080401</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69" si="47">E69+F69+($K$76*H69+$M$76)*$L$76</f>
+        <f t="shared" ref="L69" si="47">E69+F69+($K$78*H69+$M$78)*$L$78</f>
         <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69" si="48">L69/(1-G69)/(1-$O$76)/$N$76</f>
+        <f t="shared" ref="M69" si="48">L69/(1-G69)/(1-$O$78)/$N$78</f>
         <v>7.5234441602727999</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69" si="49">L69/(1-G69)/(1-$P$76)/$N$76</f>
+        <f t="shared" ref="N69" si="49">L69/(1-G69)/(1-$P$78)/$N$78</f>
         <v>8.1430219146482106</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69" si="50">L69/(1-G69)/$N$76</f>
+        <f t="shared" ref="O69" si="50">L69/(1-G69)/$N$78</f>
         <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69" si="51">O69*$N$76-L69</f>
+        <f t="shared" ref="P69" si="51">O69*$N$78-L69</f>
         <v>11.766666666666699</v>
       </c>
       <c r="Q69">
@@ -7973,7 +7940,7 @@
         <v>21</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E70">
         <v>27.5</v>
@@ -7991,31 +7958,31 @@
         <v>0.25</v>
       </c>
       <c r="J70" s="11">
-        <f>(E70+F70+($K$76*H70+$M$76)*$L$76)/(1-G70)/(1-$O$76)/(1-I70)/$N$76</f>
+        <f>(E70+F70+($K$78*H70+$M$78)*$L$78)/(1-G70)/(1-$O$78)/(1-I70)/$N$78</f>
         <v>12.7308894572322</v>
       </c>
       <c r="K70" s="12">
-        <f>(E70+F70+($K$76*H70+$M$76)*$L$76)/(1-G70)/(1-$P$76)/(1-I70)/$N$76</f>
+        <f>(E70+F70+($K$78*H70+$M$78)*$L$78)/(1-G70)/(1-$P$78)/(1-I70)/$N$78</f>
         <v>13.779315647827801</v>
       </c>
       <c r="L70" s="1">
-        <f>E70+F70+($K$76*H70+$M$76)*$L$76</f>
+        <f>E70+F70+($K$78*H70+$M$78)*$L$78</f>
         <v>44.8</v>
       </c>
       <c r="M70" s="13">
-        <f>L70/(1-G70)/(1-$O$76)/$N$76</f>
+        <f>L70/(1-G70)/(1-$O$78)/$N$78</f>
         <v>9.5481670929241194</v>
       </c>
       <c r="N70" s="13">
-        <f>L70/(1-G70)/(1-$P$76)/$N$76</f>
+        <f>L70/(1-G70)/(1-$P$78)/$N$78</f>
         <v>10.334486735870801</v>
       </c>
       <c r="O70" s="13">
-        <f>L70/(1-G70)/$N$76</f>
+        <f>L70/(1-G70)/$N$78</f>
         <v>8.7843137254902004</v>
       </c>
       <c r="P70" s="14">
-        <f>O70*$N$76-L70</f>
+        <f>O70*$N$78-L70</f>
         <v>14.9333333333333</v>
       </c>
       <c r="Q70">
@@ -8034,7 +8001,7 @@
         <v>18</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E71">
         <v>19.5</v>
@@ -8052,31 +8019,31 @@
         <v>0.25</v>
       </c>
       <c r="J71" s="11">
-        <f>(E71+F71+($K$76*H71+$M$76)*$L$76)/(1-G71)/(1-$O$76)/(1-I71)/$N$76</f>
+        <f>(E71+F71+($K$78*H71+$M$78)*$L$78)/(1-G71)/(1-$O$78)/(1-I71)/$N$78</f>
         <v>9.9744245524296709</v>
       </c>
       <c r="K71" s="12">
-        <f>(E71+F71+($K$76*H71+$M$76)*$L$76)/(1-G71)/(1-$P$76)/(1-I71)/$N$76</f>
+        <f>(E71+F71+($K$78*H71+$M$78)*$L$78)/(1-G71)/(1-$P$78)/(1-I71)/$N$78</f>
         <v>10.7958477508651</v>
       </c>
       <c r="L71" s="1">
-        <f>E71+F71+($K$76*H71+$M$76)*$L$76</f>
+        <f>E71+F71+($K$78*H71+$M$78)*$L$78</f>
         <v>35.1</v>
       </c>
       <c r="M71" s="13">
-        <f>L71/(1-G71)/(1-$O$76)/$N$76</f>
+        <f>L71/(1-G71)/(1-$O$78)/$N$78</f>
         <v>7.4808184143222496</v>
       </c>
       <c r="N71" s="13">
-        <f>L71/(1-G71)/(1-$P$76)/$N$76</f>
+        <f>L71/(1-G71)/(1-$P$78)/$N$78</f>
         <v>8.0968858131487895</v>
       </c>
       <c r="O71" s="13">
-        <f>L71/(1-G71)/$N$76</f>
+        <f>L71/(1-G71)/$N$78</f>
         <v>6.8823529411764701</v>
       </c>
       <c r="P71" s="14">
-        <f>O71*$N$76-L71</f>
+        <f>O71*$N$78-L71</f>
         <v>11.7</v>
       </c>
       <c r="Q71">
@@ -8095,7 +8062,7 @@
         <v>36</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E72">
         <v>23</v>
@@ -8113,31 +8080,31 @@
         <v>0.25</v>
       </c>
       <c r="J72" s="11">
-        <f>(E72+F72+($K$76*H72+$M$76)*$L$76)/(1-G72)/(1-$O$76)/(1-I72)/$N$76</f>
+        <f>(E72+F72+($K$78*H72+$M$78)*$L$78)/(1-G72)/(1-$O$78)/(1-I72)/$N$78</f>
         <v>12.375674907644216</v>
       </c>
       <c r="K72" s="12">
-        <f>(E72+F72+($K$76*H72+$M$76)*$L$76)/(1-G72)/(1-$P$76)/(1-I72)/$N$76</f>
+        <f>(E72+F72+($K$78*H72+$M$78)*$L$78)/(1-G72)/(1-$P$78)/(1-I72)/$N$78</f>
         <v>13.394848135332564</v>
       </c>
       <c r="L72" s="1">
-        <f>E72+F72+($K$76*H72+$M$76)*$L$76</f>
+        <f>E72+F72+($K$78*H72+$M$78)*$L$78</f>
         <v>43.55</v>
       </c>
       <c r="M72" s="13">
-        <f>L72/(1-G72)/(1-$O$76)/$N$76</f>
+        <f>L72/(1-G72)/(1-$O$78)/$N$78</f>
         <v>9.2817561807331614</v>
       </c>
       <c r="N72" s="13">
-        <f>L72/(1-G72)/(1-$P$76)/$N$76</f>
+        <f>L72/(1-G72)/(1-$P$78)/$N$78</f>
         <v>10.046136101499423</v>
       </c>
       <c r="O72" s="13">
-        <f>L72/(1-G72)/$N$76</f>
+        <f>L72/(1-G72)/$N$78</f>
         <v>8.5392156862745097</v>
       </c>
       <c r="P72" s="14">
-        <f>O72*$N$76-L72</f>
+        <f>O72*$N$78-L72</f>
         <v>14.516666666666666</v>
       </c>
       <c r="Q72">
@@ -8149,66 +8116,190 @@
       <c r="S72" s="18"/>
     </row>
     <row r="73" spans="2:20" ht="90.75" customHeight="1">
-      <c r="C73" s="1"/>
-      <c r="D73" s="9"/>
-      <c r="G73" s="3"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="14"/>
-      <c r="S73" s="18"/>
+      <c r="B73">
+        <v>17021601</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E73">
+        <v>22</v>
+      </c>
+      <c r="F73">
+        <v>2</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H73">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I73" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J73" s="11">
+        <f>(E73+F73+($K$78*H73+$M$78)*$L$78)/(1-G73)/(1-$O$78)/(1-I73)/$N$78</f>
+        <v>19.394714407502132</v>
+      </c>
+      <c r="K73" s="12">
+        <f>(E73+F73+($K$78*H73+$M$78)*$L$78)/(1-G73)/(1-$P$78)/(1-I73)/$N$78</f>
+        <v>20.991926182237602</v>
+      </c>
+      <c r="L73" s="1">
+        <f>E73+F73+($K$78*H73+$M$78)*$L$78</f>
+        <v>54.599999999999994</v>
+      </c>
+      <c r="M73" s="13">
+        <f>L73/(1-G73)/(1-$O$78)/$N$78</f>
+        <v>11.636828644501279</v>
+      </c>
+      <c r="N73" s="13">
+        <f>L73/(1-G73)/(1-$P$78)/$N$78</f>
+        <v>12.59515570934256</v>
+      </c>
+      <c r="O73" s="13">
+        <f>L73/(1-G73)/$N$78</f>
+        <v>10.705882352941176</v>
+      </c>
+      <c r="P73" s="14">
+        <f>O73*$N$78-L73</f>
+        <v>18.200000000000003</v>
+      </c>
+      <c r="Q73">
+        <v>40</v>
+      </c>
+      <c r="R73">
+        <v>25</v>
+      </c>
+      <c r="S73" s="18" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="75" spans="2:20">
-      <c r="K75" s="16" t="s">
+    <row r="74" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B74">
+        <v>17021602</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E74">
+        <v>60</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H74">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I74" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J74" s="11">
+        <f>(E74+F74+($K$78*H74+$M$78)*$L$78)/(1-G74)/(1-$O$78)/(1-I74)/$N$78</f>
+        <v>38.479726129582268</v>
+      </c>
+      <c r="K74" s="12">
+        <f>(E74+F74+($K$78*H74+$M$78)*$L$78)/(1-G74)/(1-$P$78)/(1-I74)/$N$78</f>
+        <v>41.648644752018463</v>
+      </c>
+      <c r="L74" s="1">
+        <f>E74+F74+($K$78*H74+$M$78)*$L$78</f>
+        <v>115.55000000000001</v>
+      </c>
+      <c r="M74" s="13">
+        <f>L74/(1-G74)/(1-$O$78)/$N$78</f>
+        <v>23.087835677749361</v>
+      </c>
+      <c r="N74" s="13">
+        <f>L74/(1-G74)/(1-$P$78)/$N$78</f>
+        <v>24.989186851211073</v>
+      </c>
+      <c r="O74" s="13">
+        <f>L74/(1-G74)/$N$78</f>
+        <v>21.240808823529413</v>
+      </c>
+      <c r="P74" s="14">
+        <f>O74*$N$78-L74</f>
+        <v>28.887499999999989</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>25</v>
+      </c>
+      <c r="S74" s="18"/>
+    </row>
+    <row r="75" spans="2:20" ht="90.75" customHeight="1">
+      <c r="C75" s="1"/>
+      <c r="D75" s="9"/>
+      <c r="G75" s="3"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="14"/>
+      <c r="S75" s="18"/>
+    </row>
+    <row r="77" spans="2:20">
+      <c r="K77" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="L77" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="L75" s="16" t="s">
+      <c r="M77" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="M75" s="16" t="s">
+      <c r="N77" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="N75" s="16" t="s">
+      <c r="O77" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="O75" s="16" t="s">
+      <c r="P77" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="P75" s="16" t="s">
-        <v>101</v>
-      </c>
     </row>
-    <row r="76" spans="2:20">
-      <c r="K76" s="17">
+    <row r="78" spans="2:20">
+      <c r="K78" s="17">
         <v>100</v>
       </c>
-      <c r="L76" s="15">
+      <c r="L78" s="15">
         <v>0.85</v>
       </c>
-      <c r="M76">
+      <c r="M78">
         <v>8</v>
       </c>
-      <c r="N76">
+      <c r="N78">
         <v>6.8</v>
       </c>
-      <c r="O76" s="15">
+      <c r="O78" s="15">
         <v>0.08</v>
       </c>
-      <c r="P76" s="15">
+      <c r="P78" s="15">
         <v>0.15</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C73">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C75">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -8276,127 +8367,28 @@
     <hyperlink ref="D69" r:id="rId58"/>
     <hyperlink ref="D70" r:id="rId59"/>
     <hyperlink ref="D71" r:id="rId60"/>
+    <hyperlink ref="T65" r:id="rId61"/>
+    <hyperlink ref="D73" r:id="rId62"/>
+    <hyperlink ref="S73" r:id="rId63"/>
+    <hyperlink ref="D74" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId61"/>
+  <drawing r:id="rId65"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:E6"/>
+      <selection activeCell="F8" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="22.5">
-      <c r="A1" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -8410,7 +8402,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
17021803 by ski suit 4-14
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="18540" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="107">
   <si>
     <t>产品标题</t>
   </si>
@@ -337,23 +337,22 @@
   </si>
   <si>
     <t>wish费率</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/521671959315.html?spm=a2615.7691456.0.0.ACiBQW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  <numFmts count="4">
     <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;US$&quot;* #,##0.00_ ;_-&quot;US$&quot;* \-#,##0.00\ ;_-&quot;US$&quot;* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,142 +386,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,194 +411,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -730,251 +420,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -991,37 +445,37 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1030,70 +484,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="3">
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1115,7 +524,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1157,7 +566,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1199,7 +608,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1241,7 +650,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1283,7 +692,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1325,7 +734,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1367,7 +776,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1409,7 +818,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1451,7 +860,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1493,7 +902,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1535,7 +944,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1577,7 +986,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1619,7 +1028,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId13" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1661,7 +1070,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId14" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1703,7 +1112,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId15" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1745,7 +1154,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId16" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1787,7 +1196,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId17" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1829,7 +1238,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId18" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1871,7 +1280,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId19" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1913,7 +1322,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId20" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1955,7 +1364,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId21" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1997,7 +1406,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId22" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2039,7 +1448,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId23" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2081,7 +1490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId24" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2123,7 +1532,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId25" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2165,7 +1574,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId26" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2207,7 +1616,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId27" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2249,7 +1658,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId28" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2291,7 +1700,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId29" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2333,7 +1742,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId30" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2375,7 +1784,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId31" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2417,7 +1826,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId32" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2459,7 +1868,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId33" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2501,7 +1910,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId34" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2543,7 +1952,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId35" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2585,7 +1994,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId36" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2627,7 +2036,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId37" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2669,7 +2078,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId38" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2711,7 +2120,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId39" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2753,7 +2162,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId40" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2795,7 +2204,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId41" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2837,7 +2246,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId42" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2879,7 +2288,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId43" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2921,7 +2330,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId44" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2963,7 +2372,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId45" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3005,7 +2414,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId46" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3047,7 +2456,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId47" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3089,7 +2498,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId48" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3131,7 +2540,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId49" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3173,7 +2582,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId50" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3215,7 +2624,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId51" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3257,7 +2666,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId52" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3295,7 +2704,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId53" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3333,7 +2742,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId54" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3371,7 +2780,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId55" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3409,7 +2818,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId56" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3451,7 +2860,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId57" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3489,7 +2898,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId58" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3527,7 +2936,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId59" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3569,7 +2978,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId60" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3607,7 +3016,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId61" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3645,7 +3054,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId62" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3683,7 +3092,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId63" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3721,7 +3130,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId64" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3759,7 +3168,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId65" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3797,7 +3206,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId66" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId66" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3835,7 +3244,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId67" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId67" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3877,7 +3286,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId68" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId68" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3915,7 +3324,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId69" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId69" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3957,7 +3366,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId70" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId70" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3999,7 +3408,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId71" cstate="email"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId71" cstate="email"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4037,7 +3446,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId72" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId72" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4075,7 +3484,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId73" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId73" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4113,7 +3522,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId74"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId74"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4155,7 +3564,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId75"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId75"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4172,6 +3581,44 @@
         <a:ln w="9525">
           <a:noFill/>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>57978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1035326</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>1051891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="图片 76" descr="光影魔术手拼图.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId76" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41413" y="85203195"/>
+          <a:ext cx="993913" cy="993913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4463,37 +3910,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="P75" sqref="P75:P76"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.1272727272727" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="17.3727272727273" customWidth="1"/>
-    <col min="5" max="5" width="7.25454545454545" customWidth="1"/>
-    <col min="6" max="6" width="8.87272727272727" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="7.25" customWidth="1"/>
+    <col min="6" max="6" width="8.875" customWidth="1"/>
     <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="7.37272727272727" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="11.1272727272727" customWidth="1"/>
-    <col min="12" max="12" width="7.62727272727273" customWidth="1"/>
-    <col min="13" max="13" width="11.8727272727273" customWidth="1"/>
-    <col min="14" max="15" width="11.6272727272727" customWidth="1"/>
-    <col min="16" max="16" width="9.87272727272727" customWidth="1"/>
+    <col min="11" max="11" width="11.125" customWidth="1"/>
+    <col min="12" max="12" width="7.625" customWidth="1"/>
+    <col min="13" max="13" width="11.875" customWidth="1"/>
+    <col min="14" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="9.875" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="6.87272727272727" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4549,7 +3994,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="86.25" customHeight="1" spans="1:18">
+    <row r="2" spans="1:19" ht="86.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>16072601</v>
@@ -4577,11 +4022,11 @@
       </c>
       <c r="J2" s="11">
         <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$81*H2+$M$81)*$L$81)/(1-G2)/(1-$O$81)/(1-I2)/$N$81</f>
-        <v>16.8747806027782</v>
+        <v>16.874780602778198</v>
       </c>
       <c r="K2" s="12">
         <f t="shared" ref="K2" si="1">(E2+F2+($K$81*H2+$M$81)*$L$81)/(1-G2)/(1-$P$81)/(1-I2)/$N$81</f>
-        <v>18.2644684171246</v>
+        <v>18.264468417124601</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2" si="2">E2+F2+($K$81*H2+$M$81)*$L$81</f>
@@ -4593,7 +4038,7 @@
       </c>
       <c r="N2" s="13">
         <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$81)/$N$81</f>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O2" s="13">
         <f>L2/(1-G2)/$N$81</f>
@@ -4601,7 +4046,7 @@
       </c>
       <c r="P2" s="14">
         <f>O2*$N$81-L2</f>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -4610,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="86.25" customHeight="1" spans="1:18">
+    <row r="3" spans="1:19" ht="86.25" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <v>16072701</v>
@@ -4638,27 +4083,27 @@
       </c>
       <c r="J3" s="11">
         <f t="shared" si="0"/>
-        <v>11.02585961921</v>
+        <v>11.025859619209999</v>
       </c>
       <c r="K3" s="12">
         <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$81*H3+$M$81)*$L$81)/(1-G3)/(1-$P$81)/(1-I3)/$N$81</f>
-        <v>11.9338715878508</v>
+        <v>11.933871587850801</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L6" si="6">E3+F3+($K$81*H3+$M$81)*$L$81</f>
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
         <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$81)/$N$81</f>
-        <v>8.2693947144075</v>
+        <v>8.2693947144075004</v>
       </c>
       <c r="N3" s="13">
         <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$81)/$N$81</f>
-        <v>8.95040369088812</v>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
         <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$81</f>
-        <v>7.6078431372549</v>
+        <v>7.6078431372548998</v>
       </c>
       <c r="P3" s="14">
         <f t="shared" ref="P3:P6" si="10">O3*$N$81-L3</f>
@@ -4671,7 +4116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="69.75" customHeight="1" spans="1:18">
+    <row r="4" spans="1:19" ht="69.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>16072901</v>
@@ -4699,11 +4144,11 @@
       </c>
       <c r="J4" s="11">
         <f t="shared" si="0"/>
-        <v>19.1206917549629</v>
+        <v>19.120691754962898</v>
       </c>
       <c r="K4" s="12">
         <f t="shared" si="5"/>
-        <v>20.6953369583127</v>
+        <v>20.695336958312701</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="6"/>
@@ -4711,11 +4156,11 @@
       </c>
       <c r="M4" s="13">
         <f t="shared" si="7"/>
-        <v>13.384484228474</v>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" si="8"/>
-        <v>14.4867358708189</v>
+        <v>14.486735870818899</v>
       </c>
       <c r="O4" s="13">
         <f t="shared" si="9"/>
@@ -4723,7 +4168,7 @@
       </c>
       <c r="P4" s="14">
         <f t="shared" si="10"/>
-        <v>20.9333333333333</v>
+        <v>20.933333333333302</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -4732,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="78" customHeight="1" spans="1:18">
+    <row r="5" spans="1:19" ht="78" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>16073001</v>
@@ -4760,11 +4205,11 @@
       </c>
       <c r="J5" s="11">
         <f t="shared" si="0"/>
-        <v>18.2538488541197</v>
+        <v>18.253848854119699</v>
       </c>
       <c r="K5" s="12">
         <f t="shared" si="5"/>
-        <v>19.7571069950472</v>
+        <v>19.757106995047199</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="6"/>
@@ -4776,7 +4221,7 @@
       </c>
       <c r="N5" s="13">
         <f t="shared" si="8"/>
-        <v>16.7935409457901</v>
+        <v>16.793540945790099</v>
       </c>
       <c r="O5" s="13">
         <f t="shared" si="9"/>
@@ -4784,7 +4229,7 @@
       </c>
       <c r="P5" s="14">
         <f t="shared" si="10"/>
-        <v>24.2666666666667</v>
+        <v>24.266666666666701</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -4793,7 +4238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="78" customHeight="1" spans="1:19">
+    <row r="6" spans="1:19" ht="78" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>16073002</v>
@@ -4825,7 +4270,7 @@
       </c>
       <c r="K6" s="12">
         <f t="shared" si="5"/>
-        <v>16.6140850803989</v>
+        <v>16.614085080398901</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="6"/>
@@ -4845,7 +4290,7 @@
       </c>
       <c r="P6" s="14">
         <f t="shared" si="10"/>
-        <v>16.325</v>
+        <v>16.324999999999999</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -4857,7 +4302,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="69" customHeight="1" spans="1:18">
+    <row r="7" spans="1:19" ht="69" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>16080301</v>
@@ -4885,11 +4330,11 @@
       </c>
       <c r="J7" s="11">
         <f t="shared" si="0"/>
-        <v>17.2508901258713</v>
+        <v>17.250890125871301</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$81*H7+$M$81)*$L$81)/(1-G7)/(1-$P$81)/(1-I7)/$N$81</f>
-        <v>18.671551665649</v>
+        <v>18.671551665649002</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L49" si="12">E7+F7+($K$81*H7+$M$81)*$L$81</f>
@@ -4897,7 +4342,7 @@
       </c>
       <c r="M7" s="13">
         <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$81)/$N$81</f>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$81)/$N$81</f>
@@ -4905,11 +4350,11 @@
       </c>
       <c r="O7" s="13">
         <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$81</f>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P7" s="14">
         <f t="shared" ref="P7:P49" si="16">O7*$N$81-L7</f>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -4918,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="2:18">
+    <row r="8" spans="1:19" ht="78" customHeight="1">
       <c r="B8">
         <v>16080401</v>
       </c>
@@ -4945,11 +4390,11 @@
       </c>
       <c r="J8" s="11">
         <f t="shared" si="0"/>
-        <v>35.5858375959079</v>
+        <v>35.585837595907897</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="11"/>
-        <v>38.5164359861592</v>
+        <v>38.516435986159202</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="12"/>
@@ -4957,19 +4402,19 @@
       </c>
       <c r="M8" s="13">
         <f t="shared" si="13"/>
-        <v>17.792918797954</v>
+        <v>17.792918797954002</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="14"/>
-        <v>19.2582179930796</v>
+        <v>19.258217993079601</v>
       </c>
       <c r="O8" s="13">
         <f t="shared" si="15"/>
-        <v>16.3694852941176</v>
+        <v>16.369485294117599</v>
       </c>
       <c r="P8" s="14">
         <f t="shared" si="16"/>
-        <v>22.2625</v>
+        <v>22.262499999999999</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -4978,7 +4423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="92.25" customHeight="1" spans="2:18">
+    <row r="9" spans="1:19" ht="92.25" customHeight="1">
       <c r="B9">
         <v>16100801</v>
       </c>
@@ -5005,11 +4450,11 @@
       </c>
       <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>21.0597826086956</v>
+        <v>21.059782608695599</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="11"/>
-        <v>22.7941176470588</v>
+        <v>22.794117647058801</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="12"/>
@@ -5017,11 +4462,11 @@
       </c>
       <c r="M9" s="13">
         <f t="shared" si="13"/>
-        <v>16.8478260869565</v>
+        <v>16.847826086956498</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="14"/>
-        <v>18.2352941176471</v>
+        <v>18.235294117647101</v>
       </c>
       <c r="O9" s="13">
         <f t="shared" si="15"/>
@@ -5038,7 +4483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="89.25" customHeight="1" spans="2:18">
+    <row r="10" spans="1:19" ht="89.25" customHeight="1">
       <c r="B10">
         <v>16100901</v>
       </c>
@@ -5065,11 +4510,11 @@
       </c>
       <c r="J10" s="11">
         <f t="shared" si="0"/>
-        <v>37.3888685909146</v>
+        <v>37.388868590914598</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="11"/>
-        <v>40.467951886637</v>
+        <v>40.467951886637003</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="12"/>
@@ -5077,7 +4522,7 @@
       </c>
       <c r="M10" s="13">
         <f t="shared" si="13"/>
-        <v>26.1722080136402</v>
+        <v>26.172208013640201</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="14"/>
@@ -5085,11 +4530,11 @@
       </c>
       <c r="O10" s="13">
         <f t="shared" si="15"/>
-        <v>24.078431372549</v>
+        <v>24.078431372549002</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="16"/>
-        <v>40.9333333333333</v>
+        <v>40.933333333333302</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -5098,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="95.25" customHeight="1" spans="2:18">
+    <row r="11" spans="1:19" ht="95.25" customHeight="1">
       <c r="B11">
         <v>16101601</v>
       </c>
@@ -5125,15 +4570,15 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="0"/>
-        <v>32.7967504137205</v>
+        <v>32.796750413720503</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="11"/>
-        <v>35.497659271321</v>
+        <v>35.497659271320998</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="12"/>
-        <v>130.8</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="13">
         <f t="shared" si="13"/>
@@ -5141,11 +4586,11 @@
       </c>
       <c r="N11" s="13">
         <f t="shared" si="14"/>
-        <v>30.1730103806228</v>
+        <v>30.173010380622799</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="15"/>
-        <v>25.6470588235294</v>
+        <v>25.647058823529399</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="16"/>
@@ -5158,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="81.75" customHeight="1" spans="2:18">
+    <row r="12" spans="1:19" ht="81.75" customHeight="1">
       <c r="B12">
         <v>16101602</v>
       </c>
@@ -5185,7 +4630,7 @@
       </c>
       <c r="J12" s="11">
         <f t="shared" si="0"/>
-        <v>32.8587576594196</v>
+        <v>32.858757659419602</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="11"/>
@@ -5193,23 +4638,23 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="12"/>
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="13"/>
-        <v>27.9299440105067</v>
+        <v>27.929944010506699</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="14"/>
-        <v>30.230057046666</v>
+        <v>30.230057046666001</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="15"/>
-        <v>25.6955484896661</v>
+        <v>25.695548489666098</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="16"/>
-        <v>45.4297297297297</v>
+        <v>45.429729729729701</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -5218,7 +4663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="89.1" customHeight="1" spans="2:18">
+    <row r="13" spans="1:19" ht="89.1" customHeight="1">
       <c r="B13">
         <v>16101701</v>
       </c>
@@ -5265,11 +4710,11 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" si="15"/>
-        <v>11.8725490196078</v>
+        <v>11.872549019607799</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="16"/>
-        <v>20.1833333333333</v>
+        <v>20.183333333333302</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -5278,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" ht="84" customHeight="1" spans="2:18">
+    <row r="14" spans="1:19" ht="84" customHeight="1">
       <c r="B14">
         <v>16101703</v>
       </c>
@@ -5305,27 +4750,27 @@
       </c>
       <c r="J14" s="11">
         <f t="shared" si="0"/>
-        <v>59.5907928388747</v>
+        <v>59.590792838874698</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="11"/>
-        <v>64.4982698961938</v>
+        <v>64.498269896193804</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="12"/>
-        <v>139.8</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="13">
         <f t="shared" si="13"/>
-        <v>29.7953964194373</v>
+        <v>29.795396419437299</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="14"/>
-        <v>32.2491349480969</v>
+        <v>32.249134948096902</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="15"/>
-        <v>27.4117647058824</v>
+        <v>27.411764705882401</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="16"/>
@@ -5338,7 +4783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" ht="90.75" customHeight="1" spans="2:18">
+    <row r="15" spans="1:19" ht="90.75" customHeight="1">
       <c r="B15">
         <v>16101702</v>
       </c>
@@ -5365,11 +4810,11 @@
       </c>
       <c r="J15" s="11">
         <f t="shared" si="0"/>
-        <v>23.0179028132992</v>
+        <v>23.017902813299202</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="11"/>
-        <v>24.9134948096886</v>
+        <v>24.913494809688601</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="12"/>
@@ -5377,11 +4822,11 @@
       </c>
       <c r="M15" s="13">
         <f t="shared" si="13"/>
-        <v>19.5652173913043</v>
+        <v>19.565217391304301</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="14"/>
-        <v>21.1764705882353</v>
+        <v>21.176470588235301</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="15"/>
@@ -5398,7 +4843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" ht="90.75" customHeight="1" spans="2:18">
+    <row r="16" spans="1:19" ht="90.75" customHeight="1">
       <c r="B16">
         <v>16101901</v>
       </c>
@@ -5429,7 +4874,7 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" si="11"/>
-        <v>12.6297577854671</v>
+        <v>12.629757785467101</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="12"/>
@@ -5437,15 +4882,15 @@
       </c>
       <c r="M16" s="13">
         <f t="shared" si="13"/>
-        <v>8.75159846547314</v>
+        <v>8.7515984654731405</v>
       </c>
       <c r="N16" s="13">
         <f t="shared" si="14"/>
-        <v>9.47231833910035</v>
+        <v>9.4723183391003491</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="15"/>
-        <v>8.05147058823529</v>
+        <v>8.0514705882352899</v>
       </c>
       <c r="P16" s="14">
         <f t="shared" si="16"/>
@@ -5458,7 +4903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="90.75" customHeight="1" spans="2:18">
+    <row r="17" spans="2:18" ht="90.75" customHeight="1">
       <c r="B17">
         <v>16110801</v>
       </c>
@@ -5485,11 +4930,11 @@
       </c>
       <c r="J17" s="11">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K17" s="12">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="12"/>
@@ -5497,7 +4942,7 @@
       </c>
       <c r="M17" s="13">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N17" s="13">
         <f t="shared" si="14"/>
@@ -5505,11 +4950,11 @@
       </c>
       <c r="O17" s="13">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P17" s="14">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q17" s="15">
         <v>0.15</v>
@@ -5518,7 +4963,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="18" ht="90.75" customHeight="1" spans="2:18">
+    <row r="18" spans="2:18" ht="90.75" customHeight="1">
       <c r="B18">
         <v>16110802</v>
       </c>
@@ -5545,11 +4990,11 @@
       </c>
       <c r="J18" s="11">
         <f t="shared" si="0"/>
-        <v>16.4986710796851</v>
+        <v>16.498671079685099</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="11"/>
-        <v>17.8573851686003</v>
+        <v>17.857385168600299</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="12"/>
@@ -5557,7 +5002,7 @@
       </c>
       <c r="M18" s="13">
         <f t="shared" si="13"/>
-        <v>14.0238704177323</v>
+        <v>14.023870417732301</v>
       </c>
       <c r="N18" s="13">
         <f t="shared" si="14"/>
@@ -5565,11 +5010,11 @@
       </c>
       <c r="O18" s="13">
         <f t="shared" si="15"/>
-        <v>12.9019607843137</v>
+        <v>12.901960784313699</v>
       </c>
       <c r="P18" s="14">
         <f t="shared" si="16"/>
-        <v>21.9333333333333</v>
+        <v>21.933333333333302</v>
       </c>
       <c r="Q18" s="15">
         <v>0.15</v>
@@ -5578,7 +5023,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" ht="90.75" customHeight="1" spans="2:18">
+    <row r="19" spans="2:18" ht="90.75" customHeight="1">
       <c r="B19">
         <v>16110901</v>
       </c>
@@ -5605,27 +5050,27 @@
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>17.0716112531969</v>
+        <v>17.071611253196899</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="11"/>
-        <v>18.477508650519</v>
+        <v>18.477508650518999</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="12"/>
-        <v>40.05</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="13">
         <f t="shared" si="13"/>
-        <v>8.53580562659847</v>
+        <v>8.5358056265984708</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" si="14"/>
-        <v>9.23875432525952</v>
+        <v>9.2387543252595208</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="15"/>
-        <v>7.85294117647059</v>
+        <v>7.8529411764705896</v>
       </c>
       <c r="P19" s="14">
         <f t="shared" si="16"/>
@@ -5638,7 +5083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" ht="90.75" customHeight="1" spans="2:18">
+    <row r="20" spans="2:18" ht="90.75" customHeight="1">
       <c r="B20">
         <v>16111001</v>
       </c>
@@ -5665,11 +5110,11 @@
       </c>
       <c r="J20" s="11">
         <f t="shared" si="0"/>
-        <v>18.5117525270978</v>
+        <v>18.511752527097801</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="11"/>
-        <v>20.0362497940353</v>
+        <v>20.036249794035299</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="12"/>
@@ -5677,11 +5122,11 @@
       </c>
       <c r="M20" s="13">
         <f t="shared" si="13"/>
-        <v>12.9582267689685</v>
+        <v>12.958226768968499</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="14"/>
-        <v>14.0253748558247</v>
+        <v>14.025374855824699</v>
       </c>
       <c r="O20" s="13">
         <f t="shared" si="15"/>
@@ -5689,13 +5134,13 @@
       </c>
       <c r="P20" s="14">
         <f t="shared" si="16"/>
-        <v>20.2666666666667</v>
+        <v>20.266666666666701</v>
       </c>
       <c r="R20">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="90.75" customHeight="1" spans="2:18">
+    <row r="21" spans="2:18" ht="90.75" customHeight="1">
       <c r="B21">
         <v>16111901</v>
       </c>
@@ -5726,7 +5171,7 @@
       </c>
       <c r="K21" s="12">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="12"/>
@@ -5738,11 +5183,11 @@
       </c>
       <c r="N21" s="13">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P21" s="14">
         <f t="shared" si="16"/>
@@ -5752,7 +5197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" ht="90.95" customHeight="1" spans="2:18">
+    <row r="22" spans="2:18" ht="90.95" customHeight="1">
       <c r="B22">
         <v>16112001</v>
       </c>
@@ -5783,7 +5228,7 @@
       </c>
       <c r="K22" s="12">
         <f t="shared" si="11"/>
-        <v>28.1220509594212</v>
+        <v>28.122050959421198</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="12"/>
@@ -5795,11 +5240,11 @@
       </c>
       <c r="N22" s="13">
         <f t="shared" si="14"/>
-        <v>15.4671280276817</v>
+        <v>15.467128027681699</v>
       </c>
       <c r="O22" s="13">
         <f t="shared" si="15"/>
-        <v>13.1470588235294</v>
+        <v>13.147058823529401</v>
       </c>
       <c r="P22" s="14">
         <f t="shared" si="16"/>
@@ -5809,7 +5254,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" ht="90.95" customHeight="1" spans="2:18">
+    <row r="23" spans="2:18" ht="90.95" customHeight="1">
       <c r="B23">
         <v>16112002</v>
       </c>
@@ -5836,11 +5281,11 @@
       </c>
       <c r="J23" s="11">
         <f t="shared" si="0"/>
-        <v>27.5323568162443</v>
+        <v>27.532356816244299</v>
       </c>
       <c r="K23" s="12">
         <f t="shared" si="11"/>
-        <v>29.799727377582</v>
+        <v>29.799727377581998</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="12"/>
@@ -5848,25 +5293,25 @@
       </c>
       <c r="M23" s="13">
         <f t="shared" si="13"/>
-        <v>15.1427962489344</v>
+        <v>15.142796248934401</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="14"/>
-        <v>16.3898500576701</v>
+        <v>16.389850057670099</v>
       </c>
       <c r="O23" s="13">
         <f t="shared" si="15"/>
-        <v>13.9313725490196</v>
+        <v>13.931372549019599</v>
       </c>
       <c r="P23" s="14">
         <f t="shared" si="16"/>
-        <v>23.6833333333333</v>
+        <v>23.683333333333302</v>
       </c>
       <c r="R23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="90.75" customHeight="1" spans="2:18">
+    <row r="24" spans="2:18" ht="90.75" customHeight="1">
       <c r="B24">
         <v>16112003</v>
       </c>
@@ -5893,11 +5338,11 @@
       </c>
       <c r="J24" s="11">
         <f t="shared" si="0"/>
-        <v>26.3698364721383</v>
+        <v>26.369836472138299</v>
       </c>
       <c r="K24" s="12">
         <f t="shared" si="11"/>
-        <v>28.5414700639614</v>
+        <v>28.541470063961398</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="12"/>
@@ -5909,7 +5354,7 @@
       </c>
       <c r="N24" s="13">
         <f t="shared" si="14"/>
-        <v>15.6978085351788</v>
+        <v>15.697808535178799</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" si="15"/>
@@ -5917,13 +5362,13 @@
       </c>
       <c r="P24" s="14">
         <f t="shared" si="16"/>
-        <v>22.6833333333333</v>
+        <v>22.683333333333302</v>
       </c>
       <c r="R24">
         <v>45</v>
       </c>
     </row>
-    <row r="25" ht="90.75" customHeight="1" spans="2:18">
+    <row r="25" spans="2:18" ht="90.75" customHeight="1">
       <c r="B25">
         <v>16112301</v>
       </c>
@@ -5950,7 +5395,7 @@
       </c>
       <c r="J25" s="11">
         <f t="shared" si="0"/>
-        <v>25.4156010230179</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="12">
         <f t="shared" si="11"/>
@@ -5962,11 +5407,11 @@
       </c>
       <c r="M25" s="13">
         <f t="shared" si="13"/>
-        <v>15.2493606138107</v>
+        <v>15.249360613810699</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="14"/>
-        <v>16.5051903114187</v>
+        <v>16.505190311418701</v>
       </c>
       <c r="O25" s="13">
         <f t="shared" si="15"/>
@@ -5980,7 +5425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="90.75" customHeight="1" spans="2:18">
+    <row r="26" spans="2:18" ht="90.75" customHeight="1">
       <c r="B26">
         <v>16112302</v>
       </c>
@@ -6007,7 +5452,7 @@
       </c>
       <c r="J26" s="11">
         <f t="shared" si="0"/>
-        <v>22.7514919011083</v>
+        <v>22.751491901108299</v>
       </c>
       <c r="K26" s="12">
         <f t="shared" si="11"/>
@@ -6037,7 +5482,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" ht="90.75" customHeight="1" spans="2:18">
+    <row r="27" spans="2:18" ht="90.75" customHeight="1">
       <c r="B27">
         <v>16112401</v>
       </c>
@@ -6064,11 +5509,11 @@
       </c>
       <c r="J27" s="11">
         <f t="shared" si="0"/>
-        <v>19.3338204847156</v>
+        <v>19.333820484715599</v>
       </c>
       <c r="K27" s="12">
         <f t="shared" si="11"/>
-        <v>20.9260174658099</v>
+        <v>20.926017465809899</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="12"/>
@@ -6080,7 +5525,7 @@
       </c>
       <c r="N27" s="13">
         <f t="shared" si="14"/>
-        <v>14.6482122260669</v>
+        <v>14.648212226066899</v>
       </c>
       <c r="O27" s="13">
         <f t="shared" si="15"/>
@@ -6097,7 +5542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" ht="90.75" customHeight="1" spans="2:18">
+    <row r="28" spans="2:18" ht="90.75" customHeight="1">
       <c r="B28">
         <v>16112501</v>
       </c>
@@ -6124,11 +5569,11 @@
       </c>
       <c r="J28" s="11">
         <f t="shared" si="0"/>
-        <v>28.6948771603503</v>
+        <v>28.694877160350298</v>
       </c>
       <c r="K28" s="12">
         <f t="shared" si="11"/>
-        <v>31.0579846912027</v>
+        <v>31.057984691202702</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="12"/>
@@ -6136,7 +5581,7 @@
       </c>
       <c r="M28" s="13">
         <f t="shared" si="13"/>
-        <v>15.7821824381927</v>
+        <v>15.782182438192701</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="14"/>
@@ -6144,11 +5589,11 @@
       </c>
       <c r="O28" s="13">
         <f t="shared" si="15"/>
-        <v>14.5196078431373</v>
+        <v>14.519607843137299</v>
       </c>
       <c r="P28" s="14">
         <f t="shared" si="16"/>
-        <v>24.6833333333333</v>
+        <v>24.683333333333302</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -6157,7 +5602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="90.75" customHeight="1" spans="2:18">
+    <row r="29" spans="2:18" ht="90.75" customHeight="1">
       <c r="B29">
         <v>16112801</v>
       </c>
@@ -6196,7 +5641,7 @@
       </c>
       <c r="M29" s="13">
         <f t="shared" si="13"/>
-        <v>16.2084398976982</v>
+        <v>16.208439897698199</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="14"/>
@@ -6204,7 +5649,7 @@
       </c>
       <c r="O29" s="13">
         <f t="shared" si="15"/>
-        <v>14.9117647058824</v>
+        <v>14.911764705882399</v>
       </c>
       <c r="P29" s="14">
         <f t="shared" si="16"/>
@@ -6217,7 +5662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" ht="90.75" customHeight="1" spans="2:18">
+    <row r="30" spans="2:18" ht="90.75" customHeight="1">
       <c r="B30">
         <v>16112901</v>
       </c>
@@ -6244,11 +5689,11 @@
       </c>
       <c r="J30" s="11">
         <f t="shared" si="0"/>
-        <v>26.6604665581648</v>
+        <v>26.660466558164799</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="11"/>
-        <v>28.8560343923666</v>
+        <v>28.856034392366599</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="12"/>
@@ -6256,7 +5701,7 @@
       </c>
       <c r="M30" s="13">
         <f t="shared" si="13"/>
-        <v>14.6632566069906</v>
+        <v>14.663256606990601</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="14"/>
@@ -6264,11 +5709,11 @@
       </c>
       <c r="O30" s="13">
         <f t="shared" si="15"/>
-        <v>13.4901960784314</v>
+        <v>13.490196078431399</v>
       </c>
       <c r="P30" s="14">
         <f t="shared" si="16"/>
-        <v>22.9333333333333</v>
+        <v>22.933333333333302</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -6277,7 +5722,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" ht="90.75" customHeight="1" spans="2:18">
+    <row r="31" spans="2:18" ht="90.75" customHeight="1">
       <c r="B31">
         <v>16113001</v>
       </c>
@@ -6304,11 +5749,11 @@
       </c>
       <c r="J31" s="11">
         <f t="shared" si="0"/>
-        <v>12.8010443307758</v>
+        <v>12.801044330775801</v>
       </c>
       <c r="K31" s="12">
         <f t="shared" si="11"/>
-        <v>13.8552479815456</v>
+        <v>13.855247981545601</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="12"/>
@@ -6324,11 +5769,11 @@
       </c>
       <c r="O31" s="13">
         <f t="shared" si="15"/>
-        <v>9.42156862745098</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="14">
         <f t="shared" si="16"/>
-        <v>16.0166666666667</v>
+        <v>16.016666666666701</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -6337,7 +5782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" ht="90.75" customHeight="1" spans="2:18">
+    <row r="32" spans="2:18" ht="90.75" customHeight="1">
       <c r="B32">
         <v>16113002</v>
       </c>
@@ -6368,7 +5813,7 @@
       </c>
       <c r="K32" s="12">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="12"/>
@@ -6376,7 +5821,7 @@
       </c>
       <c r="M32" s="13">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="14"/>
@@ -6384,11 +5829,11 @@
       </c>
       <c r="O32" s="13">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="14">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -6397,7 +5842,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="90.75" customHeight="1" spans="2:18">
+    <row r="33" spans="2:18" ht="90.75" customHeight="1">
       <c r="B33">
         <v>16113003</v>
       </c>
@@ -6428,7 +5873,7 @@
       </c>
       <c r="K33" s="12">
         <f t="shared" si="11"/>
-        <v>28.2269057355563</v>
+        <v>28.226905735556301</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="12"/>
@@ -6440,7 +5885,7 @@
       </c>
       <c r="N33" s="13">
         <f t="shared" si="14"/>
-        <v>15.5247981545559</v>
+        <v>15.524798154555899</v>
       </c>
       <c r="O33" s="13">
         <f t="shared" si="15"/>
@@ -6448,7 +5893,7 @@
       </c>
       <c r="P33" s="14">
         <f t="shared" si="16"/>
-        <v>22.4333333333333</v>
+        <v>22.433333333333302</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -6457,7 +5902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" ht="90.75" customHeight="1" spans="2:18">
+    <row r="34" spans="2:18" ht="90.75" customHeight="1">
       <c r="B34">
         <v>16113004</v>
       </c>
@@ -6484,11 +5929,11 @@
       </c>
       <c r="J34" s="11">
         <f t="shared" si="0"/>
-        <v>19.9772662688264</v>
+        <v>19.977266268826401</v>
       </c>
       <c r="K34" s="12">
         <f t="shared" si="11"/>
-        <v>21.6224529027297</v>
+        <v>21.622452902729702</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="12"/>
@@ -6508,7 +5953,7 @@
       </c>
       <c r="P34" s="14">
         <f t="shared" si="16"/>
-        <v>23.4333333333333</v>
+        <v>23.433333333333302</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -6517,7 +5962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" ht="90.75" customHeight="1" spans="2:18">
+    <row r="35" spans="2:18" ht="90.75" customHeight="1">
       <c r="B35">
         <v>16120201</v>
       </c>
@@ -6544,11 +5989,11 @@
       </c>
       <c r="J35" s="11">
         <f t="shared" si="0"/>
-        <v>16.0645780051151</v>
+        <v>16.064578005115099</v>
       </c>
       <c r="K35" s="12">
         <f t="shared" si="11"/>
-        <v>17.3875432525952</v>
+        <v>17.387543252595201</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="12"/>
@@ -6556,25 +6001,25 @@
       </c>
       <c r="M35" s="13">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="R35">
         <v>20</v>
       </c>
     </row>
-    <row r="36" ht="90.75" customHeight="1" spans="2:17">
+    <row r="36" spans="2:18" ht="90.75" customHeight="1">
       <c r="B36">
         <v>16120301</v>
       </c>
@@ -6603,7 +6048,7 @@
       </c>
       <c r="K36" s="12">
         <f t="shared" si="11"/>
-        <v>26.5492293173954</v>
+        <v>26.549229317395401</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="12"/>
@@ -6611,7 +6056,7 @@
       </c>
       <c r="M36" s="13">
         <f t="shared" si="13"/>
-        <v>13.4910485933504</v>
+        <v>13.491048593350399</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="14"/>
@@ -6619,7 +6064,7 @@
       </c>
       <c r="O36" s="13">
         <f t="shared" si="15"/>
-        <v>12.4117647058824</v>
+        <v>12.411764705882399</v>
       </c>
       <c r="P36" s="14">
         <f t="shared" si="16"/>
@@ -6629,7 +6074,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" ht="90.75" customHeight="1" spans="2:17">
+    <row r="37" spans="2:18" ht="90.75" customHeight="1">
       <c r="B37">
         <v>16120302</v>
       </c>
@@ -6654,11 +6099,11 @@
       </c>
       <c r="J37" s="11">
         <f t="shared" si="0"/>
-        <v>7.33962063086104</v>
+        <v>7.3396206308610399</v>
       </c>
       <c r="K37" s="12">
         <f t="shared" si="11"/>
-        <v>7.94405997693195</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="12"/>
@@ -6666,15 +6111,15 @@
       </c>
       <c r="M37" s="13">
         <f t="shared" si="13"/>
-        <v>5.87169650468883</v>
+        <v>5.8716965046888303</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="14"/>
-        <v>6.35524798154556</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="13">
         <f t="shared" si="15"/>
-        <v>5.40196078431373</v>
+        <v>5.4019607843137303</v>
       </c>
       <c r="P37" s="14">
         <f t="shared" si="16"/>
@@ -6684,7 +6129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" ht="90.75" customHeight="1" spans="2:18">
+    <row r="38" spans="2:18" ht="90.75" customHeight="1">
       <c r="B38">
         <v>16120401</v>
       </c>
@@ -6709,19 +6154,19 @@
       </c>
       <c r="J38" s="11">
         <f t="shared" si="0"/>
-        <v>16.3256606990622</v>
+        <v>16.325660699062201</v>
       </c>
       <c r="K38" s="12">
         <f t="shared" si="11"/>
-        <v>17.6701268742791</v>
+        <v>17.670126874279099</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="12"/>
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="13">
         <f t="shared" si="13"/>
-        <v>8.16283034953112</v>
+        <v>8.1628303495311201</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="14"/>
@@ -6729,11 +6174,11 @@
       </c>
       <c r="O38" s="13">
         <f t="shared" si="15"/>
-        <v>7.50980392156863</v>
+        <v>7.5098039215686301</v>
       </c>
       <c r="P38" s="14">
         <f t="shared" si="16"/>
-        <v>12.7666666666667</v>
+        <v>12.766666666666699</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -6742,7 +6187,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" ht="84" customHeight="1" spans="2:18">
+    <row r="39" spans="2:18" ht="84" customHeight="1">
       <c r="B39">
         <v>16122001</v>
       </c>
@@ -6773,7 +6218,7 @@
       </c>
       <c r="K39" s="12">
         <f t="shared" si="11"/>
-        <v>19.5309496347559</v>
+        <v>19.530949634755899</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="12"/>
@@ -6781,7 +6226,7 @@
       </c>
       <c r="M39" s="13">
         <f t="shared" si="13"/>
-        <v>10.8269394714407</v>
+        <v>10.826939471440699</v>
       </c>
       <c r="N39" s="13">
         <f t="shared" si="14"/>
@@ -6789,11 +6234,11 @@
       </c>
       <c r="O39" s="13">
         <f t="shared" si="15"/>
-        <v>9.96078431372549</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="14">
         <f t="shared" si="16"/>
-        <v>16.9333333333333</v>
+        <v>16.933333333333302</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -6802,7 +6247,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" ht="90.75" customHeight="1" spans="2:18">
+    <row r="40" spans="2:18" ht="90.75" customHeight="1">
       <c r="B40">
         <v>17011301</v>
       </c>
@@ -6862,7 +6307,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" ht="90.75" customHeight="1" spans="2:18">
+    <row r="41" spans="2:18" ht="90.75" customHeight="1">
       <c r="B41">
         <v>17011302</v>
       </c>
@@ -6893,7 +6338,7 @@
       </c>
       <c r="K41" s="12">
         <f t="shared" si="11"/>
-        <v>12.4259900038447</v>
+        <v>12.425990003844699</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="12"/>
@@ -6901,19 +6346,19 @@
       </c>
       <c r="M41" s="13">
         <f t="shared" si="13"/>
-        <v>8.61040068201194</v>
+        <v>8.6104006820119405</v>
       </c>
       <c r="N41" s="13">
         <f t="shared" si="14"/>
-        <v>9.31949250288351</v>
+        <v>9.3194925028835094</v>
       </c>
       <c r="O41" s="13">
         <f t="shared" si="15"/>
-        <v>7.92156862745098</v>
+        <v>7.9215686274509798</v>
       </c>
       <c r="P41" s="14">
         <f t="shared" si="16"/>
-        <v>13.4666666666667</v>
+        <v>13.466666666666701</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -6922,7 +6367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" ht="90.75" customHeight="1" spans="2:18">
+    <row r="42" spans="2:18" ht="90.75" customHeight="1">
       <c r="B42">
         <v>17011303</v>
       </c>
@@ -6953,7 +6398,7 @@
       </c>
       <c r="K42" s="12">
         <f t="shared" si="11"/>
-        <v>26.8637936458006</v>
+        <v>26.863793645800602</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="12"/>
@@ -6982,7 +6427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" ht="90.75" customHeight="1" spans="2:18">
+    <row r="43" spans="2:18" ht="90.75" customHeight="1">
       <c r="B43">
         <v>17011401</v>
       </c>
@@ -7013,7 +6458,7 @@
       </c>
       <c r="K43" s="12">
         <f t="shared" si="11"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827801</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="12"/>
@@ -7021,15 +6466,15 @@
       </c>
       <c r="M43" s="13">
         <f t="shared" si="13"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241194</v>
       </c>
       <c r="N43" s="13">
         <f t="shared" si="14"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870801</v>
       </c>
       <c r="O43" s="13">
         <f t="shared" si="15"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254902004</v>
       </c>
       <c r="P43" s="14">
         <f t="shared" si="16"/>
@@ -7042,7 +6487,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" ht="90.75" customHeight="1" spans="2:18">
+    <row r="44" spans="2:18" ht="90.75" customHeight="1">
       <c r="B44">
         <v>17011501</v>
       </c>
@@ -7069,11 +6514,11 @@
       </c>
       <c r="J44" s="11">
         <f t="shared" si="0"/>
-        <v>17.1355498721228</v>
+        <v>17.135549872122802</v>
       </c>
       <c r="K44" s="12">
         <f t="shared" si="11"/>
-        <v>18.5467128027682</v>
+        <v>18.546712802768202</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="12"/>
@@ -7081,19 +6526,19 @@
       </c>
       <c r="M44" s="13">
         <f t="shared" si="13"/>
-        <v>12.8516624040921</v>
+        <v>12.851662404092099</v>
       </c>
       <c r="N44" s="13">
         <f t="shared" si="14"/>
-        <v>13.9100346020761</v>
+        <v>13.910034602076101</v>
       </c>
       <c r="O44" s="13">
         <f t="shared" si="15"/>
-        <v>11.8235294117647</v>
+        <v>11.823529411764699</v>
       </c>
       <c r="P44" s="14">
         <f t="shared" si="16"/>
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -7102,7 +6547,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="90.75" customHeight="1" spans="2:18">
+    <row r="45" spans="2:18" ht="90.75" customHeight="1">
       <c r="B45">
         <v>17011502</v>
       </c>
@@ -7129,11 +6574,11 @@
       </c>
       <c r="J45" s="11">
         <f t="shared" si="0"/>
-        <v>21.3322483143455</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="12">
         <f t="shared" si="11"/>
-        <v>23.0890217049387</v>
+        <v>23.089021704938698</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="12"/>
@@ -7141,7 +6586,7 @@
       </c>
       <c r="M45" s="13">
         <f t="shared" si="13"/>
-        <v>11.73273657289</v>
+        <v>11.732736572889999</v>
       </c>
       <c r="N45" s="13">
         <f t="shared" si="14"/>
@@ -7149,11 +6594,11 @@
       </c>
       <c r="O45" s="13">
         <f t="shared" si="15"/>
-        <v>10.7941176470588</v>
+        <v>10.794117647058799</v>
       </c>
       <c r="P45" s="14">
         <f t="shared" si="16"/>
-        <v>18.35</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -7162,7 +6607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" ht="90.75" customHeight="1" spans="2:18">
+    <row r="46" spans="2:18" ht="90.75" customHeight="1">
       <c r="B46">
         <v>17011601</v>
       </c>
@@ -7193,7 +6638,7 @@
       </c>
       <c r="K46" s="12">
         <f t="shared" si="11"/>
-        <v>22.2501834958582</v>
+        <v>22.250183495858199</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="12"/>
@@ -7205,15 +6650,15 @@
       </c>
       <c r="N46" s="13">
         <f t="shared" si="14"/>
-        <v>12.237600922722</v>
+        <v>12.237600922722001</v>
       </c>
       <c r="O46" s="13">
         <f t="shared" si="15"/>
-        <v>10.4019607843137</v>
+        <v>10.401960784313699</v>
       </c>
       <c r="P46" s="14">
         <f t="shared" si="16"/>
-        <v>17.6833333333333</v>
+        <v>17.683333333333302</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -7222,7 +6667,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="90.75" customHeight="1" spans="2:18">
+    <row r="47" spans="2:18" ht="90.75" customHeight="1">
       <c r="B47">
         <v>17011503</v>
       </c>
@@ -7253,7 +6698,7 @@
       </c>
       <c r="K47" s="12">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="12"/>
@@ -7265,15 +6710,15 @@
       </c>
       <c r="N47" s="13">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O47" s="13">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P47" s="14">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -7282,7 +6727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" ht="90.75" customHeight="1" spans="2:18">
+    <row r="48" spans="2:18" ht="90.75" customHeight="1">
       <c r="B48">
         <v>17011504</v>
       </c>
@@ -7313,7 +6758,7 @@
       </c>
       <c r="K48" s="12">
         <f t="shared" si="11"/>
-        <v>17.0271049596309</v>
+        <v>17.027104959630901</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="12"/>
@@ -7325,15 +6770,15 @@
       </c>
       <c r="N48" s="13">
         <f t="shared" si="14"/>
-        <v>12.7703287197232</v>
+        <v>12.770328719723199</v>
       </c>
       <c r="O48" s="13">
         <f t="shared" si="15"/>
-        <v>10.8547794117647</v>
+        <v>10.854779411764699</v>
       </c>
       <c r="P48" s="14">
         <f t="shared" si="16"/>
-        <v>14.7625</v>
+        <v>14.762499999999999</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -7342,7 +6787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" ht="90.75" customHeight="1" spans="2:18">
+    <row r="49" spans="2:18" ht="90.75" customHeight="1">
       <c r="B49">
         <v>17011602</v>
       </c>
@@ -7369,11 +6814,11 @@
       </c>
       <c r="J49" s="11">
         <f t="shared" si="0"/>
-        <v>16.4961636828644</v>
+        <v>16.496163682864399</v>
       </c>
       <c r="K49" s="12">
         <f t="shared" si="11"/>
-        <v>17.8546712802768</v>
+        <v>17.854671280276801</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="12"/>
@@ -7381,7 +6826,7 @@
       </c>
       <c r="M49" s="13">
         <f t="shared" si="13"/>
-        <v>12.3721227621483</v>
+        <v>12.372122762148299</v>
       </c>
       <c r="N49" s="13">
         <f t="shared" si="14"/>
@@ -7389,11 +6834,11 @@
       </c>
       <c r="O49" s="13">
         <f t="shared" si="15"/>
-        <v>11.3823529411765</v>
+        <v>11.382352941176499</v>
       </c>
       <c r="P49" s="14">
         <f t="shared" si="16"/>
-        <v>19.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -7402,7 +6847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" ht="90.75" customHeight="1" spans="2:18">
+    <row r="50" spans="2:18" ht="90.75" customHeight="1">
       <c r="B50">
         <v>17011901</v>
       </c>
@@ -7429,11 +6874,11 @@
       </c>
       <c r="J50" s="11">
         <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$81*H50+$M$81)*$L$81)/(1-G50)/(1-$O$81)/(1-I50)/$N$81</f>
-        <v>17.0696737192901</v>
+        <v>17.069673719290101</v>
       </c>
       <c r="K50" s="12">
         <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$81*H50+$M$81)*$L$81)/(1-G50)/(1-$P$81)/(1-I50)/$N$81</f>
-        <v>18.4754115549963</v>
+        <v>18.475411554996299</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" ref="L50:L58" si="19">E50+F50+($K$81*H50+$M$81)*$L$81</f>
@@ -7441,7 +6886,7 @@
       </c>
       <c r="M50" s="13">
         <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$81)/$N$81</f>
-        <v>9.38832054560955</v>
+        <v>9.3883205456095506</v>
       </c>
       <c r="N50" s="13">
         <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$81)/$N$81</f>
@@ -7449,7 +6894,7 @@
       </c>
       <c r="O50" s="13">
         <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$81</f>
-        <v>8.63725490196078</v>
+        <v>8.6372549019607803</v>
       </c>
       <c r="P50" s="14">
         <f t="shared" ref="P50:P58" si="23">O50*$N$81-L50</f>
@@ -7462,7 +6907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" ht="90.75" customHeight="1" spans="2:18">
+    <row r="51" spans="2:18" ht="90.75" customHeight="1">
       <c r="B51">
         <v>17011902</v>
       </c>
@@ -7493,7 +6938,7 @@
       </c>
       <c r="K51" s="12">
         <f t="shared" si="18"/>
-        <v>15.5132641291811</v>
+        <v>15.513264129181101</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="19"/>
@@ -7509,7 +6954,7 @@
       </c>
       <c r="O51" s="13">
         <f t="shared" si="22"/>
-        <v>9.88970588235294</v>
+        <v>9.8897058823529402</v>
       </c>
       <c r="P51" s="14">
         <f t="shared" si="23"/>
@@ -7522,7 +6967,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" ht="90.75" customHeight="1" spans="2:18">
+    <row r="52" spans="2:18" ht="90.75" customHeight="1">
       <c r="B52">
         <v>17020501</v>
       </c>
@@ -7561,19 +7006,19 @@
       </c>
       <c r="M52" s="13">
         <f t="shared" si="20"/>
-        <v>17.5931106138107</v>
+        <v>17.593110613810701</v>
       </c>
       <c r="N52" s="13">
         <f t="shared" si="21"/>
-        <v>19.041955017301</v>
+        <v>19.041955017300999</v>
       </c>
       <c r="O52" s="13">
         <f t="shared" si="22"/>
-        <v>16.1856617647059</v>
+        <v>16.185661764705898</v>
       </c>
       <c r="P52" s="14">
         <f t="shared" si="23"/>
-        <v>22.0125</v>
+        <v>22.012499999999999</v>
       </c>
       <c r="Q52">
         <v>30</v>
@@ -7582,7 +7027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" ht="90.75" customHeight="1" spans="2:18">
+    <row r="53" spans="2:18" ht="90.75" customHeight="1">
       <c r="B53">
         <v>17020502</v>
       </c>
@@ -7609,11 +7054,11 @@
       </c>
       <c r="J53" s="11">
         <f t="shared" si="17"/>
-        <v>24.2774455319885</v>
+        <v>24.277445531988501</v>
       </c>
       <c r="K53" s="12">
         <f t="shared" si="18"/>
-        <v>26.2767645757994</v>
+        <v>26.276764575799401</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" si="19"/>
@@ -7625,15 +7070,15 @@
       </c>
       <c r="N53" s="13">
         <f t="shared" si="21"/>
-        <v>18.3937352030596</v>
+        <v>18.393735203059599</v>
       </c>
       <c r="O53" s="13">
         <f t="shared" si="22"/>
-        <v>15.6346749226006</v>
+        <v>15.634674922600601</v>
       </c>
       <c r="P53" s="14">
         <f t="shared" si="23"/>
-        <v>25.5157894736842</v>
+        <v>25.515789473684201</v>
       </c>
       <c r="Q53">
         <v>30</v>
@@ -7642,7 +7087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" ht="90.75" customHeight="1" spans="2:18">
+    <row r="54" spans="2:18" ht="90.75" customHeight="1">
       <c r="B54">
         <v>17020601</v>
       </c>
@@ -7669,11 +7114,11 @@
       </c>
       <c r="J54" s="11">
         <f t="shared" si="17"/>
-        <v>18.9950980392157</v>
+        <v>18.995098039215701</v>
       </c>
       <c r="K54" s="12">
         <f t="shared" si="18"/>
-        <v>20.5594002306805</v>
+        <v>20.559400230680499</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" si="19"/>
@@ -7689,11 +7134,11 @@
       </c>
       <c r="O54" s="13">
         <f t="shared" si="22"/>
-        <v>13.1066176470588</v>
+        <v>13.106617647058799</v>
       </c>
       <c r="P54" s="14">
         <f t="shared" si="23"/>
-        <v>17.825</v>
+        <v>17.824999999999999</v>
       </c>
       <c r="Q54">
         <v>30</v>
@@ -7702,7 +7147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" ht="90.75" customHeight="1" spans="2:18">
+    <row r="55" spans="2:18" ht="90.75" customHeight="1">
       <c r="B55">
         <v>17020701</v>
       </c>
@@ -7729,11 +7174,11 @@
       </c>
       <c r="J55" s="11">
         <f t="shared" si="17"/>
-        <v>24.4907745706978</v>
+        <v>24.490774570697798</v>
       </c>
       <c r="K55" s="12">
         <f t="shared" si="18"/>
-        <v>26.5076618882847</v>
+        <v>26.507661888284701</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="19"/>
@@ -7745,11 +7190,11 @@
       </c>
       <c r="N55" s="13">
         <f t="shared" si="21"/>
-        <v>18.5553633217993</v>
+        <v>18.555363321799302</v>
       </c>
       <c r="O55" s="13">
         <f t="shared" si="22"/>
-        <v>15.7720588235294</v>
+        <v>15.772058823529401</v>
       </c>
       <c r="P55" s="14">
         <f t="shared" si="23"/>
@@ -7762,7 +7207,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" ht="90.75" customHeight="1" spans="2:18">
+    <row r="56" spans="2:18" ht="90.75" customHeight="1">
       <c r="B56">
         <v>17020801</v>
       </c>
@@ -7789,7 +7234,7 @@
       </c>
       <c r="J56" s="11">
         <f t="shared" si="17"/>
-        <v>12.9475703324808</v>
+        <v>12.947570332480799</v>
       </c>
       <c r="K56" s="12">
         <f t="shared" si="18"/>
@@ -7801,15 +7246,15 @@
       </c>
       <c r="M56" s="13">
         <f t="shared" si="20"/>
-        <v>9.71067774936061</v>
+        <v>9.7106777493606096</v>
       </c>
       <c r="N56" s="13">
         <f t="shared" si="21"/>
-        <v>10.5103806228374</v>
+        <v>10.510380622837401</v>
       </c>
       <c r="O56" s="13">
         <f t="shared" si="22"/>
-        <v>8.93382352941176</v>
+        <v>8.9338235294117592</v>
       </c>
       <c r="P56" s="14">
         <f t="shared" si="23"/>
@@ -7822,7 +7267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" ht="90.75" customHeight="1" spans="2:18">
+    <row r="57" spans="2:18" ht="90.75" customHeight="1">
       <c r="B57">
         <v>17020901</v>
       </c>
@@ -7849,7 +7294,7 @@
       </c>
       <c r="J57" s="11">
         <f t="shared" si="17"/>
-        <v>19.6538595675424</v>
+        <v>19.653859567542401</v>
       </c>
       <c r="K57" s="12">
         <f t="shared" si="18"/>
@@ -7861,7 +7306,7 @@
       </c>
       <c r="M57" s="13">
         <f t="shared" si="20"/>
-        <v>10.8096227621483</v>
+        <v>10.809622762148299</v>
       </c>
       <c r="N57" s="13">
         <f t="shared" si="21"/>
@@ -7869,7 +7314,7 @@
       </c>
       <c r="O57" s="13">
         <f t="shared" si="22"/>
-        <v>9.94485294117647</v>
+        <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="14">
         <f t="shared" si="23"/>
@@ -7882,7 +7327,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" ht="90.75" customHeight="1" spans="2:18">
+    <row r="58" spans="2:18" ht="90.75" customHeight="1">
       <c r="B58">
         <v>17020901</v>
       </c>
@@ -7909,11 +7354,11 @@
       </c>
       <c r="J58" s="11">
         <f t="shared" si="17"/>
-        <v>24.9094202898551</v>
+        <v>24.909420289855099</v>
       </c>
       <c r="K58" s="12">
         <f t="shared" si="18"/>
-        <v>26.9607843137255</v>
+        <v>26.960784313725501</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" si="19"/>
@@ -7925,7 +7370,7 @@
       </c>
       <c r="N58" s="13">
         <f t="shared" si="21"/>
-        <v>16.1764705882353</v>
+        <v>16.176470588235301</v>
       </c>
       <c r="O58" s="13">
         <f t="shared" si="22"/>
@@ -7942,7 +7387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" ht="90.75" customHeight="1" spans="2:18">
+    <row r="59" spans="2:18" ht="90.75" customHeight="1">
       <c r="B59">
         <v>17021104</v>
       </c>
@@ -7973,7 +7418,7 @@
       </c>
       <c r="K59" s="12">
         <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$81*H59+$M$81)*$L$81)/(1-G59)/(1-$P$81)/(1-I59)/$N$81</f>
-        <v>16.9303015323777</v>
+        <v>16.930301532377701</v>
       </c>
       <c r="L59" s="1">
         <f t="shared" ref="L59:L60" si="26">E59+F59+($K$81*H59+$M$81)*$L$81</f>
@@ -7989,7 +7434,7 @@
       </c>
       <c r="O59" s="13">
         <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$81</f>
-        <v>10.0735294117647</v>
+        <v>10.073529411764699</v>
       </c>
       <c r="P59" s="14">
         <f t="shared" ref="P59:P60" si="30">O59*$N$81-L59</f>
@@ -8002,7 +7447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" ht="90.75" customHeight="1" spans="2:18">
+    <row r="60" spans="2:18" ht="90.75" customHeight="1">
       <c r="B60">
         <v>17021105</v>
       </c>
@@ -8033,7 +7478,7 @@
       </c>
       <c r="K60" s="12">
         <f t="shared" si="25"/>
-        <v>16.9303015323777</v>
+        <v>16.930301532377701</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" si="26"/>
@@ -8049,7 +7494,7 @@
       </c>
       <c r="O60" s="13">
         <f t="shared" si="29"/>
-        <v>10.0735294117647</v>
+        <v>10.073529411764699</v>
       </c>
       <c r="P60" s="14">
         <f t="shared" si="30"/>
@@ -8062,7 +7507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" ht="90.75" customHeight="1" spans="2:18">
+    <row r="61" spans="2:18" ht="90.75" customHeight="1">
       <c r="B61">
         <v>17021101</v>
       </c>
@@ -8093,7 +7538,7 @@
       </c>
       <c r="K61" s="12">
         <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$81*H61+$M$81)*$L$81)/(1-G61)/(1-$P$81)/(1-I61)/$N$81</f>
-        <v>12.2404844290657</v>
+        <v>12.240484429065701</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" ref="L61:L66" si="33">E61+F61+($K$81*H61+$M$81)*$L$81</f>
@@ -8101,19 +7546,19 @@
       </c>
       <c r="M61" s="13">
         <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$81)/$N$81</f>
-        <v>8.4818574168798</v>
+        <v>8.4818574168797998</v>
       </c>
       <c r="N61" s="13">
         <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$81)/$N$81</f>
-        <v>9.18036332179931</v>
+        <v>9.1803633217993106</v>
       </c>
       <c r="O61" s="13">
         <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$81</f>
-        <v>7.80330882352941</v>
+        <v>7.8033088235294104</v>
       </c>
       <c r="P61" s="14">
         <f t="shared" ref="P61:P66" si="37">O61*$N$81-L61</f>
-        <v>10.6125</v>
+        <v>10.612500000000001</v>
       </c>
       <c r="Q61">
         <v>25</v>
@@ -8122,7 +7567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" ht="90.75" customHeight="1" spans="2:18">
+    <row r="62" spans="2:18" ht="90.75" customHeight="1">
       <c r="B62">
         <v>17021102</v>
       </c>
@@ -8153,7 +7598,7 @@
       </c>
       <c r="K62" s="12">
         <f t="shared" si="32"/>
-        <v>12.7028066128412</v>
+        <v>12.702806612841201</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" si="33"/>
@@ -8161,19 +7606,19 @@
       </c>
       <c r="M62" s="13">
         <f t="shared" si="34"/>
-        <v>8.80221653878943</v>
+        <v>8.8022165387894304</v>
       </c>
       <c r="N62" s="13">
         <f t="shared" si="35"/>
-        <v>9.52710495963091</v>
+        <v>9.5271049596309094</v>
       </c>
       <c r="O62" s="13">
         <f t="shared" si="36"/>
-        <v>8.09803921568627</v>
+        <v>8.0980392156862706</v>
       </c>
       <c r="P62" s="14">
         <f t="shared" si="37"/>
-        <v>13.7666666666667</v>
+        <v>13.766666666666699</v>
       </c>
       <c r="Q62">
         <v>25</v>
@@ -8182,7 +7627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" ht="90.75" customHeight="1" spans="2:18">
+    <row r="63" spans="2:18" ht="90.75" customHeight="1">
       <c r="B63">
         <v>17021103</v>
       </c>
@@ -8213,7 +7658,7 @@
       </c>
       <c r="K63" s="12">
         <f t="shared" si="32"/>
-        <v>15.8785082660515</v>
+        <v>15.878508266051499</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" si="33"/>
@@ -8221,19 +7666,19 @@
       </c>
       <c r="M63" s="13">
         <f t="shared" si="34"/>
-        <v>8.80221653878943</v>
+        <v>8.8022165387894304</v>
       </c>
       <c r="N63" s="13">
         <f t="shared" si="35"/>
-        <v>9.52710495963091</v>
+        <v>9.5271049596309094</v>
       </c>
       <c r="O63" s="13">
         <f t="shared" si="36"/>
-        <v>8.09803921568627</v>
+        <v>8.0980392156862706</v>
       </c>
       <c r="P63" s="14">
         <f t="shared" si="37"/>
-        <v>13.7666666666667</v>
+        <v>13.766666666666699</v>
       </c>
       <c r="Q63">
         <v>25</v>
@@ -8242,7 +7687,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" ht="90.75" customHeight="1" spans="2:18">
+    <row r="64" spans="2:18" ht="90.75" customHeight="1">
       <c r="B64">
         <v>17021106</v>
       </c>
@@ -8269,7 +7714,7 @@
       </c>
       <c r="J64" s="11">
         <f t="shared" si="31"/>
-        <v>15.3985507246377</v>
+        <v>15.398550724637699</v>
       </c>
       <c r="K64" s="12">
         <f t="shared" si="32"/>
@@ -8281,7 +7726,7 @@
       </c>
       <c r="M64" s="13">
         <f t="shared" si="34"/>
-        <v>11.5489130434783</v>
+        <v>11.548913043478301</v>
       </c>
       <c r="N64" s="13">
         <f t="shared" si="35"/>
@@ -8302,7 +7747,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" ht="90.75" customHeight="1" spans="2:20">
+    <row r="65" spans="2:20" ht="90.75" customHeight="1">
       <c r="B65">
         <v>17021201</v>
       </c>
@@ -8329,11 +7774,11 @@
       </c>
       <c r="J65" s="11">
         <f t="shared" si="31"/>
-        <v>17.2087048685514</v>
+        <v>17.208704868551401</v>
       </c>
       <c r="K65" s="12">
         <f t="shared" si="32"/>
-        <v>18.6258923283145</v>
+        <v>18.625892328314499</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" si="33"/>
@@ -8349,11 +7794,11 @@
       </c>
       <c r="O65" s="13">
         <f t="shared" si="36"/>
-        <v>9.49920508744038</v>
+        <v>9.4992050874403802</v>
       </c>
       <c r="P65" s="14">
         <f t="shared" si="37"/>
-        <v>16.7945945945946</v>
+        <v>16.794594594594599</v>
       </c>
       <c r="Q65">
         <v>40</v>
@@ -8368,7 +7813,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" ht="90.75" customHeight="1" spans="2:19">
+    <row r="66" spans="2:20" ht="90.75" customHeight="1">
       <c r="B66">
         <v>17021301</v>
       </c>
@@ -8395,11 +7840,11 @@
       </c>
       <c r="J66" s="11">
         <f t="shared" si="31"/>
-        <v>20.266258677384</v>
+        <v>20.266258677383998</v>
       </c>
       <c r="K66" s="12">
         <f t="shared" si="32"/>
-        <v>21.9352446861097</v>
+        <v>21.935244686109701</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" si="33"/>
@@ -8411,11 +7856,11 @@
       </c>
       <c r="N66" s="13">
         <f t="shared" si="35"/>
-        <v>15.3546712802768</v>
+        <v>15.354671280276801</v>
       </c>
       <c r="O66" s="13">
         <f t="shared" si="36"/>
-        <v>13.0514705882353</v>
+        <v>13.051470588235301</v>
       </c>
       <c r="P66" s="14">
         <f t="shared" si="37"/>
@@ -8429,7 +7874,7 @@
       </c>
       <c r="S66" s="18"/>
     </row>
-    <row r="67" ht="90.75" customHeight="1" spans="2:19">
+    <row r="67" spans="2:20" ht="90.75" customHeight="1">
       <c r="B67">
         <v>17021401</v>
       </c>
@@ -8468,15 +7913,15 @@
       </c>
       <c r="M67" s="13">
         <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$81)/$N$81</f>
-        <v>6.2766410912191</v>
+        <v>6.2766410912191004</v>
       </c>
       <c r="N67" s="13">
         <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$81)/$N$81</f>
-        <v>6.79354094579008</v>
+        <v>6.7935409457900802</v>
       </c>
       <c r="O67" s="13">
         <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$81</f>
-        <v>5.77450980392157</v>
+        <v>5.7745098039215703</v>
       </c>
       <c r="P67" s="14">
         <f t="shared" ref="P67:P68" si="44">O67*$N$81-L67</f>
@@ -8490,7 +7935,7 @@
       </c>
       <c r="S67" s="18"/>
     </row>
-    <row r="68" ht="90.75" customHeight="1" spans="2:19">
+    <row r="68" spans="2:20" ht="90.75" customHeight="1">
       <c r="B68">
         <v>17021402</v>
       </c>
@@ -8517,11 +7962,11 @@
       </c>
       <c r="J68" s="11">
         <f t="shared" si="38"/>
-        <v>13.7952414167248</v>
+        <v>13.795241416724799</v>
       </c>
       <c r="K68" s="12">
         <f t="shared" si="39"/>
-        <v>14.9313201216315</v>
+        <v>14.931320121631501</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" si="40"/>
@@ -8529,19 +7974,19 @@
       </c>
       <c r="M68" s="13">
         <f t="shared" si="41"/>
-        <v>7.58738277919864</v>
+        <v>7.5873827791986397</v>
       </c>
       <c r="N68" s="13">
         <f t="shared" si="42"/>
-        <v>8.21222606689735</v>
+        <v>8.2122260668973492</v>
       </c>
       <c r="O68" s="13">
         <f t="shared" si="43"/>
-        <v>6.98039215686275</v>
+        <v>6.9803921568627496</v>
       </c>
       <c r="P68" s="14">
         <f t="shared" si="44"/>
-        <v>11.8666666666667</v>
+        <v>11.866666666666699</v>
       </c>
       <c r="Q68">
         <v>45</v>
@@ -8551,7 +7996,7 @@
       </c>
       <c r="S68" s="18"/>
     </row>
-    <row r="69" ht="90.75" customHeight="1" spans="2:19">
+    <row r="69" spans="2:20" ht="90.75" customHeight="1">
       <c r="B69">
         <v>17021403</v>
       </c>
@@ -8578,31 +8023,31 @@
       </c>
       <c r="J69" s="11">
         <f t="shared" ref="J69:J75" si="45">(E69+F69+($K$81*H69+$M$81)*$L$81)/(1-G69)/(1-$O$81)/(1-I69)/$N$81</f>
-        <v>12.5390736004547</v>
+        <v>12.539073600454699</v>
       </c>
       <c r="K69" s="12">
         <f t="shared" ref="K69:K75" si="46">(E69+F69+($K$81*H69+$M$81)*$L$81)/(1-G69)/(1-$P$81)/(1-I69)/$N$81</f>
-        <v>13.5717031910804</v>
+        <v>13.571703191080401</v>
       </c>
       <c r="L69" s="1">
         <f t="shared" ref="L69:L75" si="47">E69+F69+($K$81*H69+$M$81)*$L$81</f>
-        <v>35.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
         <f t="shared" ref="M69:M75" si="48">L69/(1-G69)/(1-$O$81)/$N$81</f>
-        <v>7.5234441602728</v>
+        <v>7.5234441602727999</v>
       </c>
       <c r="N69" s="13">
         <f t="shared" ref="N69:N75" si="49">L69/(1-G69)/(1-$P$81)/$N$81</f>
-        <v>8.14302191464821</v>
+        <v>8.1430219146482106</v>
       </c>
       <c r="O69" s="13">
         <f t="shared" ref="O69:O75" si="50">L69/(1-G69)/$N$81</f>
-        <v>6.92156862745098</v>
+        <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
         <f t="shared" ref="P69:P75" si="51">O69*$N$81-L69</f>
-        <v>11.7666666666667</v>
+        <v>11.766666666666699</v>
       </c>
       <c r="Q69">
         <v>25</v>
@@ -8612,7 +8057,7 @@
       </c>
       <c r="S69" s="18"/>
     </row>
-    <row r="70" ht="90.75" customHeight="1" spans="2:19">
+    <row r="70" spans="2:20" ht="90.75" customHeight="1">
       <c r="B70">
         <v>17021501</v>
       </c>
@@ -8643,7 +8088,7 @@
       </c>
       <c r="K70" s="12">
         <f t="shared" si="46"/>
-        <v>13.7793156478278</v>
+        <v>13.779315647827801</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" si="47"/>
@@ -8651,15 +8096,15 @@
       </c>
       <c r="M70" s="13">
         <f t="shared" si="48"/>
-        <v>9.54816709292412</v>
+        <v>9.5481670929241194</v>
       </c>
       <c r="N70" s="13">
         <f t="shared" si="49"/>
-        <v>10.3344867358708</v>
+        <v>10.334486735870801</v>
       </c>
       <c r="O70" s="13">
         <f t="shared" si="50"/>
-        <v>8.7843137254902</v>
+        <v>8.7843137254902004</v>
       </c>
       <c r="P70" s="14">
         <f t="shared" si="51"/>
@@ -8673,7 +8118,7 @@
       </c>
       <c r="S70" s="18"/>
     </row>
-    <row r="71" ht="90.75" customHeight="1" spans="2:19">
+    <row r="71" spans="2:20" ht="90.75" customHeight="1">
       <c r="B71">
         <v>17021502</v>
       </c>
@@ -8700,7 +8145,7 @@
       </c>
       <c r="J71" s="11">
         <f t="shared" si="45"/>
-        <v>9.97442455242967</v>
+        <v>9.9744245524296709</v>
       </c>
       <c r="K71" s="12">
         <f t="shared" si="46"/>
@@ -8712,15 +8157,15 @@
       </c>
       <c r="M71" s="13">
         <f t="shared" si="48"/>
-        <v>7.48081841432225</v>
+        <v>7.4808184143222496</v>
       </c>
       <c r="N71" s="13">
         <f t="shared" si="49"/>
-        <v>8.09688581314879</v>
+        <v>8.0968858131487895</v>
       </c>
       <c r="O71" s="13">
         <f t="shared" si="50"/>
-        <v>6.88235294117647</v>
+        <v>6.8823529411764701</v>
       </c>
       <c r="P71" s="14">
         <f t="shared" si="51"/>
@@ -8734,7 +8179,7 @@
       </c>
       <c r="S71" s="18"/>
     </row>
-    <row r="72" ht="90.75" customHeight="1" spans="2:19">
+    <row r="72" spans="2:20" ht="90.75" customHeight="1">
       <c r="B72">
         <v>17021503</v>
       </c>
@@ -8773,7 +8218,7 @@
       </c>
       <c r="M72" s="13">
         <f t="shared" si="48"/>
-        <v>9.28175618073316</v>
+        <v>9.2817561807331597</v>
       </c>
       <c r="N72" s="13">
         <f t="shared" si="49"/>
@@ -8781,11 +8226,11 @@
       </c>
       <c r="O72" s="13">
         <f t="shared" si="50"/>
-        <v>8.53921568627451</v>
+        <v>8.5392156862745097</v>
       </c>
       <c r="P72" s="14">
         <f t="shared" si="51"/>
-        <v>14.5166666666667</v>
+        <v>14.516666666666699</v>
       </c>
       <c r="Q72">
         <v>40</v>
@@ -8795,7 +8240,7 @@
       </c>
       <c r="S72" s="18"/>
     </row>
-    <row r="73" ht="90.75" customHeight="1" spans="2:19">
+    <row r="73" spans="2:20" ht="90.75" customHeight="1">
       <c r="B73">
         <v>17021601</v>
       </c>
@@ -8815,7 +8260,7 @@
         <v>0.25</v>
       </c>
       <c r="H73">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I73" s="15">
         <v>0.4</v>
@@ -8826,7 +8271,7 @@
       </c>
       <c r="K73" s="12">
         <f t="shared" si="46"/>
-        <v>20.9919261822376</v>
+        <v>20.991926182237599</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" si="47"/>
@@ -8838,11 +8283,11 @@
       </c>
       <c r="N73" s="13">
         <f t="shared" si="49"/>
-        <v>12.5951557093426</v>
+        <v>12.595155709342601</v>
       </c>
       <c r="O73" s="13">
         <f t="shared" si="50"/>
-        <v>10.7058823529412</v>
+        <v>10.705882352941201</v>
       </c>
       <c r="P73" s="14">
         <f t="shared" si="51"/>
@@ -8858,7 +8303,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" ht="90.75" customHeight="1" spans="2:19">
+    <row r="74" spans="2:20" ht="90.75" customHeight="1">
       <c r="B74">
         <v>17021602</v>
       </c>
@@ -8878,18 +8323,18 @@
         <v>0.2</v>
       </c>
       <c r="H74">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I74" s="15">
         <v>0.4</v>
       </c>
       <c r="J74" s="11">
         <f t="shared" si="45"/>
-        <v>38.4797261295823</v>
+        <v>38.479726129582303</v>
       </c>
       <c r="K74" s="12">
         <f t="shared" si="46"/>
-        <v>41.6486447520185</v>
+        <v>41.648644752018498</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" si="47"/>
@@ -8901,15 +8346,15 @@
       </c>
       <c r="N74" s="13">
         <f t="shared" si="49"/>
-        <v>24.9891868512111</v>
+        <v>24.989186851211102</v>
       </c>
       <c r="O74" s="13">
         <f t="shared" si="50"/>
-        <v>21.2408088235294</v>
+        <v>21.240808823529399</v>
       </c>
       <c r="P74" s="14">
         <f t="shared" si="51"/>
-        <v>28.8875</v>
+        <v>28.887499999999999</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -8919,7 +8364,7 @@
       </c>
       <c r="S74" s="18"/>
     </row>
-    <row r="75" ht="90.75" customHeight="1" spans="2:19">
+    <row r="75" spans="2:20" ht="90.75" customHeight="1">
       <c r="B75">
         <v>17021701</v>
       </c>
@@ -8939,18 +8384,18 @@
         <v>0.2</v>
       </c>
       <c r="H75">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I75" s="15">
         <v>0.4</v>
       </c>
       <c r="J75" s="11">
         <f t="shared" si="45"/>
-        <v>17.1835038363171</v>
+        <v>17.183503836317101</v>
       </c>
       <c r="K75" s="12">
         <f t="shared" si="46"/>
-        <v>18.598615916955</v>
+        <v>18.598615916955001</v>
       </c>
       <c r="L75" s="1">
         <f t="shared" si="47"/>
@@ -8962,11 +8407,11 @@
       </c>
       <c r="N75" s="13">
         <f t="shared" si="49"/>
-        <v>11.159169550173</v>
+        <v>11.159169550173001</v>
       </c>
       <c r="O75" s="13">
         <f t="shared" si="50"/>
-        <v>9.48529411764706</v>
+        <v>9.4852941176470598</v>
       </c>
       <c r="P75" s="14">
         <f t="shared" si="51"/>
@@ -8980,7 +8425,7 @@
       </c>
       <c r="S75" s="18"/>
     </row>
-    <row r="76" ht="90.75" customHeight="1" spans="2:19">
+    <row r="76" spans="2:20" ht="90.75" customHeight="1">
       <c r="B76">
         <v>17021702</v>
       </c>
@@ -9007,7 +8452,7 @@
       </c>
       <c r="J76" s="11">
         <f>(E76+F76+($K$81*H76+$M$81)*$L$81)/(1-G76)/(1-$O$81)/(1-I76)/$N$81</f>
-        <v>13.1340579710145</v>
+        <v>13.134057971014499</v>
       </c>
       <c r="K76" s="12">
         <f>(E76+F76+($K$81*H76+$M$81)*$L$81)/(1-G76)/(1-$P$81)/(1-I76)/$N$81</f>
@@ -9019,11 +8464,11 @@
       </c>
       <c r="M76" s="13">
         <f>L76/(1-G76)/(1-$O$81)/$N$81</f>
-        <v>9.85054347826087</v>
+        <v>9.8505434782608692</v>
       </c>
       <c r="N76" s="13">
         <f>L76/(1-G76)/(1-$P$81)/$N$81</f>
-        <v>10.6617647058824</v>
+        <v>10.661764705882399</v>
       </c>
       <c r="O76" s="13">
         <f>L76/(1-G76)/$N$81</f>
@@ -9031,25 +8476,72 @@
       </c>
       <c r="P76" s="14">
         <f>O76*$N$81-L76</f>
-        <v>12.325</v>
+        <v>12.324999999999999</v>
       </c>
       <c r="S76" s="18"/>
     </row>
-    <row r="77" ht="90.75" customHeight="1" spans="3:19">
-      <c r="C77" s="1"/>
-      <c r="D77" s="9"/>
-      <c r="G77" s="3"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="12"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="14"/>
+    <row r="77" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B77">
+        <v>17021703</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77">
+        <v>190</v>
+      </c>
+      <c r="F77">
+        <v>6</v>
+      </c>
+      <c r="G77" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H77">
+        <v>1.5</v>
+      </c>
+      <c r="I77" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J77" s="11">
+        <f t="shared" ref="J77" si="52">(E77+F77+($K$81*H77+$M$81)*$L$81)/(1-G77)/(1-$O$81)/(1-I77)/$N$81</f>
+        <v>87.995524296675171</v>
+      </c>
+      <c r="K77" s="12">
+        <f t="shared" ref="K77" si="53">(E77+F77+($K$81*H77+$M$81)*$L$81)/(1-G77)/(1-$P$81)/(1-I77)/$N$81</f>
+        <v>95.242214532871969</v>
+      </c>
+      <c r="L77" s="1">
+        <f t="shared" ref="L77" si="54">E77+F77+($K$81*H77+$M$81)*$L$81</f>
+        <v>330.29999999999995</v>
+      </c>
+      <c r="M77" s="13">
+        <f t="shared" ref="M77" si="55">L77/(1-G77)/(1-$O$81)/$N$81</f>
+        <v>65.996643222506378</v>
+      </c>
+      <c r="N77" s="13">
+        <f t="shared" ref="N77" si="56">L77/(1-G77)/(1-$P$81)/$N$81</f>
+        <v>71.431660899653977</v>
+      </c>
+      <c r="O77" s="13">
+        <f t="shared" ref="O77" si="57">L77/(1-G77)/$N$81</f>
+        <v>60.716911764705877</v>
+      </c>
+      <c r="P77" s="14">
+        <f t="shared" ref="P77" si="58">O77*$N$81-L77</f>
+        <v>82.574999999999989</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>25</v>
+      </c>
       <c r="S77" s="18"/>
     </row>
-    <row r="78" ht="90.75" customHeight="1" spans="3:19">
+    <row r="78" spans="2:20" ht="90.75" customHeight="1">
       <c r="C78" s="1"/>
       <c r="D78" s="9"/>
       <c r="G78" s="3"/>
@@ -9063,9 +8555,8 @@
       <c r="P78" s="14"/>
       <c r="S78" s="18"/>
     </row>
-    <row r="79" spans="7:16">
+    <row r="79" spans="2:20">
       <c r="G79" s="15"/>
-      <c r="H79"/>
       <c r="I79" s="15"/>
       <c r="J79" s="11"/>
       <c r="L79" s="1"/>
@@ -9073,7 +8564,7 @@
       <c r="O79" s="13"/>
       <c r="P79" s="14"/>
     </row>
-    <row r="80" spans="11:16">
+    <row r="80" spans="2:20">
       <c r="K80" s="16" t="s">
         <v>100</v>
       </c>
@@ -9114,11 +8605,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C76 C77 C78 C2:C75">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C78">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -9126,110 +8618,105 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId2" display="https://detail.1688.com/offer/43388465240.html?spm=a2615.7691456.0.0.SVo0SF"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://detail.1688.com/offer/532946594199.html?spm=a2615.7691456.0.0.KfqxAP"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="S6" r:id="rId4" display="https://item.taobao.com/item.htm?spm=a230r.1.0.0.NVkYXr&amp;id=535812571550&amp;ns=1#detail"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://detail.1688.com/offer/521926765457.html?spm=a2615.7691456.0.0.Iw9wYb"/>
-    <hyperlink ref="D9" r:id="rId6" display="https://detail.1688.com/offer/539601777542.html?spm=b26110380.8015204.1688002.1.tV3mIo"/>
-    <hyperlink ref="D10" r:id="rId7" display="https://detail.1688.com/offer/534650922032.html"/>
-    <hyperlink ref="D11" r:id="rId8" display="https://detail.1688.com/offer/525196220868.html?spm=b26110380.8015204.xshy005.911.FMmHAe"/>
-    <hyperlink ref="D12" r:id="rId9" display="https://detail.1688.com/offer/525739109360.html?spm=b26110380.sw311.0.0.2w3SJa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://detail.1688.com/offer/536964765017.html?spm=b26110380.8015204.1688002.2.0qEfTf"/>
-    <hyperlink ref="D14" r:id="rId11" display="https://detail.1688.com/offer/523084291442.html?spm=b26110380.8015204.tkhy006.2.7zxqcs"/>
-    <hyperlink ref="D15" r:id="rId12" display="https://detail.1688.com/offer/539464650849.html?spm=b26110380.8015204.tkhy006.13.LriGRm"/>
-    <hyperlink ref="D16" r:id="rId13" display="https://detail.1688.com/offer/539024831638.html?spm=a2615.7691456.0.0.erl0H2"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://detail.1688.com/offer/37436493140.html?spm=a261y.7663282.0.0.Bdoqfg"/>
-    <hyperlink ref="D20" r:id="rId15" display="https://detail.1688.com/offer/525328573875.html?spm=a2615.2177701.0.0.inGNvk"/>
-    <hyperlink ref="D21" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D22" r:id="rId17" display="https://detail.1688.com/offer/539748592006.html?spm=a2615.7691456.0.0.gzA0aC"/>
-    <hyperlink ref="D23" r:id="rId18" display="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
-    <hyperlink ref="D24" r:id="rId16" display="https://detail.1688.com/offer/531099455627.html?spm=b26110380.sw311.0.0.NlP3tV"/>
-    <hyperlink ref="D25" r:id="rId19" display="https://detail.1688.com/offer/537712350771.html?spm=a261y.7663282.0.0.HGrgRG&amp;sk=consign"/>
-    <hyperlink ref="D26" r:id="rId20" display="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
-    <hyperlink ref="D18" r:id="rId21" display="https://detail.1688.com/offer/537572849225.html?spm=a2615.7691456.0.0.0jr1X8"/>
-    <hyperlink ref="D28" r:id="rId22" display="https://detail.1688.com/offer/538358020263.html?spm=a2615.7691456.0.0.BXbA7w"/>
-    <hyperlink ref="D29" r:id="rId23" display="https://detail.1688.com/offer/536605241945.html?spm=b26110380.8015204.xshy005.79.X6yxQK"/>
-    <hyperlink ref="D30" r:id="rId24" display="https://detail.1688.com/offer/522617209176.html?spm=0.0.0.0.OkHehB&amp;sk=consign"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://detail.1688.com/offer/536564720843.html?spm=a261y.7663282.0.0.CfpkXA&amp;sk=consign"/>
-    <hyperlink ref="D32" r:id="rId26" display="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
-    <hyperlink ref="D33" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://detail.1688.com/offer/537733197961.html?spm=b26110380.8015204.tkhy006.2.6IBVa5"/>
-    <hyperlink ref="D37" r:id="rId28" display="https://detail.1688.com/offer/39363390916.html?spm=b26110380.sw56474001.0.0.AOuyqk"/>
-    <hyperlink ref="D38" r:id="rId29" display="https://detail.1688.com/offer/523975460031.html?spm=b26110380.8015204.1688002.1.dPdaJX"/>
-    <hyperlink ref="D39" r:id="rId30" display="https://detail.1688.com/offer/531232169182.html?spm=a261y.7663282.0.0.1DCfuw"/>
-    <hyperlink ref="D40" r:id="rId31" display="https://detail.1688.com/offer/531965973421.html?spm=a2615.7691456.0.0.MQ5cDO"/>
-    <hyperlink ref="D41" r:id="rId32" display="https://detail.1688.com/offer/538656905495.html?spm=b26110380.sw1037004.0.0.dRfQA7&amp;sk=consign"/>
-    <hyperlink ref="D42" r:id="rId33" display="https://detail.1688.com/offer/534135284523.html?spm=a2615.2177701.0.0.bCxxaP"/>
-    <hyperlink ref="D43" r:id="rId34" display="https://detail.1688.com/offer/524129595472.html?spm=a2615.7691456.0.0.5vRcmp"/>
-    <hyperlink ref="D44" r:id="rId35" display="https://detail.1688.com/offer/538321839564.html?spm=b26110380.sw1037005.0.0.jmc4NW"/>
-    <hyperlink ref="D45" r:id="rId36" display="https://detail.1688.com/offer/525494755952.html?spm=a2615.7691456.0.0.2qsBMx"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://detail.1688.com/offer/525529106954.html?spm=a2615.7691456.0.0.4Tm2o6"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://detail.1688.com/offer/527560763616.html?spm=b26110380.sw311.0.0.p4j2tp"/>
-    <hyperlink ref="D50" r:id="rId39" display="https://detail.1688.com/offer/542627436877.html?spm=b26110380.sw1037004.0.0.aYzCim&amp;sk=consign"/>
-    <hyperlink ref="D52" r:id="rId40" display="https://detail.1688.com/offer/543024612109.html?spm=0.0.0.0.QG7IU6"/>
-    <hyperlink ref="D51" r:id="rId41" display="https://detail.1688.com/offer/543614766781.html?spm=b26110380.8015204.tkhy006.2.m9SOm8"/>
-    <hyperlink ref="D53" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D54" r:id="rId43" display="https://detail.1688.com/offer/45277079052.html?spm=a261y.7663282.0.0.8G3JEy&amp;sk=consign"/>
-    <hyperlink ref="D55" r:id="rId42" display="https://detail.1688.com/offer/45242512122.html?spm=a2615.7691456.0.0.SHHrUO"/>
-    <hyperlink ref="D56" r:id="rId44" display="https://detail.1688.com/offer/38711199781.html?spm=b26110380.8015204.tkhy006.2.g0hkme"/>
-    <hyperlink ref="D57" r:id="rId45" display="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
-    <hyperlink ref="D58" r:id="rId46" display="https://detail.1688.com/offer/536596301611.html?spm=a2615.7691456.0.0.HFQWm0"/>
-    <hyperlink ref="D60" r:id="rId47" display="https://detail.1688.com/offer/543879481659.html?spm=a2615.7691456.0.0.UWc1Wy"/>
-    <hyperlink ref="D63" r:id="rId48" display="https://detail.1688.com/offer/542163784708.html?spm=0.0.0.0.D3IAEt"/>
-    <hyperlink ref="D59" r:id="rId49" display="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
-    <hyperlink ref="D64" r:id="rId50" display="https://detail.1688.com/offer/520727227145.html?spm=b26110380.7927930.tkhy006.2.4cRHSy"/>
-    <hyperlink ref="D65" r:id="rId51" display="https://detail.1688.com/offer/45288474070.html?spm=0.0.0.0.ROTFEe"/>
-    <hyperlink ref="S65" r:id="rId52" display="https://detail.1688.com/offer/542800642320.html?spm=b26110380.7927930.xshy005.529.St2Fw9"/>
-    <hyperlink ref="D66" r:id="rId53" display="https://detail.1688.com/offer/537836876907.html?spm=0.0.0.0.aEJnan"/>
-    <hyperlink ref="D68" r:id="rId54" display="https://detail.1688.com/offer/529253294546.html?spm=a2615.7691456.0.0.Q2HHFu"/>
-    <hyperlink ref="D69" r:id="rId55" display="https://detail.1688.com/offer/544238732440.html?spm=0.0.0.0.XUpSK3"/>
-    <hyperlink ref="D70" r:id="rId56" display="https://detail.1688.com/offer/536547771377.html?spm=a2615.7691456.0.0.0h3eHa"/>
-    <hyperlink ref="D71" r:id="rId57" display="https://detail.1688.com/offer/530505809495.html?spm=a2615.7691456.0.0.mwCaVr"/>
-    <hyperlink ref="T65" r:id="rId58" display="https://detail.1688.com/offer/45422676746.html?spm=b26110380.8015204.xshy005.17.K9Fn6R"/>
-    <hyperlink ref="D73" r:id="rId59" display="https://detail.1688.com/offer/540415830695.html?spm=a2615.7691456.0.0.fxjODa"/>
-    <hyperlink ref="S73" r:id="rId51" display="https://detail.1688.com/offer/45288474070.html?spm=0.0.0.0.ROTFEe"/>
-    <hyperlink ref="D74" r:id="rId59" display="https://detail.1688.com/offer/540415830695.html?spm=a2615.7691456.0.0.fxjODa"/>
-    <hyperlink ref="D75" r:id="rId60" display="https://detail.1688.com/offer/542457925937.html?spm=a2615.7691456.0.0.f0Y32d"/>
-    <hyperlink ref="D76" r:id="rId61" display="https://detail.1688.com/offer/543920170819.html?spm=a261y.7663282.0.0.TL5U4u&amp;sk=consign"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="S6" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D21" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18" tooltip="https://detail.1688.com/offer/542005628301.html?spm=a2615.7691456.0.0.E27Va6"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21" tooltip="https://detail.1688.com/offer/535604104982.html?spm=a2615.7691456.0.0.ceDRcB"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D30" r:id="rId25"/>
+    <hyperlink ref="D31" r:id="rId26"/>
+    <hyperlink ref="D32" r:id="rId27" tooltip="https://detail.1688.com/offer/522866160965.html?spm=b26110380.8015204.1688002.2.oTUzYR"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D39" r:id="rId32"/>
+    <hyperlink ref="D40" r:id="rId33"/>
+    <hyperlink ref="D41" r:id="rId34"/>
+    <hyperlink ref="D42" r:id="rId35"/>
+    <hyperlink ref="D43" r:id="rId36"/>
+    <hyperlink ref="D44" r:id="rId37"/>
+    <hyperlink ref="D45" r:id="rId38"/>
+    <hyperlink ref="D46" r:id="rId39"/>
+    <hyperlink ref="D49" r:id="rId40"/>
+    <hyperlink ref="D50" r:id="rId41"/>
+    <hyperlink ref="D52" r:id="rId42"/>
+    <hyperlink ref="D51" r:id="rId43"/>
+    <hyperlink ref="D53" r:id="rId44"/>
+    <hyperlink ref="D54" r:id="rId45"/>
+    <hyperlink ref="D55" r:id="rId46"/>
+    <hyperlink ref="D56" r:id="rId47"/>
+    <hyperlink ref="D57" r:id="rId48" tooltip="https://detail.1688.com/offer/1148584816.html?spm=0.0.0.0.oGhpUj"/>
+    <hyperlink ref="D58" r:id="rId49"/>
+    <hyperlink ref="D60" r:id="rId50"/>
+    <hyperlink ref="D63" r:id="rId51"/>
+    <hyperlink ref="D59" r:id="rId52" tooltip="https://detail.1688.com/offer/543452736487.html?spm=a2615.7691456.0.0.UWc1Wy"/>
+    <hyperlink ref="D64" r:id="rId53"/>
+    <hyperlink ref="D65" r:id="rId54"/>
+    <hyperlink ref="S65" r:id="rId55"/>
+    <hyperlink ref="D66" r:id="rId56"/>
+    <hyperlink ref="D68" r:id="rId57"/>
+    <hyperlink ref="D69" r:id="rId58"/>
+    <hyperlink ref="D70" r:id="rId59"/>
+    <hyperlink ref="D71" r:id="rId60"/>
+    <hyperlink ref="T65" r:id="rId61"/>
+    <hyperlink ref="D73" r:id="rId62"/>
+    <hyperlink ref="S73" r:id="rId63"/>
+    <hyperlink ref="D74" r:id="rId64"/>
+    <hyperlink ref="D75" r:id="rId65"/>
+    <hyperlink ref="D76" r:id="rId66"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId67"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17022501 长袖 by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="116">
   <si>
     <t>产品标题</t>
   </si>
@@ -363,6 +363,16 @@
   <si>
     <t>https://detail.1688.com/offer/40127471168.html?spm=b26110380.sw1688.0.0.WdursY</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/540563368484.html?spm=a2615.7691456.0.0.HOgtg8</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/532221881280.html?spm=a261y.7663282.0.0.O7Bcm0&amp;sk=consign</t>
+  </si>
+  <si>
+    <t>T-shirt</t>
   </si>
 </sst>
 </file>
@@ -3840,6 +3850,82 @@
         <a:xfrm>
           <a:off x="91108" y="90951327"/>
           <a:ext cx="927652" cy="925198"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57979</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>977349</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>1018762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="图片 82" descr="QQ截图20170223231359.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId82" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57979" y="92152305"/>
+          <a:ext cx="919370" cy="919370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1010478</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>1010479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="图片 83" descr="QQ截图20170224211515.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId83" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="82826" y="93287023"/>
+          <a:ext cx="927652" cy="927652"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4136,11 +4222,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T86"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I83" sqref="I83"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4246,31 +4332,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$86*H2+$M$86)*$L$86)/(1-G2)/(1-$O$86)/(1-I2)/$N$86</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$88*H2+$M$88)*$L$88)/(1-G2)/(1-$O$88)/(1-I2)/$N$88</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$86*H2+$M$86)*$L$86)/(1-G2)/(1-$P$86)/(1-I2)/$N$86</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$88*H2+$M$88)*$L$88)/(1-G2)/(1-$P$88)/(1-I2)/$N$88</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$86*H2+$M$86)*$L$86</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$88*H2+$M$88)*$L$88</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$88)/$N$88</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$88)/$N$88</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$86</f>
+        <f>L2/(1-G2)/$N$88</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$86-L2</f>
+        <f>O2*$N$88-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -4311,27 +4397,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$86*H3+$M$86)*$L$86)/(1-G3)/(1-$P$86)/(1-I3)/$N$86</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$88*H3+$M$88)*$L$88)/(1-G3)/(1-$P$88)/(1-I3)/$N$88</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$86*H3+$M$86)*$L$86</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$88*H3+$M$88)*$L$88</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$88)/$N$88</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$88)/$N$88</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$86</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$88</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$86-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$88-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -4558,27 +4644,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$86*H7+$M$86)*$L$86)/(1-G7)/(1-$P$86)/(1-I7)/$N$86</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$88*H7+$M$88)*$L$88)/(1-G7)/(1-$P$88)/(1-I7)/$N$88</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$86*H7+$M$86)*$L$86</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$88*H7+$M$88)*$L$88</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$88)/$N$88</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$88)/$N$88</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$86</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$88</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$86-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$88-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -7098,31 +7184,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$86*H50+$M$86)*$L$86)/(1-G50)/(1-$O$86)/(1-I50)/$N$86</f>
+        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$88*H50+$M$88)*$L$88)/(1-G50)/(1-$O$88)/(1-I50)/$N$88</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$86*H50+$M$86)*$L$86)/(1-G50)/(1-$P$86)/(1-I50)/$N$86</f>
+        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$88*H50+$M$88)*$L$88)/(1-G50)/(1-$P$88)/(1-I50)/$N$88</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$86*H50+$M$86)*$L$86</f>
+        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$88*H50+$M$88)*$L$88</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$88)/$N$88</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$88)/$N$88</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$86</f>
+        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$88</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="23">O50*$N$86-L50</f>
+        <f t="shared" ref="P50:P58" si="23">O50*$N$88-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -7641,31 +7727,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$86*H59+$M$86)*$L$86)/(1-G59)/(1-$O$86)/(1-I59)/$N$86</f>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$88*H59+$M$88)*$L$88)/(1-G59)/(1-$O$88)/(1-I59)/$N$88</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$86*H59+$M$86)*$L$86)/(1-G59)/(1-$P$86)/(1-I59)/$N$86</f>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$88*H59+$M$88)*$L$88)/(1-G59)/(1-$P$88)/(1-I59)/$N$88</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$86*H59+$M$86)*$L$86</f>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$88*H59+$M$88)*$L$88</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$88)/$N$88</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$88)/$N$88</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$86</f>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$88</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" ref="P59:P60" si="30">O59*$N$86-L59</f>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$88-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -7761,31 +7847,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$86*H61+$M$86)*$L$86)/(1-G61)/(1-$O$86)/(1-I61)/$N$86</f>
+        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$88*H61+$M$88)*$L$88)/(1-G61)/(1-$O$88)/(1-I61)/$N$88</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$86*H61+$M$86)*$L$86)/(1-G61)/(1-$P$86)/(1-I61)/$N$86</f>
+        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$88*H61+$M$88)*$L$88)/(1-G61)/(1-$P$88)/(1-I61)/$N$88</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$86*H61+$M$86)*$L$86</f>
+        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$88*H61+$M$88)*$L$88</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$88)/$N$88</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$88)/$N$88</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$86</f>
+        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$88</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="37">O61*$N$86-L61</f>
+        <f t="shared" ref="P61:P66" si="37">O61*$N$88-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -8128,31 +8214,31 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$86*H67+$M$86)*$L$86)/(1-G67)/(1-$O$86)/(1-I67)/$N$86</f>
+        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$88*H67+$M$88)*$L$88)/(1-G67)/(1-$O$88)/(1-I67)/$N$88</f>
         <v>10.461068485365161</v>
       </c>
       <c r="K67" s="12">
-        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$86*H67+$M$86)*$L$86)/(1-G67)/(1-$P$86)/(1-I67)/$N$86</f>
+        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$88*H67+$M$88)*$L$88)/(1-G67)/(1-$P$88)/(1-I67)/$N$88</f>
         <v>11.322568242983468</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$86*H67+$M$86)*$L$86</f>
+        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$88*H67+$M$88)*$L$88</f>
         <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$88)/$N$88</f>
         <v>6.276641091219096</v>
       </c>
       <c r="N67" s="13">
-        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$88)/$N$88</f>
         <v>6.7935409457900811</v>
       </c>
       <c r="O67" s="13">
-        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$86</f>
+        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$88</f>
         <v>5.7745098039215685</v>
       </c>
       <c r="P67" s="14">
-        <f t="shared" ref="P67:P68" si="44">O67*$N$86-L67</f>
+        <f t="shared" ref="P67:P68" si="44">O67*$N$88-L67</f>
         <v>9.8166666666666664</v>
       </c>
       <c r="Q67">
@@ -8250,31 +8336,31 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69:J76" si="45">(E69+F69+($K$86*H69+$M$86)*$L$86)/(1-G69)/(1-$O$86)/(1-I69)/$N$86</f>
+        <f t="shared" ref="J69:J76" si="45">(E69+F69+($K$88*H69+$M$88)*$L$88)/(1-G69)/(1-$O$88)/(1-I69)/$N$88</f>
         <v>12.539073600454673</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69:K76" si="46">(E69+F69+($K$86*H69+$M$86)*$L$86)/(1-G69)/(1-$P$86)/(1-I69)/$N$86</f>
+        <f t="shared" ref="K69:K76" si="46">(E69+F69+($K$88*H69+$M$88)*$L$88)/(1-G69)/(1-$P$88)/(1-I69)/$N$88</f>
         <v>13.571703191080355</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69:L76" si="47">E69+F69+($K$86*H69+$M$86)*$L$86</f>
+        <f t="shared" ref="L69:L76" si="47">E69+F69+($K$88*H69+$M$88)*$L$88</f>
         <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69:M76" si="48">L69/(1-G69)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M69:M76" si="48">L69/(1-G69)/(1-$O$88)/$N$88</f>
         <v>7.5234441602728035</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69:N76" si="49">L69/(1-G69)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N69:N76" si="49">L69/(1-G69)/(1-$P$88)/$N$88</f>
         <v>8.1430219146482123</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69:O76" si="50">L69/(1-G69)/$N$86</f>
+        <f t="shared" ref="O69:O76" si="50">L69/(1-G69)/$N$88</f>
         <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P76" si="51">O69*$N$86-L69</f>
+        <f t="shared" ref="P69:P76" si="51">O69*$N$88-L69</f>
         <v>11.766666666666666</v>
       </c>
       <c r="Q69">
@@ -8740,31 +8826,31 @@
         <v>0.25</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" ref="J77:J79" si="52">(E77+F77+($K$86*H77+$M$86)*$L$86)/(1-G77)/(1-$O$86)/(1-I77)/$N$86</f>
+        <f t="shared" ref="J77:J79" si="52">(E77+F77+($K$88*H77+$M$88)*$L$88)/(1-G77)/(1-$O$88)/(1-I77)/$N$88</f>
         <v>87.995524296675171</v>
       </c>
       <c r="K77" s="12">
-        <f t="shared" ref="K77:K79" si="53">(E77+F77+($K$86*H77+$M$86)*$L$86)/(1-G77)/(1-$P$86)/(1-I77)/$N$86</f>
+        <f t="shared" ref="K77:K79" si="53">(E77+F77+($K$88*H77+$M$88)*$L$88)/(1-G77)/(1-$P$88)/(1-I77)/$N$88</f>
         <v>95.242214532871969</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" ref="L77:L79" si="54">E77+F77+($K$86*H77+$M$86)*$L$86</f>
+        <f t="shared" ref="L77:L79" si="54">E77+F77+($K$88*H77+$M$88)*$L$88</f>
         <v>330.29999999999995</v>
       </c>
       <c r="M77" s="13">
-        <f t="shared" ref="M77:M79" si="55">L77/(1-G77)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M77:M79" si="55">L77/(1-G77)/(1-$O$88)/$N$88</f>
         <v>65.996643222506378</v>
       </c>
       <c r="N77" s="13">
-        <f t="shared" ref="N77:N79" si="56">L77/(1-G77)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N77:N79" si="56">L77/(1-G77)/(1-$P$88)/$N$88</f>
         <v>71.431660899653977</v>
       </c>
       <c r="O77" s="13">
-        <f t="shared" ref="O77:O79" si="57">L77/(1-G77)/$N$86</f>
+        <f t="shared" ref="O77:O79" si="57">L77/(1-G77)/$N$88</f>
         <v>60.716911764705877</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" ref="P77:P79" si="58">O77*$N$86-L77</f>
+        <f t="shared" ref="P77:P79" si="58">O77*$N$88-L77</f>
         <v>82.574999999999989</v>
       </c>
       <c r="Q77">
@@ -8923,31 +9009,31 @@
         <v>0.45</v>
       </c>
       <c r="J80" s="11">
-        <f t="shared" ref="J80" si="59">(E80+F80+($K$86*H80+$M$86)*$L$86)/(1-G80)/(1-$O$86)/(1-I80)/$N$86</f>
+        <f t="shared" ref="J80" si="59">(E80+F80+($K$88*H80+$M$88)*$L$88)/(1-G80)/(1-$O$88)/(1-I80)/$N$88</f>
         <v>13.291482600945512</v>
       </c>
       <c r="K80" s="12">
-        <f t="shared" ref="K80" si="60">(E80+F80+($K$86*H80+$M$86)*$L$86)/(1-G80)/(1-$P$86)/(1-I80)/$N$86</f>
+        <f t="shared" ref="K80" si="60">(E80+F80+($K$88*H80+$M$88)*$L$88)/(1-G80)/(1-$P$88)/(1-I80)/$N$88</f>
         <v>14.386075285729262</v>
       </c>
       <c r="L80" s="1">
-        <f t="shared" ref="L80" si="61">E80+F80+($K$86*H80+$M$86)*$L$86</f>
+        <f t="shared" ref="L80" si="61">E80+F80+($K$88*H80+$M$88)*$L$88</f>
         <v>34.299999999999997</v>
       </c>
       <c r="M80" s="13">
-        <f t="shared" ref="M80" si="62">L80/(1-G80)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M80" si="62">L80/(1-G80)/(1-$O$88)/$N$88</f>
         <v>7.3103154305200322</v>
       </c>
       <c r="N80" s="13">
-        <f t="shared" ref="N80" si="63">L80/(1-G80)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N80" si="63">L80/(1-G80)/(1-$P$88)/$N$88</f>
         <v>7.9123414071510947</v>
       </c>
       <c r="O80" s="13">
-        <f t="shared" ref="O80" si="64">L80/(1-G80)/$N$86</f>
+        <f t="shared" ref="O80" si="64">L80/(1-G80)/$N$88</f>
         <v>6.7254901960784306</v>
       </c>
       <c r="P80" s="14">
-        <f t="shared" ref="P80" si="65">O80*$N$86-L80</f>
+        <f t="shared" ref="P80" si="65">O80*$N$88-L80</f>
         <v>11.43333333333333</v>
       </c>
       <c r="Q80">
@@ -8984,31 +9070,31 @@
         <v>0.25</v>
       </c>
       <c r="J81" s="11">
-        <f t="shared" ref="J81" si="66">(E81+F81+($K$86*H81+$M$86)*$L$86)/(1-G81)/(1-$O$86)/(1-I81)/$N$86</f>
+        <f t="shared" ref="J81" si="66">(E81+F81+($K$88*H81+$M$88)*$L$88)/(1-G81)/(1-$O$88)/(1-I81)/$N$88</f>
         <v>28.452685421994886</v>
       </c>
       <c r="K81" s="12">
-        <f t="shared" ref="K81" si="67">(E81+F81+($K$86*H81+$M$86)*$L$86)/(1-G81)/(1-$P$86)/(1-I81)/$N$86</f>
+        <f t="shared" ref="K81" si="67">(E81+F81+($K$88*H81+$M$88)*$L$88)/(1-G81)/(1-$P$88)/(1-I81)/$N$88</f>
         <v>30.79584775086505</v>
       </c>
       <c r="L81" s="1">
-        <f t="shared" ref="L81" si="68">E81+F81+($K$86*H81+$M$86)*$L$86</f>
+        <f t="shared" ref="L81" si="68">E81+F81+($K$88*H81+$M$88)*$L$88</f>
         <v>106.8</v>
       </c>
       <c r="M81" s="13">
-        <f t="shared" ref="M81" si="69">L81/(1-G81)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M81" si="69">L81/(1-G81)/(1-$O$88)/$N$88</f>
         <v>21.339514066496164</v>
       </c>
       <c r="N81" s="13">
-        <f t="shared" ref="N81" si="70">L81/(1-G81)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N81" si="70">L81/(1-G81)/(1-$P$88)/$N$88</f>
         <v>23.096885813148791</v>
       </c>
       <c r="O81" s="13">
-        <f t="shared" ref="O81" si="71">L81/(1-G81)/$N$86</f>
+        <f t="shared" ref="O81" si="71">L81/(1-G81)/$N$88</f>
         <v>19.632352941176471</v>
       </c>
       <c r="P81" s="14">
-        <f t="shared" ref="P81" si="72">O81*$N$86-L81</f>
+        <f t="shared" ref="P81" si="72">O81*$N$88-L81</f>
         <v>26.700000000000003</v>
       </c>
       <c r="Q81">
@@ -9045,31 +9131,31 @@
         <v>0.25</v>
       </c>
       <c r="J82" s="11">
-        <f t="shared" ref="J82" si="73">(E82+F82+($K$86*H82+$M$86)*$L$86)/(1-G82)/(1-$O$86)/(1-I82)/$N$86</f>
+        <f t="shared" ref="J82" si="73">(E82+F82+($K$88*H82+$M$88)*$L$88)/(1-G82)/(1-$O$88)/(1-I82)/$N$88</f>
         <v>17.396632566069901</v>
       </c>
       <c r="K82" s="12">
-        <f t="shared" ref="K82" si="74">(E82+F82+($K$86*H82+$M$86)*$L$86)/(1-G82)/(1-$P$86)/(1-I82)/$N$86</f>
+        <f t="shared" ref="K82" si="74">(E82+F82+($K$88*H82+$M$88)*$L$88)/(1-G82)/(1-$P$88)/(1-I82)/$N$88</f>
         <v>18.829296424452131</v>
       </c>
       <c r="L82" s="1">
-        <f t="shared" ref="L82" si="75">E82+F82+($K$86*H82+$M$86)*$L$86</f>
+        <f t="shared" ref="L82" si="75">E82+F82+($K$88*H82+$M$88)*$L$88</f>
         <v>65.3</v>
       </c>
       <c r="M82" s="13">
-        <f t="shared" ref="M82" si="76">L82/(1-G82)/(1-$O$86)/$N$86</f>
+        <f t="shared" ref="M82" si="76">L82/(1-G82)/(1-$O$88)/$N$88</f>
         <v>13.047474424552426</v>
       </c>
       <c r="N82" s="13">
-        <f t="shared" ref="N82" si="77">L82/(1-G82)/(1-$P$86)/$N$86</f>
+        <f t="shared" ref="N82" si="77">L82/(1-G82)/(1-$P$88)/$N$88</f>
         <v>14.121972318339099</v>
       </c>
       <c r="O82" s="13">
-        <f t="shared" ref="O82" si="78">L82/(1-G82)/$N$86</f>
+        <f t="shared" ref="O82" si="78">L82/(1-G82)/$N$88</f>
         <v>12.003676470588234</v>
       </c>
       <c r="P82" s="14">
-        <f t="shared" ref="P82" si="79">O82*$N$86-L82</f>
+        <f t="shared" ref="P82" si="79">O82*$N$88-L82</f>
         <v>16.324999999999989</v>
       </c>
       <c r="Q82">
@@ -9081,65 +9167,187 @@
       <c r="S82" s="18"/>
     </row>
     <row r="83" spans="2:19" ht="90.75" customHeight="1">
-      <c r="C83" s="1"/>
-      <c r="D83" s="9"/>
-      <c r="G83" s="3"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="12"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="14"/>
+      <c r="B83">
+        <v>17022301</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83">
+        <v>28</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H83">
+        <v>0.5</v>
+      </c>
+      <c r="I83" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="J83" s="11">
+        <f t="shared" ref="J83" si="80">(E83+F83+($K$88*H83+$M$88)*$L$88)/(1-G83)/(1-$O$88)/(1-I83)/$N$88</f>
+        <v>22.635412860796489</v>
+      </c>
+      <c r="K83" s="12">
+        <f t="shared" ref="K83" si="81">(E83+F83+($K$88*H83+$M$88)*$L$88)/(1-G83)/(1-$P$88)/(1-I83)/$N$88</f>
+        <v>24.499505684626794</v>
+      </c>
+      <c r="L83" s="1">
+        <f t="shared" ref="L83" si="82">E83+F83+($K$88*H83+$M$88)*$L$88</f>
+        <v>79.3</v>
+      </c>
+      <c r="M83" s="13">
+        <f t="shared" ref="M83" si="83">L83/(1-G83)/(1-$O$88)/$N$88</f>
+        <v>15.844789002557542</v>
+      </c>
+      <c r="N83" s="13">
+        <f t="shared" ref="N83" si="84">L83/(1-G83)/(1-$P$88)/$N$88</f>
+        <v>17.149653979238753</v>
+      </c>
+      <c r="O83" s="13">
+        <f t="shared" ref="O83" si="85">L83/(1-G83)/$N$88</f>
+        <v>14.57720588235294</v>
+      </c>
+      <c r="P83" s="14">
+        <f t="shared" ref="P83" si="86">O83*$N$88-L83</f>
+        <v>19.824999999999989</v>
+      </c>
+      <c r="Q83">
+        <v>25</v>
+      </c>
+      <c r="R83">
+        <v>30</v>
+      </c>
       <c r="S83" s="18"/>
     </row>
-    <row r="84" spans="2:19">
-      <c r="G84" s="15"/>
-      <c r="I84" s="15"/>
-      <c r="J84" s="11"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="14"/>
+    <row r="84" spans="2:19" ht="90.75" customHeight="1">
+      <c r="B84">
+        <v>17022401</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84">
+        <v>15</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H84">
+        <v>0.23</v>
+      </c>
+      <c r="I84" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J84" s="11">
+        <f t="shared" ref="J84" si="87">(E84+F84+($K$88*H84+$M$88)*$L$88)/(1-G84)/(1-$O$88)/(1-I84)/$N$88</f>
+        <v>15.043336175049729</v>
+      </c>
+      <c r="K84" s="12">
+        <f t="shared" ref="K84" si="88">(E84+F84+($K$88*H84+$M$88)*$L$88)/(1-G84)/(1-$P$88)/(1-I84)/$N$88</f>
+        <v>16.282199154171472</v>
+      </c>
+      <c r="L84" s="1">
+        <f t="shared" ref="L84" si="89">E84+F84+($K$88*H84+$M$88)*$L$88</f>
+        <v>42.349999999999994</v>
+      </c>
+      <c r="M84" s="13">
+        <f t="shared" ref="M84" si="90">L84/(1-G84)/(1-$O$88)/$N$88</f>
+        <v>9.026001705029838</v>
+      </c>
+      <c r="N84" s="13">
+        <f t="shared" ref="N84" si="91">L84/(1-G84)/(1-$P$88)/$N$88</f>
+        <v>9.7693194925028823</v>
+      </c>
+      <c r="O84" s="13">
+        <f t="shared" ref="O84" si="92">L84/(1-G84)/$N$88</f>
+        <v>8.3039215686274499</v>
+      </c>
+      <c r="P84" s="14">
+        <f t="shared" ref="P84" si="93">O84*$N$88-L84</f>
+        <v>14.11666666666666</v>
+      </c>
+      <c r="Q84">
+        <v>40</v>
+      </c>
+      <c r="R84">
+        <v>30</v>
+      </c>
+      <c r="S84" s="18"/>
     </row>
-    <row r="85" spans="2:19">
-      <c r="K85" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L85" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="M85" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="N85" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="O85" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="P85" s="16" t="s">
-        <v>107</v>
-      </c>
+    <row r="85" spans="2:19" ht="90.75" customHeight="1">
+      <c r="C85" s="1"/>
+      <c r="D85" s="9"/>
+      <c r="G85" s="3"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="11"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="14"/>
+      <c r="S85" s="18"/>
     </row>
     <row r="86" spans="2:19">
-      <c r="K86" s="17">
+      <c r="G86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="11"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="13"/>
+      <c r="O86" s="13"/>
+      <c r="P86" s="14"/>
+    </row>
+    <row r="87" spans="2:19">
+      <c r="K87" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L87" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M87" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="N87" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O87" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="P87" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="2:19">
+      <c r="K88" s="17">
         <v>100</v>
       </c>
-      <c r="L86" s="15">
+      <c r="L88" s="15">
         <v>0.85</v>
       </c>
-      <c r="M86">
+      <c r="M88">
         <v>8</v>
       </c>
-      <c r="N86">
+      <c r="N88">
         <v>6.8</v>
       </c>
-      <c r="O86" s="15">
+      <c r="O88" s="15">
         <v>0.08</v>
       </c>
-      <c r="P86" s="15">
+      <c r="P88" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -9149,7 +9357,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C83">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C85">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -9229,10 +9437,11 @@
     <hyperlink ref="D80" r:id="rId70"/>
     <hyperlink ref="D81" r:id="rId71"/>
     <hyperlink ref="D82" r:id="rId72"/>
+    <hyperlink ref="D83" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId73"/>
+  <drawing r:id="rId74"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17022504 cartoon 8 socks by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>产品标题</t>
   </si>
@@ -386,6 +386,10 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/535621646058.html?spm=a261y.7663282.0.0.lbAPWL&amp;sk=consign</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/525774337749.html?spm=0.0.0.0.v042e3</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -4054,6 +4058,44 @@
         <a:xfrm>
           <a:off x="107674" y="96749152"/>
           <a:ext cx="800563" cy="795132"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190502</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>215349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>808325</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>836544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="图片 88" descr="QQ截图20170225213645.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId87" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190502" y="98024675"/>
+          <a:ext cx="617823" cy="621195"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4350,11 +4392,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:T91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D90" sqref="D90"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4460,31 +4502,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$90*H2+$M$90)*$L$90)/(1-G2)/(1-$O$90)/(1-I2)/$N$90</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$91*H2+$M$91)*$L$91)/(1-G2)/(1-$O$91)/(1-I2)/$N$91</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2" si="1">(E2+F2+($K$90*H2+$M$90)*$L$90)/(1-G2)/(1-$P$90)/(1-I2)/$N$90</f>
+        <f t="shared" ref="K2" si="1">(E2+F2+($K$91*H2+$M$91)*$L$91)/(1-G2)/(1-$P$91)/(1-I2)/$N$91</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="2">E2+F2+($K$90*H2+$M$90)*$L$90</f>
+        <f t="shared" ref="L2" si="2">E2+F2+($K$91*H2+$M$91)*$L$91</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M2" si="3">L2/(1-G2)/(1-$O$91)/$N$91</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N2" si="4">L2/(1-G2)/(1-$P$91)/$N$91</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$90</f>
+        <f>L2/(1-G2)/$N$91</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$90-L2</f>
+        <f>O2*$N$91-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -4525,27 +4567,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$90*H3+$M$90)*$L$90)/(1-G3)/(1-$P$90)/(1-I3)/$N$90</f>
+        <f t="shared" ref="K3:K6" si="5">(E3+F3+($K$91*H3+$M$91)*$L$91)/(1-G3)/(1-$P$91)/(1-I3)/$N$91</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$90*H3+$M$90)*$L$90</f>
+        <f t="shared" ref="L3:L6" si="6">E3+F3+($K$91*H3+$M$91)*$L$91</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M3:M6" si="7">L3/(1-G3)/(1-$O$91)/$N$91</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N3:N6" si="8">L3/(1-G3)/(1-$P$91)/$N$91</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$90</f>
+        <f t="shared" ref="O3:O6" si="9">L3/(1-G3)/$N$91</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f t="shared" ref="P3:P6" si="10">O3*$N$90-L3</f>
+        <f t="shared" ref="P3:P6" si="10">O3*$N$91-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -4772,27 +4814,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$90*H7+$M$90)*$L$90)/(1-G7)/(1-$P$90)/(1-I7)/$N$90</f>
+        <f t="shared" ref="K7:K49" si="11">(E7+F7+($K$91*H7+$M$91)*$L$91)/(1-G7)/(1-$P$91)/(1-I7)/$N$91</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$90*H7+$M$90)*$L$90</f>
+        <f t="shared" ref="L7:L49" si="12">E7+F7+($K$91*H7+$M$91)*$L$91</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M7:M49" si="13">L7/(1-G7)/(1-$O$91)/$N$91</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N7:N49" si="14">L7/(1-G7)/(1-$P$91)/$N$91</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$90</f>
+        <f t="shared" ref="O7:O49" si="15">L7/(1-G7)/$N$91</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="16">O7*$N$90-L7</f>
+        <f t="shared" ref="P7:P49" si="16">O7*$N$91-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -7312,31 +7354,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$90*H50+$M$90)*$L$90)/(1-G50)/(1-$O$90)/(1-I50)/$N$90</f>
+        <f t="shared" ref="J50:J58" si="17">(E50+F50+($K$91*H50+$M$91)*$L$91)/(1-G50)/(1-$O$91)/(1-I50)/$N$91</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$90*H50+$M$90)*$L$90)/(1-G50)/(1-$P$90)/(1-I50)/$N$90</f>
+        <f t="shared" ref="K50:K58" si="18">(E50+F50+($K$91*H50+$M$91)*$L$91)/(1-G50)/(1-$P$91)/(1-I50)/$N$91</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$90*H50+$M$90)*$L$90</f>
+        <f t="shared" ref="L50:L58" si="19">E50+F50+($K$91*H50+$M$91)*$L$91</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M50:M58" si="20">L50/(1-G50)/(1-$O$91)/$N$91</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N50:N58" si="21">L50/(1-G50)/(1-$P$91)/$N$91</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$90</f>
+        <f t="shared" ref="O50:O58" si="22">L50/(1-G50)/$N$91</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="23">O50*$N$90-L50</f>
+        <f t="shared" ref="P50:P58" si="23">O50*$N$91-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -7855,31 +7897,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$90*H59+$M$90)*$L$90)/(1-G59)/(1-$O$90)/(1-I59)/$N$90</f>
+        <f t="shared" ref="J59:J60" si="24">(E59+F59+($K$91*H59+$M$91)*$L$91)/(1-G59)/(1-$O$91)/(1-I59)/$N$91</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$90*H59+$M$90)*$L$90)/(1-G59)/(1-$P$90)/(1-I59)/$N$90</f>
+        <f t="shared" ref="K59:K60" si="25">(E59+F59+($K$91*H59+$M$91)*$L$91)/(1-G59)/(1-$P$91)/(1-I59)/$N$91</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$90*H59+$M$90)*$L$90</f>
+        <f t="shared" ref="L59:L60" si="26">E59+F59+($K$91*H59+$M$91)*$L$91</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M59:M60" si="27">L59/(1-G59)/(1-$O$91)/$N$91</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N59:N60" si="28">L59/(1-G59)/(1-$P$91)/$N$91</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$90</f>
+        <f t="shared" ref="O59:O60" si="29">L59/(1-G59)/$N$91</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f t="shared" ref="P59:P60" si="30">O59*$N$90-L59</f>
+        <f t="shared" ref="P59:P60" si="30">O59*$N$91-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -7975,31 +8017,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$90*H61+$M$90)*$L$90)/(1-G61)/(1-$O$90)/(1-I61)/$N$90</f>
+        <f t="shared" ref="J61:J66" si="31">(E61+F61+($K$91*H61+$M$91)*$L$91)/(1-G61)/(1-$O$91)/(1-I61)/$N$91</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$90*H61+$M$90)*$L$90)/(1-G61)/(1-$P$90)/(1-I61)/$N$90</f>
+        <f t="shared" ref="K61:K66" si="32">(E61+F61+($K$91*H61+$M$91)*$L$91)/(1-G61)/(1-$P$91)/(1-I61)/$N$91</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$90*H61+$M$90)*$L$90</f>
+        <f t="shared" ref="L61:L66" si="33">E61+F61+($K$91*H61+$M$91)*$L$91</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M61:M66" si="34">L61/(1-G61)/(1-$O$91)/$N$91</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N61:N66" si="35">L61/(1-G61)/(1-$P$91)/$N$91</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$90</f>
+        <f t="shared" ref="O61:O66" si="36">L61/(1-G61)/$N$91</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="37">O61*$N$90-L61</f>
+        <f t="shared" ref="P61:P66" si="37">O61*$N$91-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -8342,31 +8384,31 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$90*H67+$M$90)*$L$90)/(1-G67)/(1-$O$90)/(1-I67)/$N$90</f>
+        <f t="shared" ref="J67:J68" si="38">(E67+F67+($K$91*H67+$M$91)*$L$91)/(1-G67)/(1-$O$91)/(1-I67)/$N$91</f>
         <v>10.461068485365161</v>
       </c>
       <c r="K67" s="12">
-        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$90*H67+$M$90)*$L$90)/(1-G67)/(1-$P$90)/(1-I67)/$N$90</f>
+        <f t="shared" ref="K67:K68" si="39">(E67+F67+($K$91*H67+$M$91)*$L$91)/(1-G67)/(1-$P$91)/(1-I67)/$N$91</f>
         <v>11.322568242983468</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$90*H67+$M$90)*$L$90</f>
+        <f t="shared" ref="L67:L68" si="40">E67+F67+($K$91*H67+$M$91)*$L$91</f>
         <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M67:M68" si="41">L67/(1-G67)/(1-$O$91)/$N$91</f>
         <v>6.276641091219096</v>
       </c>
       <c r="N67" s="13">
-        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N67:N68" si="42">L67/(1-G67)/(1-$P$91)/$N$91</f>
         <v>6.7935409457900811</v>
       </c>
       <c r="O67" s="13">
-        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$90</f>
+        <f t="shared" ref="O67:O68" si="43">L67/(1-G67)/$N$91</f>
         <v>5.7745098039215685</v>
       </c>
       <c r="P67" s="14">
-        <f t="shared" ref="P67:P68" si="44">O67*$N$90-L67</f>
+        <f t="shared" ref="P67:P68" si="44">O67*$N$91-L67</f>
         <v>9.8166666666666664</v>
       </c>
       <c r="Q67">
@@ -8464,31 +8506,31 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69:J76" si="45">(E69+F69+($K$90*H69+$M$90)*$L$90)/(1-G69)/(1-$O$90)/(1-I69)/$N$90</f>
+        <f t="shared" ref="J69:J76" si="45">(E69+F69+($K$91*H69+$M$91)*$L$91)/(1-G69)/(1-$O$91)/(1-I69)/$N$91</f>
         <v>12.539073600454673</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69:K76" si="46">(E69+F69+($K$90*H69+$M$90)*$L$90)/(1-G69)/(1-$P$90)/(1-I69)/$N$90</f>
+        <f t="shared" ref="K69:K76" si="46">(E69+F69+($K$91*H69+$M$91)*$L$91)/(1-G69)/(1-$P$91)/(1-I69)/$N$91</f>
         <v>13.571703191080355</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69:L76" si="47">E69+F69+($K$90*H69+$M$90)*$L$90</f>
+        <f t="shared" ref="L69:L76" si="47">E69+F69+($K$91*H69+$M$91)*$L$91</f>
         <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69:M76" si="48">L69/(1-G69)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M69:M76" si="48">L69/(1-G69)/(1-$O$91)/$N$91</f>
         <v>7.5234441602728035</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69:N76" si="49">L69/(1-G69)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N69:N76" si="49">L69/(1-G69)/(1-$P$91)/$N$91</f>
         <v>8.1430219146482123</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69:O76" si="50">L69/(1-G69)/$N$90</f>
+        <f t="shared" ref="O69:O76" si="50">L69/(1-G69)/$N$91</f>
         <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P76" si="51">O69*$N$90-L69</f>
+        <f t="shared" ref="P69:P76" si="51">O69*$N$91-L69</f>
         <v>11.766666666666666</v>
       </c>
       <c r="Q69">
@@ -8954,31 +8996,31 @@
         <v>0.25</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" ref="J77:J79" si="52">(E77+F77+($K$90*H77+$M$90)*$L$90)/(1-G77)/(1-$O$90)/(1-I77)/$N$90</f>
+        <f t="shared" ref="J77:J79" si="52">(E77+F77+($K$91*H77+$M$91)*$L$91)/(1-G77)/(1-$O$91)/(1-I77)/$N$91</f>
         <v>87.995524296675171</v>
       </c>
       <c r="K77" s="12">
-        <f t="shared" ref="K77:K79" si="53">(E77+F77+($K$90*H77+$M$90)*$L$90)/(1-G77)/(1-$P$90)/(1-I77)/$N$90</f>
+        <f t="shared" ref="K77:K79" si="53">(E77+F77+($K$91*H77+$M$91)*$L$91)/(1-G77)/(1-$P$91)/(1-I77)/$N$91</f>
         <v>95.242214532871969</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" ref="L77:L79" si="54">E77+F77+($K$90*H77+$M$90)*$L$90</f>
+        <f t="shared" ref="L77:L79" si="54">E77+F77+($K$91*H77+$M$91)*$L$91</f>
         <v>330.29999999999995</v>
       </c>
       <c r="M77" s="13">
-        <f t="shared" ref="M77:M79" si="55">L77/(1-G77)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M77:M79" si="55">L77/(1-G77)/(1-$O$91)/$N$91</f>
         <v>65.996643222506378</v>
       </c>
       <c r="N77" s="13">
-        <f t="shared" ref="N77:N79" si="56">L77/(1-G77)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N77:N79" si="56">L77/(1-G77)/(1-$P$91)/$N$91</f>
         <v>71.431660899653977</v>
       </c>
       <c r="O77" s="13">
-        <f t="shared" ref="O77:O79" si="57">L77/(1-G77)/$N$90</f>
+        <f t="shared" ref="O77:O79" si="57">L77/(1-G77)/$N$91</f>
         <v>60.716911764705877</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" ref="P77:P79" si="58">O77*$N$90-L77</f>
+        <f t="shared" ref="P77:P79" si="58">O77*$N$91-L77</f>
         <v>82.574999999999989</v>
       </c>
       <c r="Q77">
@@ -9137,31 +9179,31 @@
         <v>0.45</v>
       </c>
       <c r="J80" s="11">
-        <f t="shared" ref="J80" si="59">(E80+F80+($K$90*H80+$M$90)*$L$90)/(1-G80)/(1-$O$90)/(1-I80)/$N$90</f>
+        <f t="shared" ref="J80" si="59">(E80+F80+($K$91*H80+$M$91)*$L$91)/(1-G80)/(1-$O$91)/(1-I80)/$N$91</f>
         <v>13.291482600945512</v>
       </c>
       <c r="K80" s="12">
-        <f t="shared" ref="K80" si="60">(E80+F80+($K$90*H80+$M$90)*$L$90)/(1-G80)/(1-$P$90)/(1-I80)/$N$90</f>
+        <f t="shared" ref="K80" si="60">(E80+F80+($K$91*H80+$M$91)*$L$91)/(1-G80)/(1-$P$91)/(1-I80)/$N$91</f>
         <v>14.386075285729262</v>
       </c>
       <c r="L80" s="1">
-        <f t="shared" ref="L80" si="61">E80+F80+($K$90*H80+$M$90)*$L$90</f>
+        <f t="shared" ref="L80" si="61">E80+F80+($K$91*H80+$M$91)*$L$91</f>
         <v>34.299999999999997</v>
       </c>
       <c r="M80" s="13">
-        <f t="shared" ref="M80" si="62">L80/(1-G80)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M80" si="62">L80/(1-G80)/(1-$O$91)/$N$91</f>
         <v>7.3103154305200322</v>
       </c>
       <c r="N80" s="13">
-        <f t="shared" ref="N80" si="63">L80/(1-G80)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N80" si="63">L80/(1-G80)/(1-$P$91)/$N$91</f>
         <v>7.9123414071510947</v>
       </c>
       <c r="O80" s="13">
-        <f t="shared" ref="O80" si="64">L80/(1-G80)/$N$90</f>
+        <f t="shared" ref="O80" si="64">L80/(1-G80)/$N$91</f>
         <v>6.7254901960784306</v>
       </c>
       <c r="P80" s="14">
-        <f t="shared" ref="P80" si="65">O80*$N$90-L80</f>
+        <f t="shared" ref="P80" si="65">O80*$N$91-L80</f>
         <v>11.43333333333333</v>
       </c>
       <c r="Q80">
@@ -9198,31 +9240,31 @@
         <v>0.25</v>
       </c>
       <c r="J81" s="11">
-        <f t="shared" ref="J81" si="66">(E81+F81+($K$90*H81+$M$90)*$L$90)/(1-G81)/(1-$O$90)/(1-I81)/$N$90</f>
+        <f t="shared" ref="J81" si="66">(E81+F81+($K$91*H81+$M$91)*$L$91)/(1-G81)/(1-$O$91)/(1-I81)/$N$91</f>
         <v>28.452685421994886</v>
       </c>
       <c r="K81" s="12">
-        <f t="shared" ref="K81" si="67">(E81+F81+($K$90*H81+$M$90)*$L$90)/(1-G81)/(1-$P$90)/(1-I81)/$N$90</f>
+        <f t="shared" ref="K81" si="67">(E81+F81+($K$91*H81+$M$91)*$L$91)/(1-G81)/(1-$P$91)/(1-I81)/$N$91</f>
         <v>30.79584775086505</v>
       </c>
       <c r="L81" s="1">
-        <f t="shared" ref="L81" si="68">E81+F81+($K$90*H81+$M$90)*$L$90</f>
+        <f t="shared" ref="L81" si="68">E81+F81+($K$91*H81+$M$91)*$L$91</f>
         <v>106.8</v>
       </c>
       <c r="M81" s="13">
-        <f t="shared" ref="M81" si="69">L81/(1-G81)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M81" si="69">L81/(1-G81)/(1-$O$91)/$N$91</f>
         <v>21.339514066496164</v>
       </c>
       <c r="N81" s="13">
-        <f t="shared" ref="N81" si="70">L81/(1-G81)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N81" si="70">L81/(1-G81)/(1-$P$91)/$N$91</f>
         <v>23.096885813148791</v>
       </c>
       <c r="O81" s="13">
-        <f t="shared" ref="O81" si="71">L81/(1-G81)/$N$90</f>
+        <f t="shared" ref="O81" si="71">L81/(1-G81)/$N$91</f>
         <v>19.632352941176471</v>
       </c>
       <c r="P81" s="14">
-        <f t="shared" ref="P81" si="72">O81*$N$90-L81</f>
+        <f t="shared" ref="P81" si="72">O81*$N$91-L81</f>
         <v>26.700000000000003</v>
       </c>
       <c r="Q81">
@@ -9259,31 +9301,31 @@
         <v>0.25</v>
       </c>
       <c r="J82" s="11">
-        <f t="shared" ref="J82" si="73">(E82+F82+($K$90*H82+$M$90)*$L$90)/(1-G82)/(1-$O$90)/(1-I82)/$N$90</f>
+        <f t="shared" ref="J82" si="73">(E82+F82+($K$91*H82+$M$91)*$L$91)/(1-G82)/(1-$O$91)/(1-I82)/$N$91</f>
         <v>17.396632566069901</v>
       </c>
       <c r="K82" s="12">
-        <f t="shared" ref="K82" si="74">(E82+F82+($K$90*H82+$M$90)*$L$90)/(1-G82)/(1-$P$90)/(1-I82)/$N$90</f>
+        <f t="shared" ref="K82" si="74">(E82+F82+($K$91*H82+$M$91)*$L$91)/(1-G82)/(1-$P$91)/(1-I82)/$N$91</f>
         <v>18.829296424452131</v>
       </c>
       <c r="L82" s="1">
-        <f t="shared" ref="L82" si="75">E82+F82+($K$90*H82+$M$90)*$L$90</f>
+        <f t="shared" ref="L82" si="75">E82+F82+($K$91*H82+$M$91)*$L$91</f>
         <v>65.3</v>
       </c>
       <c r="M82" s="13">
-        <f t="shared" ref="M82" si="76">L82/(1-G82)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M82" si="76">L82/(1-G82)/(1-$O$91)/$N$91</f>
         <v>13.047474424552426</v>
       </c>
       <c r="N82" s="13">
-        <f t="shared" ref="N82" si="77">L82/(1-G82)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N82" si="77">L82/(1-G82)/(1-$P$91)/$N$91</f>
         <v>14.121972318339099</v>
       </c>
       <c r="O82" s="13">
-        <f t="shared" ref="O82" si="78">L82/(1-G82)/$N$90</f>
+        <f t="shared" ref="O82" si="78">L82/(1-G82)/$N$91</f>
         <v>12.003676470588234</v>
       </c>
       <c r="P82" s="14">
-        <f t="shared" ref="P82" si="79">O82*$N$90-L82</f>
+        <f t="shared" ref="P82" si="79">O82*$N$91-L82</f>
         <v>16.324999999999989</v>
       </c>
       <c r="Q82">
@@ -9320,31 +9362,31 @@
         <v>0.3</v>
       </c>
       <c r="J83" s="11">
-        <f t="shared" ref="J83" si="80">(E83+F83+($K$90*H83+$M$90)*$L$90)/(1-G83)/(1-$O$90)/(1-I83)/$N$90</f>
+        <f t="shared" ref="J83" si="80">(E83+F83+($K$91*H83+$M$91)*$L$91)/(1-G83)/(1-$O$91)/(1-I83)/$N$91</f>
         <v>22.635412860796489</v>
       </c>
       <c r="K83" s="12">
-        <f t="shared" ref="K83" si="81">(E83+F83+($K$90*H83+$M$90)*$L$90)/(1-G83)/(1-$P$90)/(1-I83)/$N$90</f>
+        <f t="shared" ref="K83" si="81">(E83+F83+($K$91*H83+$M$91)*$L$91)/(1-G83)/(1-$P$91)/(1-I83)/$N$91</f>
         <v>24.499505684626794</v>
       </c>
       <c r="L83" s="1">
-        <f t="shared" ref="L83" si="82">E83+F83+($K$90*H83+$M$90)*$L$90</f>
+        <f t="shared" ref="L83" si="82">E83+F83+($K$91*H83+$M$91)*$L$91</f>
         <v>79.3</v>
       </c>
       <c r="M83" s="13">
-        <f t="shared" ref="M83" si="83">L83/(1-G83)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M83" si="83">L83/(1-G83)/(1-$O$91)/$N$91</f>
         <v>15.844789002557542</v>
       </c>
       <c r="N83" s="13">
-        <f t="shared" ref="N83" si="84">L83/(1-G83)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N83" si="84">L83/(1-G83)/(1-$P$91)/$N$91</f>
         <v>17.149653979238753</v>
       </c>
       <c r="O83" s="13">
-        <f t="shared" ref="O83" si="85">L83/(1-G83)/$N$90</f>
+        <f t="shared" ref="O83" si="85">L83/(1-G83)/$N$91</f>
         <v>14.57720588235294</v>
       </c>
       <c r="P83" s="14">
-        <f t="shared" ref="P83" si="86">O83*$N$90-L83</f>
+        <f t="shared" ref="P83" si="86">O83*$N$91-L83</f>
         <v>19.824999999999989</v>
       </c>
       <c r="Q83">
@@ -9381,31 +9423,31 @@
         <v>0.4</v>
       </c>
       <c r="J84" s="11">
-        <f t="shared" ref="J84" si="87">(E84+F84+($K$90*H84+$M$90)*$L$90)/(1-G84)/(1-$O$90)/(1-I84)/$N$90</f>
+        <f t="shared" ref="J84" si="87">(E84+F84+($K$91*H84+$M$91)*$L$91)/(1-G84)/(1-$O$91)/(1-I84)/$N$91</f>
         <v>15.043336175049729</v>
       </c>
       <c r="K84" s="12">
-        <f t="shared" ref="K84" si="88">(E84+F84+($K$90*H84+$M$90)*$L$90)/(1-G84)/(1-$P$90)/(1-I84)/$N$90</f>
+        <f t="shared" ref="K84" si="88">(E84+F84+($K$91*H84+$M$91)*$L$91)/(1-G84)/(1-$P$91)/(1-I84)/$N$91</f>
         <v>16.282199154171472</v>
       </c>
       <c r="L84" s="1">
-        <f t="shared" ref="L84" si="89">E84+F84+($K$90*H84+$M$90)*$L$90</f>
+        <f t="shared" ref="L84" si="89">E84+F84+($K$91*H84+$M$91)*$L$91</f>
         <v>42.349999999999994</v>
       </c>
       <c r="M84" s="13">
-        <f t="shared" ref="M84" si="90">L84/(1-G84)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M84" si="90">L84/(1-G84)/(1-$O$91)/$N$91</f>
         <v>9.026001705029838</v>
       </c>
       <c r="N84" s="13">
-        <f t="shared" ref="N84" si="91">L84/(1-G84)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N84" si="91">L84/(1-G84)/(1-$P$91)/$N$91</f>
         <v>9.7693194925028823</v>
       </c>
       <c r="O84" s="13">
-        <f t="shared" ref="O84" si="92">L84/(1-G84)/$N$90</f>
+        <f t="shared" ref="O84" si="92">L84/(1-G84)/$N$91</f>
         <v>8.3039215686274499</v>
       </c>
       <c r="P84" s="14">
-        <f t="shared" ref="P84" si="93">O84*$N$90-L84</f>
+        <f t="shared" ref="P84" si="93">O84*$N$91-L84</f>
         <v>14.11666666666666</v>
       </c>
       <c r="Q84">
@@ -9442,31 +9484,31 @@
         <v>0.25</v>
       </c>
       <c r="J85" s="11">
-        <f t="shared" ref="J85" si="94">(E85+F85+($K$90*H85+$M$90)*$L$90)/(1-G85)/(1-$O$90)/(1-I85)/$N$90</f>
+        <f t="shared" ref="J85" si="94">(E85+F85+($K$91*H85+$M$91)*$L$91)/(1-G85)/(1-$O$91)/(1-I85)/$N$91</f>
         <v>19.261508951406647</v>
       </c>
       <c r="K85" s="12">
-        <f t="shared" ref="K85" si="95">(E85+F85+($K$90*H85+$M$90)*$L$90)/(1-G85)/(1-$P$90)/(1-I85)/$N$90</f>
+        <f t="shared" ref="K85" si="95">(E85+F85+($K$91*H85+$M$91)*$L$91)/(1-G85)/(1-$P$91)/(1-I85)/$N$91</f>
         <v>20.847750865051903</v>
       </c>
       <c r="L85" s="1">
-        <f t="shared" ref="L85" si="96">E85+F85+($K$90*H85+$M$90)*$L$90</f>
+        <f t="shared" ref="L85" si="96">E85+F85+($K$91*H85+$M$91)*$L$91</f>
         <v>72.3</v>
       </c>
       <c r="M85" s="13">
-        <f t="shared" ref="M85" si="97">L85/(1-G85)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M85" si="97">L85/(1-G85)/(1-$O$91)/$N$91</f>
         <v>14.446131713554985</v>
       </c>
       <c r="N85" s="13">
-        <f t="shared" ref="N85" si="98">L85/(1-G85)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N85" si="98">L85/(1-G85)/(1-$P$91)/$N$91</f>
         <v>15.635813148788927</v>
       </c>
       <c r="O85" s="13">
-        <f t="shared" ref="O85" si="99">L85/(1-G85)/$N$90</f>
+        <f t="shared" ref="O85" si="99">L85/(1-G85)/$N$91</f>
         <v>13.290441176470587</v>
       </c>
       <c r="P85" s="14">
-        <f t="shared" ref="P85" si="100">O85*$N$90-L85</f>
+        <f t="shared" ref="P85" si="100">O85*$N$91-L85</f>
         <v>18.074999999999989</v>
       </c>
       <c r="Q85">
@@ -9479,7 +9521,7 @@
     </row>
     <row r="86" spans="2:19" ht="90.75" customHeight="1">
       <c r="B86">
-        <v>17022501</v>
+        <v>17022502</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>118</v>
@@ -9503,31 +9545,31 @@
         <v>0.25</v>
       </c>
       <c r="J86" s="11">
-        <f t="shared" ref="J86" si="101">(E86+F86+($K$90*H86+$M$90)*$L$90)/(1-G86)/(1-$O$90)/(1-I86)/$N$90</f>
+        <f t="shared" ref="J86" si="101">(E86+F86+($K$91*H86+$M$91)*$L$91)/(1-G86)/(1-$O$91)/(1-I86)/$N$91</f>
         <v>16.900207725466181</v>
       </c>
       <c r="K86" s="12">
-        <f t="shared" ref="K86" si="102">(E86+F86+($K$90*H86+$M$90)*$L$90)/(1-G86)/(1-$P$90)/(1-I86)/$N$90</f>
+        <f t="shared" ref="K86" si="102">(E86+F86+($K$91*H86+$M$91)*$L$91)/(1-G86)/(1-$P$91)/(1-I86)/$N$91</f>
         <v>18.291989538151636</v>
       </c>
       <c r="L86" s="1">
-        <f t="shared" ref="L86" si="103">E86+F86+($K$90*H86+$M$90)*$L$90</f>
+        <f t="shared" ref="L86" si="103">E86+F86+($K$91*H86+$M$91)*$L$91</f>
         <v>56.3</v>
       </c>
       <c r="M86" s="13">
-        <f t="shared" ref="M86" si="104">L86/(1-G86)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M86" si="104">L86/(1-G86)/(1-$O$91)/$N$91</f>
         <v>12.675155794099638</v>
       </c>
       <c r="N86" s="13">
-        <f t="shared" ref="N86" si="105">L86/(1-G86)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N86" si="105">L86/(1-G86)/(1-$P$91)/$N$91</f>
         <v>13.718992153613726</v>
       </c>
       <c r="O86" s="13">
-        <f t="shared" ref="O86" si="106">L86/(1-G86)/$N$90</f>
+        <f t="shared" ref="O86" si="106">L86/(1-G86)/$N$91</f>
         <v>11.661143330571667</v>
       </c>
       <c r="P86" s="14">
-        <f t="shared" ref="P86" si="107">O86*$N$90-L86</f>
+        <f t="shared" ref="P86" si="107">O86*$N$91-L86</f>
         <v>22.99577464788733</v>
       </c>
       <c r="Q86">
@@ -9564,31 +9606,31 @@
         <v>0.25</v>
       </c>
       <c r="J87" s="11">
-        <f t="shared" ref="J87" si="108">(E87+F87+($K$90*H87+$M$90)*$L$90)/(1-G87)/(1-$O$90)/(1-I87)/$N$90</f>
+        <f t="shared" ref="J87" si="108">(E87+F87+($K$91*H87+$M$91)*$L$91)/(1-G87)/(1-$O$91)/(1-I87)/$N$91</f>
         <v>9.0579710144927521</v>
       </c>
       <c r="K87" s="12">
-        <f t="shared" ref="K87" si="109">(E87+F87+($K$90*H87+$M$90)*$L$90)/(1-G87)/(1-$P$90)/(1-I87)/$N$90</f>
+        <f t="shared" ref="K87" si="109">(E87+F87+($K$91*H87+$M$91)*$L$91)/(1-G87)/(1-$P$91)/(1-I87)/$N$91</f>
         <v>9.8039215686274499</v>
       </c>
       <c r="L87" s="1">
-        <f t="shared" ref="L87" si="110">E87+F87+($K$90*H87+$M$90)*$L$90</f>
+        <f t="shared" ref="L87" si="110">E87+F87+($K$91*H87+$M$91)*$L$91</f>
         <v>32.299999999999997</v>
       </c>
       <c r="M87" s="13">
-        <f t="shared" ref="M87" si="111">L87/(1-G87)/(1-$O$90)/$N$90</f>
+        <f t="shared" ref="M87" si="111">L87/(1-G87)/(1-$O$91)/$N$91</f>
         <v>6.7934782608695636</v>
       </c>
       <c r="N87" s="13">
-        <f t="shared" ref="N87" si="112">L87/(1-G87)/(1-$P$90)/$N$90</f>
+        <f t="shared" ref="N87" si="112">L87/(1-G87)/(1-$P$91)/$N$91</f>
         <v>7.352941176470587</v>
       </c>
       <c r="O87" s="13">
-        <f t="shared" ref="O87" si="113">L87/(1-G87)/$N$90</f>
+        <f t="shared" ref="O87" si="113">L87/(1-G87)/$N$91</f>
         <v>6.2499999999999991</v>
       </c>
       <c r="P87" s="14">
-        <f t="shared" ref="P87" si="114">O87*$N$90-L87</f>
+        <f t="shared" ref="P87" si="114">O87*$N$91-L87</f>
         <v>10.199999999999996</v>
       </c>
       <c r="Q87">
@@ -9599,52 +9641,113 @@
       </c>
       <c r="S87" s="18"/>
     </row>
-    <row r="88" spans="2:19">
-      <c r="G88" s="15"/>
-      <c r="I88" s="15"/>
-      <c r="J88" s="11"/>
-      <c r="L88" s="1"/>
-      <c r="M88" s="13"/>
-      <c r="O88" s="13"/>
-      <c r="P88" s="14"/>
+    <row r="88" spans="2:19" ht="90.75" customHeight="1">
+      <c r="B88">
+        <v>17022504</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88">
+        <v>11.2</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="H88">
+        <v>0.1</v>
+      </c>
+      <c r="I88" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="J88" s="11">
+        <f t="shared" ref="J88" si="115">(E88+F88+($K$91*H88+$M$91)*$L$91)/(1-G88)/(1-$O$91)/(1-I88)/$N$91</f>
+        <v>6.6002703470734163</v>
+      </c>
+      <c r="K88" s="12">
+        <f t="shared" ref="K88" si="116">(E88+F88+($K$91*H88+$M$91)*$L$91)/(1-G88)/(1-$P$91)/(1-I88)/$N$91</f>
+        <v>7.1438220227147564</v>
+      </c>
+      <c r="L88" s="1">
+        <f t="shared" ref="L88" si="117">E88+F88+($K$91*H88+$M$91)*$L$91</f>
+        <v>27.5</v>
+      </c>
+      <c r="M88" s="13">
+        <f t="shared" ref="M88" si="118">L88/(1-G88)/(1-$O$91)/$N$91</f>
+        <v>5.9402433123660749</v>
+      </c>
+      <c r="N88" s="13">
+        <f t="shared" ref="N88" si="119">L88/(1-G88)/(1-$P$91)/$N$91</f>
+        <v>6.4294398204432808</v>
+      </c>
+      <c r="O88" s="13">
+        <f t="shared" ref="O88" si="120">L88/(1-G88)/$N$91</f>
+        <v>5.4650238473767887</v>
+      </c>
+      <c r="P88" s="14">
+        <f t="shared" ref="P88" si="121">O88*$N$91-L88</f>
+        <v>9.6621621621621614</v>
+      </c>
+      <c r="Q88">
+        <v>25</v>
+      </c>
+      <c r="R88">
+        <v>30</v>
+      </c>
+      <c r="S88" s="18"/>
     </row>
     <row r="89" spans="2:19">
-      <c r="K89" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L89" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="M89" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="N89" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="O89" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="P89" s="16" t="s">
-        <v>107</v>
-      </c>
+      <c r="G89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="11"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="13"/>
+      <c r="O89" s="13"/>
+      <c r="P89" s="14"/>
     </row>
     <row r="90" spans="2:19">
-      <c r="K90" s="17">
+      <c r="K90" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L90" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M90" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="N90" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O90" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="P90" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="2:19">
+      <c r="K91" s="17">
         <v>100</v>
       </c>
-      <c r="L90" s="15">
+      <c r="L91" s="15">
         <v>0.85</v>
       </c>
-      <c r="M90">
+      <c r="M91">
         <v>8</v>
       </c>
-      <c r="N90">
+      <c r="N91">
         <v>6.8</v>
       </c>
-      <c r="O90" s="15">
+      <c r="O91" s="15">
         <v>0.08</v>
       </c>
-      <c r="P90" s="15">
+      <c r="P91" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -9654,7 +9757,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C87">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C88">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套,婴儿用品"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -9737,10 +9840,11 @@
     <hyperlink ref="D83" r:id="rId73"/>
     <hyperlink ref="D86" r:id="rId74"/>
     <hyperlink ref="D87" r:id="rId75"/>
+    <hyperlink ref="D88" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId76"/>
+  <drawing r:id="rId77"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17022701 cat dress by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="143">
   <si>
     <t>产品标题</t>
   </si>
@@ -396,6 +396,63 @@
   <si>
     <t>https://detail.1688.com/offer/42014445347.html?spm=a2615.7691456.0.0.5dnJHf</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/520514501927.html?spm=b26110380.8015204.tkhy006.2.ROkh4O</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/529046187326.html?spm=a261y.7663282.0.0.Mjtd5V</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/kids-girl-clothes-children-coat-2015-autumn-spring-outwear-kids-jackets-winter-jacket-children-s-clothing/32298507027.html?spm=2114.01010208.3.353.gW5w6m&amp;ws_ab_test=searchweb0_0,searchweb201602_2_10066_10000073_10065_10068_10000074_10000132_10000033_10000030_119_10000167_10000026_10000175_10000126_10000129_10000023_10000123_432_10000069_10000068_10060_10062_10056_10055_10000062_10054_10000063_10059_10000120_10099_10000020_10000156_10000158_10000013_10000117_10103_10102_10000016_10000114_10096_10000111_10000056_10000059_10052_10053_10050_10107_10051_10106_10000097_10000094_10000090_10000147_10000091_10000144_10084_10000150_10000101_10083_10000100_10080_10000153_10000104_10082_10000045_10081_10110_10000108_10111_10000191_10112_10113_10000197_10114_10000089_10000086_10000179_10000083_10000042_10000135_10000080_10078_10079_10000039_10073_10000140_10070_10000036_10122_10123_10126_10124_10000187-10102,searchweb201603_9,afswitch_1,ppcSwitch_5,single_sort_1_default&amp;btsid=6ebea945-c99d-4502-99f7-3fa18e9e1a9c&amp;algo_expid=7be5f30f-786e-458a-b82b-f977929de5f2-36&amp;algo_pvid=7be5f30f-786e-458a-b82b-f977929de5f2</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/520936774201.html?spm=b26110380.7927930.xshy005.1.uG7fI8</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>衣长</t>
+  </si>
+  <si>
+    <t>胸围</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/544047922082.html?spm=a261y.7663282.0.0.T2b6je&amp;sk=consign</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/37031027317.html?spm=b26110380.sw1037192.0.0.LAWL4X</t>
+  </si>
+  <si>
+    <t>尺码</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/536504597436.html?spm=a2615.7691456.0.0.rrHOhg</t>
+  </si>
+  <si>
+    <t>105cm</t>
+  </si>
+  <si>
+    <t>115cm</t>
+  </si>
+  <si>
+    <t>125cm</t>
+  </si>
+  <si>
+    <t>135cm</t>
+  </si>
+  <si>
+    <t>肩宽（肩点到袖口）</t>
+  </si>
+  <si>
+    <t>建议身高</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/533260101909.html?spm=a360q.7751291.0.0.0tLJft</t>
   </si>
 </sst>
 </file>
@@ -408,7 +465,7 @@
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +478,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -429,6 +487,7 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -437,6 +496,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -445,6 +505,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -452,17 +513,31 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,13 +550,45 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -496,7 +603,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -557,6 +664,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -4218,6 +4340,234 @@
         <a:xfrm>
           <a:off x="82826" y="101395695"/>
           <a:ext cx="836543" cy="836543"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>207066</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>913128</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>960782</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="图片 91" descr="QQ截图20170226121514.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId91" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="157370" y="102621523"/>
+          <a:ext cx="755758" cy="753716"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>149088</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>207065</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>893513</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="图片 92" descr="QQ截图20170226194126.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId92" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="149088" y="103772804"/>
+          <a:ext cx="744425" cy="745435"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>165653</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>215349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>894521</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>944217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="图片 93" descr="QQ截图20170226211849.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId93" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="165653" y="104932371"/>
+          <a:ext cx="728868" cy="728868"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66262</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>861392</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>982445</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="图片 94" descr="QQ截图20170226215050.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId94" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66262" y="106058804"/>
+          <a:ext cx="795130" cy="791945"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91110</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>124240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>902806</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>935936</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="图片 95" descr="QQ截图20170226225847.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId95" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91110" y="107143827"/>
+          <a:ext cx="811696" cy="811696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>107673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>960782</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>1002194</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="图片 96" descr="QQ截图20170227231806.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId96" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66261" y="108278543"/>
+          <a:ext cx="894521" cy="894521"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4514,11 +4864,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T94"/>
+  <dimension ref="A1:T100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G95" sqref="G95"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4624,32 +4974,32 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$94*H2+$M$94)*$L$94)/(1-G2)/(1-$O$94)/(1-I2)/$N$94</f>
-        <v>15.169750764756031</v>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$100*H2+$M$100)*$L$100)/(1-G2)/(1-$O$100)/(1-I2)/$N$100</f>
+        <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f>(E2+F2+($K$94*H2+$M$94)*$L$94)/(1-G2)/(1-$P$94)/(1-I2)/$N$94</f>
-        <v>16.419024357147705</v>
+        <f>(E2+F2+($K$100*H2+$M$100)*$L$100)/(1-G2)/(1-$P$100)/(1-I2)/$N$100</f>
+        <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f>E2+F2+($K$94*H2+$M$94)*$L$94</f>
-        <v>60.5</v>
+        <f>E2+F2+($K$100*H2+$M$100)*$L$100</f>
+        <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f>L2/(1-G2)/(1-$O$94)/$N$94</f>
-        <v>12.894288150042627</v>
+        <f>L2/(1-G2)/(1-$O$100)/$N$100</f>
+        <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f>L2/(1-G2)/(1-$P$94)/$N$94</f>
-        <v>13.956170703575548</v>
+        <f>L2/(1-G2)/(1-$P$100)/$N$100</f>
+        <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$94</f>
-        <v>11.862745098039216</v>
+        <f>L2/(1-G2)/$N$100</f>
+        <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$94-L2</f>
-        <v>20.166666666666671</v>
+        <f>O2*$N$100-L2</f>
+        <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
@@ -4686,31 +5036,31 @@
       </c>
       <c r="J3" s="11">
         <f t="shared" si="0"/>
-        <v>9.0934924694515473</v>
+        <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f>(E3+F3+($K$94*H3+$M$94)*$L$94)/(1-G3)/(1-$P$94)/(1-I3)/$N$94</f>
-        <v>9.8423683198769716</v>
+        <f>(E3+F3+($K$100*H3+$M$100)*$L$100)/(1-G3)/(1-$P$100)/(1-I3)/$N$100</f>
+        <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f>E3+F3+($K$94*H3+$M$94)*$L$94</f>
-        <v>32</v>
+        <f>E3+F3+($K$100*H3+$M$100)*$L$100</f>
+        <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f>L3/(1-G3)/(1-$O$94)/$N$94</f>
-        <v>6.8201193520886605</v>
+        <f>L3/(1-G3)/(1-$O$100)/$N$100</f>
+        <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f>L3/(1-G3)/(1-$P$94)/$N$94</f>
-        <v>7.3817762399077278</v>
+        <f>L3/(1-G3)/(1-$P$100)/$N$100</f>
+        <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f>L3/(1-G3)/$N$94</f>
-        <v>6.2745098039215685</v>
+        <f>L3/(1-G3)/$N$100</f>
+        <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f>O3*$N$94-L3</f>
-        <v>10.666666666666664</v>
+        <f>O3*$N$100-L3</f>
+        <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
         <v>1</v>
@@ -4747,31 +5097,31 @@
       </c>
       <c r="J4" s="11">
         <f t="shared" si="0"/>
-        <v>17.050298380221658</v>
+        <v>19.120691754962856</v>
       </c>
       <c r="K4" s="12">
-        <f>(E4+F4+($K$94*H4+$M$94)*$L$94)/(1-G4)/(1-$P$94)/(1-I4)/$N$94</f>
-        <v>18.454440599769324</v>
+        <f>(E4+F4+($K$100*H4+$M$100)*$L$100)/(1-G4)/(1-$P$100)/(1-I4)/$N$100</f>
+        <v>20.69533695831274</v>
       </c>
       <c r="L4" s="1">
-        <f>E4+F4+($K$94*H4+$M$94)*$L$94</f>
-        <v>56</v>
+        <f>E4+F4+($K$100*H4+$M$100)*$L$100</f>
+        <v>62.8</v>
       </c>
       <c r="M4" s="13">
-        <f>L4/(1-G4)/(1-$O$94)/$N$94</f>
-        <v>11.935208866155159</v>
+        <f>L4/(1-G4)/(1-$O$100)/$N$100</f>
+        <v>13.384484228473999</v>
       </c>
       <c r="N4" s="13">
-        <f>L4/(1-G4)/(1-$P$94)/$N$94</f>
-        <v>12.918108419838527</v>
+        <f>L4/(1-G4)/(1-$P$100)/$N$100</f>
+        <v>14.486735870818917</v>
       </c>
       <c r="O4" s="13">
-        <f>L4/(1-G4)/$N$94</f>
-        <v>10.980392156862747</v>
+        <f>L4/(1-G4)/$N$100</f>
+        <v>12.313725490196079</v>
       </c>
       <c r="P4" s="14">
-        <f>O4*$N$94-L4</f>
-        <v>18.666666666666671</v>
+        <f>O4*$N$100-L4</f>
+        <v>20.933333333333337</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
@@ -4808,31 +5158,31 @@
       </c>
       <c r="J5" s="11">
         <f t="shared" si="0"/>
-        <v>16.548819016097486</v>
+        <v>18.253848854119653</v>
       </c>
       <c r="K5" s="12">
-        <f>(E5+F5+($K$94*H5+$M$94)*$L$94)/(1-G5)/(1-$P$94)/(1-I5)/$N$94</f>
-        <v>17.911662935070222</v>
+        <f>(E5+F5+($K$100*H5+$M$100)*$L$100)/(1-G5)/(1-$P$100)/(1-I5)/$N$100</f>
+        <v>19.757106995047156</v>
       </c>
       <c r="L5" s="1">
-        <f>E5+F5+($K$94*H5+$M$94)*$L$94</f>
-        <v>66</v>
+        <f>E5+F5+($K$100*H5+$M$100)*$L$100</f>
+        <v>72.8</v>
       </c>
       <c r="M5" s="13">
-        <f>L5/(1-G5)/(1-$O$94)/$N$94</f>
-        <v>14.066496163682864</v>
+        <f>L5/(1-G5)/(1-$O$100)/$N$100</f>
+        <v>15.515771526001704</v>
       </c>
       <c r="N5" s="13">
-        <f>L5/(1-G5)/(1-$P$94)/$N$94</f>
-        <v>15.224913494809689</v>
+        <f>L5/(1-G5)/(1-$P$100)/$N$100</f>
+        <v>16.793540945790081</v>
       </c>
       <c r="O5" s="13">
-        <f>L5/(1-G5)/$N$94</f>
-        <v>12.941176470588236</v>
+        <f>L5/(1-G5)/$N$100</f>
+        <v>14.274509803921568</v>
       </c>
       <c r="P5" s="14">
-        <f>O5*$N$94-L5</f>
-        <v>22</v>
+        <f>O5*$N$100-L5</f>
+        <v>24.266666666666666</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -4869,31 +5219,31 @@
       </c>
       <c r="J6" s="11">
         <f t="shared" si="0"/>
-        <v>13.751504438092372</v>
+        <v>15.34996991123815</v>
       </c>
       <c r="K6" s="12">
-        <f>(E6+F6+($K$94*H6+$M$94)*$L$94)/(1-G6)/(1-$P$94)/(1-I6)/$N$94</f>
-        <v>14.883981274170567</v>
+        <f>(E6+F6+($K$100*H6+$M$100)*$L$100)/(1-G6)/(1-$P$100)/(1-I6)/$N$100</f>
+        <v>16.61408508039894</v>
       </c>
       <c r="L6" s="1">
-        <f>E6+F6+($K$94*H6+$M$94)*$L$94</f>
-        <v>58.5</v>
+        <f>E6+F6+($K$100*H6+$M$100)*$L$100</f>
+        <v>65.3</v>
       </c>
       <c r="M6" s="13">
-        <f>L6/(1-G6)/(1-$O$94)/$N$94</f>
-        <v>11.688778772378516</v>
+        <f>L6/(1-G6)/(1-$O$100)/$N$100</f>
+        <v>13.047474424552426</v>
       </c>
       <c r="N6" s="13">
-        <f>L6/(1-G6)/(1-$P$94)/$N$94</f>
-        <v>12.651384083044983</v>
+        <f>L6/(1-G6)/(1-$P$100)/$N$100</f>
+        <v>14.121972318339099</v>
       </c>
       <c r="O6" s="13">
-        <f>L6/(1-G6)/$N$94</f>
-        <v>10.753676470588236</v>
+        <f>L6/(1-G6)/$N$100</f>
+        <v>12.003676470588234</v>
       </c>
       <c r="P6" s="14">
-        <f>O6*$N$94-L6</f>
-        <v>14.625</v>
+        <f>O6*$N$100-L6</f>
+        <v>16.324999999999989</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -4933,31 +5283,31 @@
       </c>
       <c r="J7" s="11">
         <f t="shared" si="0"/>
-        <v>15.545860287849157</v>
+        <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$94*H7+$M$94)*$L$94)/(1-G7)/(1-$P$94)/(1-I7)/$N$94</f>
-        <v>16.826107605672028</v>
+        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$100*H7+$M$100)*$L$100)/(1-G7)/(1-$P$100)/(1-I7)/$N$100</f>
+        <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$94*H7+$M$94)*$L$94</f>
-        <v>62</v>
+        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$100*H7+$M$100)*$L$100</f>
+        <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$94)/$N$94</f>
-        <v>13.213981244671784</v>
+        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$100)/$N$100</f>
+        <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$94)/$N$94</f>
-        <v>14.302191464821224</v>
+        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$100)/$N$100</f>
+        <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$94</f>
-        <v>12.15686274509804</v>
+        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$100</f>
+        <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="6">O7*$N$94-L7</f>
-        <v>20.666666666666671</v>
+        <f t="shared" ref="P7:P49" si="6">O7*$N$100-L7</f>
+        <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
         <v>1</v>
@@ -4993,31 +5343,31 @@
       </c>
       <c r="J8" s="11">
         <f t="shared" si="0"/>
-        <v>32.868446291560105</v>
+        <v>35.585837595907925</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="1"/>
-        <v>35.575259515570934</v>
+        <v>38.516435986159166</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="2"/>
-        <v>82.25</v>
+        <v>89.05</v>
       </c>
       <c r="M8" s="13">
         <f t="shared" si="3"/>
-        <v>16.434223145780052</v>
+        <v>17.792918797953963</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="4"/>
-        <v>17.787629757785467</v>
+        <v>19.258217993079583</v>
       </c>
       <c r="O8" s="13">
         <f t="shared" si="5"/>
-        <v>15.119485294117647</v>
+        <v>16.369485294117645</v>
       </c>
       <c r="P8" s="14">
         <f t="shared" si="6"/>
-        <v>20.5625</v>
+        <v>22.262499999999989</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -5053,31 +5403,31 @@
       </c>
       <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>19.248188405797098</v>
+        <v>21.059782608695649</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="1"/>
-        <v>20.833333333333332</v>
+        <v>22.794117647058822</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="2"/>
-        <v>72.25</v>
+        <v>79.05</v>
       </c>
       <c r="M9" s="13">
         <f t="shared" si="3"/>
-        <v>15.39855072463768</v>
+        <v>16.84782608695652</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="4"/>
-        <v>16.666666666666668</v>
+        <v>18.235294117647058</v>
       </c>
       <c r="O9" s="13">
         <f t="shared" si="5"/>
-        <v>14.166666666666666</v>
+        <v>15.5</v>
       </c>
       <c r="P9" s="14">
         <f t="shared" si="6"/>
-        <v>24.083333333333329</v>
+        <v>26.349999999999994</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -5113,31 +5463,31 @@
       </c>
       <c r="J10" s="11">
         <f t="shared" si="0"/>
-        <v>35.318475216173425</v>
+        <v>37.388868590914626</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="1"/>
-        <v>38.227055528093601</v>
+        <v>40.46795188663701</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="2"/>
-        <v>116</v>
+        <v>122.8</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="3"/>
-        <v>24.722932651321397</v>
+        <v>26.172208013640237</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="4"/>
-        <v>26.758938869665513</v>
+        <v>28.327566320645907</v>
       </c>
       <c r="O10" s="13">
         <f t="shared" si="5"/>
-        <v>22.745098039215687</v>
+        <v>24.078431372549019</v>
       </c>
       <c r="P10" s="14">
         <f t="shared" si="6"/>
-        <v>38.666666666666657</v>
+        <v>40.933333333333323</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -5173,31 +5523,31 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="0"/>
-        <v>31.091720575698314</v>
+        <v>32.796750413720474</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="1"/>
-        <v>33.652215211344057</v>
+        <v>35.497659271320991</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="2"/>
-        <v>124</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="M11" s="13">
         <f t="shared" si="3"/>
-        <v>26.427962489343567</v>
+        <v>27.877237851662404</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="4"/>
-        <v>28.604382929642448</v>
+        <v>30.173010380622841</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="5"/>
-        <v>24.313725490196081</v>
+        <v>25.647058823529413</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="6"/>
-        <v>41.333333333333343</v>
+        <v>43.599999999999994</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -5233,31 +5583,31 @@
       </c>
       <c r="J12" s="11">
         <f t="shared" si="0"/>
-        <v>31.130686877640393</v>
+        <v>32.858757659419616</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="1"/>
-        <v>33.694390502857843</v>
+        <v>35.5647729960777</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="2"/>
-        <v>122.5</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="M12" s="13">
         <f t="shared" si="3"/>
-        <v>26.461083845994334</v>
+        <v>27.929944010506674</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="4"/>
-        <v>28.640231927429163</v>
+        <v>30.230057046666044</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="5"/>
-        <v>24.344197138314787</v>
+        <v>25.695548489666137</v>
       </c>
       <c r="P12" s="14">
         <f t="shared" si="6"/>
-        <v>43.040540540540547</v>
+        <v>45.429729729729729</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -5293,31 +5643,31 @@
       </c>
       <c r="J13" s="11">
         <f t="shared" si="0"/>
-        <v>13.47725791083697</v>
+        <v>15.182287748859135</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" si="1"/>
-        <v>14.587149738788252</v>
+        <v>16.432593798765183</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="2"/>
-        <v>53.75</v>
+        <v>60.55</v>
       </c>
       <c r="M13" s="13">
         <f t="shared" si="3"/>
-        <v>11.455669224211425</v>
+        <v>12.904944586530265</v>
       </c>
       <c r="N13" s="13">
         <f t="shared" si="4"/>
-        <v>12.399077277970013</v>
+        <v>13.967704728950405</v>
       </c>
       <c r="O13" s="13">
         <f t="shared" si="5"/>
-        <v>10.539215686274511</v>
+        <v>11.872549019607844</v>
       </c>
       <c r="P13" s="14">
         <f t="shared" si="6"/>
-        <v>17.916666666666671</v>
+        <v>20.183333333333337</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -5353,31 +5703,31 @@
       </c>
       <c r="J14" s="11">
         <f t="shared" si="0"/>
-        <v>56.692242114237004</v>
+        <v>59.590792838874677</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="1"/>
-        <v>61.361014994232995</v>
+        <v>64.498269896193776</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="2"/>
-        <v>133</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="M14" s="13">
         <f t="shared" si="3"/>
-        <v>28.346121057118502</v>
+        <v>29.795396419437338</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="4"/>
-        <v>30.680507497116498</v>
+        <v>32.249134948096888</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="5"/>
-        <v>26.078431372549023</v>
+        <v>27.411764705882355</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="6"/>
-        <v>44.333333333333343</v>
+        <v>46.599999999999994</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -5413,31 +5763,31 @@
       </c>
       <c r="J15" s="11">
         <f t="shared" si="0"/>
-        <v>21.31287297527707</v>
+        <v>23.017902813299234</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="1"/>
-        <v>23.068050749711652</v>
+        <v>24.913494809688583</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>91.8</v>
       </c>
       <c r="M15" s="13">
         <f t="shared" si="3"/>
-        <v>18.115942028985508</v>
+        <v>19.565217391304348</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="4"/>
-        <v>19.607843137254903</v>
+        <v>21.176470588235293</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="5"/>
-        <v>16.666666666666668</v>
+        <v>18</v>
       </c>
       <c r="P15" s="14">
         <f t="shared" si="6"/>
-        <v>28.333333333333343</v>
+        <v>30.599999999999994</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -5473,31 +5823,31 @@
       </c>
       <c r="J16" s="11">
         <f t="shared" si="0"/>
-        <v>9.8572037510656436</v>
+        <v>11.668797953964194</v>
       </c>
       <c r="K16" s="12">
         <f t="shared" si="1"/>
-        <v>10.668973471741637</v>
+        <v>12.629757785467127</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>43.8</v>
       </c>
       <c r="M16" s="13">
         <f t="shared" si="3"/>
-        <v>7.3929028132992327</v>
+        <v>8.751598465473144</v>
       </c>
       <c r="N16" s="13">
         <f t="shared" si="4"/>
-        <v>8.0017301038062296</v>
+        <v>9.4723183391003456</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="5"/>
-        <v>6.8014705882352944</v>
+        <v>8.0514705882352935</v>
       </c>
       <c r="P16" s="14">
         <f t="shared" si="6"/>
-        <v>9.25</v>
+        <v>10.949999999999996</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -5533,31 +5883,31 @@
       </c>
       <c r="J17" s="11">
         <f t="shared" si="0"/>
-        <v>14.793641241662906</v>
+        <v>16.498671079685071</v>
       </c>
       <c r="K17" s="12">
         <f t="shared" si="1"/>
-        <v>16.011941108623382</v>
+        <v>17.857385168600313</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>65.8</v>
       </c>
       <c r="M17" s="13">
         <f t="shared" si="3"/>
-        <v>12.57459505541347</v>
+        <v>14.02387041773231</v>
       </c>
       <c r="N17" s="13">
         <f t="shared" si="4"/>
-        <v>13.610149942329874</v>
+        <v>15.178777393310266</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="5"/>
-        <v>11.568627450980394</v>
+        <v>12.901960784313726</v>
       </c>
       <c r="P17" s="14">
         <f t="shared" si="6"/>
-        <v>19.666666666666671</v>
+        <v>21.933333333333337</v>
       </c>
       <c r="Q17" s="15">
         <v>0.15</v>
@@ -5593,31 +5943,31 @@
       </c>
       <c r="J18" s="11">
         <f t="shared" si="0"/>
-        <v>14.793641241662906</v>
+        <v>16.498671079685071</v>
       </c>
       <c r="K18" s="12">
         <f t="shared" si="1"/>
-        <v>16.011941108623382</v>
+        <v>17.857385168600313</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>65.8</v>
       </c>
       <c r="M18" s="13">
         <f t="shared" si="3"/>
-        <v>12.57459505541347</v>
+        <v>14.02387041773231</v>
       </c>
       <c r="N18" s="13">
         <f t="shared" si="4"/>
-        <v>13.610149942329874</v>
+        <v>15.178777393310266</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="5"/>
-        <v>11.568627450980394</v>
+        <v>12.901960784313726</v>
       </c>
       <c r="P18" s="14">
         <f t="shared" si="6"/>
-        <v>19.666666666666671</v>
+        <v>21.933333333333337</v>
       </c>
       <c r="Q18" s="15">
         <v>0.15</v>
@@ -5653,31 +6003,31 @@
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>14.173060528559251</v>
+        <v>17.071611253196931</v>
       </c>
       <c r="K19" s="12">
         <f t="shared" si="1"/>
-        <v>15.340253748558249</v>
+        <v>18.477508650519031</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="2"/>
-        <v>33.25</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="M19" s="13">
         <f t="shared" si="3"/>
-        <v>7.0865302642796255</v>
+        <v>8.5358056265984654</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" si="4"/>
-        <v>7.6701268742791244</v>
+        <v>9.2387543252595155</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="5"/>
-        <v>6.5196078431372557</v>
+        <v>7.8529411764705879</v>
       </c>
       <c r="P19" s="14">
         <f t="shared" si="6"/>
-        <v>11.083333333333336</v>
+        <v>13.350000000000001</v>
       </c>
       <c r="Q19">
         <v>15</v>
@@ -5713,31 +6063,31 @@
       </c>
       <c r="J20" s="11">
         <f t="shared" si="0"/>
-        <v>16.441359152356597</v>
+        <v>18.511752527097798</v>
       </c>
       <c r="K20" s="12">
         <f t="shared" si="1"/>
-        <v>17.795353435491847</v>
+        <v>20.03624979403526</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>60.8</v>
       </c>
       <c r="M20" s="13">
         <f t="shared" si="3"/>
-        <v>11.508951406649617</v>
+        <v>12.958226768968457</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="4"/>
-        <v>12.456747404844291</v>
+        <v>14.025374855824683</v>
       </c>
       <c r="O20" s="13">
         <f t="shared" si="5"/>
-        <v>10.588235294117647</v>
+        <v>11.921568627450981</v>
       </c>
       <c r="P20" s="14">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>20.266666666666666</v>
       </c>
       <c r="R20">
         <v>30</v>
@@ -5770,31 +6120,31 @@
       </c>
       <c r="J21" s="11">
         <f t="shared" si="0"/>
-        <v>23.347283577462601</v>
+        <v>25.982329690769582</v>
       </c>
       <c r="K21" s="12">
         <f t="shared" si="1"/>
-        <v>25.270001048547758</v>
+        <v>28.122050959421202</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="2"/>
-        <v>60.25</v>
+        <v>67.05</v>
       </c>
       <c r="M21" s="13">
         <f t="shared" si="3"/>
-        <v>12.841005967604433</v>
+        <v>14.290281329923273</v>
       </c>
       <c r="N21" s="13">
         <f t="shared" si="4"/>
-        <v>13.898500576701268</v>
+        <v>15.46712802768166</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" si="5"/>
-        <v>11.813725490196077</v>
+        <v>13.147058823529411</v>
       </c>
       <c r="P21" s="14">
         <f t="shared" si="6"/>
-        <v>20.083333333333329</v>
+        <v>22.349999999999994</v>
       </c>
       <c r="R21">
         <v>45</v>
@@ -5827,31 +6177,31 @@
       </c>
       <c r="J22" s="11">
         <f t="shared" si="0"/>
-        <v>23.347283577462601</v>
+        <v>25.982329690769582</v>
       </c>
       <c r="K22" s="12">
         <f t="shared" si="1"/>
-        <v>25.270001048547758</v>
+        <v>28.122050959421202</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="2"/>
-        <v>60.25</v>
+        <v>67.05</v>
       </c>
       <c r="M22" s="13">
         <f t="shared" si="3"/>
-        <v>12.841005967604433</v>
+        <v>14.290281329923273</v>
       </c>
       <c r="N22" s="13">
         <f t="shared" si="4"/>
-        <v>13.898500576701268</v>
+        <v>15.46712802768166</v>
       </c>
       <c r="O22" s="13">
         <f t="shared" si="5"/>
-        <v>11.813725490196077</v>
+        <v>13.147058823529411</v>
       </c>
       <c r="P22" s="14">
         <f t="shared" si="6"/>
-        <v>20.083333333333329</v>
+        <v>22.349999999999994</v>
       </c>
       <c r="R22">
         <v>45</v>
@@ -5884,31 +6234,31 @@
       </c>
       <c r="J23" s="11">
         <f t="shared" si="0"/>
-        <v>24.897310702937304</v>
+        <v>27.532356816244285</v>
       </c>
       <c r="K23" s="12">
         <f t="shared" si="1"/>
-        <v>26.947677466708608</v>
+        <v>29.799727377582048</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="2"/>
-        <v>64.25</v>
+        <v>71.05</v>
       </c>
       <c r="M23" s="13">
         <f t="shared" si="3"/>
-        <v>13.693520886615516</v>
+        <v>15.142796248934356</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="4"/>
-        <v>14.821222606689737</v>
+        <v>16.389850057670127</v>
       </c>
       <c r="O23" s="13">
         <f t="shared" si="5"/>
-        <v>12.598039215686276</v>
+        <v>13.931372549019608</v>
       </c>
       <c r="P23" s="14">
         <f t="shared" si="6"/>
-        <v>21.416666666666671</v>
+        <v>23.683333333333337</v>
       </c>
       <c r="R23">
         <v>45</v>
@@ -5941,31 +6291,31 @@
       </c>
       <c r="J24" s="11">
         <f t="shared" si="0"/>
-        <v>23.73479035883128</v>
+        <v>26.36983647213826</v>
       </c>
       <c r="K24" s="12">
         <f t="shared" si="1"/>
-        <v>25.689420153087973</v>
+        <v>28.541470063961413</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="2"/>
-        <v>61.25</v>
+        <v>68.05</v>
       </c>
       <c r="M24" s="13">
         <f t="shared" si="3"/>
-        <v>13.054134697357204</v>
+        <v>14.503410059676044</v>
       </c>
       <c r="N24" s="13">
         <f t="shared" si="4"/>
-        <v>14.129181084198388</v>
+        <v>15.697808535178778</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" si="5"/>
-        <v>12.009803921568629</v>
+        <v>13.343137254901961</v>
       </c>
       <c r="P24" s="14">
         <f t="shared" si="6"/>
-        <v>20.416666666666671</v>
+        <v>22.683333333333337</v>
       </c>
       <c r="R24">
         <v>45</v>
@@ -5998,31 +6348,31 @@
       </c>
       <c r="J25" s="11">
         <f t="shared" si="0"/>
-        <v>23.000142085819835</v>
+        <v>25.415601023017899</v>
       </c>
       <c r="K25" s="12">
         <f t="shared" si="1"/>
-        <v>24.894271434063825</v>
+        <v>27.508650519031143</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="2"/>
-        <v>64.75</v>
+        <v>71.55</v>
       </c>
       <c r="M25" s="13">
         <f t="shared" si="3"/>
-        <v>13.8000852514919</v>
+        <v>15.24936061381074</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="4"/>
-        <v>14.936562860438293</v>
+        <v>16.505190311418687</v>
       </c>
       <c r="O25" s="13">
         <f t="shared" si="5"/>
-        <v>12.696078431372548</v>
+        <v>14.029411764705882</v>
       </c>
       <c r="P25" s="14">
         <f t="shared" si="6"/>
-        <v>21.583333333333329</v>
+        <v>23.849999999999994</v>
       </c>
       <c r="R25">
         <v>40</v>
@@ -6055,31 +6405,31 @@
       </c>
       <c r="J26" s="11">
         <f t="shared" si="0"/>
-        <v>20.336032963910203</v>
+        <v>22.751491901108267</v>
       </c>
       <c r="K26" s="12">
         <f t="shared" si="1"/>
-        <v>22.010765090349864</v>
+        <v>24.625144175317189</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="2"/>
-        <v>57.25</v>
+        <v>64.05</v>
       </c>
       <c r="M26" s="13">
         <f t="shared" si="3"/>
-        <v>12.201619778346119</v>
+        <v>13.650895140664959</v>
       </c>
       <c r="N26" s="13">
         <f t="shared" si="4"/>
-        <v>13.206459054209919</v>
+        <v>14.775086505190311</v>
       </c>
       <c r="O26" s="13">
         <f t="shared" si="5"/>
-        <v>11.225490196078431</v>
+        <v>12.558823529411764</v>
       </c>
       <c r="P26" s="14">
         <f t="shared" si="6"/>
-        <v>19.083333333333329</v>
+        <v>21.349999999999994</v>
       </c>
       <c r="R26">
         <v>40</v>
@@ -6112,31 +6462,31 @@
       </c>
       <c r="J27" s="11">
         <f t="shared" si="0"/>
-        <v>17.26342710997443</v>
+        <v>19.333820484715627</v>
       </c>
       <c r="K27" s="12">
         <f t="shared" si="1"/>
-        <v>18.68512110726644</v>
+        <v>20.926017465809856</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="2"/>
-        <v>56.7</v>
+        <v>63.5</v>
       </c>
       <c r="M27" s="13">
         <f t="shared" si="3"/>
-        <v>12.084398976982099</v>
+        <v>13.533674339300937</v>
       </c>
       <c r="N27" s="13">
         <f t="shared" si="4"/>
-        <v>13.079584775086508</v>
+        <v>14.648212226066898</v>
       </c>
       <c r="O27" s="13">
         <f t="shared" si="5"/>
-        <v>11.117647058823531</v>
+        <v>12.450980392156863</v>
       </c>
       <c r="P27" s="14">
         <f t="shared" si="6"/>
-        <v>18.900000000000006</v>
+        <v>21.166666666666671</v>
       </c>
       <c r="Q27">
         <v>40</v>
@@ -6172,31 +6522,31 @@
       </c>
       <c r="J28" s="11">
         <f t="shared" si="0"/>
-        <v>26.059831047043325</v>
+        <v>28.694877160350305</v>
       </c>
       <c r="K28" s="12">
         <f t="shared" si="1"/>
-        <v>28.205934780329248</v>
+        <v>31.057984691202684</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="2"/>
-        <v>67.25</v>
+        <v>74.05</v>
       </c>
       <c r="M28" s="13">
         <f t="shared" si="3"/>
-        <v>14.332907075873829</v>
+        <v>15.782182438192669</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="4"/>
-        <v>15.513264129181087</v>
+        <v>17.081891580161475</v>
       </c>
       <c r="O28" s="13">
         <f t="shared" si="5"/>
-        <v>13.186274509803923</v>
+        <v>14.519607843137255</v>
       </c>
       <c r="P28" s="14">
         <f t="shared" si="6"/>
-        <v>22.416666666666671</v>
+        <v>24.683333333333337</v>
       </c>
       <c r="Q28">
         <v>45</v>
@@ -6232,31 +6582,31 @@
       </c>
       <c r="J29" s="11">
         <f t="shared" si="0"/>
-        <v>19.678886047172494</v>
+        <v>21.611253196930942</v>
       </c>
       <c r="K29" s="12">
         <f t="shared" si="1"/>
-        <v>21.299500192233758</v>
+        <v>23.39100346020761</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="2"/>
-        <v>69.25</v>
+        <v>76.05</v>
       </c>
       <c r="M29" s="13">
         <f t="shared" si="3"/>
-        <v>14.759164535379369</v>
+        <v>16.208439897698209</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="4"/>
-        <v>15.974625144175317</v>
+        <v>17.543252595155707</v>
       </c>
       <c r="O29" s="13">
         <f t="shared" si="5"/>
-        <v>13.578431372549019</v>
+        <v>14.911764705882351</v>
       </c>
       <c r="P29" s="14">
         <f t="shared" si="6"/>
-        <v>23.083333333333329</v>
+        <v>25.349999999999994</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -6292,31 +6642,31 @@
       </c>
       <c r="J30" s="11">
         <f t="shared" si="0"/>
-        <v>24.025420444857787</v>
+        <v>26.660466558164767</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="1"/>
-        <v>26.003984481493134</v>
+        <v>28.856034392366574</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>68.8</v>
       </c>
       <c r="M30" s="13">
         <f t="shared" si="3"/>
-        <v>13.213981244671784</v>
+        <v>14.663256606990624</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="4"/>
-        <v>14.302191464821224</v>
+        <v>15.870818915801616</v>
       </c>
       <c r="O30" s="13">
         <f t="shared" si="5"/>
-        <v>12.15686274509804</v>
+        <v>13.490196078431373</v>
       </c>
       <c r="P30" s="14">
         <f t="shared" si="6"/>
-        <v>20.666666666666671</v>
+        <v>22.933333333333337</v>
       </c>
       <c r="Q30">
         <v>30</v>
@@ -6352,31 +6702,31 @@
       </c>
       <c r="J31" s="11">
         <f t="shared" si="0"/>
-        <v>10.989450127877236</v>
+        <v>12.801044330775786</v>
       </c>
       <c r="K31" s="12">
         <f t="shared" si="1"/>
-        <v>11.894463667820068</v>
+        <v>13.85524798154556</v>
       </c>
       <c r="L31" s="1">
         <f t="shared" si="2"/>
-        <v>41.25</v>
+        <v>48.05</v>
       </c>
       <c r="M31" s="13">
         <f t="shared" si="3"/>
-        <v>8.7915601023017906</v>
+        <v>10.240835464620631</v>
       </c>
       <c r="N31" s="13">
         <f t="shared" si="4"/>
-        <v>9.5155709342560559</v>
+        <v>11.084198385236448</v>
       </c>
       <c r="O31" s="13">
         <f t="shared" si="5"/>
-        <v>8.0882352941176467</v>
+        <v>9.4215686274509807</v>
       </c>
       <c r="P31" s="14">
         <f t="shared" si="6"/>
-        <v>13.749999999999993</v>
+        <v>16.016666666666666</v>
       </c>
       <c r="Q31">
         <v>20</v>
@@ -6412,31 +6762,31 @@
       </c>
       <c r="J32" s="11">
         <f t="shared" si="0"/>
-        <v>15.629440181869848</v>
+        <v>18.044899119067917</v>
       </c>
       <c r="K32" s="12">
         <f t="shared" si="1"/>
-        <v>16.916570549788545</v>
+        <v>19.530949634755864</v>
       </c>
       <c r="L32" s="1">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>50.8</v>
       </c>
       <c r="M32" s="13">
         <f t="shared" si="3"/>
-        <v>9.3776641091219091</v>
+        <v>10.826939471440749</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="4"/>
-        <v>10.149942329873126</v>
+        <v>11.718569780853519</v>
       </c>
       <c r="O32" s="13">
         <f t="shared" si="5"/>
-        <v>8.6274509803921564</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P32" s="14">
         <f t="shared" si="6"/>
-        <v>14.666666666666664</v>
+        <v>16.933333333333337</v>
       </c>
       <c r="Q32">
         <v>20</v>
@@ -6472,31 +6822,31 @@
       </c>
       <c r="J33" s="11">
         <f t="shared" si="0"/>
-        <v>23.444160272804776</v>
+        <v>26.079206386111757</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" si="1"/>
-        <v>25.374855824682811</v>
+        <v>28.226905735556254</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="2"/>
-        <v>60.5</v>
+        <v>67.3</v>
       </c>
       <c r="M33" s="13">
         <f t="shared" si="3"/>
-        <v>12.894288150042627</v>
+        <v>14.343563512361467</v>
       </c>
       <c r="N33" s="13">
         <f t="shared" si="4"/>
-        <v>13.956170703575548</v>
+        <v>15.524798154555942</v>
       </c>
       <c r="O33" s="13">
         <f t="shared" si="5"/>
-        <v>11.862745098039216</v>
+        <v>13.19607843137255</v>
       </c>
       <c r="P33" s="14">
         <f t="shared" si="6"/>
-        <v>20.166666666666671</v>
+        <v>22.433333333333337</v>
       </c>
       <c r="Q33">
         <v>45</v>
@@ -6532,31 +6882,31 @@
       </c>
       <c r="J34" s="11">
         <f t="shared" si="0"/>
-        <v>18.044899119067917</v>
+        <v>19.977266268826373</v>
       </c>
       <c r="K34" s="12">
         <f t="shared" si="1"/>
-        <v>19.530949634755864</v>
+        <v>21.622452902729723</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="2"/>
-        <v>63.5</v>
+        <v>70.3</v>
       </c>
       <c r="M34" s="13">
         <f t="shared" si="3"/>
-        <v>13.533674339300937</v>
+        <v>14.982949701619777</v>
       </c>
       <c r="N34" s="13">
         <f t="shared" si="4"/>
-        <v>14.648212226066898</v>
+        <v>16.21683967704729</v>
       </c>
       <c r="O34" s="13">
         <f t="shared" si="5"/>
-        <v>12.450980392156863</v>
+        <v>13.784313725490197</v>
       </c>
       <c r="P34" s="14">
         <f t="shared" si="6"/>
-        <v>21.166666666666671</v>
+        <v>23.433333333333337</v>
       </c>
       <c r="Q34">
         <v>45</v>
@@ -6592,31 +6942,31 @@
       </c>
       <c r="J35" s="11">
         <f t="shared" si="0"/>
-        <v>14.252983802216537</v>
+        <v>16.064578005115088</v>
       </c>
       <c r="K35" s="12">
         <f t="shared" si="1"/>
-        <v>15.426758938869664</v>
+        <v>17.387543252595155</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="2"/>
-        <v>53.5</v>
+        <v>60.3</v>
       </c>
       <c r="M35" s="13">
         <f t="shared" si="3"/>
-        <v>11.402387041773231</v>
+        <v>12.851662404092071</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="4"/>
-        <v>12.341407151095733</v>
+        <v>13.910034602076124</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="5"/>
-        <v>10.490196078431373</v>
+        <v>11.823529411764705</v>
       </c>
       <c r="P35" s="14">
         <f t="shared" si="6"/>
-        <v>17.833333333333329</v>
+        <v>20.099999999999994</v>
       </c>
       <c r="R35">
         <v>20</v>
@@ -6647,31 +6997,31 @@
       </c>
       <c r="J36" s="11">
         <f t="shared" si="0"/>
-        <v>21.894133147330074</v>
+        <v>24.529179260637054</v>
       </c>
       <c r="K36" s="12">
         <f t="shared" si="1"/>
-        <v>23.697179406521965</v>
+        <v>26.549229317395405</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="2"/>
-        <v>56.5</v>
+        <v>63.3</v>
       </c>
       <c r="M36" s="13">
         <f t="shared" si="3"/>
-        <v>12.041773231031542</v>
+        <v>13.491048593350381</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="4"/>
-        <v>13.033448673587081</v>
+        <v>14.602076124567473</v>
       </c>
       <c r="O36" s="13">
         <f t="shared" si="5"/>
-        <v>11.078431372549019</v>
+        <v>12.411764705882351</v>
       </c>
       <c r="P36" s="14">
         <f t="shared" si="6"/>
-        <v>18.833333333333329</v>
+        <v>21.099999999999994</v>
       </c>
       <c r="Q36">
         <v>45</v>
@@ -6702,31 +7052,31 @@
       </c>
       <c r="J37" s="11">
         <f t="shared" si="0"/>
-        <v>5.5280264279624891</v>
+        <v>7.339620630861039</v>
       </c>
       <c r="K37" s="12">
         <f t="shared" si="1"/>
-        <v>5.9832756632064594</v>
+        <v>7.9440599769319498</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="2"/>
-        <v>20.75</v>
+        <v>27.55</v>
       </c>
       <c r="M37" s="13">
         <f t="shared" si="3"/>
-        <v>4.4224211423699913</v>
+        <v>5.8716965046888321</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="4"/>
-        <v>4.7866205305651679</v>
+        <v>6.3552479815455598</v>
       </c>
       <c r="O37" s="13">
         <f t="shared" si="5"/>
-        <v>4.0686274509803928</v>
+        <v>5.4019607843137258</v>
       </c>
       <c r="P37" s="14">
         <f t="shared" si="6"/>
-        <v>6.9166666666666714</v>
+        <v>9.1833333333333336</v>
       </c>
       <c r="Q37">
         <v>20</v>
@@ -6757,31 +7107,31 @@
       </c>
       <c r="J38" s="11">
         <f t="shared" si="0"/>
-        <v>13.427109974424551</v>
+        <v>16.325660699062233</v>
       </c>
       <c r="K38" s="12">
         <f t="shared" si="1"/>
-        <v>14.53287197231834</v>
+        <v>17.670126874279124</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="2"/>
-        <v>31.5</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="M38" s="13">
         <f t="shared" si="3"/>
-        <v>6.7135549872122757</v>
+        <v>8.1628303495311165</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="4"/>
-        <v>7.2664359861591699</v>
+        <v>8.8350634371395618</v>
       </c>
       <c r="O38" s="13">
         <f t="shared" si="5"/>
-        <v>6.1764705882352944</v>
+        <v>7.5098039215686274</v>
       </c>
       <c r="P38" s="14">
         <f t="shared" si="6"/>
-        <v>10.5</v>
+        <v>12.766666666666666</v>
       </c>
       <c r="Q38">
         <v>20</v>
@@ -6817,31 +7167,31 @@
       </c>
       <c r="J39" s="11">
         <f t="shared" si="0"/>
-        <v>15.629440181869848</v>
+        <v>18.044899119067917</v>
       </c>
       <c r="K39" s="12">
         <f t="shared" si="1"/>
-        <v>16.916570549788545</v>
+        <v>19.530949634755864</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>50.8</v>
       </c>
       <c r="M39" s="13">
         <f t="shared" si="3"/>
-        <v>9.3776641091219091</v>
+        <v>10.826939471440749</v>
       </c>
       <c r="N39" s="13">
         <f t="shared" si="4"/>
-        <v>10.149942329873126</v>
+        <v>11.718569780853519</v>
       </c>
       <c r="O39" s="13">
         <f t="shared" si="5"/>
-        <v>8.6274509803921564</v>
+        <v>9.9607843137254903</v>
       </c>
       <c r="P39" s="14">
         <f t="shared" si="6"/>
-        <v>14.666666666666664</v>
+        <v>16.933333333333337</v>
       </c>
       <c r="Q39">
         <v>20</v>
@@ -6877,31 +7227,31 @@
       </c>
       <c r="J40" s="11">
         <f t="shared" si="0"/>
-        <v>15.88777803611563</v>
+        <v>18.522824149422608</v>
       </c>
       <c r="K40" s="12">
         <f t="shared" si="1"/>
-        <v>17.196183286148681</v>
+        <v>20.048233197022117</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>47.8</v>
       </c>
       <c r="M40" s="13">
         <f t="shared" si="3"/>
-        <v>8.7382779198635969</v>
+        <v>10.187553282182437</v>
       </c>
       <c r="N40" s="13">
         <f t="shared" si="4"/>
-        <v>9.4579008073817761</v>
+        <v>11.026528258362168</v>
       </c>
       <c r="O40" s="13">
         <f t="shared" si="5"/>
-        <v>8.0392156862745097</v>
+        <v>9.3725490196078418</v>
       </c>
       <c r="P40" s="14">
         <f t="shared" si="6"/>
-        <v>13.666666666666664</v>
+        <v>15.933333333333323</v>
       </c>
       <c r="Q40">
         <v>20</v>
@@ -6937,31 +7287,31 @@
       </c>
       <c r="J41" s="11">
         <f t="shared" si="0"/>
-        <v>9.5481670929241265</v>
+        <v>11.480534242682578</v>
       </c>
       <c r="K41" s="12">
         <f t="shared" si="1"/>
-        <v>10.33448673587082</v>
+        <v>12.425990003844674</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="2"/>
-        <v>33.6</v>
+        <v>40.4</v>
       </c>
       <c r="M41" s="13">
         <f t="shared" si="3"/>
-        <v>7.1611253196930953</v>
+        <v>8.6104006820119352</v>
       </c>
       <c r="N41" s="13">
         <f t="shared" si="4"/>
-        <v>7.7508650519031148</v>
+        <v>9.3194925028835076</v>
       </c>
       <c r="O41" s="13">
         <f t="shared" si="5"/>
-        <v>6.5882352941176476</v>
+        <v>7.9215686274509807</v>
       </c>
       <c r="P41" s="14">
         <f t="shared" si="6"/>
-        <v>11.200000000000003</v>
+        <v>13.466666666666669</v>
       </c>
       <c r="Q41">
         <v>20</v>
@@ -6997,31 +7347,31 @@
       </c>
       <c r="J42" s="11">
         <f t="shared" si="0"/>
-        <v>22.184763233356577</v>
+        <v>24.819809346663558</v>
       </c>
       <c r="K42" s="12">
         <f t="shared" si="1"/>
-        <v>24.011743734927123</v>
+        <v>26.863793645800566</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="2"/>
-        <v>57.25</v>
+        <v>64.05</v>
       </c>
       <c r="M42" s="13">
         <f t="shared" si="3"/>
-        <v>12.201619778346119</v>
+        <v>13.650895140664959</v>
       </c>
       <c r="N42" s="13">
         <f t="shared" si="4"/>
-        <v>13.206459054209919</v>
+        <v>14.775086505190311</v>
       </c>
       <c r="O42" s="13">
         <f t="shared" si="5"/>
-        <v>11.225490196078431</v>
+        <v>12.558823529411764</v>
       </c>
       <c r="P42" s="14">
         <f t="shared" si="6"/>
-        <v>19.083333333333329</v>
+        <v>21.349999999999994</v>
       </c>
       <c r="Q42">
         <v>45</v>
@@ -7057,31 +7407,31 @@
       </c>
       <c r="J43" s="11">
         <f t="shared" si="0"/>
-        <v>10.798522307473714</v>
+        <v>12.730889457232166</v>
       </c>
       <c r="K43" s="12">
         <f t="shared" si="1"/>
-        <v>11.687812379853902</v>
+        <v>13.779315647827758</v>
       </c>
       <c r="L43" s="1">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>44.8</v>
       </c>
       <c r="M43" s="13">
         <f t="shared" si="3"/>
-        <v>8.0988917306052848</v>
+        <v>9.5481670929241247</v>
       </c>
       <c r="N43" s="13">
         <f t="shared" si="4"/>
-        <v>8.7658592848904267</v>
+        <v>10.334486735870819</v>
       </c>
       <c r="O43" s="13">
         <f t="shared" si="5"/>
-        <v>7.4509803921568629</v>
+        <v>8.7843137254901951</v>
       </c>
       <c r="P43" s="14">
         <f t="shared" si="6"/>
-        <v>12.666666666666664</v>
+        <v>14.93333333333333</v>
       </c>
       <c r="Q43">
         <v>0</v>
@@ -7117,31 +7467,31 @@
       </c>
       <c r="J44" s="11">
         <f t="shared" si="0"/>
-        <v>15.203182722364309</v>
+        <v>17.135549872122759</v>
       </c>
       <c r="K44" s="12">
         <f t="shared" si="1"/>
-        <v>16.45520953479431</v>
+        <v>18.546712802768166</v>
       </c>
       <c r="L44" s="1">
         <f t="shared" si="2"/>
-        <v>53.5</v>
+        <v>60.3</v>
       </c>
       <c r="M44" s="13">
         <f t="shared" si="3"/>
-        <v>11.402387041773231</v>
+        <v>12.851662404092071</v>
       </c>
       <c r="N44" s="13">
         <f t="shared" si="4"/>
-        <v>12.341407151095733</v>
+        <v>13.910034602076124</v>
       </c>
       <c r="O44" s="13">
         <f t="shared" si="5"/>
-        <v>10.490196078431373</v>
+        <v>11.823529411764705</v>
       </c>
       <c r="P44" s="14">
         <f t="shared" si="6"/>
-        <v>17.833333333333329</v>
+        <v>20.099999999999994</v>
       </c>
       <c r="Q44">
         <v>0</v>
@@ -7177,31 +7527,31 @@
       </c>
       <c r="J45" s="11">
         <f t="shared" si="0"/>
-        <v>18.697202201038515</v>
+        <v>21.332248314345499</v>
       </c>
       <c r="K45" s="12">
         <f t="shared" si="1"/>
-        <v>20.236971794065219</v>
+        <v>23.089021704938656</v>
       </c>
       <c r="L45" s="1">
         <f t="shared" si="2"/>
-        <v>48.25</v>
+        <v>55.05</v>
       </c>
       <c r="M45" s="13">
         <f t="shared" si="3"/>
-        <v>10.283461210571184</v>
+        <v>11.732736572890024</v>
       </c>
       <c r="N45" s="13">
         <f t="shared" si="4"/>
-        <v>11.130334486735871</v>
+        <v>12.698961937716263</v>
       </c>
       <c r="O45" s="13">
         <f t="shared" si="5"/>
-        <v>9.4607843137254903</v>
+        <v>10.794117647058822</v>
       </c>
       <c r="P45" s="14">
         <f t="shared" si="6"/>
-        <v>16.083333333333329</v>
+        <v>18.349999999999994</v>
       </c>
       <c r="Q45">
         <v>45</v>
@@ -7237,31 +7587,31 @@
       </c>
       <c r="J46" s="11">
         <f t="shared" si="0"/>
-        <v>17.922188638301169</v>
+        <v>20.557234751608149</v>
       </c>
       <c r="K46" s="12">
         <f t="shared" si="1"/>
-        <v>19.398133584984798</v>
+        <v>22.250183495858234</v>
       </c>
       <c r="L46" s="1">
         <f t="shared" si="2"/>
-        <v>46.25</v>
+        <v>53.05</v>
       </c>
       <c r="M46" s="13">
         <f t="shared" si="3"/>
-        <v>9.8572037510656436</v>
+        <v>11.306479113384484</v>
       </c>
       <c r="N46" s="13">
         <f t="shared" si="4"/>
-        <v>10.668973471741637</v>
+        <v>12.237600922722031</v>
       </c>
       <c r="O46" s="13">
         <f t="shared" si="5"/>
-        <v>9.0686274509803919</v>
+        <v>10.401960784313726</v>
       </c>
       <c r="P46" s="14">
         <f t="shared" si="6"/>
-        <v>15.416666666666664</v>
+        <v>17.683333333333337</v>
       </c>
       <c r="Q46">
         <v>25</v>
@@ -7297,31 +7647,31 @@
       </c>
       <c r="J47" s="11">
         <f t="shared" si="0"/>
-        <v>13.919970161977833</v>
+        <v>15.731564364876382</v>
       </c>
       <c r="K47" s="12">
         <f t="shared" si="1"/>
-        <v>15.066320645905421</v>
+        <v>17.027104959630908</v>
       </c>
       <c r="L47" s="1">
         <f t="shared" si="2"/>
-        <v>52.25</v>
+        <v>59.05</v>
       </c>
       <c r="M47" s="13">
         <f t="shared" si="3"/>
-        <v>10.439977621483376</v>
+        <v>11.798673273657286</v>
       </c>
       <c r="N47" s="13">
         <f t="shared" si="4"/>
-        <v>11.299740484429067</v>
+        <v>12.770328719723182</v>
       </c>
       <c r="O47" s="13">
         <f t="shared" si="5"/>
-        <v>9.6047794117647065</v>
+        <v>10.854779411764705</v>
       </c>
       <c r="P47" s="14">
         <f t="shared" si="6"/>
-        <v>13.0625</v>
+        <v>14.762499999999989</v>
       </c>
       <c r="Q47">
         <v>0</v>
@@ -7357,31 +7707,31 @@
       </c>
       <c r="J48" s="11">
         <f t="shared" si="0"/>
-        <v>13.919970161977833</v>
+        <v>15.731564364876382</v>
       </c>
       <c r="K48" s="12">
         <f t="shared" si="1"/>
-        <v>15.066320645905421</v>
+        <v>17.027104959630908</v>
       </c>
       <c r="L48" s="1">
         <f t="shared" si="2"/>
-        <v>52.25</v>
+        <v>59.05</v>
       </c>
       <c r="M48" s="13">
         <f t="shared" si="3"/>
-        <v>10.439977621483376</v>
+        <v>11.798673273657286</v>
       </c>
       <c r="N48" s="13">
         <f t="shared" si="4"/>
-        <v>11.299740484429067</v>
+        <v>12.770328719723182</v>
       </c>
       <c r="O48" s="13">
         <f t="shared" si="5"/>
-        <v>9.6047794117647065</v>
+        <v>10.854779411764705</v>
       </c>
       <c r="P48" s="14">
         <f t="shared" si="6"/>
-        <v>13.0625</v>
+        <v>14.762499999999989</v>
       </c>
       <c r="Q48">
         <v>0</v>
@@ -7417,31 +7767,31 @@
       </c>
       <c r="J49" s="11">
         <f t="shared" si="0"/>
-        <v>14.563796533105997</v>
+        <v>16.496163682864449</v>
       </c>
       <c r="K49" s="12">
         <f t="shared" si="1"/>
-        <v>15.763168012302961</v>
+        <v>17.854671280276815</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" si="2"/>
-        <v>51.25</v>
+        <v>58.05</v>
       </c>
       <c r="M49" s="13">
         <f t="shared" si="3"/>
-        <v>10.922847399829497</v>
+        <v>12.372122762148337</v>
       </c>
       <c r="N49" s="13">
         <f t="shared" si="4"/>
-        <v>11.82237600922722</v>
+        <v>13.391003460207612</v>
       </c>
       <c r="O49" s="13">
         <f t="shared" si="5"/>
-        <v>10.049019607843137</v>
+        <v>11.382352941176469</v>
       </c>
       <c r="P49" s="14">
         <f t="shared" si="6"/>
-        <v>17.083333333333329</v>
+        <v>19.349999999999994</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -7476,32 +7826,32 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$94*H50+$M$94)*$L$94)/(1-G50)/(1-$O$94)/(1-I50)/$N$94</f>
-        <v>14.434627605983103</v>
+        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$100*H50+$M$100)*$L$100)/(1-G50)/(1-$O$100)/(1-I50)/$N$100</f>
+        <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$94*H50+$M$94)*$L$94)/(1-G50)/(1-$P$94)/(1-I50)/$N$94</f>
-        <v>15.623361644122888</v>
+        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$100*H50+$M$100)*$L$100)/(1-G50)/(1-$P$100)/(1-I50)/$N$100</f>
+        <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$94*H50+$M$94)*$L$94</f>
-        <v>37.25</v>
+        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$100*H50+$M$100)*$L$100</f>
+        <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$94)/$N$94</f>
-        <v>7.9390451832907072</v>
+        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$100)/$N$100</f>
+        <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$94)/$N$94</f>
-        <v>8.5928489042675888</v>
+        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$100)/$N$100</f>
+        <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$94</f>
-        <v>7.3039215686274508</v>
+        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$100</f>
+        <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="13">O50*$N$94-L50</f>
-        <v>12.416666666666664</v>
+        <f t="shared" ref="P50:P58" si="13">O50*$N$100-L50</f>
+        <v>14.68333333333333</v>
       </c>
       <c r="Q50">
         <v>25</v>
@@ -7537,31 +7887,31 @@
       </c>
       <c r="J51" s="11">
         <f t="shared" si="7"/>
-        <v>12.521312872975276</v>
+        <v>14.332907075873825</v>
       </c>
       <c r="K51" s="12">
         <f t="shared" si="8"/>
-        <v>13.552479815455596</v>
+        <v>15.51326412918108</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="9"/>
-        <v>47</v>
+        <v>53.8</v>
       </c>
       <c r="M51" s="13">
         <f t="shared" si="10"/>
-        <v>9.3909846547314579</v>
+        <v>10.749680306905368</v>
       </c>
       <c r="N51" s="13">
         <f t="shared" si="11"/>
-        <v>10.164359861591697</v>
+        <v>11.634948096885811</v>
       </c>
       <c r="O51" s="13">
         <f t="shared" si="12"/>
-        <v>8.639705882352942</v>
+        <v>9.8897058823529385</v>
       </c>
       <c r="P51" s="14">
         <f t="shared" si="13"/>
-        <v>11.750000000000007</v>
+        <v>13.449999999999989</v>
       </c>
       <c r="Q51">
         <v>0</v>
@@ -7597,31 +7947,31 @@
       </c>
       <c r="J52" s="11">
         <f t="shared" si="7"/>
-        <v>21.645886615515767</v>
+        <v>23.457480818414318</v>
       </c>
       <c r="K52" s="12">
         <f t="shared" si="8"/>
-        <v>23.428489042675896</v>
+        <v>25.389273356401382</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" si="9"/>
-        <v>81.25</v>
+        <v>88.05</v>
       </c>
       <c r="M52" s="13">
         <f t="shared" si="10"/>
-        <v>16.234414961636826</v>
+        <v>17.593110613810737</v>
       </c>
       <c r="N52" s="13">
         <f t="shared" si="11"/>
-        <v>17.571366782006919</v>
+        <v>19.041955017301035</v>
       </c>
       <c r="O52" s="13">
         <f t="shared" si="12"/>
-        <v>14.935661764705882</v>
+        <v>16.18566176470588</v>
       </c>
       <c r="P52" s="14">
         <f t="shared" si="13"/>
-        <v>20.3125</v>
+        <v>22.012499999999989</v>
       </c>
       <c r="Q52">
         <v>30</v>
@@ -7657,31 +8007,31 @@
       </c>
       <c r="J53" s="11">
         <f t="shared" si="7"/>
-        <v>22.234294175336036</v>
+        <v>24.27744553198854</v>
       </c>
       <c r="K53" s="12">
         <f t="shared" si="8"/>
-        <v>24.06535369565783</v>
+        <v>26.276764575799358</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" si="9"/>
-        <v>74</v>
+        <v>80.8</v>
       </c>
       <c r="M53" s="13">
         <f t="shared" si="10"/>
-        <v>15.564005922735225</v>
+        <v>16.994211872391976</v>
       </c>
       <c r="N53" s="13">
         <f t="shared" si="11"/>
-        <v>16.845747586960481</v>
+        <v>18.393735203059553</v>
       </c>
       <c r="O53" s="13">
         <f t="shared" si="12"/>
-        <v>14.318885448916408</v>
+        <v>15.634674922600619</v>
       </c>
       <c r="P53" s="14">
         <f t="shared" si="13"/>
-        <v>23.368421052631575</v>
+        <v>25.515789473684208</v>
       </c>
       <c r="Q53">
         <v>30</v>
@@ -7717,31 +8067,31 @@
       </c>
       <c r="J54" s="11">
         <f t="shared" si="7"/>
-        <v>17.183503836317136</v>
+        <v>18.995098039215684</v>
       </c>
       <c r="K54" s="12">
         <f t="shared" si="8"/>
-        <v>18.598615916955019</v>
+        <v>20.559400230680506</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" si="9"/>
-        <v>64.5</v>
+        <v>71.3</v>
       </c>
       <c r="M54" s="13">
         <f t="shared" si="10"/>
-        <v>12.887627877237852</v>
+        <v>14.246323529411763</v>
       </c>
       <c r="N54" s="13">
         <f t="shared" si="11"/>
-        <v>13.948961937716264</v>
+        <v>15.41955017301038</v>
       </c>
       <c r="O54" s="13">
         <f t="shared" si="12"/>
-        <v>11.856617647058824</v>
+        <v>13.106617647058822</v>
       </c>
       <c r="P54" s="14">
         <f t="shared" si="13"/>
-        <v>16.125</v>
+        <v>17.824999999999989</v>
       </c>
       <c r="Q54">
         <v>30</v>
@@ -7780,31 +8130,31 @@
       </c>
       <c r="J55" s="11">
         <f t="shared" si="7"/>
-        <v>22.549780781877971</v>
+        <v>24.490774570697841</v>
       </c>
       <c r="K55" s="12">
         <f t="shared" si="8"/>
-        <v>24.406821552150273</v>
+        <v>26.507661888284723</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="9"/>
-        <v>79</v>
+        <v>85.8</v>
       </c>
       <c r="M55" s="13">
         <f t="shared" si="10"/>
-        <v>15.784846547314578</v>
+        <v>17.14354219948849</v>
       </c>
       <c r="N55" s="13">
         <f t="shared" si="11"/>
-        <v>17.084775086505193</v>
+        <v>18.555363321799305</v>
       </c>
       <c r="O55" s="13">
         <f t="shared" si="12"/>
-        <v>14.522058823529413</v>
+        <v>15.772058823529409</v>
       </c>
       <c r="P55" s="14">
         <f t="shared" si="13"/>
-        <v>19.75</v>
+        <v>21.449999999999989</v>
       </c>
       <c r="Q55">
         <v>30</v>
@@ -7840,31 +8190,31 @@
       </c>
       <c r="J56" s="11">
         <f t="shared" si="7"/>
-        <v>11.135976129582266</v>
+        <v>12.947570332480817</v>
       </c>
       <c r="K56" s="12">
         <f t="shared" si="8"/>
-        <v>12.053056516724336</v>
+        <v>14.013840830449828</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" si="9"/>
-        <v>41.8</v>
+        <v>48.599999999999994</v>
       </c>
       <c r="M56" s="13">
         <f t="shared" si="10"/>
-        <v>8.3519820971866991</v>
+        <v>9.7106777493606113</v>
       </c>
       <c r="N56" s="13">
         <f t="shared" si="11"/>
-        <v>9.0397923875432511</v>
+        <v>10.510380622837371</v>
       </c>
       <c r="O56" s="13">
         <f t="shared" si="12"/>
-        <v>7.6838235294117636</v>
+        <v>8.9338235294117645</v>
       </c>
       <c r="P56" s="14">
         <f t="shared" si="13"/>
-        <v>10.449999999999996</v>
+        <v>12.150000000000006</v>
       </c>
       <c r="Q56">
         <v>30</v>
@@ -7900,31 +8250,31 @@
       </c>
       <c r="J57" s="11">
         <f t="shared" si="7"/>
-        <v>17.183503836317133</v>
+        <v>19.653859567542423</v>
       </c>
       <c r="K57" s="12">
         <f t="shared" si="8"/>
-        <v>18.598615916955012</v>
+        <v>21.272412708398864</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" si="9"/>
-        <v>47.3</v>
+        <v>54.099999999999994</v>
       </c>
       <c r="M57" s="13">
         <f t="shared" si="10"/>
-        <v>9.4509271099744243</v>
+        <v>10.809622762148335</v>
       </c>
       <c r="N57" s="13">
         <f t="shared" si="11"/>
-        <v>10.229238754325259</v>
+        <v>11.699826989619377</v>
       </c>
       <c r="O57" s="13">
         <f t="shared" si="12"/>
-        <v>8.6948529411764692</v>
+        <v>9.9448529411764692</v>
       </c>
       <c r="P57" s="14">
         <f t="shared" si="13"/>
-        <v>11.824999999999989</v>
+        <v>13.524999999999991</v>
       </c>
       <c r="Q57">
         <v>45</v>
@@ -7960,31 +8310,31 @@
       </c>
       <c r="J58" s="11">
         <f t="shared" si="7"/>
-        <v>22.644927536231886</v>
+        <v>24.909420289855071</v>
       </c>
       <c r="K58" s="12">
         <f t="shared" si="8"/>
-        <v>24.509803921568629</v>
+        <v>26.960784313725487</v>
       </c>
       <c r="L58" s="1">
         <f t="shared" si="9"/>
-        <v>68</v>
+        <v>74.8</v>
       </c>
       <c r="M58" s="13">
         <f t="shared" si="10"/>
-        <v>13.586956521739129</v>
+        <v>14.945652173913041</v>
       </c>
       <c r="N58" s="13">
         <f t="shared" si="11"/>
-        <v>14.705882352941178</v>
+        <v>16.176470588235293</v>
       </c>
       <c r="O58" s="13">
         <f t="shared" si="12"/>
-        <v>12.5</v>
+        <v>13.749999999999998</v>
       </c>
       <c r="P58" s="14">
         <f t="shared" si="13"/>
-        <v>17</v>
+        <v>18.699999999999989</v>
       </c>
       <c r="Q58">
         <v>0</v>
@@ -8019,32 +8369,32 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f>(E59+F59+($K$94*H59+$M$94)*$L$94)/(1-G59)/(1-$O$94)/(1-I59)/$N$94</f>
-        <v>13.70113262696383</v>
+        <f>(E59+F59+($K$100*H59+$M$100)*$L$100)/(1-G59)/(1-$O$100)/(1-I59)/$N$100</f>
+        <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f>(E59+F59+($K$94*H59+$M$94)*$L$94)/(1-G59)/(1-$P$94)/(1-I59)/$N$94</f>
-        <v>14.829461196243205</v>
+        <f>(E59+F59+($K$100*H59+$M$100)*$L$100)/(1-G59)/(1-$P$100)/(1-I59)/$N$100</f>
+        <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f>E59+F59+($K$94*H59+$M$94)*$L$94</f>
-        <v>48</v>
+        <f>E59+F59+($K$100*H59+$M$100)*$L$100</f>
+        <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f>L59/(1-G59)/(1-$O$94)/$N$94</f>
-        <v>9.5907928388746804</v>
+        <f>L59/(1-G59)/(1-$O$100)/$N$100</f>
+        <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f>L59/(1-G59)/(1-$P$94)/$N$94</f>
-        <v>10.380622837370243</v>
+        <f>L59/(1-G59)/(1-$P$100)/$N$100</f>
+        <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f>L59/(1-G59)/$N$94</f>
-        <v>8.8235294117647065</v>
+        <f>L59/(1-G59)/$N$100</f>
+        <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f>O59*$N$94-L59</f>
-        <v>12</v>
+        <f>O59*$N$100-L59</f>
+        <v>13.699999999999989</v>
       </c>
       <c r="Q59">
         <v>30</v>
@@ -8079,32 +8429,32 @@
         <v>0.3</v>
       </c>
       <c r="J60" s="11">
-        <f>(E60+F60+($K$94*H60+$M$94)*$L$94)/(1-G60)/(1-$O$94)/(1-I60)/$N$94</f>
-        <v>13.70113262696383</v>
+        <f>(E60+F60+($K$100*H60+$M$100)*$L$100)/(1-G60)/(1-$O$100)/(1-I60)/$N$100</f>
+        <v>15.642126415783704</v>
       </c>
       <c r="K60" s="12">
-        <f>(E60+F60+($K$94*H60+$M$94)*$L$94)/(1-G60)/(1-$P$94)/(1-I60)/$N$94</f>
-        <v>14.829461196243205</v>
+        <f>(E60+F60+($K$100*H60+$M$100)*$L$100)/(1-G60)/(1-$P$100)/(1-I60)/$N$100</f>
+        <v>16.930301532377655</v>
       </c>
       <c r="L60" s="1">
-        <f>E60+F60+($K$94*H60+$M$94)*$L$94</f>
-        <v>48</v>
+        <f>E60+F60+($K$100*H60+$M$100)*$L$100</f>
+        <v>54.8</v>
       </c>
       <c r="M60" s="13">
-        <f>L60/(1-G60)/(1-$O$94)/$N$94</f>
-        <v>9.5907928388746804</v>
+        <f>L60/(1-G60)/(1-$O$100)/$N$100</f>
+        <v>10.949488491048593</v>
       </c>
       <c r="N60" s="13">
-        <f>L60/(1-G60)/(1-$P$94)/$N$94</f>
-        <v>10.380622837370243</v>
+        <f>L60/(1-G60)/(1-$P$100)/$N$100</f>
+        <v>11.851211072664359</v>
       </c>
       <c r="O60" s="13">
-        <f>L60/(1-G60)/$N$94</f>
-        <v>8.8235294117647065</v>
+        <f>L60/(1-G60)/$N$100</f>
+        <v>10.073529411764705</v>
       </c>
       <c r="P60" s="14">
-        <f>O60*$N$94-L60</f>
-        <v>12</v>
+        <f>O60*$N$100-L60</f>
+        <v>13.699999999999989</v>
       </c>
       <c r="Q60">
         <v>30</v>
@@ -8139,32 +8489,32 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$94*H61+$M$94)*$L$94)/(1-G61)/(1-$O$94)/(1-I61)/$N$94</f>
-        <v>9.4975490196078418</v>
+        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$100*H61+$M$100)*$L$100)/(1-G61)/(1-$O$100)/(1-I61)/$N$100</f>
+        <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$94*H61+$M$94)*$L$94)/(1-G61)/(1-$P$94)/(1-I61)/$N$94</f>
-        <v>10.279700115340253</v>
+        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$100*H61+$M$100)*$L$100)/(1-G61)/(1-$P$100)/(1-I61)/$N$100</f>
+        <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$94*H61+$M$94)*$L$94</f>
-        <v>35.65</v>
+        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$100*H61+$M$100)*$L$100</f>
+        <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$94)/$N$94</f>
-        <v>7.1231617647058814</v>
+        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$100)/$N$100</f>
+        <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$94)/$N$94</f>
-        <v>7.7097750865051902</v>
+        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$100)/$N$100</f>
+        <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$94</f>
-        <v>6.5533088235294112</v>
+        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$100</f>
+        <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="20">O61*$N$94-L61</f>
-        <v>8.9124999999999943</v>
+        <f t="shared" ref="P61:P66" si="20">O61*$N$100-L61</f>
+        <v>10.612499999999997</v>
       </c>
       <c r="Q61">
         <v>25</v>
@@ -8200,31 +8550,31 @@
       </c>
       <c r="J62" s="11">
         <f t="shared" si="14"/>
-        <v>9.8039215686274517</v>
+        <v>11.736288718385904</v>
       </c>
       <c r="K62" s="12">
         <f t="shared" si="15"/>
-        <v>10.611303344867359</v>
+        <v>12.702806612841213</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" si="16"/>
-        <v>34.5</v>
+        <v>41.3</v>
       </c>
       <c r="M62" s="13">
         <f t="shared" si="17"/>
-        <v>7.3529411764705888</v>
+        <v>8.8022165387894287</v>
       </c>
       <c r="N62" s="13">
         <f t="shared" si="18"/>
-        <v>7.9584775086505193</v>
+        <v>9.5271049596309112</v>
       </c>
       <c r="O62" s="13">
         <f t="shared" si="19"/>
-        <v>6.7647058823529411</v>
+        <v>8.0980392156862742</v>
       </c>
       <c r="P62" s="14">
         <f t="shared" si="20"/>
-        <v>11.5</v>
+        <v>13.766666666666666</v>
       </c>
       <c r="Q62">
         <v>25</v>
@@ -8260,31 +8610,31 @@
       </c>
       <c r="J63" s="11">
         <f t="shared" si="14"/>
-        <v>12.254901960784315</v>
+        <v>14.670360897982381</v>
       </c>
       <c r="K63" s="12">
         <f t="shared" si="15"/>
-        <v>13.264129181084199</v>
+        <v>15.878508266051519</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" si="16"/>
-        <v>34.5</v>
+        <v>41.3</v>
       </c>
       <c r="M63" s="13">
         <f t="shared" si="17"/>
-        <v>7.3529411764705888</v>
+        <v>8.8022165387894287</v>
       </c>
       <c r="N63" s="13">
         <f t="shared" si="18"/>
-        <v>7.9584775086505193</v>
+        <v>9.5271049596309112</v>
       </c>
       <c r="O63" s="13">
         <f t="shared" si="19"/>
-        <v>6.7647058823529411</v>
+        <v>8.0980392156862742</v>
       </c>
       <c r="P63" s="14">
         <f t="shared" si="20"/>
-        <v>11.5</v>
+        <v>13.766666666666666</v>
       </c>
       <c r="Q63">
         <v>25</v>
@@ -8320,31 +8670,31 @@
       </c>
       <c r="J64" s="11">
         <f t="shared" si="14"/>
-        <v>13.586956521739129</v>
+        <v>15.398550724637678</v>
       </c>
       <c r="K64" s="12">
         <f t="shared" si="15"/>
-        <v>14.705882352941178</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="L64" s="1">
         <f t="shared" si="16"/>
-        <v>51</v>
+        <v>57.8</v>
       </c>
       <c r="M64" s="13">
         <f t="shared" si="17"/>
-        <v>10.190217391304348</v>
+        <v>11.548913043478258</v>
       </c>
       <c r="N64" s="13">
         <f t="shared" si="18"/>
-        <v>11.029411764705882</v>
+        <v>12.499999999999998</v>
       </c>
       <c r="O64" s="13">
         <f t="shared" si="19"/>
-        <v>9.375</v>
+        <v>10.624999999999998</v>
       </c>
       <c r="P64" s="14">
         <f t="shared" si="20"/>
-        <v>12.75</v>
+        <v>14.449999999999989</v>
       </c>
       <c r="Q64">
         <v>25</v>
@@ -8380,31 +8730,31 @@
       </c>
       <c r="J65" s="11">
         <f t="shared" si="14"/>
-        <v>14.219682438192669</v>
+        <v>16.484175191815854</v>
       </c>
       <c r="K65" s="12">
         <f t="shared" si="15"/>
-        <v>15.390715109573243</v>
+        <v>17.841695501730104</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" si="16"/>
-        <v>42.7</v>
+        <v>49.5</v>
       </c>
       <c r="M65" s="13">
         <f t="shared" si="17"/>
-        <v>8.5318094629156018</v>
+        <v>9.890505115089514</v>
       </c>
       <c r="N65" s="13">
         <f t="shared" si="18"/>
-        <v>9.2344290657439458</v>
+        <v>10.705017301038064</v>
       </c>
       <c r="O65" s="13">
         <f t="shared" si="19"/>
-        <v>7.8492647058823533</v>
+        <v>9.0992647058823533</v>
       </c>
       <c r="P65" s="14">
         <f t="shared" si="20"/>
-        <v>10.674999999999997</v>
+        <v>12.375</v>
       </c>
       <c r="Q65">
         <v>40</v>
@@ -8446,31 +8796,31 @@
       </c>
       <c r="J66" s="11">
         <f t="shared" si="14"/>
-        <v>18.325264888564124</v>
+        <v>20.266258677383998</v>
       </c>
       <c r="K66" s="12">
         <f t="shared" si="15"/>
-        <v>19.834404349975287</v>
+        <v>21.935244686109741</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" si="16"/>
-        <v>64.2</v>
+        <v>71</v>
       </c>
       <c r="M66" s="13">
         <f t="shared" si="17"/>
-        <v>12.827685421994886</v>
+        <v>14.186381074168798</v>
       </c>
       <c r="N66" s="13">
         <f t="shared" si="18"/>
-        <v>13.884083044982701</v>
+        <v>15.354671280276818</v>
       </c>
       <c r="O66" s="13">
         <f t="shared" si="19"/>
-        <v>11.801470588235295</v>
+        <v>13.051470588235295</v>
       </c>
       <c r="P66" s="14">
         <f t="shared" si="20"/>
-        <v>16.049999999999997</v>
+        <v>17.75</v>
       </c>
       <c r="Q66">
         <v>30</v>
@@ -8506,32 +8856,32 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f>(E67+F67+($K$94*H67+$M$94)*$L$94)/(1-G67)/(1-$O$94)/(1-I67)/$N$94</f>
-        <v>8.0456095481670928</v>
+        <f>(E67+F67+($K$100*H67+$M$100)*$L$100)/(1-G67)/(1-$O$100)/(1-I67)/$N$100</f>
+        <v>10.461068485365161</v>
       </c>
       <c r="K67" s="12">
-        <f>(E67+F67+($K$94*H67+$M$94)*$L$94)/(1-G67)/(1-$P$94)/(1-I67)/$N$94</f>
-        <v>8.7081891580161486</v>
+        <f>(E67+F67+($K$100*H67+$M$100)*$L$100)/(1-G67)/(1-$P$100)/(1-I67)/$N$100</f>
+        <v>11.322568242983468</v>
       </c>
       <c r="L67" s="1">
-        <f>E67+F67+($K$94*H67+$M$94)*$L$94</f>
-        <v>22.65</v>
+        <f>E67+F67+($K$100*H67+$M$100)*$L$100</f>
+        <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f>L67/(1-G67)/(1-$O$94)/$N$94</f>
-        <v>4.8273657289002552</v>
+        <f>L67/(1-G67)/(1-$O$100)/$N$100</f>
+        <v>6.276641091219096</v>
       </c>
       <c r="N67" s="13">
-        <f>L67/(1-G67)/(1-$P$94)/$N$94</f>
-        <v>5.2249134948096891</v>
+        <f>L67/(1-G67)/(1-$P$100)/$N$100</f>
+        <v>6.7935409457900811</v>
       </c>
       <c r="O67" s="13">
-        <f>L67/(1-G67)/$N$94</f>
-        <v>4.4411764705882355</v>
+        <f>L67/(1-G67)/$N$100</f>
+        <v>5.7745098039215685</v>
       </c>
       <c r="P67" s="14">
-        <f>O67*$N$94-L67</f>
-        <v>7.5500000000000007</v>
+        <f>O67*$N$100-L67</f>
+        <v>9.8166666666666664</v>
       </c>
       <c r="Q67">
         <v>25</v>
@@ -8567,32 +8917,32 @@
         <v>0.45</v>
       </c>
       <c r="J68" s="11">
-        <f>(E68+F68+($K$94*H68+$M$94)*$L$94)/(1-G68)/(1-$O$94)/(1-I68)/$N$94</f>
-        <v>11.160195303417808</v>
+        <f>(E68+F68+($K$100*H68+$M$100)*$L$100)/(1-G68)/(1-$O$100)/(1-I68)/$N$100</f>
+        <v>13.795241416724791</v>
       </c>
       <c r="K68" s="12">
-        <f>(E68+F68+($K$94*H68+$M$94)*$L$94)/(1-G68)/(1-$P$94)/(1-I68)/$N$94</f>
-        <v>12.0792702107581</v>
+        <f>(E68+F68+($K$100*H68+$M$100)*$L$100)/(1-G68)/(1-$P$100)/(1-I68)/$N$100</f>
+        <v>14.93132012163154</v>
       </c>
       <c r="L68" s="1">
-        <f>E68+F68+($K$94*H68+$M$94)*$L$94</f>
-        <v>28.8</v>
+        <f>E68+F68+($K$100*H68+$M$100)*$L$100</f>
+        <v>35.6</v>
       </c>
       <c r="M68" s="13">
-        <f>L68/(1-G68)/(1-$O$94)/$N$94</f>
-        <v>6.1381074168797944</v>
+        <f>L68/(1-G68)/(1-$O$100)/$N$100</f>
+        <v>7.5873827791986361</v>
       </c>
       <c r="N68" s="13">
-        <f>L68/(1-G68)/(1-$P$94)/$N$94</f>
-        <v>6.6435986159169556</v>
+        <f>L68/(1-G68)/(1-$P$100)/$N$100</f>
+        <v>8.2122260668973475</v>
       </c>
       <c r="O68" s="13">
-        <f>L68/(1-G68)/$N$94</f>
-        <v>5.6470588235294121</v>
+        <f>L68/(1-G68)/$N$100</f>
+        <v>6.9803921568627452</v>
       </c>
       <c r="P68" s="14">
-        <f>O68*$N$94-L68</f>
-        <v>9.5999999999999979</v>
+        <f>O68*$N$100-L68</f>
+        <v>11.866666666666667</v>
       </c>
       <c r="Q68">
         <v>45</v>
@@ -8628,32 +8978,32 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$94*H69+$M$94)*$L$94)/(1-G69)/(1-$O$94)/(1-I69)/$N$94</f>
-        <v>10.123614663256607</v>
+        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$100*H69+$M$100)*$L$100)/(1-G69)/(1-$O$100)/(1-I69)/$N$100</f>
+        <v>12.539073600454673</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$94*H69+$M$94)*$L$94)/(1-G69)/(1-$P$94)/(1-I69)/$N$94</f>
-        <v>10.957324106113035</v>
+        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$100*H69+$M$100)*$L$100)/(1-G69)/(1-$P$100)/(1-I69)/$N$100</f>
+        <v>13.571703191080355</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$94*H69+$M$94)*$L$94</f>
-        <v>28.5</v>
+        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$100*H69+$M$100)*$L$100</f>
+        <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$94)/$N$94</f>
-        <v>6.0741687979539636</v>
+        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$100)/$N$100</f>
+        <v>7.5234441602728035</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$94)/$N$94</f>
-        <v>6.5743944636678213</v>
+        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$100)/$N$100</f>
+        <v>8.1430219146482123</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$94</f>
-        <v>5.5882352941176476</v>
+        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$100</f>
+        <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P76" si="27">O69*$N$94-L69</f>
-        <v>9.5</v>
+        <f t="shared" ref="P69:P76" si="27">O69*$N$100-L69</f>
+        <v>11.766666666666666</v>
       </c>
       <c r="Q69">
         <v>25</v>
@@ -8690,31 +9040,31 @@
       </c>
       <c r="J70" s="11">
         <f t="shared" si="21"/>
-        <v>10.798522307473714</v>
+        <v>12.730889457232166</v>
       </c>
       <c r="K70" s="12">
         <f t="shared" si="22"/>
-        <v>11.687812379853902</v>
+        <v>13.779315647827758</v>
       </c>
       <c r="L70" s="1">
         <f t="shared" si="23"/>
-        <v>38</v>
+        <v>44.8</v>
       </c>
       <c r="M70" s="13">
         <f t="shared" si="24"/>
-        <v>8.0988917306052848</v>
+        <v>9.5481670929241247</v>
       </c>
       <c r="N70" s="13">
         <f t="shared" si="25"/>
-        <v>8.7658592848904267</v>
+        <v>10.334486735870819</v>
       </c>
       <c r="O70" s="13">
         <f t="shared" si="26"/>
-        <v>7.4509803921568629</v>
+        <v>8.7843137254901951</v>
       </c>
       <c r="P70" s="14">
         <f t="shared" si="27"/>
-        <v>12.666666666666664</v>
+        <v>14.93333333333333</v>
       </c>
       <c r="Q70">
         <v>40</v>
@@ -8751,31 +9101,31 @@
       </c>
       <c r="J71" s="11">
         <f t="shared" si="21"/>
-        <v>8.0420574026712135</v>
+        <v>9.9744245524296673</v>
       </c>
       <c r="K71" s="12">
         <f t="shared" si="22"/>
-        <v>8.704344482891198</v>
+        <v>10.795847750865054</v>
       </c>
       <c r="L71" s="1">
         <f t="shared" si="23"/>
-        <v>28.3</v>
+        <v>35.1</v>
       </c>
       <c r="M71" s="13">
         <f t="shared" si="24"/>
-        <v>6.0315430520034097</v>
+        <v>7.4808184143222505</v>
       </c>
       <c r="N71" s="13">
         <f t="shared" si="25"/>
-        <v>6.5282583621683976</v>
+        <v>8.0968858131487895</v>
       </c>
       <c r="O71" s="13">
         <f t="shared" si="26"/>
-        <v>5.549019607843138</v>
+        <v>6.882352941176471</v>
       </c>
       <c r="P71" s="14">
         <f t="shared" si="27"/>
-        <v>9.4333333333333336</v>
+        <v>11.700000000000003</v>
       </c>
       <c r="Q71">
         <v>25</v>
@@ -8812,31 +9162,31 @@
       </c>
       <c r="J72" s="11">
         <f t="shared" si="21"/>
-        <v>10.443307757885764</v>
+        <v>12.375674907644216</v>
       </c>
       <c r="K72" s="12">
         <f t="shared" si="22"/>
-        <v>11.303344867358708</v>
+        <v>13.394848135332564</v>
       </c>
       <c r="L72" s="1">
         <f t="shared" si="23"/>
-        <v>36.75</v>
+        <v>43.55</v>
       </c>
       <c r="M72" s="13">
         <f t="shared" si="24"/>
-        <v>7.8324808184143224</v>
+        <v>9.2817561807331614</v>
       </c>
       <c r="N72" s="13">
         <f t="shared" si="25"/>
-        <v>8.4775086505190309</v>
+        <v>10.046136101499423</v>
       </c>
       <c r="O72" s="13">
         <f t="shared" si="26"/>
-        <v>7.2058823529411766</v>
+        <v>8.5392156862745097</v>
       </c>
       <c r="P72" s="14">
         <f t="shared" si="27"/>
-        <v>12.25</v>
+        <v>14.516666666666666</v>
       </c>
       <c r="Q72">
         <v>40</v>
@@ -8873,31 +9223,31 @@
       </c>
       <c r="J73" s="11">
         <f t="shared" si="21"/>
-        <v>16.979255470304061</v>
+        <v>19.394714407502132</v>
       </c>
       <c r="K73" s="12">
         <f t="shared" si="22"/>
-        <v>18.377547097270277</v>
+        <v>20.991926182237602</v>
       </c>
       <c r="L73" s="1">
         <f t="shared" si="23"/>
-        <v>47.8</v>
+        <v>54.599999999999994</v>
       </c>
       <c r="M73" s="13">
         <f t="shared" si="24"/>
-        <v>10.187553282182437</v>
+        <v>11.636828644501279</v>
       </c>
       <c r="N73" s="13">
         <f t="shared" si="25"/>
-        <v>11.026528258362168</v>
+        <v>12.59515570934256</v>
       </c>
       <c r="O73" s="13">
         <f t="shared" si="26"/>
-        <v>9.3725490196078418</v>
+        <v>10.705882352941176</v>
       </c>
       <c r="P73" s="14">
         <f t="shared" si="27"/>
-        <v>15.933333333333323</v>
+        <v>18.200000000000003</v>
       </c>
       <c r="Q73">
         <v>40</v>
@@ -8936,31 +9286,31 @@
       </c>
       <c r="J74" s="11">
         <f t="shared" si="21"/>
-        <v>36.21523337595908</v>
+        <v>38.479726129582268</v>
       </c>
       <c r="K74" s="12">
         <f t="shared" si="22"/>
-        <v>39.197664359861598</v>
+        <v>41.648644752018463</v>
       </c>
       <c r="L74" s="1">
         <f t="shared" si="23"/>
-        <v>108.75</v>
+        <v>115.55000000000001</v>
       </c>
       <c r="M74" s="13">
         <f t="shared" si="24"/>
-        <v>21.729140025575447</v>
+        <v>23.087835677749361</v>
       </c>
       <c r="N74" s="13">
         <f t="shared" si="25"/>
-        <v>23.518598615916957</v>
+        <v>24.989186851211073</v>
       </c>
       <c r="O74" s="13">
         <f t="shared" si="26"/>
-        <v>19.990808823529413</v>
+        <v>21.240808823529413</v>
       </c>
       <c r="P74" s="14">
         <f t="shared" si="27"/>
-        <v>27.1875</v>
+        <v>28.887499999999989</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -8997,31 +9347,31 @@
       </c>
       <c r="J75" s="11">
         <f t="shared" si="21"/>
-        <v>14.919011082693943</v>
+        <v>17.183503836317129</v>
       </c>
       <c r="K75" s="12">
         <f t="shared" si="22"/>
-        <v>16.147635524798154</v>
+        <v>18.598615916955012</v>
       </c>
       <c r="L75" s="1">
         <f t="shared" si="23"/>
-        <v>44.8</v>
+        <v>51.599999999999994</v>
       </c>
       <c r="M75" s="13">
         <f t="shared" si="24"/>
-        <v>8.9514066496163665</v>
+        <v>10.310102301790279</v>
       </c>
       <c r="N75" s="13">
         <f t="shared" si="25"/>
-        <v>9.688581314878892</v>
+        <v>11.159169550173008</v>
       </c>
       <c r="O75" s="13">
         <f t="shared" si="26"/>
-        <v>8.235294117647058</v>
+        <v>9.4852941176470562</v>
       </c>
       <c r="P75" s="14">
         <f t="shared" si="27"/>
-        <v>11.199999999999996</v>
+        <v>12.899999999999991</v>
       </c>
       <c r="Q75">
         <v>25</v>
@@ -9058,31 +9408,31 @@
       </c>
       <c r="J76" s="11">
         <f t="shared" si="21"/>
-        <v>14.822134387351774</v>
+        <v>17.292490118577071</v>
       </c>
       <c r="K76" s="12">
         <f t="shared" si="22"/>
-        <v>16.042780748663098</v>
+        <v>18.71657754010695</v>
       </c>
       <c r="L76" s="1">
         <f t="shared" si="23"/>
-        <v>40.799999999999997</v>
+        <v>47.599999999999994</v>
       </c>
       <c r="M76" s="13">
         <f t="shared" si="24"/>
-        <v>8.1521739130434767</v>
+        <v>9.5108695652173907</v>
       </c>
       <c r="N76" s="13">
         <f t="shared" si="25"/>
-        <v>8.8235294117647047</v>
+        <v>10.294117647058824</v>
       </c>
       <c r="O76" s="13">
         <f t="shared" si="26"/>
-        <v>7.4999999999999991</v>
+        <v>8.75</v>
       </c>
       <c r="P76" s="14">
         <f t="shared" si="27"/>
-        <v>10.199999999999996</v>
+        <v>11.900000000000006</v>
       </c>
       <c r="Q76">
         <v>25</v>
@@ -9118,32 +9468,32 @@
         <v>0.25</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$94*H77+$M$94)*$L$94)/(1-G77)/(1-$O$94)/(1-I77)/$N$94</f>
-        <v>86.183930093776638</v>
+        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$100*H77+$M$100)*$L$100)/(1-G77)/(1-$O$100)/(1-I77)/$N$100</f>
+        <v>87.995524296675171</v>
       </c>
       <c r="K77" s="12">
-        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$94*H77+$M$94)*$L$94)/(1-G77)/(1-$P$94)/(1-I77)/$N$94</f>
-        <v>93.281430219146486</v>
+        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$100*H77+$M$100)*$L$100)/(1-G77)/(1-$P$100)/(1-I77)/$N$100</f>
+        <v>95.242214532871969</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$94*H77+$M$94)*$L$94</f>
-        <v>323.5</v>
+        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$100*H77+$M$100)*$L$100</f>
+        <v>330.29999999999995</v>
       </c>
       <c r="M77" s="13">
-        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$94)/$N$94</f>
-        <v>64.637947570332486</v>
+        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$100)/$N$100</f>
+        <v>65.996643222506378</v>
       </c>
       <c r="N77" s="13">
-        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$94)/$N$94</f>
-        <v>69.961072664359861</v>
+        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$100)/$N$100</f>
+        <v>71.431660899653977</v>
       </c>
       <c r="O77" s="13">
-        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$94</f>
-        <v>59.466911764705884</v>
+        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$100</f>
+        <v>60.716911764705877</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" ref="P77:P90" si="34">O77*$N$94-L77</f>
-        <v>80.875</v>
+        <f t="shared" ref="P77:P90" si="34">O77*$N$100-L77</f>
+        <v>82.574999999999989</v>
       </c>
       <c r="Q77">
         <v>0</v>
@@ -9180,31 +9530,31 @@
       </c>
       <c r="J78" s="11">
         <f t="shared" si="28"/>
-        <v>31.827223643080426</v>
+        <v>33.759590792838878</v>
       </c>
       <c r="K78" s="12">
         <f t="shared" si="29"/>
-        <v>34.448289119569402</v>
+        <v>36.539792387543258</v>
       </c>
       <c r="L78" s="1">
         <f t="shared" si="30"/>
-        <v>112</v>
+        <v>118.8</v>
       </c>
       <c r="M78" s="13">
         <f t="shared" si="31"/>
-        <v>23.870417732310319</v>
+        <v>25.319693094629155</v>
       </c>
       <c r="N78" s="13">
         <f t="shared" si="32"/>
-        <v>25.836216839677054</v>
+        <v>27.404844290657444</v>
       </c>
       <c r="O78" s="13">
         <f t="shared" si="33"/>
-        <v>21.960784313725494</v>
+        <v>23.294117647058826</v>
       </c>
       <c r="P78" s="14">
         <f t="shared" si="34"/>
-        <v>37.333333333333343</v>
+        <v>39.600000000000009</v>
       </c>
       <c r="Q78">
         <v>40</v>
@@ -9241,31 +9591,31 @@
       </c>
       <c r="J79" s="11">
         <f t="shared" si="28"/>
-        <v>25.225783248081843</v>
+        <v>27.490276001705027</v>
       </c>
       <c r="K79" s="12">
         <f t="shared" si="29"/>
-        <v>27.303200692041525</v>
+        <v>29.754181084198382</v>
       </c>
       <c r="L79" s="1">
         <f t="shared" si="30"/>
-        <v>75.75</v>
+        <v>82.55</v>
       </c>
       <c r="M79" s="13">
         <f t="shared" si="31"/>
-        <v>15.135469948849105</v>
+        <v>16.494165601023017</v>
       </c>
       <c r="N79" s="13">
         <f t="shared" si="32"/>
-        <v>16.381920415224915</v>
+        <v>17.852508650519027</v>
       </c>
       <c r="O79" s="13">
         <f t="shared" si="33"/>
-        <v>13.924632352941178</v>
+        <v>15.174632352941174</v>
       </c>
       <c r="P79" s="14">
         <f t="shared" si="34"/>
-        <v>18.9375</v>
+        <v>20.637499999999989</v>
       </c>
       <c r="Q79">
         <v>25</v>
@@ -9302,31 +9652,31 @@
       </c>
       <c r="J80" s="11">
         <f t="shared" si="28"/>
-        <v>10.656436487638532</v>
+        <v>13.291482600945512</v>
       </c>
       <c r="K80" s="12">
         <f t="shared" si="29"/>
-        <v>11.534025374855824</v>
+        <v>14.386075285729262</v>
       </c>
       <c r="L80" s="1">
         <f t="shared" si="30"/>
-        <v>27.5</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="M80" s="13">
         <f t="shared" si="31"/>
-        <v>5.8610400682011932</v>
+        <v>7.3103154305200322</v>
       </c>
       <c r="N80" s="13">
         <f t="shared" si="32"/>
-        <v>6.3437139561707028</v>
+        <v>7.9123414071510947</v>
       </c>
       <c r="O80" s="13">
         <f t="shared" si="33"/>
-        <v>5.3921568627450975</v>
+        <v>6.7254901960784306</v>
       </c>
       <c r="P80" s="14">
         <f t="shared" si="34"/>
-        <v>9.1666666666666643</v>
+        <v>11.43333333333333</v>
       </c>
       <c r="Q80">
         <v>40</v>
@@ -9336,7 +9686,7 @@
       </c>
       <c r="S80" s="19"/>
     </row>
-    <row r="81" spans="2:19" ht="90.75" customHeight="1">
+    <row r="81" spans="2:20" ht="90.75" customHeight="1">
       <c r="B81">
         <v>17022001</v>
       </c>
@@ -9363,31 +9713,31 @@
       </c>
       <c r="J81" s="11">
         <f t="shared" si="28"/>
-        <v>26.641091219096339</v>
+        <v>28.452685421994886</v>
       </c>
       <c r="K81" s="12">
         <f t="shared" si="29"/>
-        <v>28.835063437139564</v>
+        <v>30.79584775086505</v>
       </c>
       <c r="L81" s="1">
         <f t="shared" si="30"/>
-        <v>100</v>
+        <v>106.8</v>
       </c>
       <c r="M81" s="13">
         <f t="shared" si="31"/>
-        <v>19.98081841432225</v>
+        <v>21.339514066496164</v>
       </c>
       <c r="N81" s="13">
         <f t="shared" si="32"/>
-        <v>21.626297577854672</v>
+        <v>23.096885813148791</v>
       </c>
       <c r="O81" s="13">
         <f t="shared" si="33"/>
-        <v>18.382352941176471</v>
+        <v>19.632352941176471</v>
       </c>
       <c r="P81" s="14">
         <f t="shared" si="34"/>
-        <v>25</v>
+        <v>26.700000000000003</v>
       </c>
       <c r="Q81">
         <v>25</v>
@@ -9397,7 +9747,7 @@
       </c>
       <c r="S81" s="19"/>
     </row>
-    <row r="82" spans="2:19" ht="90.75" customHeight="1">
+    <row r="82" spans="2:20" ht="90.75" customHeight="1">
       <c r="B82">
         <v>17022201</v>
       </c>
@@ -9424,31 +9774,31 @@
       </c>
       <c r="J82" s="11">
         <f t="shared" si="28"/>
-        <v>15.585038363171353</v>
+        <v>17.396632566069901</v>
       </c>
       <c r="K82" s="12">
         <f t="shared" si="29"/>
-        <v>16.868512110726645</v>
+        <v>18.829296424452131</v>
       </c>
       <c r="L82" s="1">
         <f t="shared" si="30"/>
-        <v>58.5</v>
+        <v>65.3</v>
       </c>
       <c r="M82" s="13">
         <f t="shared" si="31"/>
-        <v>11.688778772378516</v>
+        <v>13.047474424552426</v>
       </c>
       <c r="N82" s="13">
         <f t="shared" si="32"/>
-        <v>12.651384083044983</v>
+        <v>14.121972318339099</v>
       </c>
       <c r="O82" s="13">
         <f t="shared" si="33"/>
-        <v>10.753676470588236</v>
+        <v>12.003676470588234</v>
       </c>
       <c r="P82" s="14">
         <f t="shared" si="34"/>
-        <v>14.625</v>
+        <v>16.324999999999989</v>
       </c>
       <c r="Q82">
         <v>25</v>
@@ -9458,7 +9808,7 @@
       </c>
       <c r="S82" s="19"/>
     </row>
-    <row r="83" spans="2:19" ht="90.75" customHeight="1">
+    <row r="83" spans="2:20" ht="90.75" customHeight="1">
       <c r="B83">
         <v>17022301</v>
       </c>
@@ -9485,31 +9835,31 @@
       </c>
       <c r="J83" s="11">
         <f t="shared" si="28"/>
-        <v>20.694419071976615</v>
+        <v>22.635412860796489</v>
       </c>
       <c r="K83" s="12">
         <f t="shared" si="29"/>
-        <v>22.39866534849234</v>
+        <v>24.499505684626794</v>
       </c>
       <c r="L83" s="1">
         <f t="shared" si="30"/>
-        <v>72.5</v>
+        <v>79.3</v>
       </c>
       <c r="M83" s="13">
         <f t="shared" si="31"/>
-        <v>14.486093350383632</v>
+        <v>15.844789002557542</v>
       </c>
       <c r="N83" s="13">
         <f t="shared" si="32"/>
-        <v>15.679065743944639</v>
+        <v>17.149653979238753</v>
       </c>
       <c r="O83" s="13">
         <f t="shared" si="33"/>
-        <v>13.327205882352942</v>
+        <v>14.57720588235294</v>
       </c>
       <c r="P83" s="14">
         <f t="shared" si="34"/>
-        <v>18.125</v>
+        <v>19.824999999999989</v>
       </c>
       <c r="Q83">
         <v>25</v>
@@ -9519,7 +9869,7 @@
       </c>
       <c r="S83" s="19"/>
     </row>
-    <row r="84" spans="2:19" ht="90.75" customHeight="1">
+    <row r="84" spans="2:20" ht="90.75" customHeight="1">
       <c r="B84">
         <v>17022401</v>
       </c>
@@ -9546,31 +9896,31 @@
       </c>
       <c r="J84" s="11">
         <f t="shared" si="28"/>
-        <v>12.627877237851663</v>
+        <v>15.043336175049729</v>
       </c>
       <c r="K84" s="12">
         <f t="shared" si="29"/>
-        <v>13.667820069204154</v>
+        <v>16.282199154171472</v>
       </c>
       <c r="L84" s="1">
         <f t="shared" si="30"/>
-        <v>35.549999999999997</v>
+        <v>42.349999999999994</v>
       </c>
       <c r="M84" s="13">
         <f t="shared" si="31"/>
-        <v>7.5767263427109972</v>
+        <v>9.026001705029838</v>
       </c>
       <c r="N84" s="13">
         <f t="shared" si="32"/>
-        <v>8.2006920415224922</v>
+        <v>9.7693194925028823</v>
       </c>
       <c r="O84" s="13">
         <f t="shared" si="33"/>
-        <v>6.9705882352941178</v>
+        <v>8.3039215686274499</v>
       </c>
       <c r="P84" s="14">
         <f t="shared" si="34"/>
-        <v>11.850000000000001</v>
+        <v>14.11666666666666</v>
       </c>
       <c r="Q84">
         <v>40</v>
@@ -9580,7 +9930,7 @@
       </c>
       <c r="S84" s="19"/>
     </row>
-    <row r="85" spans="2:19" ht="90.75" customHeight="1">
+    <row r="85" spans="2:20" ht="90.75" customHeight="1">
       <c r="B85">
         <v>17022501</v>
       </c>
@@ -9607,31 +9957,31 @@
       </c>
       <c r="J85" s="11">
         <f t="shared" si="28"/>
-        <v>17.4499147485081</v>
+        <v>19.261508951406647</v>
       </c>
       <c r="K85" s="12">
         <f t="shared" si="29"/>
-        <v>18.886966551326413</v>
+        <v>20.847750865051903</v>
       </c>
       <c r="L85" s="1">
         <f t="shared" si="30"/>
-        <v>65.5</v>
+        <v>72.3</v>
       </c>
       <c r="M85" s="13">
         <f t="shared" si="31"/>
-        <v>13.087436061381073</v>
+        <v>14.446131713554985</v>
       </c>
       <c r="N85" s="13">
         <f t="shared" si="32"/>
-        <v>14.165224913494811</v>
+        <v>15.635813148788927</v>
       </c>
       <c r="O85" s="13">
         <f t="shared" si="33"/>
-        <v>12.040441176470589</v>
+        <v>13.290441176470587</v>
       </c>
       <c r="P85" s="14">
         <f t="shared" si="34"/>
-        <v>16.375</v>
+        <v>18.074999999999989</v>
       </c>
       <c r="Q85">
         <v>25</v>
@@ -9641,7 +9991,7 @@
       </c>
       <c r="S85" s="19"/>
     </row>
-    <row r="86" spans="2:19" ht="90.75" customHeight="1">
+    <row r="86" spans="2:20" ht="90.75" customHeight="1">
       <c r="B86">
         <v>17022502</v>
       </c>
@@ -9668,31 +10018,31 @@
       </c>
       <c r="J86" s="11">
         <f t="shared" si="28"/>
-        <v>14.858974820791756</v>
+        <v>16.900207725466181</v>
       </c>
       <c r="K86" s="12">
         <f t="shared" si="29"/>
-        <v>16.082655100151079</v>
+        <v>18.291989538151636</v>
       </c>
       <c r="L86" s="1">
         <f t="shared" si="30"/>
-        <v>49.5</v>
+        <v>56.3</v>
       </c>
       <c r="M86" s="13">
         <f t="shared" si="31"/>
-        <v>11.144231115593817</v>
+        <v>12.675155794099638</v>
       </c>
       <c r="N86" s="13">
         <f t="shared" si="32"/>
-        <v>12.06199132511331</v>
+        <v>13.718992153613726</v>
       </c>
       <c r="O86" s="13">
         <f t="shared" si="33"/>
-        <v>10.252692626346313</v>
+        <v>11.661143330571667</v>
       </c>
       <c r="P86" s="14">
         <f t="shared" si="34"/>
-        <v>20.218309859154928</v>
+        <v>22.99577464788733</v>
       </c>
       <c r="Q86">
         <v>25</v>
@@ -9702,7 +10052,7 @@
       </c>
       <c r="S86" s="19"/>
     </row>
-    <row r="87" spans="2:19" ht="90.75" customHeight="1">
+    <row r="87" spans="2:20" ht="90.75" customHeight="1">
       <c r="B87">
         <v>17022503</v>
       </c>
@@ -9729,31 +10079,31 @@
       </c>
       <c r="J87" s="11">
         <f t="shared" si="28"/>
-        <v>7.1510297482837535</v>
+        <v>9.0579710144927521</v>
       </c>
       <c r="K87" s="12">
         <f t="shared" si="29"/>
-        <v>7.7399380804953557</v>
+        <v>9.8039215686274499</v>
       </c>
       <c r="L87" s="1">
         <f t="shared" si="30"/>
-        <v>25.5</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="M87" s="13">
         <f t="shared" si="31"/>
-        <v>5.3632723112128149</v>
+        <v>6.7934782608695636</v>
       </c>
       <c r="N87" s="13">
         <f t="shared" si="32"/>
-        <v>5.8049535603715174</v>
+        <v>7.352941176470587</v>
       </c>
       <c r="O87" s="13">
         <f t="shared" si="33"/>
-        <v>4.9342105263157894</v>
+        <v>6.2499999999999991</v>
       </c>
       <c r="P87" s="14">
         <f t="shared" si="34"/>
-        <v>8.0526315789473699</v>
+        <v>10.199999999999996</v>
       </c>
       <c r="Q87">
         <v>25</v>
@@ -9763,7 +10113,7 @@
       </c>
       <c r="S87" s="19"/>
     </row>
-    <row r="88" spans="2:19" ht="90.75" customHeight="1">
+    <row r="88" spans="2:20" ht="90.75" customHeight="1">
       <c r="B88">
         <v>17022504</v>
       </c>
@@ -9790,31 +10140,31 @@
       </c>
       <c r="J88" s="11">
         <f t="shared" si="28"/>
-        <v>4.9682034976152618</v>
+        <v>6.6002703470734163</v>
       </c>
       <c r="K88" s="12">
         <f t="shared" si="29"/>
-        <v>5.3773496680071071</v>
+        <v>7.1438220227147564</v>
       </c>
       <c r="L88" s="1">
         <f t="shared" si="30"/>
-        <v>20.7</v>
+        <v>27.5</v>
       </c>
       <c r="M88" s="13">
         <f t="shared" si="31"/>
-        <v>4.4713831478537358</v>
+        <v>5.9402433123660749</v>
       </c>
       <c r="N88" s="13">
         <f t="shared" si="32"/>
-        <v>4.8396147012063961</v>
+        <v>6.4294398204432808</v>
       </c>
       <c r="O88" s="13">
         <f t="shared" si="33"/>
-        <v>4.1136724960254369</v>
+        <v>5.4650238473767887</v>
       </c>
       <c r="P88" s="14">
         <f t="shared" si="34"/>
-        <v>7.2729729729729726</v>
+        <v>9.6621621621621614</v>
       </c>
       <c r="Q88">
         <v>0</v>
@@ -9824,7 +10174,7 @@
       </c>
       <c r="S88" s="19"/>
     </row>
-    <row r="89" spans="2:19" ht="90.75" customHeight="1">
+    <row r="89" spans="2:20" ht="90.75" customHeight="1">
       <c r="B89">
         <v>17022505</v>
       </c>
@@ -9851,31 +10201,31 @@
       </c>
       <c r="J89" s="11">
         <f t="shared" si="28"/>
-        <v>15.258079516391536</v>
+        <v>17.728435247616829</v>
       </c>
       <c r="K89" s="12">
         <f t="shared" si="29"/>
-        <v>16.514627241270841</v>
+        <v>19.188424032714686</v>
       </c>
       <c r="L89" s="1">
         <f t="shared" si="30"/>
-        <v>42</v>
+        <v>48.8</v>
       </c>
       <c r="M89" s="13">
         <f t="shared" si="31"/>
-        <v>8.3919437340153458</v>
+        <v>9.7506393861892562</v>
       </c>
       <c r="N89" s="13">
         <f t="shared" si="32"/>
-        <v>9.0830449826989614</v>
+        <v>10.553633217993077</v>
       </c>
       <c r="O89" s="13">
         <f t="shared" si="33"/>
-        <v>7.7205882352941178</v>
+        <v>8.970588235294116</v>
       </c>
       <c r="P89" s="14">
         <f t="shared" si="34"/>
-        <v>10.5</v>
+        <v>12.199999999999989</v>
       </c>
       <c r="Q89">
         <v>45</v>
@@ -9885,7 +10235,7 @@
       </c>
       <c r="S89" s="19"/>
     </row>
-    <row r="90" spans="2:19" ht="90.75" customHeight="1">
+    <row r="90" spans="2:20" ht="90.75" customHeight="1">
       <c r="B90">
         <v>17022506</v>
       </c>
@@ -9912,31 +10262,31 @@
       </c>
       <c r="J90" s="11">
         <f t="shared" si="28"/>
-        <v>5.2048279265939783</v>
+        <v>6.7303809395611802</v>
       </c>
       <c r="K90" s="12">
         <f t="shared" si="29"/>
-        <v>5.6334608146664236</v>
+        <v>7.2846476051721005</v>
       </c>
       <c r="L90" s="1">
         <f t="shared" si="30"/>
-        <v>23.2</v>
+        <v>30</v>
       </c>
       <c r="M90" s="13">
         <f t="shared" si="31"/>
-        <v>4.9445865302642797</v>
+        <v>6.3938618925831205</v>
       </c>
       <c r="N90" s="13">
         <f t="shared" si="32"/>
-        <v>5.3517877739331023</v>
+        <v>6.9204152249134951</v>
       </c>
       <c r="O90" s="13">
         <f t="shared" si="33"/>
-        <v>4.5490196078431371</v>
+        <v>5.882352941176471</v>
       </c>
       <c r="P90" s="14">
         <f t="shared" si="34"/>
-        <v>7.7333333333333307</v>
+        <v>10</v>
       </c>
       <c r="Q90">
         <v>0</v>
@@ -9946,7 +10296,7 @@
       </c>
       <c r="S90" s="19"/>
     </row>
-    <row r="91" spans="2:19" ht="90.75" customHeight="1">
+    <row r="91" spans="2:20" ht="90.75" customHeight="1">
       <c r="B91">
         <v>17022507</v>
       </c>
@@ -9972,32 +10322,32 @@
         <v>0.2</v>
       </c>
       <c r="J91" s="11">
-        <f t="shared" ref="J91" si="35">(E91+F91+($K$94*H91+$M$94)*$L$94)/(1-G91)/(1-$O$94)/(1-I91)/$N$94</f>
-        <v>4.9952046035805617</v>
+        <f t="shared" ref="J91" si="35">(E91+F91+($K$100*H91+$M$100)*$L$100)/(1-G91)/(1-$O$100)/(1-I91)/$N$100</f>
+        <v>6.9361983924004385</v>
       </c>
       <c r="K91" s="12">
-        <f t="shared" ref="K91" si="36">(E91+F91+($K$94*H91+$M$94)*$L$94)/(1-G91)/(1-$P$94)/(1-I91)/$N$94</f>
-        <v>5.4065743944636679</v>
+        <f t="shared" ref="K91" si="36">(E91+F91+($K$100*H91+$M$100)*$L$100)/(1-G91)/(1-$P$100)/(1-I91)/$N$100</f>
+        <v>7.5074147305981214</v>
       </c>
       <c r="L91" s="1">
-        <f t="shared" ref="L91" si="37">E91+F91+($K$94*H91+$M$94)*$L$94</f>
-        <v>17.5</v>
+        <f t="shared" ref="L91" si="37">E91+F91+($K$100*H91+$M$100)*$L$100</f>
+        <v>24.299999999999997</v>
       </c>
       <c r="M91" s="13">
-        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$94)/$N$94</f>
-        <v>3.99616368286445</v>
+        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$100)/$N$100</f>
+        <v>5.5489587139203511</v>
       </c>
       <c r="N91" s="13">
-        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$94)/$N$94</f>
-        <v>4.3252595155709344</v>
+        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$100)/$N$100</f>
+        <v>6.0059317844784976</v>
       </c>
       <c r="O91" s="13">
-        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$94</f>
-        <v>3.6764705882352944</v>
+        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$100</f>
+        <v>5.1050420168067232</v>
       </c>
       <c r="P91" s="14">
-        <f t="shared" ref="P91" si="41">O91*$N$94-L91</f>
-        <v>7.5</v>
+        <f t="shared" ref="P91" si="41">O91*$N$100-L91</f>
+        <v>10.414285714285718</v>
       </c>
       <c r="Q91">
         <v>0</v>
@@ -10007,52 +10357,422 @@
       </c>
       <c r="S91" s="19"/>
     </row>
-    <row r="92" spans="2:19">
-      <c r="G92" s="15"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="11"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="13"/>
-      <c r="O92" s="13"/>
-      <c r="P92" s="14"/>
+    <row r="92" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B92">
+        <v>17022601</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E92">
+        <v>34</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
+      <c r="G92" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H92">
+        <v>0.5</v>
+      </c>
+      <c r="I92" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J92" s="11">
+        <f t="shared" ref="J92" si="42">(E92+F92+($K$100*H92+$M$100)*$L$100)/(1-G92)/(1-$O$100)/(1-I92)/$N$100</f>
+        <v>24.239840863881785</v>
+      </c>
+      <c r="K92" s="12">
+        <f t="shared" ref="K92" si="43">(E92+F92+($K$100*H92+$M$100)*$L$100)/(1-G92)/(1-$P$100)/(1-I92)/$N$100</f>
+        <v>26.236063052672051</v>
+      </c>
+      <c r="L92" s="1">
+        <f t="shared" ref="L92" si="44">E92+F92+($K$100*H92+$M$100)*$L$100</f>
+        <v>85.3</v>
+      </c>
+      <c r="M92" s="13">
+        <f t="shared" ref="M92" si="45">L92/(1-G92)/(1-$O$100)/$N$100</f>
+        <v>18.17988064791134</v>
+      </c>
+      <c r="N92" s="13">
+        <f t="shared" ref="N92" si="46">L92/(1-G92)/(1-$P$100)/$N$100</f>
+        <v>19.677047289504038</v>
+      </c>
+      <c r="O92" s="13">
+        <f t="shared" ref="O92" si="47">L92/(1-G92)/$N$100</f>
+        <v>16.725490196078432</v>
+      </c>
+      <c r="P92" s="14">
+        <f t="shared" ref="P92" si="48">O92*$N$100-L92</f>
+        <v>28.433333333333337</v>
+      </c>
+      <c r="Q92">
+        <v>30</v>
+      </c>
+      <c r="R92">
+        <v>25</v>
+      </c>
+      <c r="S92" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="T92" s="20" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="93" spans="2:19">
-      <c r="K93" s="17" t="s">
+    <row r="93" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B93">
+        <v>17022602</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E93">
+        <v>20</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H93">
+        <v>0.1</v>
+      </c>
+      <c r="I93" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="J93" s="11">
+        <f t="shared" ref="J93" si="49">(E93+F93+($K$100*H93+$M$100)*$L$100)/(1-G93)/(1-$O$100)/(1-I93)/$N$100</f>
+        <v>11.356716599683351</v>
+      </c>
+      <c r="K93" s="12">
+        <f t="shared" ref="K93" si="50">(E93+F93+($K$100*H93+$M$100)*$L$100)/(1-G93)/(1-$P$100)/(1-I93)/$N$100</f>
+        <v>12.29197561377492</v>
+      </c>
+      <c r="L93" s="1">
+        <f t="shared" ref="L93" si="51">E93+F93+($K$100*H93+$M$100)*$L$100</f>
+        <v>37.299999999999997</v>
+      </c>
+      <c r="M93" s="13">
+        <f t="shared" ref="M93" si="52">L93/(1-G93)/(1-$O$100)/$N$100</f>
+        <v>7.9497016197783452</v>
+      </c>
+      <c r="N93" s="13">
+        <f t="shared" ref="N93" si="53">L93/(1-G93)/(1-$P$100)/$N$100</f>
+        <v>8.6043829296424441</v>
+      </c>
+      <c r="O93" s="13">
+        <f t="shared" ref="O93" si="54">L93/(1-G93)/$N$100</f>
+        <v>7.3137254901960773</v>
+      </c>
+      <c r="P93" s="14">
+        <f t="shared" ref="P93" si="55">O93*$N$100-L93</f>
+        <v>12.43333333333333</v>
+      </c>
+      <c r="Q93">
+        <v>40</v>
+      </c>
+      <c r="R93">
+        <v>30</v>
+      </c>
+      <c r="S93" s="19"/>
+      <c r="T93" s="20"/>
+    </row>
+    <row r="94" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B94">
+        <v>17022603</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E94">
+        <v>29</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H94">
+        <v>0.3</v>
+      </c>
+      <c r="I94" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J94" s="11">
+        <f t="shared" ref="J94" si="56">(E94+F94+($K$100*H94+$M$100)*$L$100)/(1-G94)/(1-$O$100)/(1-I94)/$N$100</f>
+        <v>20.74674978687127</v>
+      </c>
+      <c r="K94" s="12">
+        <f t="shared" ref="K94" si="57">(E94+F94+($K$100*H94+$M$100)*$L$100)/(1-G94)/(1-$P$100)/(1-I94)/$N$100</f>
+        <v>22.455305651672433</v>
+      </c>
+      <c r="L94" s="1">
+        <f t="shared" ref="L94" si="58">E94+F94+($K$100*H94+$M$100)*$L$100</f>
+        <v>62.3</v>
+      </c>
+      <c r="M94" s="13">
+        <f t="shared" ref="M94" si="59">L94/(1-G94)/(1-$O$100)/$N$100</f>
+        <v>12.448049872122761</v>
+      </c>
+      <c r="N94" s="13">
+        <f t="shared" ref="N94" si="60">L94/(1-G94)/(1-$P$100)/$N$100</f>
+        <v>13.47318339100346</v>
+      </c>
+      <c r="O94" s="13">
+        <f t="shared" ref="O94" si="61">L94/(1-G94)/$N$100</f>
+        <v>11.45220588235294</v>
+      </c>
+      <c r="P94" s="14">
+        <f t="shared" ref="P94" si="62">O94*$N$100-L94</f>
+        <v>15.574999999999989</v>
+      </c>
+      <c r="Q94">
+        <v>40</v>
+      </c>
+      <c r="R94">
+        <v>30</v>
+      </c>
+      <c r="S94" s="19"/>
+      <c r="T94" s="20"/>
+    </row>
+    <row r="95" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B95">
+        <v>17022604</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E95">
+        <v>30</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="G95" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H95">
+        <v>0.3</v>
+      </c>
+      <c r="I95" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J95" s="11">
+        <f t="shared" ref="J95" si="63">(E95+F95+($K$100*H95+$M$100)*$L$100)/(1-G95)/(1-$O$100)/(1-I95)/$N$100</f>
+        <v>17.988064791133844</v>
+      </c>
+      <c r="K95" s="12">
+        <f t="shared" ref="K95" si="64">(E95+F95+($K$100*H95+$M$100)*$L$100)/(1-G95)/(1-$P$100)/(1-I95)/$N$100</f>
+        <v>19.46943483275663</v>
+      </c>
+      <c r="L95" s="1">
+        <f t="shared" ref="L95" si="65">E95+F95+($K$100*H95+$M$100)*$L$100</f>
+        <v>63.3</v>
+      </c>
+      <c r="M95" s="13">
+        <f t="shared" ref="M95" si="66">L95/(1-G95)/(1-$O$100)/$N$100</f>
+        <v>13.491048593350381</v>
+      </c>
+      <c r="N95" s="13">
+        <f t="shared" ref="N95" si="67">L95/(1-G95)/(1-$P$100)/$N$100</f>
+        <v>14.602076124567473</v>
+      </c>
+      <c r="O95" s="13">
+        <f t="shared" ref="O95" si="68">L95/(1-G95)/$N$100</f>
+        <v>12.411764705882351</v>
+      </c>
+      <c r="P95" s="14">
+        <f t="shared" ref="P95" si="69">O95*$N$100-L95</f>
+        <v>21.099999999999994</v>
+      </c>
+      <c r="R95">
+        <v>25</v>
+      </c>
+      <c r="S95" s="19"/>
+      <c r="T95" s="20"/>
+    </row>
+    <row r="96" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B96">
+        <v>17022605</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E96">
+        <v>21</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H96">
+        <v>0.2</v>
+      </c>
+      <c r="I96" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="J96" s="11">
+        <f t="shared" ref="J96" si="70">(E96+F96+($K$100*H96+$M$100)*$L$100)/(1-G96)/(1-$O$100)/(1-I96)/$N$100</f>
+        <v>12.201619778346119</v>
+      </c>
+      <c r="K96" s="12">
+        <f t="shared" ref="K96" si="71">(E96+F96+($K$100*H96+$M$100)*$L$100)/(1-G96)/(1-$P$100)/(1-I96)/$N$100</f>
+        <v>13.206459054209919</v>
+      </c>
+      <c r="L96" s="1">
+        <f t="shared" ref="L96" si="72">E96+F96+($K$100*H96+$M$100)*$L$100</f>
+        <v>45.8</v>
+      </c>
+      <c r="M96" s="13">
+        <f t="shared" ref="M96" si="73">L96/(1-G96)/(1-$O$100)/$N$100</f>
+        <v>9.1512148337595889</v>
+      </c>
+      <c r="N96" s="13">
+        <f t="shared" ref="N96" si="74">L96/(1-G96)/(1-$P$100)/$N$100</f>
+        <v>9.9048442906574383</v>
+      </c>
+      <c r="O96" s="13">
+        <f t="shared" ref="O96" si="75">L96/(1-G96)/$N$100</f>
+        <v>8.4191176470588225</v>
+      </c>
+      <c r="P96" s="14">
+        <f t="shared" ref="P96" si="76">O96*$N$100-L96</f>
+        <v>11.449999999999996</v>
+      </c>
+      <c r="R96">
+        <v>25</v>
+      </c>
+      <c r="S96" s="19"/>
+      <c r="T96" s="20"/>
+    </row>
+    <row r="97" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B97">
+        <v>17022701</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E97">
+        <v>32</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H97">
+        <v>0.18</v>
+      </c>
+      <c r="I97" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="J97" s="11">
+        <f t="shared" ref="J97" si="77">(E97+F97+($K$100*H97+$M$100)*$L$100)/(1-G97)/(1-$O$100)/(1-I97)/$N$100</f>
+        <v>14.802596230307978</v>
+      </c>
+      <c r="K97" s="12">
+        <f t="shared" ref="K97" si="78">(E97+F97+($K$100*H97+$M$100)*$L$100)/(1-G97)/(1-$P$100)/(1-I97)/$N$100</f>
+        <v>16.021633566921576</v>
+      </c>
+      <c r="L97" s="1">
+        <f t="shared" ref="L97" si="79">E97+F97+($K$100*H97+$M$100)*$L$100</f>
+        <v>55.099999999999994</v>
+      </c>
+      <c r="M97" s="13">
+        <f t="shared" ref="M97" si="80">L97/(1-G97)/(1-$O$100)/$N$100</f>
+        <v>10.361817361215584</v>
+      </c>
+      <c r="N97" s="13">
+        <f t="shared" ref="N97" si="81">L97/(1-G97)/(1-$P$100)/$N$100</f>
+        <v>11.215143496845103</v>
+      </c>
+      <c r="O97" s="13">
+        <f t="shared" ref="O97" si="82">L97/(1-G97)/$N$100</f>
+        <v>9.5328719723183379</v>
+      </c>
+      <c r="P97" s="14">
+        <f t="shared" ref="P97" si="83">O97*$N$100-L97</f>
+        <v>9.7235294117647015</v>
+      </c>
+      <c r="Q97">
+        <v>30</v>
+      </c>
+      <c r="R97">
+        <v>25</v>
+      </c>
+      <c r="S97" s="19"/>
+      <c r="T97" s="20"/>
+    </row>
+    <row r="98" spans="2:20">
+      <c r="G98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="11"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="13"/>
+      <c r="O98" s="13"/>
+      <c r="P98" s="14"/>
+    </row>
+    <row r="99" spans="2:20">
+      <c r="K99" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L93" s="17" t="s">
+      <c r="L99" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="M93" s="17" t="s">
+      <c r="M99" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="N93" s="17" t="s">
+      <c r="N99" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="O93" s="17" t="s">
+      <c r="O99" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="P93" s="17" t="s">
+      <c r="P99" s="17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="94" spans="2:19">
-      <c r="K94" s="18">
+    <row r="100" spans="2:20">
+      <c r="K100" s="18">
         <v>100</v>
       </c>
-      <c r="L94" s="15">
+      <c r="L100" s="15">
         <v>0.85</v>
       </c>
-      <c r="M94">
-        <v>0</v>
-      </c>
-      <c r="N94">
+      <c r="M100">
+        <v>8</v>
+      </c>
+      <c r="N100">
         <v>6.8</v>
       </c>
-      <c r="O94" s="15">
+      <c r="O100" s="15">
         <v>0.08</v>
       </c>
-      <c r="P94" s="15">
+      <c r="P100" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -10062,7 +10782,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C91">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C97">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套,婴儿用品"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -10149,26 +10869,136 @@
     <hyperlink ref="D89" r:id="rId77"/>
     <hyperlink ref="D90" r:id="rId78"/>
     <hyperlink ref="D91" r:id="rId79"/>
+    <hyperlink ref="D92" r:id="rId80"/>
+    <hyperlink ref="D93" r:id="rId81"/>
+    <hyperlink ref="D94" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <drawing r:id="rId80"/>
+  <drawing r:id="rId83"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="A1:F8"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="72">
+      <c r="A1" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="22">
+        <v>100</v>
+      </c>
+      <c r="B2" s="22">
+        <v>44</v>
+      </c>
+      <c r="C2" s="22">
+        <v>66</v>
+      </c>
+      <c r="D2" s="22">
+        <v>44</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="22">
+        <v>110</v>
+      </c>
+      <c r="B3" s="22">
+        <v>47</v>
+      </c>
+      <c r="C3" s="22">
+        <v>70</v>
+      </c>
+      <c r="D3" s="22">
+        <v>47</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="22">
+        <v>120</v>
+      </c>
+      <c r="B4" s="22">
+        <v>50</v>
+      </c>
+      <c r="C4" s="22">
+        <v>76</v>
+      </c>
+      <c r="D4" s="22">
+        <v>52</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18">
+      <c r="A5" s="22">
+        <v>130</v>
+      </c>
+      <c r="B5" s="22">
+        <v>53</v>
+      </c>
+      <c r="C5" s="22">
+        <v>78</v>
+      </c>
+      <c r="D5" s="22">
+        <v>53</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17022802 boy vest by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="170">
   <si>
     <t>产品标题</t>
   </si>
@@ -412,12 +412,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>衣长</t>
-  </si>
-  <si>
-    <t>胸围</t>
-  </si>
-  <si>
     <t>https://detail.1688.com/offer/544047922082.html?spm=a261y.7663282.0.0.T2b6je&amp;sk=consign</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -425,34 +419,121 @@
     <t>https://detail.1688.com/offer/37031027317.html?spm=b26110380.sw1037192.0.0.LAWL4X</t>
   </si>
   <si>
-    <t>尺码</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>https://detail.1688.com/offer/536504597436.html?spm=a2615.7691456.0.0.rrHOhg</t>
   </si>
   <si>
-    <t>105cm</t>
-  </si>
-  <si>
-    <t>115cm</t>
-  </si>
-  <si>
-    <t>125cm</t>
-  </si>
-  <si>
-    <t>135cm</t>
-  </si>
-  <si>
-    <t>肩宽（肩点到袖口）</t>
-  </si>
-  <si>
-    <t>建议身高</t>
-  </si>
-  <si>
     <t>https://detail.1688.com/offer/533260101909.html?spm=a360q.7751291.0.0.0tLJft</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t> Dress length</t>
+  </si>
+  <si>
+    <t> Shoulder</t>
+  </si>
+  <si>
+    <t> Bust</t>
+  </si>
+  <si>
+    <t> Suggest Height</t>
+  </si>
+  <si>
+    <t> 86</t>
+  </si>
+  <si>
+    <t> 40cm</t>
+  </si>
+  <si>
+    <t> 19cm</t>
+  </si>
+  <si>
+    <t> 42cm</t>
+  </si>
+  <si>
+    <t> 80-85cm</t>
+  </si>
+  <si>
+    <t> 92</t>
+  </si>
+  <si>
+    <t> 45cm</t>
+  </si>
+  <si>
+    <t> 20cm</t>
+  </si>
+  <si>
+    <t> 46cm</t>
+  </si>
+  <si>
+    <t> 85-90cm</t>
+  </si>
+  <si>
+    <t> 98</t>
+  </si>
+  <si>
+    <t> 50cm</t>
+  </si>
+  <si>
+    <t> 21cm</t>
+  </si>
+  <si>
+    <t> 49cm</t>
+  </si>
+  <si>
+    <t> 90-95cm</t>
+  </si>
+  <si>
+    <t> 104</t>
+  </si>
+  <si>
+    <t> 53cm</t>
+  </si>
+  <si>
+    <t> 22cm</t>
+  </si>
+  <si>
+    <t> 52cm</t>
+  </si>
+  <si>
+    <t> 95-100cm</t>
+  </si>
+  <si>
+    <t> 110</t>
+  </si>
+  <si>
+    <t> 59cm</t>
+  </si>
+  <si>
+    <t> 23cm</t>
+  </si>
+  <si>
+    <t> 56cm</t>
+  </si>
+  <si>
+    <t> 100-110cm</t>
+  </si>
+  <si>
+    <t> 116</t>
+  </si>
+  <si>
+    <t> 64cm</t>
+  </si>
+  <si>
+    <t> 24cm</t>
+  </si>
+  <si>
+    <t> 60cm</t>
+  </si>
+  <si>
+    <t> 110-115cm</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/531314044561.html?spm=a2615.7691456.0.0.dxZKIY</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/43272851910.html?spm=a360q.7751291.0.0.q4HoxL</t>
   </si>
 </sst>
 </file>
@@ -465,7 +546,7 @@
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="\¥#,##0.00_);[Red]\(\¥#,##0.00\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,10 +612,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Tahoma"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -557,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -580,17 +667,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -603,7 +679,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -670,14 +746,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4568,6 +4641,82 @@
         <a:xfrm>
           <a:off x="66261" y="108278543"/>
           <a:ext cx="894521" cy="894521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>165653</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>157370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>969065</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>960782</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="图片 97" descr="QQ截图20170228212547.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId97" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="165653" y="109479522"/>
+          <a:ext cx="803412" cy="803412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57978</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>124240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>1017550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="99" name="图片 98" descr="QQ截图20170228231729.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId98" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57978" y="110597675"/>
+          <a:ext cx="894522" cy="893310"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4864,11 +5013,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T100"/>
+  <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
+      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4974,31 +5123,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$100*H2+$M$100)*$L$100)/(1-G2)/(1-$O$100)/(1-I2)/$N$100</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$102*H2+$M$102)*$L$102)/(1-G2)/(1-$O$102)/(1-I2)/$N$102</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f>(E2+F2+($K$100*H2+$M$100)*$L$100)/(1-G2)/(1-$P$100)/(1-I2)/$N$100</f>
+        <f>(E2+F2+($K$102*H2+$M$102)*$L$102)/(1-G2)/(1-$P$102)/(1-I2)/$N$102</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f>E2+F2+($K$100*H2+$M$100)*$L$100</f>
+        <f>E2+F2+($K$102*H2+$M$102)*$L$102</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f>L2/(1-G2)/(1-$O$100)/$N$100</f>
+        <f>L2/(1-G2)/(1-$O$102)/$N$102</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f>L2/(1-G2)/(1-$P$100)/$N$100</f>
+        <f>L2/(1-G2)/(1-$P$102)/$N$102</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$100</f>
+        <f>L2/(1-G2)/$N$102</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$100-L2</f>
+        <f>O2*$N$102-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -5039,27 +5188,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f>(E3+F3+($K$100*H3+$M$100)*$L$100)/(1-G3)/(1-$P$100)/(1-I3)/$N$100</f>
+        <f>(E3+F3+($K$102*H3+$M$102)*$L$102)/(1-G3)/(1-$P$102)/(1-I3)/$N$102</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f>E3+F3+($K$100*H3+$M$100)*$L$100</f>
+        <f>E3+F3+($K$102*H3+$M$102)*$L$102</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f>L3/(1-G3)/(1-$O$100)/$N$100</f>
+        <f>L3/(1-G3)/(1-$O$102)/$N$102</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f>L3/(1-G3)/(1-$P$100)/$N$100</f>
+        <f>L3/(1-G3)/(1-$P$102)/$N$102</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f>L3/(1-G3)/$N$100</f>
+        <f>L3/(1-G3)/$N$102</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f>O3*$N$100-L3</f>
+        <f>O3*$N$102-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -5100,27 +5249,27 @@
         <v>19.120691754962856</v>
       </c>
       <c r="K4" s="12">
-        <f>(E4+F4+($K$100*H4+$M$100)*$L$100)/(1-G4)/(1-$P$100)/(1-I4)/$N$100</f>
+        <f>(E4+F4+($K$102*H4+$M$102)*$L$102)/(1-G4)/(1-$P$102)/(1-I4)/$N$102</f>
         <v>20.69533695831274</v>
       </c>
       <c r="L4" s="1">
-        <f>E4+F4+($K$100*H4+$M$100)*$L$100</f>
+        <f>E4+F4+($K$102*H4+$M$102)*$L$102</f>
         <v>62.8</v>
       </c>
       <c r="M4" s="13">
-        <f>L4/(1-G4)/(1-$O$100)/$N$100</f>
+        <f>L4/(1-G4)/(1-$O$102)/$N$102</f>
         <v>13.384484228473999</v>
       </c>
       <c r="N4" s="13">
-        <f>L4/(1-G4)/(1-$P$100)/$N$100</f>
+        <f>L4/(1-G4)/(1-$P$102)/$N$102</f>
         <v>14.486735870818917</v>
       </c>
       <c r="O4" s="13">
-        <f>L4/(1-G4)/$N$100</f>
+        <f>L4/(1-G4)/$N$102</f>
         <v>12.313725490196079</v>
       </c>
       <c r="P4" s="14">
-        <f>O4*$N$100-L4</f>
+        <f>O4*$N$102-L4</f>
         <v>20.933333333333337</v>
       </c>
       <c r="Q4" s="1">
@@ -5161,27 +5310,27 @@
         <v>18.253848854119653</v>
       </c>
       <c r="K5" s="12">
-        <f>(E5+F5+($K$100*H5+$M$100)*$L$100)/(1-G5)/(1-$P$100)/(1-I5)/$N$100</f>
+        <f>(E5+F5+($K$102*H5+$M$102)*$L$102)/(1-G5)/(1-$P$102)/(1-I5)/$N$102</f>
         <v>19.757106995047156</v>
       </c>
       <c r="L5" s="1">
-        <f>E5+F5+($K$100*H5+$M$100)*$L$100</f>
+        <f>E5+F5+($K$102*H5+$M$102)*$L$102</f>
         <v>72.8</v>
       </c>
       <c r="M5" s="13">
-        <f>L5/(1-G5)/(1-$O$100)/$N$100</f>
+        <f>L5/(1-G5)/(1-$O$102)/$N$102</f>
         <v>15.515771526001704</v>
       </c>
       <c r="N5" s="13">
-        <f>L5/(1-G5)/(1-$P$100)/$N$100</f>
+        <f>L5/(1-G5)/(1-$P$102)/$N$102</f>
         <v>16.793540945790081</v>
       </c>
       <c r="O5" s="13">
-        <f>L5/(1-G5)/$N$100</f>
+        <f>L5/(1-G5)/$N$102</f>
         <v>14.274509803921568</v>
       </c>
       <c r="P5" s="14">
-        <f>O5*$N$100-L5</f>
+        <f>O5*$N$102-L5</f>
         <v>24.266666666666666</v>
       </c>
       <c r="Q5" s="1">
@@ -5222,27 +5371,27 @@
         <v>15.34996991123815</v>
       </c>
       <c r="K6" s="12">
-        <f>(E6+F6+($K$100*H6+$M$100)*$L$100)/(1-G6)/(1-$P$100)/(1-I6)/$N$100</f>
+        <f>(E6+F6+($K$102*H6+$M$102)*$L$102)/(1-G6)/(1-$P$102)/(1-I6)/$N$102</f>
         <v>16.61408508039894</v>
       </c>
       <c r="L6" s="1">
-        <f>E6+F6+($K$100*H6+$M$100)*$L$100</f>
+        <f>E6+F6+($K$102*H6+$M$102)*$L$102</f>
         <v>65.3</v>
       </c>
       <c r="M6" s="13">
-        <f>L6/(1-G6)/(1-$O$100)/$N$100</f>
+        <f>L6/(1-G6)/(1-$O$102)/$N$102</f>
         <v>13.047474424552426</v>
       </c>
       <c r="N6" s="13">
-        <f>L6/(1-G6)/(1-$P$100)/$N$100</f>
+        <f>L6/(1-G6)/(1-$P$102)/$N$102</f>
         <v>14.121972318339099</v>
       </c>
       <c r="O6" s="13">
-        <f>L6/(1-G6)/$N$100</f>
+        <f>L6/(1-G6)/$N$102</f>
         <v>12.003676470588234</v>
       </c>
       <c r="P6" s="14">
-        <f>O6*$N$100-L6</f>
+        <f>O6*$N$102-L6</f>
         <v>16.324999999999989</v>
       </c>
       <c r="Q6" s="1">
@@ -5286,27 +5435,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$100*H7+$M$100)*$L$100)/(1-G7)/(1-$P$100)/(1-I7)/$N$100</f>
+        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$102*H7+$M$102)*$L$102)/(1-G7)/(1-$P$102)/(1-I7)/$N$102</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$100*H7+$M$100)*$L$100</f>
+        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$102*H7+$M$102)*$L$102</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$102)/$N$102</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$102)/$N$102</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$100</f>
+        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$102</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="6">O7*$N$100-L7</f>
+        <f t="shared" ref="P7:P49" si="6">O7*$N$102-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -7826,31 +7975,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$100*H50+$M$100)*$L$100)/(1-G50)/(1-$O$100)/(1-I50)/$N$100</f>
+        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$102*H50+$M$102)*$L$102)/(1-G50)/(1-$O$102)/(1-I50)/$N$102</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$100*H50+$M$100)*$L$100)/(1-G50)/(1-$P$100)/(1-I50)/$N$100</f>
+        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$102*H50+$M$102)*$L$102)/(1-G50)/(1-$P$102)/(1-I50)/$N$102</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$100*H50+$M$100)*$L$100</f>
+        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$102*H50+$M$102)*$L$102</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$102)/$N$102</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$102)/$N$102</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$100</f>
+        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$102</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="13">O50*$N$100-L50</f>
+        <f t="shared" ref="P50:P58" si="13">O50*$N$102-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -8369,31 +8518,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f>(E59+F59+($K$100*H59+$M$100)*$L$100)/(1-G59)/(1-$O$100)/(1-I59)/$N$100</f>
+        <f>(E59+F59+($K$102*H59+$M$102)*$L$102)/(1-G59)/(1-$O$102)/(1-I59)/$N$102</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f>(E59+F59+($K$100*H59+$M$100)*$L$100)/(1-G59)/(1-$P$100)/(1-I59)/$N$100</f>
+        <f>(E59+F59+($K$102*H59+$M$102)*$L$102)/(1-G59)/(1-$P$102)/(1-I59)/$N$102</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f>E59+F59+($K$100*H59+$M$100)*$L$100</f>
+        <f>E59+F59+($K$102*H59+$M$102)*$L$102</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f>L59/(1-G59)/(1-$O$100)/$N$100</f>
+        <f>L59/(1-G59)/(1-$O$102)/$N$102</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f>L59/(1-G59)/(1-$P$100)/$N$100</f>
+        <f>L59/(1-G59)/(1-$P$102)/$N$102</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f>L59/(1-G59)/$N$100</f>
+        <f>L59/(1-G59)/$N$102</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f>O59*$N$100-L59</f>
+        <f>O59*$N$102-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -8429,31 +8578,31 @@
         <v>0.3</v>
       </c>
       <c r="J60" s="11">
-        <f>(E60+F60+($K$100*H60+$M$100)*$L$100)/(1-G60)/(1-$O$100)/(1-I60)/$N$100</f>
+        <f>(E60+F60+($K$102*H60+$M$102)*$L$102)/(1-G60)/(1-$O$102)/(1-I60)/$N$102</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K60" s="12">
-        <f>(E60+F60+($K$100*H60+$M$100)*$L$100)/(1-G60)/(1-$P$100)/(1-I60)/$N$100</f>
+        <f>(E60+F60+($K$102*H60+$M$102)*$L$102)/(1-G60)/(1-$P$102)/(1-I60)/$N$102</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L60" s="1">
-        <f>E60+F60+($K$100*H60+$M$100)*$L$100</f>
+        <f>E60+F60+($K$102*H60+$M$102)*$L$102</f>
         <v>54.8</v>
       </c>
       <c r="M60" s="13">
-        <f>L60/(1-G60)/(1-$O$100)/$N$100</f>
+        <f>L60/(1-G60)/(1-$O$102)/$N$102</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N60" s="13">
-        <f>L60/(1-G60)/(1-$P$100)/$N$100</f>
+        <f>L60/(1-G60)/(1-$P$102)/$N$102</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O60" s="13">
-        <f>L60/(1-G60)/$N$100</f>
+        <f>L60/(1-G60)/$N$102</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P60" s="14">
-        <f>O60*$N$100-L60</f>
+        <f>O60*$N$102-L60</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q60">
@@ -8489,31 +8638,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$100*H61+$M$100)*$L$100)/(1-G61)/(1-$O$100)/(1-I61)/$N$100</f>
+        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$102*H61+$M$102)*$L$102)/(1-G61)/(1-$O$102)/(1-I61)/$N$102</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$100*H61+$M$100)*$L$100)/(1-G61)/(1-$P$100)/(1-I61)/$N$100</f>
+        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$102*H61+$M$102)*$L$102)/(1-G61)/(1-$P$102)/(1-I61)/$N$102</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$100*H61+$M$100)*$L$100</f>
+        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$102*H61+$M$102)*$L$102</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$102)/$N$102</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$102)/$N$102</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$100</f>
+        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$102</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="20">O61*$N$100-L61</f>
+        <f t="shared" ref="P61:P66" si="20">O61*$N$102-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -8856,31 +9005,31 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f>(E67+F67+($K$100*H67+$M$100)*$L$100)/(1-G67)/(1-$O$100)/(1-I67)/$N$100</f>
+        <f>(E67+F67+($K$102*H67+$M$102)*$L$102)/(1-G67)/(1-$O$102)/(1-I67)/$N$102</f>
         <v>10.461068485365161</v>
       </c>
       <c r="K67" s="12">
-        <f>(E67+F67+($K$100*H67+$M$100)*$L$100)/(1-G67)/(1-$P$100)/(1-I67)/$N$100</f>
+        <f>(E67+F67+($K$102*H67+$M$102)*$L$102)/(1-G67)/(1-$P$102)/(1-I67)/$N$102</f>
         <v>11.322568242983468</v>
       </c>
       <c r="L67" s="1">
-        <f>E67+F67+($K$100*H67+$M$100)*$L$100</f>
+        <f>E67+F67+($K$102*H67+$M$102)*$L$102</f>
         <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f>L67/(1-G67)/(1-$O$100)/$N$100</f>
+        <f>L67/(1-G67)/(1-$O$102)/$N$102</f>
         <v>6.276641091219096</v>
       </c>
       <c r="N67" s="13">
-        <f>L67/(1-G67)/(1-$P$100)/$N$100</f>
+        <f>L67/(1-G67)/(1-$P$102)/$N$102</f>
         <v>6.7935409457900811</v>
       </c>
       <c r="O67" s="13">
-        <f>L67/(1-G67)/$N$100</f>
+        <f>L67/(1-G67)/$N$102</f>
         <v>5.7745098039215685</v>
       </c>
       <c r="P67" s="14">
-        <f>O67*$N$100-L67</f>
+        <f>O67*$N$102-L67</f>
         <v>9.8166666666666664</v>
       </c>
       <c r="Q67">
@@ -8917,31 +9066,31 @@
         <v>0.45</v>
       </c>
       <c r="J68" s="11">
-        <f>(E68+F68+($K$100*H68+$M$100)*$L$100)/(1-G68)/(1-$O$100)/(1-I68)/$N$100</f>
+        <f>(E68+F68+($K$102*H68+$M$102)*$L$102)/(1-G68)/(1-$O$102)/(1-I68)/$N$102</f>
         <v>13.795241416724791</v>
       </c>
       <c r="K68" s="12">
-        <f>(E68+F68+($K$100*H68+$M$100)*$L$100)/(1-G68)/(1-$P$100)/(1-I68)/$N$100</f>
+        <f>(E68+F68+($K$102*H68+$M$102)*$L$102)/(1-G68)/(1-$P$102)/(1-I68)/$N$102</f>
         <v>14.93132012163154</v>
       </c>
       <c r="L68" s="1">
-        <f>E68+F68+($K$100*H68+$M$100)*$L$100</f>
+        <f>E68+F68+($K$102*H68+$M$102)*$L$102</f>
         <v>35.6</v>
       </c>
       <c r="M68" s="13">
-        <f>L68/(1-G68)/(1-$O$100)/$N$100</f>
+        <f>L68/(1-G68)/(1-$O$102)/$N$102</f>
         <v>7.5873827791986361</v>
       </c>
       <c r="N68" s="13">
-        <f>L68/(1-G68)/(1-$P$100)/$N$100</f>
+        <f>L68/(1-G68)/(1-$P$102)/$N$102</f>
         <v>8.2122260668973475</v>
       </c>
       <c r="O68" s="13">
-        <f>L68/(1-G68)/$N$100</f>
+        <f>L68/(1-G68)/$N$102</f>
         <v>6.9803921568627452</v>
       </c>
       <c r="P68" s="14">
-        <f>O68*$N$100-L68</f>
+        <f>O68*$N$102-L68</f>
         <v>11.866666666666667</v>
       </c>
       <c r="Q68">
@@ -8978,31 +9127,31 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$100*H69+$M$100)*$L$100)/(1-G69)/(1-$O$100)/(1-I69)/$N$100</f>
+        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$102*H69+$M$102)*$L$102)/(1-G69)/(1-$O$102)/(1-I69)/$N$102</f>
         <v>12.539073600454673</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$100*H69+$M$100)*$L$100)/(1-G69)/(1-$P$100)/(1-I69)/$N$100</f>
+        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$102*H69+$M$102)*$L$102)/(1-G69)/(1-$P$102)/(1-I69)/$N$102</f>
         <v>13.571703191080355</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$100*H69+$M$100)*$L$100</f>
+        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$102*H69+$M$102)*$L$102</f>
         <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$102)/$N$102</f>
         <v>7.5234441602728035</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$102)/$N$102</f>
         <v>8.1430219146482123</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$100</f>
+        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$102</f>
         <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P76" si="27">O69*$N$100-L69</f>
+        <f t="shared" ref="P69:P76" si="27">O69*$N$102-L69</f>
         <v>11.766666666666666</v>
       </c>
       <c r="Q69">
@@ -9468,31 +9617,31 @@
         <v>0.25</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$100*H77+$M$100)*$L$100)/(1-G77)/(1-$O$100)/(1-I77)/$N$100</f>
+        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$102*H77+$M$102)*$L$102)/(1-G77)/(1-$O$102)/(1-I77)/$N$102</f>
         <v>87.995524296675171</v>
       </c>
       <c r="K77" s="12">
-        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$100*H77+$M$100)*$L$100)/(1-G77)/(1-$P$100)/(1-I77)/$N$100</f>
+        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$102*H77+$M$102)*$L$102)/(1-G77)/(1-$P$102)/(1-I77)/$N$102</f>
         <v>95.242214532871969</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$100*H77+$M$100)*$L$100</f>
+        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$102*H77+$M$102)*$L$102</f>
         <v>330.29999999999995</v>
       </c>
       <c r="M77" s="13">
-        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$102)/$N$102</f>
         <v>65.996643222506378</v>
       </c>
       <c r="N77" s="13">
-        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$102)/$N$102</f>
         <v>71.431660899653977</v>
       </c>
       <c r="O77" s="13">
-        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$100</f>
+        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$102</f>
         <v>60.716911764705877</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" ref="P77:P90" si="34">O77*$N$100-L77</f>
+        <f t="shared" ref="P77:P90" si="34">O77*$N$102-L77</f>
         <v>82.574999999999989</v>
       </c>
       <c r="Q77">
@@ -10322,31 +10471,31 @@
         <v>0.2</v>
       </c>
       <c r="J91" s="11">
-        <f t="shared" ref="J91" si="35">(E91+F91+($K$100*H91+$M$100)*$L$100)/(1-G91)/(1-$O$100)/(1-I91)/$N$100</f>
+        <f t="shared" ref="J91" si="35">(E91+F91+($K$102*H91+$M$102)*$L$102)/(1-G91)/(1-$O$102)/(1-I91)/$N$102</f>
         <v>6.9361983924004385</v>
       </c>
       <c r="K91" s="12">
-        <f t="shared" ref="K91" si="36">(E91+F91+($K$100*H91+$M$100)*$L$100)/(1-G91)/(1-$P$100)/(1-I91)/$N$100</f>
+        <f t="shared" ref="K91" si="36">(E91+F91+($K$102*H91+$M$102)*$L$102)/(1-G91)/(1-$P$102)/(1-I91)/$N$102</f>
         <v>7.5074147305981214</v>
       </c>
       <c r="L91" s="1">
-        <f t="shared" ref="L91" si="37">E91+F91+($K$100*H91+$M$100)*$L$100</f>
+        <f t="shared" ref="L91" si="37">E91+F91+($K$102*H91+$M$102)*$L$102</f>
         <v>24.299999999999997</v>
       </c>
       <c r="M91" s="13">
-        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$102)/$N$102</f>
         <v>5.5489587139203511</v>
       </c>
       <c r="N91" s="13">
-        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$102)/$N$102</f>
         <v>6.0059317844784976</v>
       </c>
       <c r="O91" s="13">
-        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$100</f>
+        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$102</f>
         <v>5.1050420168067232</v>
       </c>
       <c r="P91" s="14">
-        <f t="shared" ref="P91" si="41">O91*$N$100-L91</f>
+        <f t="shared" ref="P91" si="41">O91*$N$102-L91</f>
         <v>10.414285714285718</v>
       </c>
       <c r="Q91">
@@ -10383,31 +10532,31 @@
         <v>0.25</v>
       </c>
       <c r="J92" s="11">
-        <f t="shared" ref="J92" si="42">(E92+F92+($K$100*H92+$M$100)*$L$100)/(1-G92)/(1-$O$100)/(1-I92)/$N$100</f>
+        <f t="shared" ref="J92" si="42">(E92+F92+($K$102*H92+$M$102)*$L$102)/(1-G92)/(1-$O$102)/(1-I92)/$N$102</f>
         <v>24.239840863881785</v>
       </c>
       <c r="K92" s="12">
-        <f t="shared" ref="K92" si="43">(E92+F92+($K$100*H92+$M$100)*$L$100)/(1-G92)/(1-$P$100)/(1-I92)/$N$100</f>
+        <f t="shared" ref="K92" si="43">(E92+F92+($K$102*H92+$M$102)*$L$102)/(1-G92)/(1-$P$102)/(1-I92)/$N$102</f>
         <v>26.236063052672051</v>
       </c>
       <c r="L92" s="1">
-        <f t="shared" ref="L92" si="44">E92+F92+($K$100*H92+$M$100)*$L$100</f>
+        <f t="shared" ref="L92" si="44">E92+F92+($K$102*H92+$M$102)*$L$102</f>
         <v>85.3</v>
       </c>
       <c r="M92" s="13">
-        <f t="shared" ref="M92" si="45">L92/(1-G92)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M92" si="45">L92/(1-G92)/(1-$O$102)/$N$102</f>
         <v>18.17988064791134</v>
       </c>
       <c r="N92" s="13">
-        <f t="shared" ref="N92" si="46">L92/(1-G92)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N92" si="46">L92/(1-G92)/(1-$P$102)/$N$102</f>
         <v>19.677047289504038</v>
       </c>
       <c r="O92" s="13">
-        <f t="shared" ref="O92" si="47">L92/(1-G92)/$N$100</f>
+        <f t="shared" ref="O92" si="47">L92/(1-G92)/$N$102</f>
         <v>16.725490196078432</v>
       </c>
       <c r="P92" s="14">
-        <f t="shared" ref="P92" si="48">O92*$N$100-L92</f>
+        <f t="shared" ref="P92" si="48">O92*$N$102-L92</f>
         <v>28.433333333333337</v>
       </c>
       <c r="Q92">
@@ -10449,31 +10598,31 @@
         <v>0.3</v>
       </c>
       <c r="J93" s="11">
-        <f t="shared" ref="J93" si="49">(E93+F93+($K$100*H93+$M$100)*$L$100)/(1-G93)/(1-$O$100)/(1-I93)/$N$100</f>
+        <f t="shared" ref="J93" si="49">(E93+F93+($K$102*H93+$M$102)*$L$102)/(1-G93)/(1-$O$102)/(1-I93)/$N$102</f>
         <v>11.356716599683351</v>
       </c>
       <c r="K93" s="12">
-        <f t="shared" ref="K93" si="50">(E93+F93+($K$100*H93+$M$100)*$L$100)/(1-G93)/(1-$P$100)/(1-I93)/$N$100</f>
+        <f t="shared" ref="K93" si="50">(E93+F93+($K$102*H93+$M$102)*$L$102)/(1-G93)/(1-$P$102)/(1-I93)/$N$102</f>
         <v>12.29197561377492</v>
       </c>
       <c r="L93" s="1">
-        <f t="shared" ref="L93" si="51">E93+F93+($K$100*H93+$M$100)*$L$100</f>
+        <f t="shared" ref="L93" si="51">E93+F93+($K$102*H93+$M$102)*$L$102</f>
         <v>37.299999999999997</v>
       </c>
       <c r="M93" s="13">
-        <f t="shared" ref="M93" si="52">L93/(1-G93)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M93" si="52">L93/(1-G93)/(1-$O$102)/$N$102</f>
         <v>7.9497016197783452</v>
       </c>
       <c r="N93" s="13">
-        <f t="shared" ref="N93" si="53">L93/(1-G93)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N93" si="53">L93/(1-G93)/(1-$P$102)/$N$102</f>
         <v>8.6043829296424441</v>
       </c>
       <c r="O93" s="13">
-        <f t="shared" ref="O93" si="54">L93/(1-G93)/$N$100</f>
+        <f t="shared" ref="O93" si="54">L93/(1-G93)/$N$102</f>
         <v>7.3137254901960773</v>
       </c>
       <c r="P93" s="14">
-        <f t="shared" ref="P93" si="55">O93*$N$100-L93</f>
+        <f t="shared" ref="P93" si="55">O93*$N$102-L93</f>
         <v>12.43333333333333</v>
       </c>
       <c r="Q93">
@@ -10493,7 +10642,7 @@
         <v>28</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E94">
         <v>29</v>
@@ -10511,31 +10660,31 @@
         <v>0.4</v>
       </c>
       <c r="J94" s="11">
-        <f t="shared" ref="J94" si="56">(E94+F94+($K$100*H94+$M$100)*$L$100)/(1-G94)/(1-$O$100)/(1-I94)/$N$100</f>
+        <f t="shared" ref="J94" si="56">(E94+F94+($K$102*H94+$M$102)*$L$102)/(1-G94)/(1-$O$102)/(1-I94)/$N$102</f>
         <v>20.74674978687127</v>
       </c>
       <c r="K94" s="12">
-        <f t="shared" ref="K94" si="57">(E94+F94+($K$100*H94+$M$100)*$L$100)/(1-G94)/(1-$P$100)/(1-I94)/$N$100</f>
+        <f t="shared" ref="K94" si="57">(E94+F94+($K$102*H94+$M$102)*$L$102)/(1-G94)/(1-$P$102)/(1-I94)/$N$102</f>
         <v>22.455305651672433</v>
       </c>
       <c r="L94" s="1">
-        <f t="shared" ref="L94" si="58">E94+F94+($K$100*H94+$M$100)*$L$100</f>
+        <f t="shared" ref="L94" si="58">E94+F94+($K$102*H94+$M$102)*$L$102</f>
         <v>62.3</v>
       </c>
       <c r="M94" s="13">
-        <f t="shared" ref="M94" si="59">L94/(1-G94)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M94" si="59">L94/(1-G94)/(1-$O$102)/$N$102</f>
         <v>12.448049872122761</v>
       </c>
       <c r="N94" s="13">
-        <f t="shared" ref="N94" si="60">L94/(1-G94)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N94" si="60">L94/(1-G94)/(1-$P$102)/$N$102</f>
         <v>13.47318339100346</v>
       </c>
       <c r="O94" s="13">
-        <f t="shared" ref="O94" si="61">L94/(1-G94)/$N$100</f>
+        <f t="shared" ref="O94" si="61">L94/(1-G94)/$N$102</f>
         <v>11.45220588235294</v>
       </c>
       <c r="P94" s="14">
-        <f t="shared" ref="P94" si="62">O94*$N$100-L94</f>
+        <f t="shared" ref="P94" si="62">O94*$N$102-L94</f>
         <v>15.574999999999989</v>
       </c>
       <c r="Q94">
@@ -10555,7 +10704,7 @@
         <v>28</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E95">
         <v>30</v>
@@ -10573,31 +10722,31 @@
         <v>0.25</v>
       </c>
       <c r="J95" s="11">
-        <f t="shared" ref="J95" si="63">(E95+F95+($K$100*H95+$M$100)*$L$100)/(1-G95)/(1-$O$100)/(1-I95)/$N$100</f>
+        <f t="shared" ref="J95" si="63">(E95+F95+($K$102*H95+$M$102)*$L$102)/(1-G95)/(1-$O$102)/(1-I95)/$N$102</f>
         <v>17.988064791133844</v>
       </c>
       <c r="K95" s="12">
-        <f t="shared" ref="K95" si="64">(E95+F95+($K$100*H95+$M$100)*$L$100)/(1-G95)/(1-$P$100)/(1-I95)/$N$100</f>
+        <f t="shared" ref="K95" si="64">(E95+F95+($K$102*H95+$M$102)*$L$102)/(1-G95)/(1-$P$102)/(1-I95)/$N$102</f>
         <v>19.46943483275663</v>
       </c>
       <c r="L95" s="1">
-        <f t="shared" ref="L95" si="65">E95+F95+($K$100*H95+$M$100)*$L$100</f>
+        <f t="shared" ref="L95" si="65">E95+F95+($K$102*H95+$M$102)*$L$102</f>
         <v>63.3</v>
       </c>
       <c r="M95" s="13">
-        <f t="shared" ref="M95" si="66">L95/(1-G95)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M95" si="66">L95/(1-G95)/(1-$O$102)/$N$102</f>
         <v>13.491048593350381</v>
       </c>
       <c r="N95" s="13">
-        <f t="shared" ref="N95" si="67">L95/(1-G95)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N95" si="67">L95/(1-G95)/(1-$P$102)/$N$102</f>
         <v>14.602076124567473</v>
       </c>
       <c r="O95" s="13">
-        <f t="shared" ref="O95" si="68">L95/(1-G95)/$N$100</f>
+        <f t="shared" ref="O95" si="68">L95/(1-G95)/$N$102</f>
         <v>12.411764705882351</v>
       </c>
       <c r="P95" s="14">
-        <f t="shared" ref="P95" si="69">O95*$N$100-L95</f>
+        <f t="shared" ref="P95" si="69">O95*$N$102-L95</f>
         <v>21.099999999999994</v>
       </c>
       <c r="R95">
@@ -10614,7 +10763,7 @@
         <v>28</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E96">
         <v>21</v>
@@ -10632,31 +10781,31 @@
         <v>0.25</v>
       </c>
       <c r="J96" s="11">
-        <f t="shared" ref="J96" si="70">(E96+F96+($K$100*H96+$M$100)*$L$100)/(1-G96)/(1-$O$100)/(1-I96)/$N$100</f>
+        <f t="shared" ref="J96" si="70">(E96+F96+($K$102*H96+$M$102)*$L$102)/(1-G96)/(1-$O$102)/(1-I96)/$N$102</f>
         <v>12.201619778346119</v>
       </c>
       <c r="K96" s="12">
-        <f t="shared" ref="K96" si="71">(E96+F96+($K$100*H96+$M$100)*$L$100)/(1-G96)/(1-$P$100)/(1-I96)/$N$100</f>
+        <f t="shared" ref="K96" si="71">(E96+F96+($K$102*H96+$M$102)*$L$102)/(1-G96)/(1-$P$102)/(1-I96)/$N$102</f>
         <v>13.206459054209919</v>
       </c>
       <c r="L96" s="1">
-        <f t="shared" ref="L96" si="72">E96+F96+($K$100*H96+$M$100)*$L$100</f>
+        <f t="shared" ref="L96" si="72">E96+F96+($K$102*H96+$M$102)*$L$102</f>
         <v>45.8</v>
       </c>
       <c r="M96" s="13">
-        <f t="shared" ref="M96" si="73">L96/(1-G96)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M96" si="73">L96/(1-G96)/(1-$O$102)/$N$102</f>
         <v>9.1512148337595889</v>
       </c>
       <c r="N96" s="13">
-        <f t="shared" ref="N96" si="74">L96/(1-G96)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N96" si="74">L96/(1-G96)/(1-$P$102)/$N$102</f>
         <v>9.9048442906574383</v>
       </c>
       <c r="O96" s="13">
-        <f t="shared" ref="O96" si="75">L96/(1-G96)/$N$100</f>
+        <f t="shared" ref="O96" si="75">L96/(1-G96)/$N$102</f>
         <v>8.4191176470588225</v>
       </c>
       <c r="P96" s="14">
-        <f t="shared" ref="P96" si="76">O96*$N$100-L96</f>
+        <f t="shared" ref="P96" si="76">O96*$N$102-L96</f>
         <v>11.449999999999996</v>
       </c>
       <c r="R96">
@@ -10673,7 +10822,7 @@
         <v>21</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="E97">
         <v>32</v>
@@ -10691,31 +10840,31 @@
         <v>0.3</v>
       </c>
       <c r="J97" s="11">
-        <f t="shared" ref="J97" si="77">(E97+F97+($K$100*H97+$M$100)*$L$100)/(1-G97)/(1-$O$100)/(1-I97)/$N$100</f>
+        <f t="shared" ref="J97" si="77">(E97+F97+($K$102*H97+$M$102)*$L$102)/(1-G97)/(1-$O$102)/(1-I97)/$N$102</f>
         <v>14.802596230307978</v>
       </c>
       <c r="K97" s="12">
-        <f t="shared" ref="K97" si="78">(E97+F97+($K$100*H97+$M$100)*$L$100)/(1-G97)/(1-$P$100)/(1-I97)/$N$100</f>
+        <f t="shared" ref="K97" si="78">(E97+F97+($K$102*H97+$M$102)*$L$102)/(1-G97)/(1-$P$102)/(1-I97)/$N$102</f>
         <v>16.021633566921576</v>
       </c>
       <c r="L97" s="1">
-        <f t="shared" ref="L97" si="79">E97+F97+($K$100*H97+$M$100)*$L$100</f>
+        <f t="shared" ref="L97" si="79">E97+F97+($K$102*H97+$M$102)*$L$102</f>
         <v>55.099999999999994</v>
       </c>
       <c r="M97" s="13">
-        <f t="shared" ref="M97" si="80">L97/(1-G97)/(1-$O$100)/$N$100</f>
+        <f t="shared" ref="M97" si="80">L97/(1-G97)/(1-$O$102)/$N$102</f>
         <v>10.361817361215584</v>
       </c>
       <c r="N97" s="13">
-        <f t="shared" ref="N97" si="81">L97/(1-G97)/(1-$P$100)/$N$100</f>
+        <f t="shared" ref="N97" si="81">L97/(1-G97)/(1-$P$102)/$N$102</f>
         <v>11.215143496845103</v>
       </c>
       <c r="O97" s="13">
-        <f t="shared" ref="O97" si="82">L97/(1-G97)/$N$100</f>
+        <f t="shared" ref="O97" si="82">L97/(1-G97)/$N$102</f>
         <v>9.5328719723183379</v>
       </c>
       <c r="P97" s="14">
-        <f t="shared" ref="P97" si="83">O97*$N$100-L97</f>
+        <f t="shared" ref="P97" si="83">O97*$N$102-L97</f>
         <v>9.7235294117647015</v>
       </c>
       <c r="Q97">
@@ -10727,52 +10876,176 @@
       <c r="S97" s="19"/>
       <c r="T97" s="20"/>
     </row>
-    <row r="98" spans="2:20">
-      <c r="G98" s="15"/>
-      <c r="I98" s="15"/>
-      <c r="J98" s="11"/>
-      <c r="L98" s="1"/>
-      <c r="M98" s="13"/>
-      <c r="O98" s="13"/>
-      <c r="P98" s="14"/>
+    <row r="98" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B98">
+        <v>17022801</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E98">
+        <v>20</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H98">
+        <v>0.15</v>
+      </c>
+      <c r="I98" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J98" s="11">
+        <f t="shared" ref="J98" si="84">(E98+F98+($K$102*H98+$M$102)*$L$102)/(1-G98)/(1-$O$102)/(1-I98)/$N$102</f>
+        <v>13.503703111679453</v>
+      </c>
+      <c r="K98" s="12">
+        <f t="shared" ref="K98" si="85">(E98+F98+($K$102*H98+$M$102)*$L$102)/(1-G98)/(1-$P$102)/(1-I98)/$N$102</f>
+        <v>14.615772779700114</v>
+      </c>
+      <c r="L98" s="1">
+        <f t="shared" ref="L98" si="86">E98+F98+($K$102*H98+$M$102)*$L$102</f>
+        <v>40.549999999999997</v>
+      </c>
+      <c r="M98" s="13">
+        <f t="shared" ref="M98" si="87">L98/(1-G98)/(1-$O$102)/$N$102</f>
+        <v>8.1022218670076711</v>
+      </c>
+      <c r="N98" s="13">
+        <f t="shared" ref="N98" si="88">L98/(1-G98)/(1-$P$102)/$N$102</f>
+        <v>8.7694636678200677</v>
+      </c>
+      <c r="O98" s="13">
+        <f t="shared" ref="O98" si="89">L98/(1-G98)/$N$102</f>
+        <v>7.454044117647058</v>
+      </c>
+      <c r="P98" s="14">
+        <f t="shared" ref="P98" si="90">O98*$N$102-L98</f>
+        <v>10.137499999999996</v>
+      </c>
+      <c r="Q98">
+        <v>40</v>
+      </c>
+      <c r="R98">
+        <v>30</v>
+      </c>
+      <c r="S98" s="19"/>
+      <c r="T98" s="20"/>
     </row>
-    <row r="99" spans="2:20">
-      <c r="K99" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="L99" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="M99" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="N99" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="O99" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="P99" s="17" t="s">
-        <v>121</v>
-      </c>
+    <row r="99" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B99">
+        <v>17022802</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E99">
+        <v>31</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="G99" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H99">
+        <v>0.2</v>
+      </c>
+      <c r="I99" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="J99" s="11">
+        <f t="shared" ref="J99" si="91">(E99+F99+($K$102*H99+$M$102)*$L$102)/(1-G99)/(1-$O$102)/(1-I99)/$N$102</f>
+        <v>18.58216112531969</v>
+      </c>
+      <c r="K99" s="12">
+        <f t="shared" ref="K99" si="92">(E99+F99+($K$102*H99+$M$102)*$L$102)/(1-G99)/(1-$P$102)/(1-I99)/$N$102</f>
+        <v>20.112456747404842</v>
+      </c>
+      <c r="L99" s="1">
+        <f t="shared" ref="L99" si="93">E99+F99+($K$102*H99+$M$102)*$L$102</f>
+        <v>55.8</v>
+      </c>
+      <c r="M99" s="13">
+        <f t="shared" ref="M99" si="94">L99/(1-G99)/(1-$O$102)/$N$102</f>
+        <v>11.149296675191813</v>
+      </c>
+      <c r="N99" s="13">
+        <f t="shared" ref="N99" si="95">L99/(1-G99)/(1-$P$102)/$N$102</f>
+        <v>12.067474048442905</v>
+      </c>
+      <c r="O99" s="13">
+        <f t="shared" ref="O99" si="96">L99/(1-G99)/$N$102</f>
+        <v>10.257352941176469</v>
+      </c>
+      <c r="P99" s="14">
+        <f t="shared" ref="P99" si="97">O99*$N$102-L99</f>
+        <v>13.949999999999989</v>
+      </c>
+      <c r="Q99">
+        <v>40</v>
+      </c>
+      <c r="R99">
+        <v>30</v>
+      </c>
+      <c r="S99" s="19"/>
+      <c r="T99" s="20"/>
     </row>
     <row r="100" spans="2:20">
-      <c r="K100" s="18">
+      <c r="G100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="11"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="13"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="14"/>
+    </row>
+    <row r="101" spans="2:20">
+      <c r="K101" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="L101" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="M101" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="N101" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="O101" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="P101" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="102" spans="2:20">
+      <c r="K102" s="18">
         <v>100</v>
       </c>
-      <c r="L100" s="15">
+      <c r="L102" s="15">
         <v>0.85</v>
       </c>
-      <c r="M100">
+      <c r="M102">
         <v>8</v>
       </c>
-      <c r="N100">
+      <c r="N102">
         <v>6.8</v>
       </c>
-      <c r="O100" s="15">
+      <c r="O102" s="15">
         <v>0.08</v>
       </c>
-      <c r="P100" s="15">
+      <c r="P102" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -10782,7 +11055,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C97">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C99">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套,婴儿用品"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">
@@ -10881,119 +11154,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="72">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>134</v>
-      </c>
+      <c r="E2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="22"/>
     </row>
-    <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="22">
-        <v>100</v>
-      </c>
-      <c r="B2" s="22">
-        <v>44</v>
-      </c>
-      <c r="C2" s="22">
-        <v>66</v>
-      </c>
-      <c r="D2" s="22">
-        <v>44</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>134</v>
-      </c>
+    <row r="3" spans="1:6">
+      <c r="A3" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="18">
-      <c r="A3" s="22">
-        <v>110</v>
-      </c>
-      <c r="B3" s="22">
-        <v>47</v>
-      </c>
-      <c r="C3" s="22">
-        <v>70</v>
-      </c>
-      <c r="D3" s="22">
-        <v>47</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>134</v>
-      </c>
+    <row r="4" spans="1:6">
+      <c r="A4" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="18">
-      <c r="A4" s="22">
-        <v>120</v>
-      </c>
-      <c r="B4" s="22">
-        <v>50</v>
-      </c>
-      <c r="C4" s="22">
-        <v>76</v>
-      </c>
-      <c r="D4" s="22">
-        <v>52</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="22">
-        <v>130</v>
-      </c>
-      <c r="B5" s="22">
-        <v>53</v>
-      </c>
-      <c r="C5" s="22">
-        <v>78</v>
-      </c>
-      <c r="D5" s="22">
-        <v>53</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="24"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>162</v>
+      </c>
       <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -11012,6 +11304,6 @@
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17030102 floral jacket by hjx
</commit_message>
<xml_diff>
--- a/产品表单.xlsx
+++ b/产品表单.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="171">
   <si>
     <t>产品标题</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>https://detail.1688.com/offer/43272851910.html?spm=a360q.7751291.0.0.q4HoxL</t>
+  </si>
+  <si>
+    <t>https://detail.1688.com/offer/528987127575.html?spm=a360q.7751291.0.0.l321Vu</t>
   </si>
 </sst>
 </file>
@@ -4717,6 +4720,44 @@
         <a:xfrm>
           <a:off x="57978" y="110597675"/>
           <a:ext cx="894522" cy="893310"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>149086</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>165653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>869673</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>881358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="100" name="图片 99" descr="QQ截图20170301222925.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId99" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="149086" y="111790370"/>
+          <a:ext cx="720587" cy="715705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5013,11 +5054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5123,31 +5164,31 @@
         <v>0.15</v>
       </c>
       <c r="J2" s="11">
-        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$102*H2+$M$102)*$L$102)/(1-G2)/(1-$O$102)/(1-I2)/$N$102</f>
+        <f t="shared" ref="J2:J49" si="0">(E2+F2+($K$103*H2+$M$103)*$L$103)/(1-G2)/(1-$O$103)/(1-I2)/$N$103</f>
         <v>16.874780602778195</v>
       </c>
       <c r="K2" s="12">
-        <f>(E2+F2+($K$102*H2+$M$102)*$L$102)/(1-G2)/(1-$P$102)/(1-I2)/$N$102</f>
+        <f>(E2+F2+($K$103*H2+$M$103)*$L$103)/(1-G2)/(1-$P$103)/(1-I2)/$N$103</f>
         <v>18.26446841712464</v>
       </c>
       <c r="L2" s="1">
-        <f>E2+F2+($K$102*H2+$M$102)*$L$102</f>
+        <f>E2+F2+($K$103*H2+$M$103)*$L$103</f>
         <v>67.3</v>
       </c>
       <c r="M2" s="13">
-        <f>L2/(1-G2)/(1-$O$102)/$N$102</f>
+        <f>L2/(1-G2)/(1-$O$103)/$N$103</f>
         <v>14.343563512361467</v>
       </c>
       <c r="N2" s="13">
-        <f>L2/(1-G2)/(1-$P$102)/$N$102</f>
+        <f>L2/(1-G2)/(1-$P$103)/$N$103</f>
         <v>15.524798154555942</v>
       </c>
       <c r="O2" s="13">
-        <f>L2/(1-G2)/$N$102</f>
+        <f>L2/(1-G2)/$N$103</f>
         <v>13.19607843137255</v>
       </c>
       <c r="P2" s="14">
-        <f>O2*$N$102-L2</f>
+        <f>O2*$N$103-L2</f>
         <v>22.433333333333337</v>
       </c>
       <c r="Q2" s="1">
@@ -5188,27 +5229,27 @@
         <v>11.025859619210001</v>
       </c>
       <c r="K3" s="12">
-        <f>(E3+F3+($K$102*H3+$M$102)*$L$102)/(1-G3)/(1-$P$102)/(1-I3)/$N$102</f>
+        <f>(E3+F3+($K$103*H3+$M$103)*$L$103)/(1-G3)/(1-$P$103)/(1-I3)/$N$103</f>
         <v>11.933871587850826</v>
       </c>
       <c r="L3" s="1">
-        <f>E3+F3+($K$102*H3+$M$102)*$L$102</f>
+        <f>E3+F3+($K$103*H3+$M$103)*$L$103</f>
         <v>38.799999999999997</v>
       </c>
       <c r="M3" s="13">
-        <f>L3/(1-G3)/(1-$O$102)/$N$102</f>
+        <f>L3/(1-G3)/(1-$O$103)/$N$103</f>
         <v>8.2693947144075022</v>
       </c>
       <c r="N3" s="13">
-        <f>L3/(1-G3)/(1-$P$102)/$N$102</f>
+        <f>L3/(1-G3)/(1-$P$103)/$N$103</f>
         <v>8.9504036908881197</v>
       </c>
       <c r="O3" s="13">
-        <f>L3/(1-G3)/$N$102</f>
+        <f>L3/(1-G3)/$N$103</f>
         <v>7.6078431372549016</v>
       </c>
       <c r="P3" s="14">
-        <f>O3*$N$102-L3</f>
+        <f>O3*$N$103-L3</f>
         <v>12.93333333333333</v>
       </c>
       <c r="Q3" s="1">
@@ -5249,27 +5290,27 @@
         <v>19.120691754962856</v>
       </c>
       <c r="K4" s="12">
-        <f>(E4+F4+($K$102*H4+$M$102)*$L$102)/(1-G4)/(1-$P$102)/(1-I4)/$N$102</f>
+        <f>(E4+F4+($K$103*H4+$M$103)*$L$103)/(1-G4)/(1-$P$103)/(1-I4)/$N$103</f>
         <v>20.69533695831274</v>
       </c>
       <c r="L4" s="1">
-        <f>E4+F4+($K$102*H4+$M$102)*$L$102</f>
+        <f>E4+F4+($K$103*H4+$M$103)*$L$103</f>
         <v>62.8</v>
       </c>
       <c r="M4" s="13">
-        <f>L4/(1-G4)/(1-$O$102)/$N$102</f>
+        <f>L4/(1-G4)/(1-$O$103)/$N$103</f>
         <v>13.384484228473999</v>
       </c>
       <c r="N4" s="13">
-        <f>L4/(1-G4)/(1-$P$102)/$N$102</f>
+        <f>L4/(1-G4)/(1-$P$103)/$N$103</f>
         <v>14.486735870818917</v>
       </c>
       <c r="O4" s="13">
-        <f>L4/(1-G4)/$N$102</f>
+        <f>L4/(1-G4)/$N$103</f>
         <v>12.313725490196079</v>
       </c>
       <c r="P4" s="14">
-        <f>O4*$N$102-L4</f>
+        <f>O4*$N$103-L4</f>
         <v>20.933333333333337</v>
       </c>
       <c r="Q4" s="1">
@@ -5310,27 +5351,27 @@
         <v>18.253848854119653</v>
       </c>
       <c r="K5" s="12">
-        <f>(E5+F5+($K$102*H5+$M$102)*$L$102)/(1-G5)/(1-$P$102)/(1-I5)/$N$102</f>
+        <f>(E5+F5+($K$103*H5+$M$103)*$L$103)/(1-G5)/(1-$P$103)/(1-I5)/$N$103</f>
         <v>19.757106995047156</v>
       </c>
       <c r="L5" s="1">
-        <f>E5+F5+($K$102*H5+$M$102)*$L$102</f>
+        <f>E5+F5+($K$103*H5+$M$103)*$L$103</f>
         <v>72.8</v>
       </c>
       <c r="M5" s="13">
-        <f>L5/(1-G5)/(1-$O$102)/$N$102</f>
+        <f>L5/(1-G5)/(1-$O$103)/$N$103</f>
         <v>15.515771526001704</v>
       </c>
       <c r="N5" s="13">
-        <f>L5/(1-G5)/(1-$P$102)/$N$102</f>
+        <f>L5/(1-G5)/(1-$P$103)/$N$103</f>
         <v>16.793540945790081</v>
       </c>
       <c r="O5" s="13">
-        <f>L5/(1-G5)/$N$102</f>
+        <f>L5/(1-G5)/$N$103</f>
         <v>14.274509803921568</v>
       </c>
       <c r="P5" s="14">
-        <f>O5*$N$102-L5</f>
+        <f>O5*$N$103-L5</f>
         <v>24.266666666666666</v>
       </c>
       <c r="Q5" s="1">
@@ -5371,27 +5412,27 @@
         <v>15.34996991123815</v>
       </c>
       <c r="K6" s="12">
-        <f>(E6+F6+($K$102*H6+$M$102)*$L$102)/(1-G6)/(1-$P$102)/(1-I6)/$N$102</f>
+        <f>(E6+F6+($K$103*H6+$M$103)*$L$103)/(1-G6)/(1-$P$103)/(1-I6)/$N$103</f>
         <v>16.61408508039894</v>
       </c>
       <c r="L6" s="1">
-        <f>E6+F6+($K$102*H6+$M$102)*$L$102</f>
+        <f>E6+F6+($K$103*H6+$M$103)*$L$103</f>
         <v>65.3</v>
       </c>
       <c r="M6" s="13">
-        <f>L6/(1-G6)/(1-$O$102)/$N$102</f>
+        <f>L6/(1-G6)/(1-$O$103)/$N$103</f>
         <v>13.047474424552426</v>
       </c>
       <c r="N6" s="13">
-        <f>L6/(1-G6)/(1-$P$102)/$N$102</f>
+        <f>L6/(1-G6)/(1-$P$103)/$N$103</f>
         <v>14.121972318339099</v>
       </c>
       <c r="O6" s="13">
-        <f>L6/(1-G6)/$N$102</f>
+        <f>L6/(1-G6)/$N$103</f>
         <v>12.003676470588234</v>
       </c>
       <c r="P6" s="14">
-        <f>O6*$N$102-L6</f>
+        <f>O6*$N$103-L6</f>
         <v>16.324999999999989</v>
       </c>
       <c r="Q6" s="1">
@@ -5435,27 +5476,27 @@
         <v>17.250890125871322</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$102*H7+$M$102)*$L$102)/(1-G7)/(1-$P$102)/(1-I7)/$N$102</f>
+        <f t="shared" ref="K7:K49" si="1">(E7+F7+($K$103*H7+$M$103)*$L$103)/(1-G7)/(1-$P$103)/(1-I7)/$N$103</f>
         <v>18.671551665648959</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$102*H7+$M$102)*$L$102</f>
+        <f t="shared" ref="L7:L49" si="2">E7+F7+($K$103*H7+$M$103)*$L$103</f>
         <v>68.8</v>
       </c>
       <c r="M7" s="13">
-        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M7:M49" si="3">L7/(1-G7)/(1-$O$103)/$N$103</f>
         <v>14.663256606990624</v>
       </c>
       <c r="N7" s="13">
-        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N7:N49" si="4">L7/(1-G7)/(1-$P$103)/$N$103</f>
         <v>15.870818915801616</v>
       </c>
       <c r="O7" s="13">
-        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$102</f>
+        <f t="shared" ref="O7:O49" si="5">L7/(1-G7)/$N$103</f>
         <v>13.490196078431373</v>
       </c>
       <c r="P7" s="14">
-        <f t="shared" ref="P7:P49" si="6">O7*$N$102-L7</f>
+        <f t="shared" ref="P7:P49" si="6">O7*$N$103-L7</f>
         <v>22.933333333333337</v>
       </c>
       <c r="Q7" s="1">
@@ -7975,31 +8016,31 @@
         <v>0.45</v>
       </c>
       <c r="J50" s="11">
-        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$102*H50+$M$102)*$L$102)/(1-G50)/(1-$O$102)/(1-I50)/$N$102</f>
+        <f t="shared" ref="J50:J58" si="7">(E50+F50+($K$103*H50+$M$103)*$L$103)/(1-G50)/(1-$O$103)/(1-I50)/$N$103</f>
         <v>17.069673719290083</v>
       </c>
       <c r="K50" s="12">
-        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$102*H50+$M$102)*$L$102)/(1-G50)/(1-$P$102)/(1-I50)/$N$102</f>
+        <f t="shared" ref="K50:K58" si="8">(E50+F50+($K$103*H50+$M$103)*$L$103)/(1-G50)/(1-$P$103)/(1-I50)/$N$103</f>
         <v>18.475411554996327</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$102*H50+$M$102)*$L$102</f>
+        <f t="shared" ref="L50:L58" si="9">E50+F50+($K$103*H50+$M$103)*$L$103</f>
         <v>44.05</v>
       </c>
       <c r="M50" s="13">
-        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M50:M58" si="10">L50/(1-G50)/(1-$O$103)/$N$103</f>
         <v>9.3883205456095471</v>
       </c>
       <c r="N50" s="13">
-        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N50:N58" si="11">L50/(1-G50)/(1-$P$103)/$N$103</f>
         <v>10.161476355247981</v>
       </c>
       <c r="O50" s="13">
-        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$102</f>
+        <f t="shared" ref="O50:O58" si="12">L50/(1-G50)/$N$103</f>
         <v>8.6372549019607838</v>
       </c>
       <c r="P50" s="14">
-        <f t="shared" ref="P50:P58" si="13">O50*$N$102-L50</f>
+        <f t="shared" ref="P50:P58" si="13">O50*$N$103-L50</f>
         <v>14.68333333333333</v>
       </c>
       <c r="Q50">
@@ -8518,31 +8559,31 @@
         <v>0.3</v>
       </c>
       <c r="J59" s="11">
-        <f>(E59+F59+($K$102*H59+$M$102)*$L$102)/(1-G59)/(1-$O$102)/(1-I59)/$N$102</f>
+        <f>(E59+F59+($K$103*H59+$M$103)*$L$103)/(1-G59)/(1-$O$103)/(1-I59)/$N$103</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K59" s="12">
-        <f>(E59+F59+($K$102*H59+$M$102)*$L$102)/(1-G59)/(1-$P$102)/(1-I59)/$N$102</f>
+        <f>(E59+F59+($K$103*H59+$M$103)*$L$103)/(1-G59)/(1-$P$103)/(1-I59)/$N$103</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L59" s="1">
-        <f>E59+F59+($K$102*H59+$M$102)*$L$102</f>
+        <f>E59+F59+($K$103*H59+$M$103)*$L$103</f>
         <v>54.8</v>
       </c>
       <c r="M59" s="13">
-        <f>L59/(1-G59)/(1-$O$102)/$N$102</f>
+        <f>L59/(1-G59)/(1-$O$103)/$N$103</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N59" s="13">
-        <f>L59/(1-G59)/(1-$P$102)/$N$102</f>
+        <f>L59/(1-G59)/(1-$P$103)/$N$103</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O59" s="13">
-        <f>L59/(1-G59)/$N$102</f>
+        <f>L59/(1-G59)/$N$103</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P59" s="14">
-        <f>O59*$N$102-L59</f>
+        <f>O59*$N$103-L59</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q59">
@@ -8578,31 +8619,31 @@
         <v>0.3</v>
       </c>
       <c r="J60" s="11">
-        <f>(E60+F60+($K$102*H60+$M$102)*$L$102)/(1-G60)/(1-$O$102)/(1-I60)/$N$102</f>
+        <f>(E60+F60+($K$103*H60+$M$103)*$L$103)/(1-G60)/(1-$O$103)/(1-I60)/$N$103</f>
         <v>15.642126415783704</v>
       </c>
       <c r="K60" s="12">
-        <f>(E60+F60+($K$102*H60+$M$102)*$L$102)/(1-G60)/(1-$P$102)/(1-I60)/$N$102</f>
+        <f>(E60+F60+($K$103*H60+$M$103)*$L$103)/(1-G60)/(1-$P$103)/(1-I60)/$N$103</f>
         <v>16.930301532377655</v>
       </c>
       <c r="L60" s="1">
-        <f>E60+F60+($K$102*H60+$M$102)*$L$102</f>
+        <f>E60+F60+($K$103*H60+$M$103)*$L$103</f>
         <v>54.8</v>
       </c>
       <c r="M60" s="13">
-        <f>L60/(1-G60)/(1-$O$102)/$N$102</f>
+        <f>L60/(1-G60)/(1-$O$103)/$N$103</f>
         <v>10.949488491048593</v>
       </c>
       <c r="N60" s="13">
-        <f>L60/(1-G60)/(1-$P$102)/$N$102</f>
+        <f>L60/(1-G60)/(1-$P$103)/$N$103</f>
         <v>11.851211072664359</v>
       </c>
       <c r="O60" s="13">
-        <f>L60/(1-G60)/$N$102</f>
+        <f>L60/(1-G60)/$N$103</f>
         <v>10.073529411764705</v>
       </c>
       <c r="P60" s="14">
-        <f>O60*$N$102-L60</f>
+        <f>O60*$N$103-L60</f>
         <v>13.699999999999989</v>
       </c>
       <c r="Q60">
@@ -8638,31 +8679,31 @@
         <v>0.25</v>
       </c>
       <c r="J61" s="11">
-        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$102*H61+$M$102)*$L$102)/(1-G61)/(1-$O$102)/(1-I61)/$N$102</f>
+        <f t="shared" ref="J61:J66" si="14">(E61+F61+($K$103*H61+$M$103)*$L$103)/(1-G61)/(1-$O$103)/(1-I61)/$N$103</f>
         <v>11.309143222506394</v>
       </c>
       <c r="K61" s="12">
-        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$102*H61+$M$102)*$L$102)/(1-G61)/(1-$P$102)/(1-I61)/$N$102</f>
+        <f t="shared" ref="K61:K66" si="15">(E61+F61+($K$103*H61+$M$103)*$L$103)/(1-G61)/(1-$P$103)/(1-I61)/$N$103</f>
         <v>12.240484429065743</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$102*H61+$M$102)*$L$102</f>
+        <f t="shared" ref="L61:L66" si="16">E61+F61+($K$103*H61+$M$103)*$L$103</f>
         <v>42.45</v>
       </c>
       <c r="M61" s="13">
-        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M61:M66" si="17">L61/(1-G61)/(1-$O$103)/$N$103</f>
         <v>8.4818574168797962</v>
       </c>
       <c r="N61" s="13">
-        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N61:N66" si="18">L61/(1-G61)/(1-$P$103)/$N$103</f>
         <v>9.1803633217993088</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$102</f>
+        <f t="shared" ref="O61:O66" si="19">L61/(1-G61)/$N$103</f>
         <v>7.8033088235294121</v>
       </c>
       <c r="P61" s="14">
-        <f t="shared" ref="P61:P66" si="20">O61*$N$102-L61</f>
+        <f t="shared" ref="P61:P66" si="20">O61*$N$103-L61</f>
         <v>10.612499999999997</v>
       </c>
       <c r="Q61">
@@ -9005,31 +9046,31 @@
         <v>0.4</v>
       </c>
       <c r="J67" s="11">
-        <f>(E67+F67+($K$102*H67+$M$102)*$L$102)/(1-G67)/(1-$O$102)/(1-I67)/$N$102</f>
+        <f>(E67+F67+($K$103*H67+$M$103)*$L$103)/(1-G67)/(1-$O$103)/(1-I67)/$N$103</f>
         <v>10.461068485365161</v>
       </c>
       <c r="K67" s="12">
-        <f>(E67+F67+($K$102*H67+$M$102)*$L$102)/(1-G67)/(1-$P$102)/(1-I67)/$N$102</f>
+        <f>(E67+F67+($K$103*H67+$M$103)*$L$103)/(1-G67)/(1-$P$103)/(1-I67)/$N$103</f>
         <v>11.322568242983468</v>
       </c>
       <c r="L67" s="1">
-        <f>E67+F67+($K$102*H67+$M$102)*$L$102</f>
+        <f>E67+F67+($K$103*H67+$M$103)*$L$103</f>
         <v>29.45</v>
       </c>
       <c r="M67" s="13">
-        <f>L67/(1-G67)/(1-$O$102)/$N$102</f>
+        <f>L67/(1-G67)/(1-$O$103)/$N$103</f>
         <v>6.276641091219096</v>
       </c>
       <c r="N67" s="13">
-        <f>L67/(1-G67)/(1-$P$102)/$N$102</f>
+        <f>L67/(1-G67)/(1-$P$103)/$N$103</f>
         <v>6.7935409457900811</v>
       </c>
       <c r="O67" s="13">
-        <f>L67/(1-G67)/$N$102</f>
+        <f>L67/(1-G67)/$N$103</f>
         <v>5.7745098039215685</v>
       </c>
       <c r="P67" s="14">
-        <f>O67*$N$102-L67</f>
+        <f>O67*$N$103-L67</f>
         <v>9.8166666666666664</v>
       </c>
       <c r="Q67">
@@ -9066,31 +9107,31 @@
         <v>0.45</v>
       </c>
       <c r="J68" s="11">
-        <f>(E68+F68+($K$102*H68+$M$102)*$L$102)/(1-G68)/(1-$O$102)/(1-I68)/$N$102</f>
+        <f>(E68+F68+($K$103*H68+$M$103)*$L$103)/(1-G68)/(1-$O$103)/(1-I68)/$N$103</f>
         <v>13.795241416724791</v>
       </c>
       <c r="K68" s="12">
-        <f>(E68+F68+($K$102*H68+$M$102)*$L$102)/(1-G68)/(1-$P$102)/(1-I68)/$N$102</f>
+        <f>(E68+F68+($K$103*H68+$M$103)*$L$103)/(1-G68)/(1-$P$103)/(1-I68)/$N$103</f>
         <v>14.93132012163154</v>
       </c>
       <c r="L68" s="1">
-        <f>E68+F68+($K$102*H68+$M$102)*$L$102</f>
+        <f>E68+F68+($K$103*H68+$M$103)*$L$103</f>
         <v>35.6</v>
       </c>
       <c r="M68" s="13">
-        <f>L68/(1-G68)/(1-$O$102)/$N$102</f>
+        <f>L68/(1-G68)/(1-$O$103)/$N$103</f>
         <v>7.5873827791986361</v>
       </c>
       <c r="N68" s="13">
-        <f>L68/(1-G68)/(1-$P$102)/$N$102</f>
+        <f>L68/(1-G68)/(1-$P$103)/$N$103</f>
         <v>8.2122260668973475</v>
       </c>
       <c r="O68" s="13">
-        <f>L68/(1-G68)/$N$102</f>
+        <f>L68/(1-G68)/$N$103</f>
         <v>6.9803921568627452</v>
       </c>
       <c r="P68" s="14">
-        <f>O68*$N$102-L68</f>
+        <f>O68*$N$103-L68</f>
         <v>11.866666666666667</v>
       </c>
       <c r="Q68">
@@ -9127,31 +9168,31 @@
         <v>0.4</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$102*H69+$M$102)*$L$102)/(1-G69)/(1-$O$102)/(1-I69)/$N$102</f>
+        <f t="shared" ref="J69:J76" si="21">(E69+F69+($K$103*H69+$M$103)*$L$103)/(1-G69)/(1-$O$103)/(1-I69)/$N$103</f>
         <v>12.539073600454673</v>
       </c>
       <c r="K69" s="12">
-        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$102*H69+$M$102)*$L$102)/(1-G69)/(1-$P$102)/(1-I69)/$N$102</f>
+        <f t="shared" ref="K69:K76" si="22">(E69+F69+($K$103*H69+$M$103)*$L$103)/(1-G69)/(1-$P$103)/(1-I69)/$N$103</f>
         <v>13.571703191080355</v>
       </c>
       <c r="L69" s="1">
-        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$102*H69+$M$102)*$L$102</f>
+        <f t="shared" ref="L69:L76" si="23">E69+F69+($K$103*H69+$M$103)*$L$103</f>
         <v>35.299999999999997</v>
       </c>
       <c r="M69" s="13">
-        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M69:M76" si="24">L69/(1-G69)/(1-$O$103)/$N$103</f>
         <v>7.5234441602728035</v>
       </c>
       <c r="N69" s="13">
-        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N69:N76" si="25">L69/(1-G69)/(1-$P$103)/$N$103</f>
         <v>8.1430219146482123</v>
       </c>
       <c r="O69" s="13">
-        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$102</f>
+        <f t="shared" ref="O69:O76" si="26">L69/(1-G69)/$N$103</f>
         <v>6.9215686274509798</v>
       </c>
       <c r="P69" s="14">
-        <f t="shared" ref="P69:P76" si="27">O69*$N$102-L69</f>
+        <f t="shared" ref="P69:P76" si="27">O69*$N$103-L69</f>
         <v>11.766666666666666</v>
       </c>
       <c r="Q69">
@@ -9617,31 +9658,31 @@
         <v>0.25</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$102*H77+$M$102)*$L$102)/(1-G77)/(1-$O$102)/(1-I77)/$N$102</f>
+        <f t="shared" ref="J77:J90" si="28">(E77+F77+($K$103*H77+$M$103)*$L$103)/(1-G77)/(1-$O$103)/(1-I77)/$N$103</f>
         <v>87.995524296675171</v>
       </c>
       <c r="K77" s="12">
-        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$102*H77+$M$102)*$L$102)/(1-G77)/(1-$P$102)/(1-I77)/$N$102</f>
+        <f t="shared" ref="K77:K90" si="29">(E77+F77+($K$103*H77+$M$103)*$L$103)/(1-G77)/(1-$P$103)/(1-I77)/$N$103</f>
         <v>95.242214532871969</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$102*H77+$M$102)*$L$102</f>
+        <f t="shared" ref="L77:L90" si="30">E77+F77+($K$103*H77+$M$103)*$L$103</f>
         <v>330.29999999999995</v>
       </c>
       <c r="M77" s="13">
-        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M77:M90" si="31">L77/(1-G77)/(1-$O$103)/$N$103</f>
         <v>65.996643222506378</v>
       </c>
       <c r="N77" s="13">
-        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N77:N90" si="32">L77/(1-G77)/(1-$P$103)/$N$103</f>
         <v>71.431660899653977</v>
       </c>
       <c r="O77" s="13">
-        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$102</f>
+        <f t="shared" ref="O77:O90" si="33">L77/(1-G77)/$N$103</f>
         <v>60.716911764705877</v>
       </c>
       <c r="P77" s="14">
-        <f t="shared" ref="P77:P90" si="34">O77*$N$102-L77</f>
+        <f t="shared" ref="P77:P90" si="34">O77*$N$103-L77</f>
         <v>82.574999999999989</v>
       </c>
       <c r="Q77">
@@ -10471,31 +10512,31 @@
         <v>0.2</v>
       </c>
       <c r="J91" s="11">
-        <f t="shared" ref="J91" si="35">(E91+F91+($K$102*H91+$M$102)*$L$102)/(1-G91)/(1-$O$102)/(1-I91)/$N$102</f>
+        <f t="shared" ref="J91" si="35">(E91+F91+($K$103*H91+$M$103)*$L$103)/(1-G91)/(1-$O$103)/(1-I91)/$N$103</f>
         <v>6.9361983924004385</v>
       </c>
       <c r="K91" s="12">
-        <f t="shared" ref="K91" si="36">(E91+F91+($K$102*H91+$M$102)*$L$102)/(1-G91)/(1-$P$102)/(1-I91)/$N$102</f>
+        <f t="shared" ref="K91" si="36">(E91+F91+($K$103*H91+$M$103)*$L$103)/(1-G91)/(1-$P$103)/(1-I91)/$N$103</f>
         <v>7.5074147305981214</v>
       </c>
       <c r="L91" s="1">
-        <f t="shared" ref="L91" si="37">E91+F91+($K$102*H91+$M$102)*$L$102</f>
+        <f t="shared" ref="L91" si="37">E91+F91+($K$103*H91+$M$103)*$L$103</f>
         <v>24.299999999999997</v>
       </c>
       <c r="M91" s="13">
-        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M91" si="38">L91/(1-G91)/(1-$O$103)/$N$103</f>
         <v>5.5489587139203511</v>
       </c>
       <c r="N91" s="13">
-        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N91" si="39">L91/(1-G91)/(1-$P$103)/$N$103</f>
         <v>6.0059317844784976</v>
       </c>
       <c r="O91" s="13">
-        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$102</f>
+        <f t="shared" ref="O91" si="40">L91/(1-G91)/$N$103</f>
         <v>5.1050420168067232</v>
       </c>
       <c r="P91" s="14">
-        <f t="shared" ref="P91" si="41">O91*$N$102-L91</f>
+        <f t="shared" ref="P91" si="41">O91*$N$103-L91</f>
         <v>10.414285714285718</v>
       </c>
       <c r="Q91">
@@ -10532,31 +10573,31 @@
         <v>0.25</v>
       </c>
       <c r="J92" s="11">
-        <f t="shared" ref="J92" si="42">(E92+F92+($K$102*H92+$M$102)*$L$102)/(1-G92)/(1-$O$102)/(1-I92)/$N$102</f>
+        <f t="shared" ref="J92" si="42">(E92+F92+($K$103*H92+$M$103)*$L$103)/(1-G92)/(1-$O$103)/(1-I92)/$N$103</f>
         <v>24.239840863881785</v>
       </c>
       <c r="K92" s="12">
-        <f t="shared" ref="K92" si="43">(E92+F92+($K$102*H92+$M$102)*$L$102)/(1-G92)/(1-$P$102)/(1-I92)/$N$102</f>
+        <f t="shared" ref="K92" si="43">(E92+F92+($K$103*H92+$M$103)*$L$103)/(1-G92)/(1-$P$103)/(1-I92)/$N$103</f>
         <v>26.236063052672051</v>
       </c>
       <c r="L92" s="1">
-        <f t="shared" ref="L92" si="44">E92+F92+($K$102*H92+$M$102)*$L$102</f>
+        <f t="shared" ref="L92" si="44">E92+F92+($K$103*H92+$M$103)*$L$103</f>
         <v>85.3</v>
       </c>
       <c r="M92" s="13">
-        <f t="shared" ref="M92" si="45">L92/(1-G92)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M92" si="45">L92/(1-G92)/(1-$O$103)/$N$103</f>
         <v>18.17988064791134</v>
       </c>
       <c r="N92" s="13">
-        <f t="shared" ref="N92" si="46">L92/(1-G92)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N92" si="46">L92/(1-G92)/(1-$P$103)/$N$103</f>
         <v>19.677047289504038</v>
       </c>
       <c r="O92" s="13">
-        <f t="shared" ref="O92" si="47">L92/(1-G92)/$N$102</f>
+        <f t="shared" ref="O92" si="47">L92/(1-G92)/$N$103</f>
         <v>16.725490196078432</v>
       </c>
       <c r="P92" s="14">
-        <f t="shared" ref="P92" si="48">O92*$N$102-L92</f>
+        <f t="shared" ref="P92" si="48">O92*$N$103-L92</f>
         <v>28.433333333333337</v>
       </c>
       <c r="Q92">
@@ -10598,31 +10639,31 @@
         <v>0.3</v>
       </c>
       <c r="J93" s="11">
-        <f t="shared" ref="J93" si="49">(E93+F93+($K$102*H93+$M$102)*$L$102)/(1-G93)/(1-$O$102)/(1-I93)/$N$102</f>
+        <f t="shared" ref="J93" si="49">(E93+F93+($K$103*H93+$M$103)*$L$103)/(1-G93)/(1-$O$103)/(1-I93)/$N$103</f>
         <v>11.356716599683351</v>
       </c>
       <c r="K93" s="12">
-        <f t="shared" ref="K93" si="50">(E93+F93+($K$102*H93+$M$102)*$L$102)/(1-G93)/(1-$P$102)/(1-I93)/$N$102</f>
+        <f t="shared" ref="K93" si="50">(E93+F93+($K$103*H93+$M$103)*$L$103)/(1-G93)/(1-$P$103)/(1-I93)/$N$103</f>
         <v>12.29197561377492</v>
       </c>
       <c r="L93" s="1">
-        <f t="shared" ref="L93" si="51">E93+F93+($K$102*H93+$M$102)*$L$102</f>
+        <f t="shared" ref="L93" si="51">E93+F93+($K$103*H93+$M$103)*$L$103</f>
         <v>37.299999999999997</v>
       </c>
       <c r="M93" s="13">
-        <f t="shared" ref="M93" si="52">L93/(1-G93)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M93" si="52">L93/(1-G93)/(1-$O$103)/$N$103</f>
         <v>7.9497016197783452</v>
       </c>
       <c r="N93" s="13">
-        <f t="shared" ref="N93" si="53">L93/(1-G93)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N93" si="53">L93/(1-G93)/(1-$P$103)/$N$103</f>
         <v>8.6043829296424441</v>
       </c>
       <c r="O93" s="13">
-        <f t="shared" ref="O93" si="54">L93/(1-G93)/$N$102</f>
+        <f t="shared" ref="O93" si="54">L93/(1-G93)/$N$103</f>
         <v>7.3137254901960773</v>
       </c>
       <c r="P93" s="14">
-        <f t="shared" ref="P93" si="55">O93*$N$102-L93</f>
+        <f t="shared" ref="P93" si="55">O93*$N$103-L93</f>
         <v>12.43333333333333</v>
       </c>
       <c r="Q93">
@@ -10660,31 +10701,31 @@
         <v>0.4</v>
       </c>
       <c r="J94" s="11">
-        <f t="shared" ref="J94" si="56">(E94+F94+($K$102*H94+$M$102)*$L$102)/(1-G94)/(1-$O$102)/(1-I94)/$N$102</f>
+        <f t="shared" ref="J94" si="56">(E94+F94+($K$103*H94+$M$103)*$L$103)/(1-G94)/(1-$O$103)/(1-I94)/$N$103</f>
         <v>20.74674978687127</v>
       </c>
       <c r="K94" s="12">
-        <f t="shared" ref="K94" si="57">(E94+F94+($K$102*H94+$M$102)*$L$102)/(1-G94)/(1-$P$102)/(1-I94)/$N$102</f>
+        <f t="shared" ref="K94" si="57">(E94+F94+($K$103*H94+$M$103)*$L$103)/(1-G94)/(1-$P$103)/(1-I94)/$N$103</f>
         <v>22.455305651672433</v>
       </c>
       <c r="L94" s="1">
-        <f t="shared" ref="L94" si="58">E94+F94+($K$102*H94+$M$102)*$L$102</f>
+        <f t="shared" ref="L94" si="58">E94+F94+($K$103*H94+$M$103)*$L$103</f>
         <v>62.3</v>
       </c>
       <c r="M94" s="13">
-        <f t="shared" ref="M94" si="59">L94/(1-G94)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M94" si="59">L94/(1-G94)/(1-$O$103)/$N$103</f>
         <v>12.448049872122761</v>
       </c>
       <c r="N94" s="13">
-        <f t="shared" ref="N94" si="60">L94/(1-G94)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N94" si="60">L94/(1-G94)/(1-$P$103)/$N$103</f>
         <v>13.47318339100346</v>
       </c>
       <c r="O94" s="13">
-        <f t="shared" ref="O94" si="61">L94/(1-G94)/$N$102</f>
+        <f t="shared" ref="O94" si="61">L94/(1-G94)/$N$103</f>
         <v>11.45220588235294</v>
       </c>
       <c r="P94" s="14">
-        <f t="shared" ref="P94" si="62">O94*$N$102-L94</f>
+        <f t="shared" ref="P94" si="62">O94*$N$103-L94</f>
         <v>15.574999999999989</v>
       </c>
       <c r="Q94">
@@ -10722,31 +10763,31 @@
         <v>0.25</v>
       </c>
       <c r="J95" s="11">
-        <f t="shared" ref="J95" si="63">(E95+F95+($K$102*H95+$M$102)*$L$102)/(1-G95)/(1-$O$102)/(1-I95)/$N$102</f>
+        <f t="shared" ref="J95" si="63">(E95+F95+($K$103*H95+$M$103)*$L$103)/(1-G95)/(1-$O$103)/(1-I95)/$N$103</f>
         <v>17.988064791133844</v>
       </c>
       <c r="K95" s="12">
-        <f t="shared" ref="K95" si="64">(E95+F95+($K$102*H95+$M$102)*$L$102)/(1-G95)/(1-$P$102)/(1-I95)/$N$102</f>
+        <f t="shared" ref="K95" si="64">(E95+F95+($K$103*H95+$M$103)*$L$103)/(1-G95)/(1-$P$103)/(1-I95)/$N$103</f>
         <v>19.46943483275663</v>
       </c>
       <c r="L95" s="1">
-        <f t="shared" ref="L95" si="65">E95+F95+($K$102*H95+$M$102)*$L$102</f>
+        <f t="shared" ref="L95" si="65">E95+F95+($K$103*H95+$M$103)*$L$103</f>
         <v>63.3</v>
       </c>
       <c r="M95" s="13">
-        <f t="shared" ref="M95" si="66">L95/(1-G95)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M95" si="66">L95/(1-G95)/(1-$O$103)/$N$103</f>
         <v>13.491048593350381</v>
       </c>
       <c r="N95" s="13">
-        <f t="shared" ref="N95" si="67">L95/(1-G95)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N95" si="67">L95/(1-G95)/(1-$P$103)/$N$103</f>
         <v>14.602076124567473</v>
       </c>
       <c r="O95" s="13">
-        <f t="shared" ref="O95" si="68">L95/(1-G95)/$N$102</f>
+        <f t="shared" ref="O95" si="68">L95/(1-G95)/$N$103</f>
         <v>12.411764705882351</v>
       </c>
       <c r="P95" s="14">
-        <f t="shared" ref="P95" si="69">O95*$N$102-L95</f>
+        <f t="shared" ref="P95" si="69">O95*$N$103-L95</f>
         <v>21.099999999999994</v>
       </c>
       <c r="R95">
@@ -10781,31 +10822,31 @@
         <v>0.25</v>
       </c>
       <c r="J96" s="11">
-        <f t="shared" ref="J96" si="70">(E96+F96+($K$102*H96+$M$102)*$L$102)/(1-G96)/(1-$O$102)/(1-I96)/$N$102</f>
+        <f t="shared" ref="J96" si="70">(E96+F96+($K$103*H96+$M$103)*$L$103)/(1-G96)/(1-$O$103)/(1-I96)/$N$103</f>
         <v>12.201619778346119</v>
       </c>
       <c r="K96" s="12">
-        <f t="shared" ref="K96" si="71">(E96+F96+($K$102*H96+$M$102)*$L$102)/(1-G96)/(1-$P$102)/(1-I96)/$N$102</f>
+        <f t="shared" ref="K96" si="71">(E96+F96+($K$103*H96+$M$103)*$L$103)/(1-G96)/(1-$P$103)/(1-I96)/$N$103</f>
         <v>13.206459054209919</v>
       </c>
       <c r="L96" s="1">
-        <f t="shared" ref="L96" si="72">E96+F96+($K$102*H96+$M$102)*$L$102</f>
+        <f t="shared" ref="L96" si="72">E96+F96+($K$103*H96+$M$103)*$L$103</f>
         <v>45.8</v>
       </c>
       <c r="M96" s="13">
-        <f t="shared" ref="M96" si="73">L96/(1-G96)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M96" si="73">L96/(1-G96)/(1-$O$103)/$N$103</f>
         <v>9.1512148337595889</v>
       </c>
       <c r="N96" s="13">
-        <f t="shared" ref="N96" si="74">L96/(1-G96)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N96" si="74">L96/(1-G96)/(1-$P$103)/$N$103</f>
         <v>9.9048442906574383</v>
       </c>
       <c r="O96" s="13">
-        <f t="shared" ref="O96" si="75">L96/(1-G96)/$N$102</f>
+        <f t="shared" ref="O96" si="75">L96/(1-G96)/$N$103</f>
         <v>8.4191176470588225</v>
       </c>
       <c r="P96" s="14">
-        <f t="shared" ref="P96" si="76">O96*$N$102-L96</f>
+        <f t="shared" ref="P96" si="76">O96*$N$103-L96</f>
         <v>11.449999999999996</v>
       </c>
       <c r="R96">
@@ -10840,31 +10881,31 @@
         <v>0.3</v>
       </c>
       <c r="J97" s="11">
-        <f t="shared" ref="J97" si="77">(E97+F97+($K$102*H97+$M$102)*$L$102)/(1-G97)/(1-$O$102)/(1-I97)/$N$102</f>
+        <f t="shared" ref="J97" si="77">(E97+F97+($K$103*H97+$M$103)*$L$103)/(1-G97)/(1-$O$103)/(1-I97)/$N$103</f>
         <v>14.802596230307978</v>
       </c>
       <c r="K97" s="12">
-        <f t="shared" ref="K97" si="78">(E97+F97+($K$102*H97+$M$102)*$L$102)/(1-G97)/(1-$P$102)/(1-I97)/$N$102</f>
+        <f t="shared" ref="K97" si="78">(E97+F97+($K$103*H97+$M$103)*$L$103)/(1-G97)/(1-$P$103)/(1-I97)/$N$103</f>
         <v>16.021633566921576</v>
       </c>
       <c r="L97" s="1">
-        <f t="shared" ref="L97" si="79">E97+F97+($K$102*H97+$M$102)*$L$102</f>
+        <f t="shared" ref="L97" si="79">E97+F97+($K$103*H97+$M$103)*$L$103</f>
         <v>55.099999999999994</v>
       </c>
       <c r="M97" s="13">
-        <f t="shared" ref="M97" si="80">L97/(1-G97)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M97" si="80">L97/(1-G97)/(1-$O$103)/$N$103</f>
         <v>10.361817361215584</v>
       </c>
       <c r="N97" s="13">
-        <f t="shared" ref="N97" si="81">L97/(1-G97)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N97" si="81">L97/(1-G97)/(1-$P$103)/$N$103</f>
         <v>11.215143496845103</v>
       </c>
       <c r="O97" s="13">
-        <f t="shared" ref="O97" si="82">L97/(1-G97)/$N$102</f>
+        <f t="shared" ref="O97" si="82">L97/(1-G97)/$N$103</f>
         <v>9.5328719723183379</v>
       </c>
       <c r="P97" s="14">
-        <f t="shared" ref="P97" si="83">O97*$N$102-L97</f>
+        <f t="shared" ref="P97" si="83">O97*$N$103-L97</f>
         <v>9.7235294117647015</v>
       </c>
       <c r="Q97">
@@ -10902,31 +10943,31 @@
         <v>0.4</v>
       </c>
       <c r="J98" s="11">
-        <f t="shared" ref="J98" si="84">(E98+F98+($K$102*H98+$M$102)*$L$102)/(1-G98)/(1-$O$102)/(1-I98)/$N$102</f>
+        <f t="shared" ref="J98" si="84">(E98+F98+($K$103*H98+$M$103)*$L$103)/(1-G98)/(1-$O$103)/(1-I98)/$N$103</f>
         <v>13.503703111679453</v>
       </c>
       <c r="K98" s="12">
-        <f t="shared" ref="K98" si="85">(E98+F98+($K$102*H98+$M$102)*$L$102)/(1-G98)/(1-$P$102)/(1-I98)/$N$102</f>
+        <f t="shared" ref="K98" si="85">(E98+F98+($K$103*H98+$M$103)*$L$103)/(1-G98)/(1-$P$103)/(1-I98)/$N$103</f>
         <v>14.615772779700114</v>
       </c>
       <c r="L98" s="1">
-        <f t="shared" ref="L98" si="86">E98+F98+($K$102*H98+$M$102)*$L$102</f>
+        <f t="shared" ref="L98" si="86">E98+F98+($K$103*H98+$M$103)*$L$103</f>
         <v>40.549999999999997</v>
       </c>
       <c r="M98" s="13">
-        <f t="shared" ref="M98" si="87">L98/(1-G98)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M98" si="87">L98/(1-G98)/(1-$O$103)/$N$103</f>
         <v>8.1022218670076711</v>
       </c>
       <c r="N98" s="13">
-        <f t="shared" ref="N98" si="88">L98/(1-G98)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N98" si="88">L98/(1-G98)/(1-$P$103)/$N$103</f>
         <v>8.7694636678200677</v>
       </c>
       <c r="O98" s="13">
-        <f t="shared" ref="O98" si="89">L98/(1-G98)/$N$102</f>
+        <f t="shared" ref="O98" si="89">L98/(1-G98)/$N$103</f>
         <v>7.454044117647058</v>
       </c>
       <c r="P98" s="14">
-        <f t="shared" ref="P98" si="90">O98*$N$102-L98</f>
+        <f t="shared" ref="P98" si="90">O98*$N$103-L98</f>
         <v>10.137499999999996</v>
       </c>
       <c r="Q98">
@@ -10964,31 +11005,31 @@
         <v>0.4</v>
       </c>
       <c r="J99" s="11">
-        <f t="shared" ref="J99" si="91">(E99+F99+($K$102*H99+$M$102)*$L$102)/(1-G99)/(1-$O$102)/(1-I99)/$N$102</f>
+        <f t="shared" ref="J99" si="91">(E99+F99+($K$103*H99+$M$103)*$L$103)/(1-G99)/(1-$O$103)/(1-I99)/$N$103</f>
         <v>18.58216112531969</v>
       </c>
       <c r="K99" s="12">
-        <f t="shared" ref="K99" si="92">(E99+F99+($K$102*H99+$M$102)*$L$102)/(1-G99)/(1-$P$102)/(1-I99)/$N$102</f>
+        <f t="shared" ref="K99" si="92">(E99+F99+($K$103*H99+$M$103)*$L$103)/(1-G99)/(1-$P$103)/(1-I99)/$N$103</f>
         <v>20.112456747404842</v>
       </c>
       <c r="L99" s="1">
-        <f t="shared" ref="L99" si="93">E99+F99+($K$102*H99+$M$102)*$L$102</f>
+        <f t="shared" ref="L99" si="93">E99+F99+($K$103*H99+$M$103)*$L$103</f>
         <v>55.8</v>
       </c>
       <c r="M99" s="13">
-        <f t="shared" ref="M99" si="94">L99/(1-G99)/(1-$O$102)/$N$102</f>
+        <f t="shared" ref="M99" si="94">L99/(1-G99)/(1-$O$103)/$N$103</f>
         <v>11.149296675191813</v>
       </c>
       <c r="N99" s="13">
-        <f t="shared" ref="N99" si="95">L99/(1-G99)/(1-$P$102)/$N$102</f>
+        <f t="shared" ref="N99" si="95">L99/(1-G99)/(1-$P$103)/$N$103</f>
         <v>12.067474048442905</v>
       </c>
       <c r="O99" s="13">
-        <f t="shared" ref="O99" si="96">L99/(1-G99)/$N$102</f>
+        <f t="shared" ref="O99" si="96">L99/(1-G99)/$N$103</f>
         <v>10.257352941176469</v>
       </c>
       <c r="P99" s="14">
-        <f t="shared" ref="P99" si="97">O99*$N$102-L99</f>
+        <f t="shared" ref="P99" si="97">O99*$N$103-L99</f>
         <v>13.949999999999989</v>
       </c>
       <c r="Q99">
@@ -11000,52 +11041,114 @@
       <c r="S99" s="19"/>
       <c r="T99" s="20"/>
     </row>
-    <row r="100" spans="2:20">
-      <c r="G100" s="15"/>
-      <c r="I100" s="15"/>
-      <c r="J100" s="11"/>
-      <c r="L100" s="1"/>
-      <c r="M100" s="13"/>
-      <c r="O100" s="13"/>
-      <c r="P100" s="14"/>
+    <row r="100" spans="2:20" ht="90.75" customHeight="1">
+      <c r="B100">
+        <v>17030102</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E100">
+        <v>32</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+      <c r="G100" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H100">
+        <v>0.3</v>
+      </c>
+      <c r="I100" s="15">
+        <v>0.26</v>
+      </c>
+      <c r="J100" s="11">
+        <f t="shared" ref="J100" si="98">(E100+F100+($K$103*H100+$M$103)*$L$103)/(1-G100)/(1-$O$103)/(1-I100)/$N$103</f>
+        <v>17.631722195341119</v>
+      </c>
+      <c r="K100" s="12">
+        <f t="shared" ref="K100" si="99">(E100+F100+($K$103*H100+$M$103)*$L$103)/(1-G100)/(1-$P$103)/(1-I100)/$N$103</f>
+        <v>19.083746376133917</v>
+      </c>
+      <c r="L100" s="1">
+        <f t="shared" ref="L100" si="100">E100+F100+($K$103*H100+$M$103)*$L$103</f>
+        <v>65.3</v>
+      </c>
+      <c r="M100" s="13">
+        <f t="shared" ref="M100" si="101">L100/(1-G100)/(1-$O$103)/$N$103</f>
+        <v>13.047474424552426</v>
+      </c>
+      <c r="N100" s="13">
+        <f t="shared" ref="N100" si="102">L100/(1-G100)/(1-$P$103)/$N$103</f>
+        <v>14.121972318339099</v>
+      </c>
+      <c r="O100" s="13">
+        <f t="shared" ref="O100" si="103">L100/(1-G100)/$N$103</f>
+        <v>12.003676470588234</v>
+      </c>
+      <c r="P100" s="14">
+        <f t="shared" ref="P100" si="104">O100*$N$103-L100</f>
+        <v>16.324999999999989</v>
+      </c>
+      <c r="Q100">
+        <v>40</v>
+      </c>
+      <c r="R100">
+        <v>25</v>
+      </c>
+      <c r="S100" s="19"/>
+      <c r="T100" s="20"/>
     </row>
     <row r="101" spans="2:20">
-      <c r="K101" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="L101" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="M101" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="N101" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="P101" s="17" t="s">
-        <v>121</v>
-      </c>
+      <c r="G101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="11"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="13"/>
+      <c r="O101" s="13"/>
+      <c r="P101" s="14"/>
     </row>
     <row r="102" spans="2:20">
-      <c r="K102" s="18">
+      <c r="K102" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="L102" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="M102" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="P102" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="103" spans="2:20">
+      <c r="K103" s="18">
         <v>100</v>
       </c>
-      <c r="L102" s="15">
+      <c r="L103" s="15">
         <v>0.85</v>
       </c>
-      <c r="M102">
+      <c r="M103">
         <v>8</v>
       </c>
-      <c r="N102">
+      <c r="N103">
         <v>6.8</v>
       </c>
-      <c r="O102" s="15">
+      <c r="O103" s="15">
         <v>0.08</v>
       </c>
-      <c r="P102" s="15">
+      <c r="P103" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -11055,7 +11158,7 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>"爬爬服"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C99">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C100">
       <formula1>"爬爬服,婴儿套装,连衣裙,套装,外套,鞋子,裤子,衬衫,T-shirt,袜子,口水巾,手套,婴儿用品"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q6 R2:R4">

</xml_diff>